<commit_message>
add information to report
add my name, email and github user name to the report file
</commit_message>
<xml_diff>
--- a/Team05Report.xlsx
+++ b/Team05Report.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="240" windowWidth="20730" windowHeight="11760" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="240" yWindow="240" windowWidth="20730" windowHeight="11760" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Team" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
     <sheet name="Sprint4" sheetId="6" r:id="rId9"/>
     <sheet name="Sprint5" sheetId="8" r:id="rId10"/>
   </sheets>
-  <calcPr calcId="124519" concurrentCalc="0"/>
+  <calcPr calcId="125725" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="282" uniqueCount="186">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="282" uniqueCount="187">
   <si>
     <t>Find marriage date</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -170,14 +170,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>Mills</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Harlan</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>Turing</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -186,10 +178,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>hmills@stevens.edu</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>hm</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -419,9 +407,6 @@
     <t>GitHub Username</t>
   </si>
   <si>
-    <t>harlanmills</t>
-  </si>
-  <si>
     <t>enigmacracker</t>
   </si>
   <si>
@@ -654,6 +639,21 @@
   </si>
   <si>
     <t>Family rule</t>
+  </si>
+  <si>
+    <t>gc</t>
+  </si>
+  <si>
+    <t>Gong</t>
+  </si>
+  <si>
+    <t>Cheng</t>
+  </si>
+  <si>
+    <t>gcheng2@stevens.edu</t>
+  </si>
+  <si>
+    <t>chenggongtc</t>
   </si>
 </sst>
 </file>
@@ -792,56 +792,56 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="49"/>
   </cellXfs>
   <cellStyles count="50">
-    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="30" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="32" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="34" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="36" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="38" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="40" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="44" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="46" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="48" builtinId="9" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="29" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="31" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="33" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="35" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="37" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="39" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="41" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="43" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="45" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="47" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="49" builtinId="8"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="已访问的超链接" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="20" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="22" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="24" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="26" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="28" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="30" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="32" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="34" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="36" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="38" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="40" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="42" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="44" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="46" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="48" builtinId="9" hidden="1"/>
+    <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle name="超链接" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="15" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="17" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="19" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="21" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="23" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="25" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="27" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="29" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="31" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="33" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="35" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="37" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="39" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="41" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="43" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="45" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="47" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="49" builtinId="8"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
@@ -921,25 +921,25 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="69126784"/>
-        <c:axId val="69128576"/>
+        <c:axId val="306886528"/>
+        <c:axId val="306888064"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="69126784"/>
+        <c:axId val="306886528"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="m/d" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="69128576"/>
+        <c:crossAx val="306888064"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
         <c:baseTimeUnit val="days"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="69128576"/>
+        <c:axId val="306888064"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -947,7 +947,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="69126784"/>
+        <c:crossAx val="306886528"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -957,7 +957,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="1" l="0.75000000000000022" r="0.75000000000000022" t="1" header="0.5" footer="0.5"/>
+    <c:pageMargins b="1" l="0.75000000000000033" r="0.75000000000000033" t="1" header="0.5" footer="0.5"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1320,8 +1320,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E9"/>
   <sheetViews>
-    <sheetView zoomScale="150" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+    <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75"/>
@@ -1346,66 +1346,66 @@
         <v>29</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
     </row>
     <row r="3" spans="1:5">
       <c r="A3" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="B3" t="s">
+        <v>106</v>
+      </c>
+      <c r="C3" t="s">
+        <v>107</v>
+      </c>
+      <c r="D3" s="14" t="s">
+        <v>109</v>
+      </c>
+      <c r="E3" t="s">
         <v>110</v>
-      </c>
-      <c r="C3" t="s">
-        <v>111</v>
-      </c>
-      <c r="D3" s="14" t="s">
-        <v>113</v>
-      </c>
-      <c r="E3" t="s">
-        <v>114</v>
       </c>
     </row>
     <row r="4" spans="1:5">
       <c r="A4" t="s">
-        <v>40</v>
+        <v>182</v>
       </c>
       <c r="B4" t="s">
-        <v>36</v>
+        <v>183</v>
       </c>
       <c r="C4" t="s">
-        <v>35</v>
-      </c>
-      <c r="D4" t="s">
-        <v>39</v>
+        <v>184</v>
+      </c>
+      <c r="D4" s="14" t="s">
+        <v>185</v>
       </c>
       <c r="E4" t="s">
-        <v>107</v>
+        <v>186</v>
       </c>
     </row>
     <row r="5" spans="1:5">
       <c r="A5" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="B5" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C5" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="D5" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="E5" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
     </row>
     <row r="9" spans="1:5">
       <c r="D9" s="4" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="E9" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
     </row>
   </sheetData>
@@ -1415,6 +1415,7 @@
   <phoneticPr fontId="2" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="D3" r:id="rId1"/>
+    <hyperlink ref="D4" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -1444,7 +1445,7 @@
         <v>8</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="D1" s="4" t="s">
         <v>9</v>
@@ -1505,34 +1506,34 @@
   <sheetData>
     <row r="1" spans="1:12" s="4" customFormat="1">
       <c r="A1" s="4" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="C1" s="4" t="s">
         <v>24</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="G1" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="H1" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="I1" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="J1" s="10" t="s">
         <v>53</v>
-      </c>
-      <c r="H1" s="10" t="s">
-        <v>55</v>
-      </c>
-      <c r="I1" s="10" t="s">
-        <v>54</v>
-      </c>
-      <c r="J1" s="10" t="s">
-        <v>56</v>
       </c>
       <c r="K1" s="11" t="s">
         <v>14</v>
@@ -1546,16 +1547,16 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="C2" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="D2" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="F2" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="G2">
         <v>150</v>
@@ -1581,13 +1582,13 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="C3" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="D3" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="G3">
         <v>200</v>
@@ -1604,13 +1605,13 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="C4" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="D4" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="L4" s="7">
         <v>40460</v>
@@ -1618,112 +1619,112 @@
     </row>
     <row r="5" spans="1:12">
       <c r="B5" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
     </row>
     <row r="6" spans="1:12">
       <c r="B6" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
     </row>
     <row r="7" spans="1:12">
       <c r="B7" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
     </row>
     <row r="8" spans="1:12">
       <c r="B8" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
     </row>
     <row r="9" spans="1:12">
       <c r="B9" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
     </row>
     <row r="10" spans="1:12">
       <c r="B10" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
     </row>
     <row r="11" spans="1:12">
       <c r="B11" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
     </row>
     <row r="12" spans="1:12">
       <c r="B12" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
     </row>
     <row r="13" spans="1:12">
       <c r="B13" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
     </row>
     <row r="14" spans="1:12">
       <c r="B14" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
     </row>
     <row r="15" spans="1:12">
       <c r="B15" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
     </row>
     <row r="16" spans="1:12">
       <c r="B16" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
     </row>
     <row r="17" spans="2:2">
       <c r="B17" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
     </row>
     <row r="18" spans="2:2">
       <c r="B18" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
     </row>
     <row r="19" spans="2:2">
       <c r="B19" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
     </row>
     <row r="20" spans="2:2">
       <c r="B20" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
     </row>
     <row r="21" spans="2:2">
       <c r="B21" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
     </row>
     <row r="22" spans="2:2">
       <c r="B22" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
     </row>
     <row r="23" spans="2:2">
       <c r="B23" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
     </row>
     <row r="24" spans="2:2">
       <c r="B24" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
     </row>
     <row r="25" spans="2:2">
       <c r="B25" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
     </row>
     <row r="26" spans="2:2">
       <c r="B26" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
     </row>
   </sheetData>
@@ -1742,7 +1743,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+    <sheetView topLeftCell="A2" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
       <selection activeCell="C7" sqref="C7:D8"/>
     </sheetView>
   </sheetViews>
@@ -1757,307 +1758,307 @@
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" s="4" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="B1" s="4" t="s">
         <v>24</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="E1" s="10" t="s">
         <v>11</v>
       </c>
       <c r="F1" s="10" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
     </row>
     <row r="2" spans="1:6">
       <c r="A2" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="B2" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="25.5">
       <c r="A3" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="B3" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
     </row>
     <row r="4" spans="1:6">
       <c r="A4" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="B4" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
     </row>
     <row r="5" spans="1:6">
       <c r="A5" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="B5" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
     </row>
     <row r="6" spans="1:6">
       <c r="A6" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="B6" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
     </row>
     <row r="7" spans="1:6">
       <c r="A7" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="B7" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
     </row>
     <row r="8" spans="1:6">
       <c r="A8" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="B8" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
     </row>
     <row r="9" spans="1:6">
       <c r="A9" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="B9" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
     </row>
     <row r="10" spans="1:6">
       <c r="A10" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="B10" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
     </row>
     <row r="11" spans="1:6">
       <c r="A11" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="B11" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="25.5">
       <c r="A12" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="B12" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="25.5">
       <c r="A13" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="B13" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
     </row>
     <row r="14" spans="1:6">
       <c r="A14" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="B14" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
     </row>
     <row r="15" spans="1:6">
       <c r="A15" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="B15" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
     </row>
     <row r="16" spans="1:6">
       <c r="A16" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="B16" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
     </row>
     <row r="17" spans="1:3">
       <c r="A17" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="B17" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
     </row>
     <row r="18" spans="1:3">
       <c r="A18" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="B18" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
     </row>
     <row r="19" spans="1:3">
       <c r="A19" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="B19" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
     </row>
     <row r="20" spans="1:3">
       <c r="A20" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="B20" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
     </row>
     <row r="21" spans="1:3">
       <c r="A21" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="B21" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
     </row>
     <row r="22" spans="1:3">
       <c r="A22" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="B22" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
     </row>
     <row r="23" spans="1:3" ht="25.5">
       <c r="A23" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="B23" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
     </row>
     <row r="24" spans="1:3">
       <c r="A24" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="B24" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
     </row>
     <row r="25" spans="1:3">
       <c r="A25" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="B25" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
     </row>
     <row r="26" spans="1:3">
       <c r="A26" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="B26" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
     </row>
     <row r="27" spans="1:3">
       <c r="A27" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
     </row>
     <row r="28" spans="1:3">
       <c r="A28" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
     </row>
   </sheetData>
@@ -2091,142 +2092,142 @@
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" s="4" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="C1" s="4" t="s">
         <v>24</v>
       </c>
       <c r="D1" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="F1" s="4" t="s">
         <v>73</v>
-      </c>
-      <c r="E1" s="5" t="s">
-        <v>74</v>
-      </c>
-      <c r="F1" s="4" t="s">
-        <v>76</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="63">
       <c r="A2" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="B2" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="C2" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="D2" s="13" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="E2" s="13" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="F2" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="31.5">
       <c r="A3" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="B3" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="C3" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="D3" s="13" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="E3" s="12" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="F3" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="63">
       <c r="A4" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="B4" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="C4" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="D4" s="13" t="s">
+        <v>76</v>
+      </c>
+      <c r="E4" s="13" t="s">
+        <v>78</v>
+      </c>
+      <c r="F4" t="s">
         <v>79</v>
-      </c>
-      <c r="E4" s="13" t="s">
-        <v>81</v>
-      </c>
-      <c r="F4" t="s">
-        <v>82</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="47.25">
       <c r="A5" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="B5" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="C5" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="D5" s="13" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="E5" s="12" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="F5" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="63">
       <c r="A6" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="B6" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="C6" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="D6" s="13" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="E6" s="13" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="F6" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="47.25">
       <c r="A7" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="B7" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="C7" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="D7" s="13" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="E7" s="12" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="F7" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
     </row>
   </sheetData>
@@ -2442,7 +2443,7 @@
         <v>16</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="D1" s="4" t="s">
         <v>17</v>
@@ -2468,19 +2469,19 @@
     </row>
     <row r="2" spans="1:10">
       <c r="A2" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="D2" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="E2" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="F2">
         <v>150</v>
@@ -2500,52 +2501,52 @@
     </row>
     <row r="4" spans="1:10">
       <c r="A4" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="D4" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="5" spans="1:10">
       <c r="A5" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="D5" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="6" spans="1:10">
       <c r="A6" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="D6" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="8" spans="1:10">
       <c r="A8" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="D8" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="E8" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="F8">
         <v>200</v>
@@ -2556,10 +2557,10 @@
     </row>
     <row r="10" spans="1:10">
       <c r="A10" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="D10" t="s">
         <v>33</v>
@@ -2570,13 +2571,13 @@
     </row>
     <row r="11" spans="1:10">
       <c r="A11" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>0</v>
       </c>
       <c r="D11" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
     </row>
     <row r="12" spans="1:10">
@@ -2592,7 +2593,7 @@
     </row>
     <row r="14" spans="1:10">
       <c r="B14" s="5" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
     </row>
     <row r="15" spans="1:10">
@@ -2601,27 +2602,27 @@
     </row>
     <row r="16" spans="1:10">
       <c r="B16" s="5" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
     </row>
     <row r="17" spans="2:2">
       <c r="B17" s="1" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
     </row>
     <row r="18" spans="2:2">
       <c r="B18" s="1" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
     </row>
     <row r="20" spans="2:2">
       <c r="B20" s="5" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
     </row>
     <row r="21" spans="2:2">
       <c r="B21" s="1" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
     </row>
   </sheetData>
@@ -2654,7 +2655,7 @@
         <v>16</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="D1" s="4" t="s">
         <v>17</v>
@@ -2708,7 +2709,7 @@
         <v>8</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="D1" s="4" t="s">
         <v>9</v>
@@ -2761,7 +2762,7 @@
         <v>8</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="D1" s="4" t="s">
         <v>9</v>

</xml_diff>

<commit_message>
Complete two user stories
User stories 1 and 2 and the tests of them are completed.
</commit_message>
<xml_diff>
--- a/Team05Report.xlsx
+++ b/Team05Report.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="240" windowWidth="20730" windowHeight="11760" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="240" yWindow="240" windowWidth="20730" windowHeight="11760" tabRatio="500" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Team" sheetId="1" r:id="rId1"/>
@@ -28,17 +28,149 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="275" uniqueCount="179">
-  <si>
-    <t>Find marriage date</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>T02.03</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Compare marriage date to birth date</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="324" uniqueCount="195">
+  <si>
+    <t>Date</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Remaining Stories</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Story Velocity</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Story ID</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Story Name</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Owner</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Status</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Est Size</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Act Size</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Act Time</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Completed</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Story ID</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Story Name</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Owner</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Status</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Est Size</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Est Time</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Act Size</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Act Time</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Completed</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Story Name</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Added</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Initials</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Last</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>First</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Email</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>LOC</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Min</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>at</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Story ID</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Owner</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Status</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>US01</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>US02</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Death before marriage</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>US03</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
@@ -46,588 +178,499 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>Date</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Remaining Stories</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Story Velocity</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Story ID</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Story Name</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Owner</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <t>Est Size</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Act Size</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Est Time</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Act Time</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Sprint</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>T01.01</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>T01.02</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>T01.03</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>T02.01</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>T02.02</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Story Description</t>
+  </si>
+  <si>
+    <t>Make sure that an individual's death date is &gt;= their birth date</t>
+  </si>
+  <si>
+    <t>Make sure that an individual's death date is &gt;= their marriage date</t>
+  </si>
+  <si>
+    <t>Make sure that an individual's marriage date is &gt;= their birth date</t>
+  </si>
+  <si>
+    <t>Input</t>
+  </si>
+  <si>
+    <t>Expected Output</t>
+  </si>
+  <si>
+    <t>No error message</t>
   </si>
   <si>
     <t>Status</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Est Size</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Act Size</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Act Time</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Completed</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Story ID</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Story Name</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Owner</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Status</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Est Size</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Est Time</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Act Size</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Act Time</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Completed</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Story Name</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Added</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Initials</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Last</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>First</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Email</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>LOC</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Passed</t>
+  </si>
+  <si>
+    <t>AT01</t>
+  </si>
+  <si>
+    <t>AT02</t>
+  </si>
+  <si>
+    <t>AT03</t>
+  </si>
+  <si>
+    <t>AT04</t>
+  </si>
+  <si>
+    <t>AT05</t>
+  </si>
+  <si>
+    <t>AT06</t>
+  </si>
+  <si>
+    <t>Acc Tests</t>
+  </si>
+  <si>
+    <t>AT ID</t>
+  </si>
+  <si>
+    <t>Meet twice a week</t>
+  </si>
+  <si>
+    <t>Text everyone when you discover a problem</t>
+  </si>
+  <si>
+    <t>Review Results</t>
+  </si>
+  <si>
+    <t>Forgetting to commit changes to GitHub</t>
+  </si>
+  <si>
+    <t>Keep doing:</t>
+  </si>
+  <si>
+    <t>Avoid:</t>
+  </si>
+  <si>
+    <t>GitHub Username</t>
+  </si>
+  <si>
+    <t>GitHub Repository:</t>
+  </si>
+  <si>
+    <t>Yanjun</t>
+  </si>
+  <si>
+    <t>Wu</t>
+  </si>
+  <si>
+    <t>yw</t>
+  </si>
+  <si>
+    <t>ywu29@stevens.edu</t>
+  </si>
+  <si>
+    <t>LSYanJun</t>
+  </si>
+  <si>
+    <t>SSW555tm052015s</t>
+  </si>
+  <si>
+    <t>US04</t>
+  </si>
+  <si>
+    <t>US05</t>
+  </si>
+  <si>
+    <t>US06</t>
+  </si>
+  <si>
+    <t>US07</t>
+  </si>
+  <si>
+    <t>US08</t>
+  </si>
+  <si>
+    <t>US09</t>
+  </si>
+  <si>
+    <t>US10</t>
+  </si>
+  <si>
+    <t>US11</t>
+  </si>
+  <si>
+    <t>US12</t>
+  </si>
+  <si>
+    <t>US13</t>
+  </si>
+  <si>
+    <t>US14</t>
+  </si>
+  <si>
+    <t>US15</t>
+  </si>
+  <si>
+    <t>US16</t>
+  </si>
+  <si>
+    <t>US17</t>
+  </si>
+  <si>
+    <t>US18</t>
+  </si>
+  <si>
+    <t>US19</t>
+  </si>
+  <si>
+    <t>US20</t>
+  </si>
+  <si>
+    <t>US21</t>
+  </si>
+  <si>
+    <t>US22</t>
+  </si>
+  <si>
+    <t>US23</t>
+  </si>
+  <si>
+    <t>US24</t>
+  </si>
+  <si>
+    <t>US25</t>
+  </si>
+  <si>
+    <t>Make sure that an individual's age is between 0 and 150</t>
+  </si>
+  <si>
+    <t>Make sure that in a family, father is a male and mother is a female</t>
+  </si>
+  <si>
+    <t>US26</t>
+  </si>
+  <si>
+    <t>Monogamy</t>
+  </si>
+  <si>
+    <t>US27</t>
+  </si>
+  <si>
+    <t>Make sure that an individual's divorce date is &gt;= their marriage date</t>
+  </si>
+  <si>
+    <t>Marriage before birth</t>
+  </si>
+  <si>
+    <t>Divorce before marriage</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Death before giving birth </t>
+  </si>
+  <si>
+    <t>An individual can't marry to their sibling unless they are not biologically related</t>
+  </si>
+  <si>
+    <t>A man can't get married until 20, a woman can't get married until 18</t>
+  </si>
+  <si>
+    <t>Death before birth</t>
+  </si>
+  <si>
+    <t>Make sure that the ID of an individual in a family or the ID of a family of an individual exists</t>
+  </si>
+  <si>
+    <t>Inexistent ID</t>
+  </si>
+  <si>
+    <t>Invalid gender</t>
+  </si>
+  <si>
+    <t>Invalid age of an individual</t>
+  </si>
+  <si>
+    <t>Invalid ages in a family</t>
+  </si>
+  <si>
+    <t>Make sure that the parents are older than children in one family</t>
+  </si>
+  <si>
+    <t>Illegal spouse</t>
+  </si>
+  <si>
+    <t>Illegal marrige age</t>
+  </si>
+  <si>
+    <t>Invalid family members</t>
+  </si>
+  <si>
+    <t>An individual can have at most one spouse</t>
+  </si>
+  <si>
+    <t>A family must contain a husband and a wife</t>
+  </si>
+  <si>
+    <t>Multiple roles in a family</t>
+  </si>
+  <si>
+    <t>Make sure an individual can play only one role in a family</t>
+  </si>
+  <si>
+    <t>Unmatched pointers</t>
+  </si>
+  <si>
+    <t>Amount of family members</t>
+  </si>
+  <si>
+    <t>A family can have at most 8 members</t>
+  </si>
+  <si>
+    <t>Age gap among the children</t>
+  </si>
+  <si>
+    <t>There should be at least 1 year age difference unless they were born on the same day</t>
+  </si>
+  <si>
+    <t>Make sure that all the dates are before today</t>
+  </si>
+  <si>
+    <t>Pregnancy limit</t>
+  </si>
+  <si>
+    <t>Wife can give birth between the age of 18 and 50</t>
+  </si>
+  <si>
+    <t>A person could be a child of only one family</t>
+  </si>
+  <si>
+    <t>A person should be linked to at least one family</t>
+  </si>
+  <si>
+    <t>Child in family</t>
+  </si>
+  <si>
+    <t>Family rule</t>
+  </si>
+  <si>
+    <t>gc</t>
+  </si>
+  <si>
+    <t>Gong</t>
+  </si>
+  <si>
+    <t>Cheng</t>
+  </si>
+  <si>
+    <t>gcheng2@stevens.edu</t>
+  </si>
+  <si>
+    <t>chenggongtc</t>
+  </si>
+  <si>
+    <t>Amog</t>
+  </si>
+  <si>
+    <t>bheemanakolli gurumallappa</t>
+  </si>
+  <si>
+    <t>abheeman@stevens.edu</t>
+  </si>
+  <si>
+    <t>amoghagurumallappa</t>
+  </si>
+  <si>
+    <t>Make sure that the pointers of an individual matches the pointers of the related families, and vice versa</t>
+  </si>
+  <si>
+    <t>Date rule</t>
+  </si>
+  <si>
+    <t>Make sure that in a family, mother's death date is &gt;= her children's birth dates and father's death date + 10 months is &gt;= his children's birth dates</t>
+  </si>
+  <si>
+    <t>Individual I1(Jacky /Mao/)  is the child of F22</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Individual I3(Katie /Brown/) is the spouse of Family F23</t>
+  </si>
+  <si>
+    <t>Error message "
+Individual I1(Jacky /Mao/) is a child of an inexistent Family F22."</t>
+  </si>
+  <si>
+    <t>Error message "
+Individual I3(Katie /Brown/) is a spouse of an inexistent Family F23."</t>
+  </si>
+  <si>
+    <t>Error message "
+Family F1 has a husband who is an inexistent Individual I18."</t>
+  </si>
+  <si>
+    <t>Error message "
+Family F2 has a child who is an inexistent Individual I15."</t>
+  </si>
+  <si>
+    <t>Error message "
+Family F3 has a wife who is an inexistent Individual I31."</t>
+  </si>
+  <si>
+    <t>Family F1's husband is Individual I18</t>
+  </si>
+  <si>
+    <t>Family F2 has a child who is Individual I15</t>
+  </si>
+  <si>
+    <t>US01</t>
+  </si>
+  <si>
+    <t>Individual I5(Emily /Mao/) is the child of F2 and the spouse of F5</t>
+  </si>
+  <si>
+    <t>AT07</t>
+  </si>
+  <si>
+    <t>US02</t>
+  </si>
+  <si>
+    <t>Family F4's husband is Individual I8(Kevin /Brown/), wife is Individual I9(Elena /Wilson/) and child is Individual I3(Katie /Brown/)</t>
+  </si>
+  <si>
+    <t>AT01~AT07</t>
+  </si>
+  <si>
+    <t>AT08</t>
+  </si>
+  <si>
+    <t>AT09</t>
+  </si>
+  <si>
+    <t>US03</t>
+  </si>
+  <si>
+    <t>AT10</t>
+  </si>
+  <si>
+    <t>AT11</t>
+  </si>
+  <si>
+    <t>AT12</t>
+  </si>
+  <si>
+    <t>Error message "
+Individual I1(Jacky /Mao/) is a spouse of Family F1, but Family F1 does not have the spouse of I1(Jacky /Mao/)."</t>
+  </si>
+  <si>
+    <t>Individual I1(Jacky /Mao/) is one of the spouse of Family F1, and Family F1's husband is Individual I18 and wife is Individual I12</t>
+  </si>
+  <si>
+    <t>Error message "
+Individual I3(Katie /Brown/) is a spouse of Family F3, but Family F3 does not have the spouse of I3(Katie /Brown/)."</t>
+  </si>
+  <si>
+    <t>Individual I3(Katie /Brown/) is one of the spouse of Family F3, and Family F3's husband is Individual I4 and wife is Individual I31</t>
+  </si>
+  <si>
+    <t>Error message "
+Individual I5(Emily /Mao/) is a child of Family F2, but Family F2 does not have the child of I5(Emily /Mao/)."</t>
+  </si>
+  <si>
+    <t>Individual I5(Emily /Mao/) is one of the child of Family F2, and Family F2's children are I1 and I15</t>
+  </si>
+  <si>
+    <t>Error message "
+Family F2's wife is Individual I3(Katie /Brown/), but Individual I3(Katie /Brown/) is not the wife of Family F2."</t>
+  </si>
+  <si>
+    <t>Family F2's wife is Individual I3(Katie /Brown/), I3(Katie /Brown/) is the spouse of F23 and F3</t>
+  </si>
+  <si>
+    <t>Error message "
+Family F2 has a child who is Individual I1(Jacky /Mao/), but Individual I1(Jacky /Mao/) is not a child of Family F2."</t>
+  </si>
+  <si>
+    <t>Family F2 has a child who is Individual I1(Jacky /Mao/), and I1(Jacky /Mao/) is the child of F22</t>
+  </si>
+  <si>
+    <t>AT13</t>
+  </si>
+  <si>
+    <t>Individual I2(Jianguo /Mao/) is one of the spouse of Family F2, and Family F2's husband is Individual I2(Jianguo /Mao/)</t>
+  </si>
+  <si>
+    <t>AT14</t>
+  </si>
+  <si>
+    <t>Family F3's wife is Individual I31</t>
+  </si>
+  <si>
+    <t>Family F3's husband is Individual I4(Edwin /Moore/), and Individual I4(Edwin /Moore/) is one of the spouse of Family F3</t>
+  </si>
+  <si>
+    <t>AT08~AT14</t>
+  </si>
+  <si>
+    <t>Done</t>
   </si>
   <si>
     <t>Code Velocity</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Min</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>gh(at)</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>gh(hm)</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>hm</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>gh</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>at</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Story ID</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Owner</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Status</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Death before birth</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>US01</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>US02</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Death before marriage</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>US03</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Marriage before birth</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Done</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Est Size</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Act Size</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Est Time</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Act Time</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Sprint</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>T01.01</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Store birth date</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>T01.02</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Store death date</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>T01.03</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Compare birth and death dates</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Coding</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>T02.01</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Find marriage record for individual</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>T02.02</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Story Description</t>
-  </si>
-  <si>
-    <t>Make sure that an individual's death date is &gt;= their birth date</t>
-  </si>
-  <si>
-    <t>Make sure that an individual's death date is &gt;= their marriage date</t>
-  </si>
-  <si>
-    <t>Make sure that an individual's marriage date is &gt;= their birth date</t>
-  </si>
-  <si>
-    <t>Input</t>
-  </si>
-  <si>
-    <t>Expected Output</t>
-  </si>
-  <si>
-    <t>No error message</t>
-  </si>
-  <si>
-    <t>Status</t>
-  </si>
-  <si>
-    <t>Passed</t>
-  </si>
-  <si>
-    <t>Individual I01 (Groucho Marx)  has birth date 01 JAN 2015 and death date 01 JAN 2014</t>
-  </si>
-  <si>
-    <t>Individual I01 (Groucho Marx) has marriage date 01 JAN 2015 and death date 01 JAN 2014</t>
-  </si>
-  <si>
-    <t>Error message "Individual I01 (Groucho Marx) has death date (01 JAN 2014) before birth date (01 JAN 2015)"</t>
-  </si>
-  <si>
-    <t>Error message "Individual I01  (Groucho Marx) has death date (01 JAN 2014) before marriage date (01 JAN 2015)"</t>
-  </si>
-  <si>
-    <t>Failed</t>
-  </si>
-  <si>
-    <t>No data</t>
-  </si>
-  <si>
-    <t>Individual I02 (Harpo Marx) has birth date 01 JAN 1950 and death date 01 JAN 2015</t>
-  </si>
-  <si>
-    <t>Individual I02 (Harpo Marx) has marriage date 01 JAN 1980 and death date 01 JAN 2015</t>
-  </si>
-  <si>
-    <t>Individual I03 Chico Marx)  has birth date 01 JAN 2015 and marriage date 01 JAN 2014</t>
-  </si>
-  <si>
-    <t>Individual I02 (Harpo Marx) has birth date 01 JAN 1950 and marriage date 01 JAN 1980</t>
-  </si>
-  <si>
-    <t>Error message "Individual I03  (Chico Marx) has marriage date (01 JAN 2014) before birth date (01 JAN 2015)"</t>
-  </si>
-  <si>
-    <t>AT01, AT02</t>
-  </si>
-  <si>
-    <t>AT01</t>
-  </si>
-  <si>
-    <t>AT02</t>
-  </si>
-  <si>
-    <t>AT03</t>
-  </si>
-  <si>
-    <t>AT04</t>
-  </si>
-  <si>
-    <t>AT05</t>
-  </si>
-  <si>
-    <t>AT06</t>
-  </si>
-  <si>
-    <t>AT03, AT04</t>
-  </si>
-  <si>
-    <t>AT05, AT06</t>
-  </si>
-  <si>
-    <t>Acc Tests</t>
-  </si>
-  <si>
-    <t>AT ID</t>
-  </si>
-  <si>
-    <t>Meet twice a week</t>
-  </si>
-  <si>
-    <t>Text everyone when you discover a problem</t>
-  </si>
-  <si>
-    <t>Review Results</t>
-  </si>
-  <si>
-    <t>Forgetting to commit changes to GitHub</t>
-  </si>
-  <si>
-    <t>Keep doing:</t>
-  </si>
-  <si>
-    <t>Avoid:</t>
-  </si>
-  <si>
-    <t>GitHub Username</t>
-  </si>
-  <si>
-    <t>GitHub Repository:</t>
-  </si>
-  <si>
-    <t>Yanjun</t>
-  </si>
-  <si>
-    <t>Wu</t>
-  </si>
-  <si>
-    <t>yw</t>
-  </si>
-  <si>
-    <t>ywu29@stevens.edu</t>
-  </si>
-  <si>
-    <t>LSYanJun</t>
-  </si>
-  <si>
-    <t>SSW555tm052015s</t>
-  </si>
-  <si>
-    <t>US04</t>
-  </si>
-  <si>
-    <t>US05</t>
-  </si>
-  <si>
-    <t>US06</t>
-  </si>
-  <si>
-    <t>US07</t>
-  </si>
-  <si>
-    <t>US08</t>
-  </si>
-  <si>
-    <t>US09</t>
-  </si>
-  <si>
-    <t>US10</t>
-  </si>
-  <si>
-    <t>US11</t>
-  </si>
-  <si>
-    <t>US12</t>
-  </si>
-  <si>
-    <t>US13</t>
-  </si>
-  <si>
-    <t>US14</t>
-  </si>
-  <si>
-    <t>US15</t>
-  </si>
-  <si>
-    <t>US16</t>
-  </si>
-  <si>
-    <t>US17</t>
-  </si>
-  <si>
-    <t>US18</t>
-  </si>
-  <si>
-    <t>US19</t>
-  </si>
-  <si>
-    <t>US20</t>
-  </si>
-  <si>
-    <t>US21</t>
-  </si>
-  <si>
-    <t>US22</t>
-  </si>
-  <si>
-    <t>US23</t>
-  </si>
-  <si>
-    <t>US24</t>
-  </si>
-  <si>
-    <t>US25</t>
-  </si>
-  <si>
-    <t>Make sure that an individual's age is between 0 and 150</t>
-  </si>
-  <si>
-    <t>Make sure that in a family, father is a male and mother is a female</t>
-  </si>
-  <si>
-    <t>US26</t>
-  </si>
-  <si>
-    <t>Monogamy</t>
-  </si>
-  <si>
-    <t>US27</t>
-  </si>
-  <si>
-    <t>Make sure that an individual's divorce date is &gt;= their marriage date</t>
-  </si>
-  <si>
-    <t>Marriage before birth</t>
-  </si>
-  <si>
-    <t>Divorce before marriage</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Death before giving birth </t>
-  </si>
-  <si>
-    <t>An individual can't marry to their sibling unless they are not biologically related</t>
-  </si>
-  <si>
-    <t>A man can't get married until 20, a woman can't get married until 18</t>
-  </si>
-  <si>
-    <t>Death before birth</t>
-  </si>
-  <si>
-    <t>Make sure that the ID of an individual in a family or the ID of a family of an individual exists</t>
-  </si>
-  <si>
-    <t>Inexistent ID</t>
-  </si>
-  <si>
-    <t>Invalid gender</t>
-  </si>
-  <si>
-    <t>Invalid age of an individual</t>
-  </si>
-  <si>
-    <t>Invalid ages in a family</t>
-  </si>
-  <si>
-    <t>Make sure that the parents are older than children in one family</t>
-  </si>
-  <si>
-    <t>Illegal spouse</t>
-  </si>
-  <si>
-    <t>Illegal marrige age</t>
-  </si>
-  <si>
-    <t>Invalid family members</t>
-  </si>
-  <si>
-    <t>An individual can have at most one spouse</t>
-  </si>
-  <si>
-    <t>A family must contain a husband and a wife</t>
-  </si>
-  <si>
-    <t>Multiple roles in a family</t>
-  </si>
-  <si>
-    <t>Make sure an individual can play only one role in a family</t>
-  </si>
-  <si>
-    <t>Unmatched pointers</t>
-  </si>
-  <si>
-    <t>Amount of family members</t>
-  </si>
-  <si>
-    <t>A family can have at most 8 members</t>
-  </si>
-  <si>
-    <t>Age gap among the children</t>
-  </si>
-  <si>
-    <t>There should be at least 1 year age difference unless they were born on the same day</t>
-  </si>
-  <si>
-    <t>Make sure that all the dates are before today</t>
-  </si>
-  <si>
-    <t>Pregnancy limit</t>
-  </si>
-  <si>
-    <t>Wife can give birth between the age of 18 and 50</t>
-  </si>
-  <si>
-    <t>A person could be a child of only one family</t>
-  </si>
-  <si>
-    <t>A person should be linked to at least one family</t>
-  </si>
-  <si>
-    <t>Child in family</t>
-  </si>
-  <si>
-    <t>Family rule</t>
-  </si>
-  <si>
-    <t>gc</t>
-  </si>
-  <si>
-    <t>Gong</t>
-  </si>
-  <si>
-    <t>Cheng</t>
-  </si>
-  <si>
-    <t>gcheng2@stevens.edu</t>
-  </si>
-  <si>
-    <t>chenggongtc</t>
-  </si>
-  <si>
-    <t>Amog</t>
-  </si>
-  <si>
-    <t>bheemanakolli gurumallappa</t>
-  </si>
-  <si>
-    <t>abheeman@stevens.edu</t>
-  </si>
-  <si>
-    <t>amoghagurumallappa</t>
-  </si>
-  <si>
-    <t>Make sure that the pointers of an individual matches the pointers of the related families, and vice versa</t>
-  </si>
-  <si>
-    <t>Date rule</t>
-  </si>
-  <si>
-    <t>Make sure that in a family, mother's death date is &gt;= her children's birth dates and father's death date + 10 months is &gt;= his children's birth dates</t>
+  </si>
+  <si>
+    <t>Link the existant family IDs to the related families</t>
+  </si>
+  <si>
+    <t>Link the existant individual IDs to the related individuals</t>
+  </si>
+  <si>
+    <t>T01.04</t>
+  </si>
+  <si>
+    <t>Check the existance of family IDs of every individual</t>
+  </si>
+  <si>
+    <t>Check the existance of individual IDs of every family</t>
+  </si>
+  <si>
+    <t>Check if the family pointers of an individual point back to the individual(as the same role in the family)</t>
+  </si>
+  <si>
+    <t>Check if the individual pointers of a family point back to the family(as the same role in the family)</t>
   </si>
 </sst>
 </file>
@@ -738,7 +781,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -764,6 +807,10 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="49"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="50">
     <cellStyle name="已访问的超链接" xfId="2" builtinId="9" hidden="1"/>
@@ -895,25 +942,25 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="265713536"/>
-        <c:axId val="265715072"/>
+        <c:axId val="305379200"/>
+        <c:axId val="305380736"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="265713536"/>
+        <c:axId val="305379200"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="m/d" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="265715072"/>
+        <c:crossAx val="305380736"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
         <c:baseTimeUnit val="days"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="265715072"/>
+        <c:axId val="305380736"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -921,7 +968,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="265713536"/>
+        <c:crossAx val="305379200"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -931,7 +978,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="1" l="0.75000000000000056" r="0.75000000000000056" t="1" header="0.5" footer="0.5"/>
+    <c:pageMargins b="1" l="0.75000000000000089" r="0.75000000000000089" t="1" header="0.5" footer="0.5"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1308,78 +1355,78 @@
   <sheetData>
     <row r="1" spans="1:5" s="4" customFormat="1">
       <c r="A1" s="4" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>100</v>
+        <v>70</v>
       </c>
     </row>
     <row r="3" spans="1:5">
       <c r="A3" t="s">
-        <v>104</v>
+        <v>74</v>
       </c>
       <c r="B3" t="s">
-        <v>102</v>
+        <v>72</v>
       </c>
       <c r="C3" t="s">
-        <v>103</v>
+        <v>73</v>
       </c>
       <c r="D3" s="14" t="s">
-        <v>105</v>
+        <v>75</v>
       </c>
       <c r="E3" t="s">
-        <v>106</v>
+        <v>76</v>
       </c>
     </row>
     <row r="4" spans="1:5">
       <c r="A4" t="s">
-        <v>167</v>
+        <v>137</v>
       </c>
       <c r="B4" t="s">
-        <v>168</v>
+        <v>138</v>
       </c>
       <c r="C4" t="s">
-        <v>169</v>
+        <v>139</v>
       </c>
       <c r="D4" s="14" t="s">
-        <v>170</v>
+        <v>140</v>
       </c>
       <c r="E4" t="s">
-        <v>171</v>
+        <v>141</v>
       </c>
     </row>
     <row r="5" spans="1:5">
       <c r="A5" t="s">
-        <v>37</v>
+        <v>28</v>
       </c>
       <c r="B5" t="s">
-        <v>172</v>
+        <v>142</v>
       </c>
       <c r="C5" t="s">
-        <v>173</v>
+        <v>143</v>
       </c>
       <c r="D5" s="14" t="s">
-        <v>174</v>
+        <v>144</v>
       </c>
       <c r="E5" t="s">
-        <v>175</v>
+        <v>145</v>
       </c>
     </row>
     <row r="9" spans="1:5">
       <c r="D9" s="4" t="s">
-        <v>101</v>
+        <v>71</v>
       </c>
       <c r="E9" t="s">
-        <v>107</v>
+        <v>77</v>
       </c>
     </row>
   </sheetData>
@@ -1414,34 +1461,34 @@
   <sheetData>
     <row r="1" spans="1:10" ht="25.5">
       <c r="A1" s="4" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="B1" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="H1" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="C1" s="5" t="s">
-        <v>92</v>
-      </c>
-      <c r="D1" s="4" t="s">
+      <c r="I1" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="E1" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="F1" s="10" t="s">
+      <c r="J1" s="10" t="s">
         <v>19</v>
-      </c>
-      <c r="G1" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="H1" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="I1" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="J1" s="10" t="s">
-        <v>23</v>
       </c>
     </row>
   </sheetData>
@@ -1460,7 +1507,7 @@
   <dimension ref="A1:L26"/>
   <sheetViews>
     <sheetView zoomScale="150" workbookViewId="0">
-      <selection activeCell="K10" sqref="K10"/>
+      <selection activeCell="M6" sqref="M6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75"/>
@@ -1481,40 +1528,40 @@
   <sheetData>
     <row r="1" spans="1:12" s="4" customFormat="1">
       <c r="A1" s="4" t="s">
-        <v>52</v>
+        <v>41</v>
       </c>
       <c r="B1" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="G1" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="H1" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="I1" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="C1" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="D1" s="4" t="s">
-        <v>92</v>
-      </c>
-      <c r="E1" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="F1" s="4" t="s">
+      <c r="J1" s="10" t="s">
         <v>40</v>
       </c>
-      <c r="G1" s="10" t="s">
-        <v>48</v>
-      </c>
-      <c r="H1" s="10" t="s">
-        <v>50</v>
-      </c>
-      <c r="I1" s="10" t="s">
-        <v>49</v>
-      </c>
-      <c r="J1" s="10" t="s">
-        <v>51</v>
-      </c>
       <c r="K1" s="11" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="L1" s="11" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
     </row>
     <row r="2" spans="1:12">
@@ -1522,19 +1569,19 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>42</v>
+        <v>32</v>
       </c>
       <c r="C2" t="s">
-        <v>143</v>
+        <v>113</v>
       </c>
       <c r="D2" t="s">
-        <v>83</v>
+        <v>163</v>
       </c>
       <c r="E2" t="s">
-        <v>167</v>
+        <v>137</v>
       </c>
       <c r="F2" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="G2">
         <v>150</v>
@@ -1543,16 +1590,16 @@
         <v>60</v>
       </c>
       <c r="I2">
-        <v>120</v>
+        <v>98</v>
       </c>
       <c r="J2">
-        <v>90</v>
+        <v>60</v>
       </c>
       <c r="K2" s="7">
-        <v>40235</v>
+        <v>40600</v>
       </c>
       <c r="L2" s="7">
-        <v>40600</v>
+        <v>40598</v>
       </c>
     </row>
     <row r="3" spans="1:12">
@@ -1560,36 +1607,42 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>43</v>
+        <v>33</v>
       </c>
       <c r="C3" t="s">
-        <v>44</v>
+        <v>125</v>
       </c>
       <c r="D3" t="s">
-        <v>90</v>
+        <v>185</v>
+      </c>
+      <c r="E3" t="s">
+        <v>137</v>
+      </c>
+      <c r="F3" t="s">
+        <v>186</v>
       </c>
       <c r="G3">
-        <v>200</v>
+        <v>50</v>
       </c>
       <c r="H3">
-        <v>120</v>
+        <v>40</v>
+      </c>
+      <c r="I3">
+        <v>72</v>
+      </c>
+      <c r="J3">
+        <v>45</v>
+      </c>
+      <c r="K3" s="16">
+        <v>40601</v>
       </c>
       <c r="L3" s="7">
-        <v>40414</v>
+        <v>40598</v>
       </c>
     </row>
     <row r="4" spans="1:12">
-      <c r="A4">
-        <v>3</v>
-      </c>
       <c r="B4" t="s">
-        <v>45</v>
-      </c>
-      <c r="C4" t="s">
-        <v>46</v>
-      </c>
-      <c r="D4" t="s">
-        <v>91</v>
+        <v>35</v>
       </c>
       <c r="L4" s="7">
         <v>40460</v>
@@ -1597,112 +1650,112 @@
     </row>
     <row r="5" spans="1:12">
       <c r="B5" t="s">
-        <v>108</v>
+        <v>78</v>
       </c>
     </row>
     <row r="6" spans="1:12">
       <c r="B6" t="s">
-        <v>109</v>
+        <v>79</v>
       </c>
     </row>
     <row r="7" spans="1:12">
       <c r="B7" t="s">
-        <v>110</v>
+        <v>80</v>
       </c>
     </row>
     <row r="8" spans="1:12">
       <c r="B8" t="s">
-        <v>111</v>
+        <v>81</v>
       </c>
     </row>
     <row r="9" spans="1:12">
       <c r="B9" t="s">
-        <v>112</v>
+        <v>82</v>
       </c>
     </row>
     <row r="10" spans="1:12">
       <c r="B10" t="s">
-        <v>113</v>
+        <v>83</v>
       </c>
     </row>
     <row r="11" spans="1:12">
       <c r="B11" t="s">
-        <v>114</v>
+        <v>84</v>
       </c>
     </row>
     <row r="12" spans="1:12">
       <c r="B12" t="s">
-        <v>115</v>
+        <v>85</v>
       </c>
     </row>
     <row r="13" spans="1:12">
       <c r="B13" t="s">
-        <v>116</v>
+        <v>86</v>
       </c>
     </row>
     <row r="14" spans="1:12">
       <c r="B14" t="s">
-        <v>117</v>
+        <v>87</v>
       </c>
     </row>
     <row r="15" spans="1:12">
       <c r="B15" t="s">
-        <v>118</v>
+        <v>88</v>
       </c>
     </row>
     <row r="16" spans="1:12">
       <c r="B16" t="s">
-        <v>119</v>
+        <v>89</v>
       </c>
     </row>
     <row r="17" spans="2:2">
       <c r="B17" t="s">
-        <v>120</v>
+        <v>90</v>
       </c>
     </row>
     <row r="18" spans="2:2">
       <c r="B18" t="s">
-        <v>121</v>
+        <v>91</v>
       </c>
     </row>
     <row r="19" spans="2:2">
       <c r="B19" t="s">
-        <v>122</v>
+        <v>92</v>
       </c>
     </row>
     <row r="20" spans="2:2">
       <c r="B20" t="s">
-        <v>123</v>
+        <v>93</v>
       </c>
     </row>
     <row r="21" spans="2:2">
       <c r="B21" t="s">
-        <v>124</v>
+        <v>94</v>
       </c>
     </row>
     <row r="22" spans="2:2">
       <c r="B22" t="s">
-        <v>125</v>
+        <v>95</v>
       </c>
     </row>
     <row r="23" spans="2:2">
       <c r="B23" t="s">
-        <v>126</v>
+        <v>96</v>
       </c>
     </row>
     <row r="24" spans="2:2">
       <c r="B24" t="s">
-        <v>127</v>
+        <v>97</v>
       </c>
     </row>
     <row r="25" spans="2:2">
       <c r="B25" t="s">
-        <v>128</v>
+        <v>98</v>
       </c>
     </row>
     <row r="26" spans="2:2">
       <c r="B26" t="s">
-        <v>129</v>
+        <v>99</v>
       </c>
     </row>
   </sheetData>
@@ -1721,8 +1774,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75"/>
@@ -1736,283 +1789,301 @@
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" s="4" t="s">
-        <v>38</v>
+        <v>29</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>63</v>
+        <v>47</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>92</v>
+        <v>62</v>
       </c>
       <c r="E1" s="10" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="F1" s="10" t="s">
-        <v>50</v>
+        <v>39</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="25.5">
       <c r="A2" t="s">
-        <v>42</v>
+        <v>32</v>
       </c>
       <c r="B2" t="s">
-        <v>143</v>
+        <v>113</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>142</v>
+        <v>112</v>
+      </c>
+      <c r="D2" t="s">
+        <v>163</v>
+      </c>
+      <c r="E2">
+        <v>150</v>
+      </c>
+      <c r="F2">
+        <v>60</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="25.5">
       <c r="A3" t="s">
-        <v>43</v>
+        <v>33</v>
       </c>
       <c r="B3" t="s">
-        <v>155</v>
+        <v>125</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>176</v>
+        <v>146</v>
+      </c>
+      <c r="D3" t="s">
+        <v>185</v>
+      </c>
+      <c r="E3">
+        <v>50</v>
+      </c>
+      <c r="F3">
+        <v>40</v>
       </c>
     </row>
     <row r="4" spans="1:6">
       <c r="A4" t="s">
-        <v>45</v>
+        <v>35</v>
       </c>
       <c r="B4" t="s">
-        <v>177</v>
+        <v>147</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>160</v>
+        <v>130</v>
       </c>
     </row>
     <row r="5" spans="1:6">
       <c r="A5" t="s">
-        <v>108</v>
+        <v>78</v>
       </c>
       <c r="B5" t="s">
-        <v>150</v>
+        <v>120</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>152</v>
+        <v>122</v>
       </c>
     </row>
     <row r="6" spans="1:6">
       <c r="A6" t="s">
-        <v>109</v>
+        <v>79</v>
       </c>
       <c r="B6" t="s">
-        <v>141</v>
+        <v>111</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>64</v>
+        <v>48</v>
       </c>
     </row>
     <row r="7" spans="1:6">
       <c r="A7" t="s">
-        <v>110</v>
+        <v>80</v>
       </c>
       <c r="B7" t="s">
-        <v>144</v>
+        <v>114</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>131</v>
+        <v>101</v>
       </c>
     </row>
     <row r="8" spans="1:6">
       <c r="A8" t="s">
-        <v>111</v>
+        <v>81</v>
       </c>
       <c r="B8" t="s">
-        <v>145</v>
+        <v>115</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>130</v>
+        <v>100</v>
       </c>
     </row>
     <row r="9" spans="1:6">
       <c r="A9" t="s">
-        <v>112</v>
+        <v>82</v>
       </c>
       <c r="B9" t="s">
-        <v>153</v>
+        <v>123</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>154</v>
+        <v>124</v>
       </c>
     </row>
     <row r="10" spans="1:6">
       <c r="A10" t="s">
-        <v>113</v>
+        <v>83</v>
       </c>
       <c r="B10" t="s">
-        <v>146</v>
+        <v>116</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>147</v>
+        <v>117</v>
       </c>
     </row>
     <row r="11" spans="1:6">
       <c r="A11" t="s">
-        <v>114</v>
+        <v>84</v>
       </c>
       <c r="B11" t="s">
-        <v>44</v>
+        <v>34</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>65</v>
+        <v>49</v>
       </c>
     </row>
     <row r="12" spans="1:6">
       <c r="A12" t="s">
-        <v>115</v>
+        <v>85</v>
       </c>
       <c r="B12" t="s">
-        <v>136</v>
+        <v>106</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>66</v>
+        <v>50</v>
       </c>
     </row>
     <row r="13" spans="1:6">
       <c r="A13" t="s">
-        <v>116</v>
+        <v>86</v>
       </c>
       <c r="B13" t="s">
-        <v>137</v>
+        <v>107</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>135</v>
+        <v>105</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="25.5">
       <c r="A14" t="s">
-        <v>117</v>
+        <v>87</v>
       </c>
       <c r="B14" t="s">
-        <v>138</v>
+        <v>108</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>178</v>
+        <v>148</v>
       </c>
     </row>
     <row r="15" spans="1:6">
       <c r="A15" t="s">
-        <v>118</v>
+        <v>88</v>
       </c>
       <c r="B15" t="s">
-        <v>133</v>
+        <v>103</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>151</v>
+        <v>121</v>
       </c>
     </row>
     <row r="16" spans="1:6">
       <c r="A16" t="s">
-        <v>119</v>
+        <v>89</v>
       </c>
       <c r="B16" t="s">
-        <v>148</v>
+        <v>118</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>139</v>
+        <v>109</v>
       </c>
     </row>
     <row r="17" spans="1:3">
       <c r="A17" t="s">
-        <v>120</v>
+        <v>90</v>
       </c>
       <c r="B17" t="s">
-        <v>149</v>
+        <v>119</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>140</v>
+        <v>110</v>
       </c>
     </row>
     <row r="18" spans="1:3">
       <c r="A18" t="s">
-        <v>121</v>
+        <v>91</v>
       </c>
       <c r="B18" t="s">
-        <v>156</v>
+        <v>126</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>157</v>
+        <v>127</v>
       </c>
     </row>
     <row r="19" spans="1:3" ht="25.5">
       <c r="A19" t="s">
-        <v>122</v>
+        <v>92</v>
       </c>
       <c r="B19" t="s">
-        <v>158</v>
+        <v>128</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>159</v>
+        <v>129</v>
       </c>
     </row>
     <row r="20" spans="1:3">
       <c r="A20" t="s">
-        <v>123</v>
+        <v>93</v>
       </c>
       <c r="B20" t="s">
-        <v>161</v>
+        <v>131</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>162</v>
+        <v>132</v>
       </c>
     </row>
     <row r="21" spans="1:3">
       <c r="A21" t="s">
-        <v>124</v>
+        <v>94</v>
       </c>
       <c r="B21" t="s">
-        <v>165</v>
+        <v>135</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>163</v>
+        <v>133</v>
       </c>
     </row>
     <row r="22" spans="1:3">
       <c r="A22" t="s">
-        <v>125</v>
+        <v>95</v>
       </c>
       <c r="B22" t="s">
-        <v>166</v>
+        <v>136</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>164</v>
+        <v>134</v>
       </c>
     </row>
     <row r="23" spans="1:3">
       <c r="A23" t="s">
-        <v>126</v>
+        <v>96</v>
       </c>
     </row>
     <row r="24" spans="1:3">
       <c r="A24" t="s">
-        <v>127</v>
+        <v>97</v>
       </c>
     </row>
     <row r="25" spans="1:3">
       <c r="A25" t="s">
-        <v>128</v>
+        <v>98</v>
       </c>
     </row>
     <row r="26" spans="1:3">
       <c r="A26" t="s">
-        <v>129</v>
+        <v>99</v>
       </c>
     </row>
     <row r="27" spans="1:3">
       <c r="A27" t="s">
-        <v>132</v>
+        <v>102</v>
       </c>
     </row>
     <row r="28" spans="1:3">
       <c r="A28" t="s">
-        <v>134</v>
+        <v>104</v>
       </c>
     </row>
   </sheetData>
@@ -2028,10 +2099,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F7"/>
+  <dimension ref="A1:F15"/>
   <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView zoomScale="145" zoomScaleNormal="145" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75"/>
@@ -2046,147 +2117,307 @@
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" s="4" t="s">
-        <v>93</v>
+        <v>63</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>38</v>
+        <v>29</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>67</v>
+        <v>51</v>
       </c>
       <c r="E1" s="5" t="s">
-        <v>68</v>
+        <v>52</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" ht="63">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="47.25">
       <c r="A2" t="s">
-        <v>84</v>
+        <v>56</v>
       </c>
       <c r="B2" t="s">
-        <v>42</v>
+        <v>32</v>
       </c>
       <c r="C2" t="s">
-        <v>41</v>
+        <v>113</v>
       </c>
       <c r="D2" s="13" t="s">
-        <v>72</v>
+        <v>149</v>
       </c>
       <c r="E2" s="13" t="s">
-        <v>74</v>
+        <v>151</v>
       </c>
       <c r="F2" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" ht="31.5">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="47.25">
       <c r="A3" t="s">
-        <v>85</v>
+        <v>57</v>
       </c>
       <c r="B3" t="s">
-        <v>42</v>
+        <v>32</v>
       </c>
       <c r="C3" t="s">
-        <v>41</v>
+        <v>113</v>
       </c>
       <c r="D3" s="13" t="s">
-        <v>78</v>
-      </c>
-      <c r="E3" s="12" t="s">
-        <v>69</v>
+        <v>150</v>
+      </c>
+      <c r="E3" s="15" t="s">
+        <v>152</v>
       </c>
       <c r="F3" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" ht="63">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="47.25">
       <c r="A4" t="s">
-        <v>86</v>
+        <v>58</v>
       </c>
       <c r="B4" t="s">
-        <v>43</v>
+        <v>158</v>
       </c>
       <c r="C4" t="s">
-        <v>44</v>
+        <v>113</v>
       </c>
       <c r="D4" s="13" t="s">
-        <v>73</v>
+        <v>156</v>
       </c>
       <c r="E4" s="13" t="s">
-        <v>75</v>
+        <v>153</v>
       </c>
       <c r="F4" t="s">
-        <v>76</v>
+        <v>55</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="47.25">
       <c r="A5" t="s">
-        <v>87</v>
+        <v>59</v>
       </c>
       <c r="B5" t="s">
-        <v>43</v>
+        <v>158</v>
       </c>
       <c r="C5" t="s">
-        <v>44</v>
+        <v>113</v>
       </c>
       <c r="D5" s="13" t="s">
-        <v>79</v>
-      </c>
-      <c r="E5" s="12" t="s">
-        <v>69</v>
+        <v>157</v>
+      </c>
+      <c r="E5" s="15" t="s">
+        <v>154</v>
       </c>
       <c r="F5" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" ht="63">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="47.25">
       <c r="A6" t="s">
-        <v>88</v>
+        <v>60</v>
       </c>
       <c r="B6" t="s">
-        <v>45</v>
+        <v>158</v>
       </c>
       <c r="C6" t="s">
-        <v>46</v>
+        <v>113</v>
       </c>
       <c r="D6" s="13" t="s">
-        <v>80</v>
+        <v>183</v>
       </c>
       <c r="E6" s="13" t="s">
-        <v>82</v>
+        <v>155</v>
       </c>
       <c r="F6" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" ht="47.25">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="31.5">
       <c r="A7" t="s">
-        <v>89</v>
+        <v>61</v>
       </c>
       <c r="B7" t="s">
-        <v>45</v>
+        <v>158</v>
       </c>
       <c r="C7" t="s">
-        <v>46</v>
+        <v>113</v>
       </c>
       <c r="D7" s="13" t="s">
-        <v>81</v>
+        <v>159</v>
       </c>
       <c r="E7" s="12" t="s">
-        <v>69</v>
+        <v>53</v>
       </c>
       <c r="F7" t="s">
-        <v>71</v>
+        <v>55</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="63">
+      <c r="A8" t="s">
+        <v>160</v>
+      </c>
+      <c r="B8" t="s">
+        <v>158</v>
+      </c>
+      <c r="C8" t="s">
+        <v>113</v>
+      </c>
+      <c r="D8" s="13" t="s">
+        <v>162</v>
+      </c>
+      <c r="E8" s="12" t="s">
+        <v>53</v>
+      </c>
+      <c r="F8" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="63">
+      <c r="A9" t="s">
+        <v>164</v>
+      </c>
+      <c r="B9" t="s">
+        <v>161</v>
+      </c>
+      <c r="C9" t="s">
+        <v>125</v>
+      </c>
+      <c r="D9" s="13" t="s">
+        <v>171</v>
+      </c>
+      <c r="E9" s="15" t="s">
+        <v>170</v>
+      </c>
+      <c r="F9" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="78.75">
+      <c r="A10" t="s">
+        <v>165</v>
+      </c>
+      <c r="B10" t="s">
+        <v>161</v>
+      </c>
+      <c r="C10" t="s">
+        <v>125</v>
+      </c>
+      <c r="D10" s="13" t="s">
+        <v>173</v>
+      </c>
+      <c r="E10" s="15" t="s">
+        <v>172</v>
+      </c>
+      <c r="F10" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="63">
+      <c r="A11" t="s">
+        <v>167</v>
+      </c>
+      <c r="B11" t="s">
+        <v>161</v>
+      </c>
+      <c r="C11" t="s">
+        <v>125</v>
+      </c>
+      <c r="D11" s="13" t="s">
+        <v>175</v>
+      </c>
+      <c r="E11" s="15" t="s">
+        <v>174</v>
+      </c>
+      <c r="F11" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="63">
+      <c r="A12" t="s">
+        <v>168</v>
+      </c>
+      <c r="B12" t="s">
+        <v>161</v>
+      </c>
+      <c r="C12" t="s">
+        <v>125</v>
+      </c>
+      <c r="D12" s="13" t="s">
+        <v>177</v>
+      </c>
+      <c r="E12" s="15" t="s">
+        <v>176</v>
+      </c>
+      <c r="F12" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="78.75">
+      <c r="A13" t="s">
+        <v>169</v>
+      </c>
+      <c r="B13" t="s">
+        <v>161</v>
+      </c>
+      <c r="C13" t="s">
+        <v>125</v>
+      </c>
+      <c r="D13" s="13" t="s">
+        <v>179</v>
+      </c>
+      <c r="E13" s="15" t="s">
+        <v>178</v>
+      </c>
+      <c r="F13" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="47.25">
+      <c r="A14" t="s">
+        <v>180</v>
+      </c>
+      <c r="B14" t="s">
+        <v>161</v>
+      </c>
+      <c r="C14" t="s">
+        <v>125</v>
+      </c>
+      <c r="D14" s="13" t="s">
+        <v>181</v>
+      </c>
+      <c r="E14" s="15" t="s">
+        <v>53</v>
+      </c>
+      <c r="F14" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" ht="47.25">
+      <c r="A15" t="s">
+        <v>182</v>
+      </c>
+      <c r="B15" t="s">
+        <v>166</v>
+      </c>
+      <c r="C15" t="s">
+        <v>125</v>
+      </c>
+      <c r="D15" s="13" t="s">
+        <v>184</v>
+      </c>
+      <c r="E15" s="15" t="s">
+        <v>53</v>
+      </c>
+      <c r="F15" t="s">
+        <v>55</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -2200,7 +2431,7 @@
   <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView zoomScale="150" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="I14" sqref="I14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75"/>
@@ -2215,22 +2446,22 @@
   <sheetData>
     <row r="1" spans="1:6" s="4" customFormat="1">
       <c r="A1" s="3" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="F1" s="8" t="s">
-        <v>31</v>
+        <v>187</v>
       </c>
     </row>
     <row r="2" spans="1:6">
@@ -2369,10 +2600,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J21"/>
+  <dimension ref="A1:J25"/>
   <sheetViews>
-    <sheetView zoomScale="150" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+    <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75"/>
@@ -2391,51 +2622,51 @@
   <sheetData>
     <row r="1" spans="1:10">
       <c r="A1" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="F1" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="G1" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="C1" s="5" t="s">
-        <v>92</v>
-      </c>
-      <c r="D1" s="4" t="s">
+      <c r="H1" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="I1" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="F1" s="10" t="s">
+      <c r="J1" s="11" t="s">
         <v>19</v>
-      </c>
-      <c r="G1" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="H1" s="10" t="s">
-        <v>21</v>
-      </c>
-      <c r="I1" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="J1" s="11" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="2" spans="1:10">
       <c r="A2" t="s">
-        <v>42</v>
+        <v>32</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>83</v>
+        <v>113</v>
+      </c>
+      <c r="C2" t="s">
+        <v>163</v>
       </c>
       <c r="D2" t="s">
-        <v>35</v>
+        <v>137</v>
       </c>
       <c r="E2" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="F2">
         <v>150</v>
@@ -2444,139 +2675,147 @@
         <v>60</v>
       </c>
       <c r="H2">
-        <v>120</v>
+        <v>98</v>
       </c>
       <c r="I2">
-        <v>90</v>
-      </c>
-      <c r="J2" s="6">
-        <v>40444</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10">
+        <v>60</v>
+      </c>
+      <c r="J2" s="7">
+        <v>40600</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" ht="25.5">
       <c r="A4" t="s">
-        <v>53</v>
+        <v>42</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>54</v>
+        <v>191</v>
       </c>
       <c r="D4" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" ht="25.5">
       <c r="A5" t="s">
-        <v>55</v>
+        <v>43</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>56</v>
+        <v>188</v>
       </c>
       <c r="D5" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" ht="25.5">
       <c r="A6" t="s">
-        <v>57</v>
+        <v>44</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>58</v>
+        <v>192</v>
       </c>
       <c r="D6" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10">
-      <c r="A8" t="s">
-        <v>43</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="D8" t="s">
-        <v>36</v>
-      </c>
-      <c r="E8" t="s">
-        <v>59</v>
-      </c>
-      <c r="F8">
-        <v>200</v>
-      </c>
-      <c r="G8">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10">
-      <c r="A10" t="s">
-        <v>60</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="D10" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" ht="25.5">
+      <c r="A7" t="s">
+        <v>190</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="D7" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10">
+      <c r="A9" t="s">
         <v>33</v>
       </c>
-      <c r="E10" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10">
+      <c r="B9" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="C9" t="s">
+        <v>185</v>
+      </c>
+      <c r="D9" t="s">
+        <v>137</v>
+      </c>
+      <c r="E9" t="s">
+        <v>186</v>
+      </c>
+      <c r="F9">
+        <v>50</v>
+      </c>
+      <c r="G9">
+        <v>40</v>
+      </c>
+      <c r="H9">
+        <v>72</v>
+      </c>
+      <c r="I9">
+        <v>45</v>
+      </c>
+      <c r="J9" s="16">
+        <v>40601</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" ht="38.25">
       <c r="A11" t="s">
-        <v>62</v>
+        <v>45</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>0</v>
+        <v>193</v>
       </c>
       <c r="D11" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" ht="38.25">
       <c r="A12" t="s">
-        <v>1</v>
+        <v>46</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>2</v>
+        <v>194</v>
       </c>
       <c r="D12" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10">
-      <c r="B14" s="5" t="s">
-        <v>96</v>
+        <v>137</v>
       </c>
     </row>
     <row r="15" spans="1:10">
-      <c r="B15" s="5"/>
       <c r="J15" s="7"/>
     </row>
-    <row r="16" spans="1:10">
-      <c r="B16" s="5" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="17" spans="2:2">
-      <c r="B17" s="1" t="s">
-        <v>94</v>
-      </c>
-    </row>
     <row r="18" spans="2:2">
-      <c r="B18" s="1" t="s">
-        <v>95</v>
-      </c>
+      <c r="B18" s="5" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="19" spans="2:2">
+      <c r="B19" s="5"/>
     </row>
     <row r="20" spans="2:2">
       <c r="B20" s="5" t="s">
-        <v>99</v>
+        <v>68</v>
       </c>
     </row>
     <row r="21" spans="2:2">
       <c r="B21" s="1" t="s">
-        <v>97</v>
+        <v>64</v>
+      </c>
+    </row>
+    <row r="22" spans="2:2">
+      <c r="B22" s="1" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="24" spans="2:2">
+      <c r="B24" s="5" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="25" spans="2:2">
+      <c r="B25" s="1" t="s">
+        <v>67</v>
       </c>
     </row>
   </sheetData>
@@ -2603,34 +2842,34 @@
   <sheetData>
     <row r="1" spans="1:10" ht="25.5">
       <c r="A1" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="F1" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="G1" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="C1" s="5" t="s">
-        <v>92</v>
-      </c>
-      <c r="D1" s="4" t="s">
+      <c r="H1" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="I1" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="F1" s="10" t="s">
+      <c r="J1" s="10" t="s">
         <v>19</v>
-      </c>
-      <c r="G1" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="H1" s="10" t="s">
-        <v>21</v>
-      </c>
-      <c r="I1" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="J1" s="10" t="s">
-        <v>23</v>
       </c>
     </row>
   </sheetData>
@@ -2657,34 +2896,34 @@
   <sheetData>
     <row r="1" spans="1:10" ht="25.5">
       <c r="A1" s="4" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="B1" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="H1" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="C1" s="5" t="s">
-        <v>92</v>
-      </c>
-      <c r="D1" s="4" t="s">
+      <c r="I1" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="E1" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="F1" s="10" t="s">
+      <c r="J1" s="10" t="s">
         <v>19</v>
-      </c>
-      <c r="G1" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="H1" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="I1" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="J1" s="10" t="s">
-        <v>23</v>
       </c>
     </row>
   </sheetData>
@@ -2710,34 +2949,34 @@
   <sheetData>
     <row r="1" spans="1:10" ht="25.5">
       <c r="A1" s="4" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="B1" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="H1" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="C1" s="5" t="s">
-        <v>92</v>
-      </c>
-      <c r="D1" s="4" t="s">
+      <c r="I1" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="E1" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="F1" s="10" t="s">
+      <c r="J1" s="10" t="s">
         <v>19</v>
-      </c>
-      <c r="G1" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="H1" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="I1" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="J1" s="10" t="s">
-        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add function to us03
</commit_message>
<xml_diff>
--- a/Team05Report.xlsx
+++ b/Team05Report.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="240" windowWidth="20730" windowHeight="11760" tabRatio="500"/>
+    <workbookView xWindow="240" yWindow="240" windowWidth="20730" windowHeight="11760" tabRatio="500" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Team" sheetId="1" r:id="rId1"/>
@@ -27,8 +27,42 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>Yanjun</author>
+  </authors>
+  <commentList>
+    <comment ref="E22" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Yanjun:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="480" uniqueCount="281">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="495" uniqueCount="287">
   <si>
     <t>Date</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -893,12 +927,6 @@
     <t>Individual I5(Emily /Mao/) was born on 11 SEP 1993 and died on 31 OCT 2014</t>
   </si>
   <si>
-    <t>AT15~AT19</t>
-  </si>
-  <si>
-    <t>AT20~AT21</t>
-  </si>
-  <si>
     <t>Get current date(year, month, day)</t>
   </si>
   <si>
@@ -927,6 +955,30 @@
   </si>
   <si>
     <t>abg</t>
+  </si>
+  <si>
+    <t>Family F1 marriage date is 2 FEB 2018</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Family F1 has an invalid marriage date (2 Feb 2018). Marriage date beforen current date. </t>
+  </si>
+  <si>
+    <t>Family F3 has an invalid divorce date(31 NOV 1987). Divorce date doesn't exist.</t>
+  </si>
+  <si>
+    <t>Family F3 marriage date is 31 NOV 1987</t>
+  </si>
+  <si>
+    <t>AT15~AT21</t>
+  </si>
+  <si>
+    <t>AT22~AT23</t>
+  </si>
+  <si>
+    <t>Completed information</t>
+  </si>
+  <si>
+    <t>Every person must have completed information(name, sex, birthday) and every family must have completed information(marriage date)</t>
   </si>
 </sst>
 </file>
@@ -937,7 +989,7 @@
     <numFmt numFmtId="164" formatCode="m/d"/>
     <numFmt numFmtId="165" formatCode="0.0"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Verdana"/>
@@ -966,6 +1018,29 @@
     <font>
       <sz val="12"/>
       <name val="Cambria"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <name val="Cambria"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Verdana"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -1037,7 +1112,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1067,6 +1142,16 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="justify"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="justify"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="50">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -1195,11 +1280,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="95289728"/>
-        <c:axId val="95291264"/>
+        <c:axId val="104432000"/>
+        <c:axId val="104433536"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="95289728"/>
+        <c:axId val="104432000"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1209,14 +1294,14 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="95291264"/>
+        <c:crossAx val="104433536"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
         <c:baseTimeUnit val="days"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="95291264"/>
+        <c:axId val="104433536"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1227,7 +1312,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="95289728"/>
+        <c:crossAx val="104432000"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1601,7 +1686,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E9"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
+    <sheetView zoomScale="150" workbookViewId="0">
       <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
@@ -1667,7 +1752,7 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="B5" t="s">
         <v>140</v>
@@ -1768,7 +1853,7 @@
   <dimension ref="A1:L26"/>
   <sheetViews>
     <sheetView zoomScale="150" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1911,8 +1996,8 @@
       <c r="C4" t="s">
         <v>193</v>
       </c>
-      <c r="D4" t="s">
-        <v>269</v>
+      <c r="D4" s="18" t="s">
+        <v>283</v>
       </c>
       <c r="E4" t="s">
         <v>194</v>
@@ -1927,7 +2012,7 @@
         <v>45</v>
       </c>
       <c r="I4">
-        <v>102</v>
+        <v>162</v>
       </c>
       <c r="J4">
         <v>60</v>
@@ -1960,8 +2045,8 @@
       <c r="C6" t="s">
         <v>109</v>
       </c>
-      <c r="D6" t="s">
-        <v>270</v>
+      <c r="D6" s="18" t="s">
+        <v>284</v>
       </c>
       <c r="E6" t="s">
         <v>194</v>
@@ -2167,6 +2252,12 @@
     <row r="23" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B23" t="s">
         <v>94</v>
+      </c>
+      <c r="C23" s="18" t="s">
+        <v>285</v>
+      </c>
+      <c r="L23" s="7">
+        <v>40602</v>
       </c>
     </row>
     <row r="24" spans="2:12" x14ac:dyDescent="0.2">
@@ -2201,7 +2292,7 @@
   <dimension ref="A1:F28"/>
   <sheetViews>
     <sheetView zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2283,8 +2374,8 @@
       <c r="C4" s="1" t="s">
         <v>128</v>
       </c>
-      <c r="D4" t="s">
-        <v>269</v>
+      <c r="D4" s="18" t="s">
+        <v>283</v>
       </c>
       <c r="E4">
         <v>80</v>
@@ -2303,8 +2394,8 @@
       <c r="C5" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="D5" t="s">
-        <v>270</v>
+      <c r="D5" s="18" t="s">
+        <v>284</v>
       </c>
       <c r="E5">
         <v>20</v>
@@ -2500,9 +2591,15 @@
         <v>132</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>94</v>
+      </c>
+      <c r="B23" s="18" t="s">
+        <v>285</v>
+      </c>
+      <c r="C23" s="20" t="s">
+        <v>286</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.2">
@@ -2542,11 +2639,11 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F78"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F80"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" zoomScale="145" zoomScaleNormal="145" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="B22" sqref="B20:D22"/>
+    <sheetView topLeftCell="A16" zoomScale="145" zoomScaleNormal="145" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="H23" sqref="H23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2799,7 +2896,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="63" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" ht="78.75" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>166</v>
       </c>
@@ -2959,329 +3056,370 @@
         <v>53</v>
       </c>
     </row>
-    <row r="21" spans="1:6" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:6" ht="47.25" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>200</v>
       </c>
       <c r="B21" t="s">
-        <v>77</v>
+        <v>163</v>
       </c>
       <c r="C21" t="s">
-        <v>109</v>
+        <v>193</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>266</v>
-      </c>
-      <c r="E21" s="1" t="s">
-        <v>267</v>
-      </c>
-      <c r="F21" t="s">
+        <v>279</v>
+      </c>
+      <c r="E21" s="17" t="s">
+        <v>280</v>
+      </c>
+      <c r="F21" s="18" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="22" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" ht="47.25" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>201</v>
       </c>
       <c r="B22" t="s">
-        <v>77</v>
+        <v>163</v>
       </c>
       <c r="C22" t="s">
-        <v>109</v>
-      </c>
-      <c r="D22" s="1" t="s">
-        <v>268</v>
-      </c>
-      <c r="E22" s="12" t="s">
-        <v>51</v>
-      </c>
-      <c r="F22" t="s">
+        <v>193</v>
+      </c>
+      <c r="D22" s="20" t="s">
+        <v>282</v>
+      </c>
+      <c r="E22" s="19" t="s">
+        <v>281</v>
+      </c>
+      <c r="F22" s="18" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:6" ht="37.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>202</v>
       </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B23" t="s">
+        <v>77</v>
+      </c>
+      <c r="C23" t="s">
+        <v>109</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>266</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>267</v>
+      </c>
+      <c r="F23" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>202</v>
+        <v>203</v>
+      </c>
+      <c r="B24" t="s">
+        <v>77</v>
+      </c>
+      <c r="C24" t="s">
+        <v>109</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>268</v>
+      </c>
+      <c r="E24" s="12" t="s">
+        <v>51</v>
+      </c>
+      <c r="F24" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
     </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
     </row>
     <row r="39" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
     </row>
     <row r="40" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
     </row>
     <row r="41" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
     </row>
     <row r="42" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
     </row>
     <row r="43" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
     </row>
     <row r="44" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
     </row>
     <row r="45" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
     </row>
     <row r="46" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
     </row>
     <row r="47" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
     </row>
     <row r="48" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
     </row>
     <row r="49" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
     </row>
     <row r="50" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
     </row>
     <row r="51" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
     </row>
     <row r="52" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
     </row>
     <row r="53" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
     </row>
     <row r="54" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
     </row>
     <row r="55" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
     </row>
     <row r="56" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
     </row>
     <row r="57" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
     </row>
     <row r="58" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
     </row>
     <row r="59" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
     </row>
     <row r="60" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
     </row>
     <row r="61" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
     </row>
     <row r="62" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
     </row>
     <row r="63" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
     </row>
     <row r="64" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
     </row>
     <row r="65" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
     </row>
     <row r="66" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
     </row>
     <row r="67" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
     </row>
     <row r="68" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
     </row>
     <row r="69" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="70" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
     </row>
     <row r="71" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
     </row>
     <row r="72" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
     </row>
     <row r="73" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
     </row>
     <row r="74" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
     </row>
     <row r="75" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
     </row>
     <row r="76" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
     </row>
     <row r="77" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
     </row>
     <row r="78" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="79" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A79" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="80" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A80" t="s">
         <v>256</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -3379,7 +3517,7 @@
   <dimension ref="A1:J32"/>
   <sheetViews>
     <sheetView topLeftCell="A7" zoomScale="150" workbookViewId="0">
-      <selection activeCell="I22" sqref="I22"/>
+      <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -3565,8 +3703,8 @@
       <c r="B14" t="s">
         <v>193</v>
       </c>
-      <c r="C14" t="s">
-        <v>269</v>
+      <c r="C14" s="18" t="s">
+        <v>283</v>
       </c>
       <c r="D14" t="s">
         <v>72</v>
@@ -3581,7 +3719,7 @@
         <v>45</v>
       </c>
       <c r="H14">
-        <v>102</v>
+        <v>162</v>
       </c>
       <c r="I14">
         <v>60</v>
@@ -3595,7 +3733,7 @@
         <v>192</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="D15" t="s">
         <v>72</v>
@@ -3604,10 +3742,10 @@
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="D16" t="s">
         <v>72</v>
@@ -3615,10 +3753,10 @@
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
+        <v>272</v>
+      </c>
+      <c r="B17" s="1" t="s">
         <v>274</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>276</v>
       </c>
       <c r="D17" t="s">
         <v>72</v>
@@ -3629,7 +3767,7 @@
         <v>187</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="D18" t="s">
         <v>72</v>
@@ -3649,8 +3787,8 @@
       <c r="B20" t="s">
         <v>109</v>
       </c>
-      <c r="C20" s="1" t="s">
-        <v>270</v>
+      <c r="C20" s="20" t="s">
+        <v>284</v>
       </c>
       <c r="D20" t="s">
         <v>72</v>
@@ -3679,7 +3817,7 @@
         <v>192</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="D21" t="s">
         <v>72</v>
@@ -3688,10 +3826,10 @@
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="D22" t="s">
         <v>72</v>
@@ -3699,10 +3837,10 @@
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="J23" s="7"/>
     </row>
@@ -3758,7 +3896,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J1"/>
   <sheetViews>
-    <sheetView topLeftCell="A25" zoomScale="150" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="150" workbookViewId="0">
       <selection activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
complete 2 user stories
along with the team report
</commit_message>
<xml_diff>
--- a/Team05Report.xlsx
+++ b/Team05Report.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="240" windowWidth="20730" windowHeight="11760" tabRatio="500" activeTab="6"/>
+    <workbookView xWindow="240" yWindow="240" windowWidth="20730" windowHeight="11760" tabRatio="500" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Team" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
     <sheet name="Sprint4" sheetId="6" r:id="rId9"/>
     <sheet name="Sprint5" sheetId="8" r:id="rId10"/>
   </sheets>
-  <calcPr calcId="145621" concurrentCalc="0"/>
+  <calcPr calcId="124519" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -62,7 +62,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="495" uniqueCount="287">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="552" uniqueCount="315">
   <si>
     <t>Date</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -930,15 +930,9 @@
     <t>Get current date(year, month, day)</t>
   </si>
   <si>
-    <t>T01.02</t>
-  </si>
-  <si>
     <t>Get every date from stored structure</t>
   </si>
   <si>
-    <t>T01.03</t>
-  </si>
-  <si>
     <t>check if the event date of individual or family is after current date</t>
   </si>
   <si>
@@ -979,17 +973,107 @@
   </si>
   <si>
     <t>Every person must have completed information(name, sex, birthday) and every family must have completed information(marriage date)</t>
+  </si>
+  <si>
+    <t>Family F1 doesn't have information of a husband</t>
+  </si>
+  <si>
+    <t>Family F3 doesn't have information of a wife</t>
+  </si>
+  <si>
+    <t>Family F2 has 2 husbands: I2 and I4</t>
+  </si>
+  <si>
+    <t>Family F1 does not have a husband.</t>
+  </si>
+  <si>
+    <t>Family F3 does not have a wife.</t>
+  </si>
+  <si>
+    <t>Family F2 has 2 husbands: I2(Jianguo /Mao/), I4(Edwin /Moore/).</t>
+  </si>
+  <si>
+    <t>Famil F2's wife I3(Katie /Brown/) is not FEMALE.</t>
+  </si>
+  <si>
+    <t>Famil F4's husdband I8(Kevin /Brown/) is not MALE.</t>
+  </si>
+  <si>
+    <t>Individual I3 of family F2 is a male</t>
+  </si>
+  <si>
+    <t>Individual I8 of family F4 is a female</t>
+  </si>
+  <si>
+    <t>AT24~A26</t>
+  </si>
+  <si>
+    <t>AT24~AT26</t>
+  </si>
+  <si>
+    <t>AT27~AT28</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Find all the husbands and wives in each family </t>
+  </si>
+  <si>
+    <t>count the amount of husbands and wives respectively</t>
+  </si>
+  <si>
+    <t>check the amount is less, equal or greater than one</t>
+  </si>
+  <si>
+    <t>Get the sex of a husband and the sex of a wife in a family</t>
+  </si>
+  <si>
+    <t>T03.01</t>
+  </si>
+  <si>
+    <t>T03.02</t>
+  </si>
+  <si>
+    <t>T03.03</t>
+  </si>
+  <si>
+    <t>T03.04</t>
+  </si>
+  <si>
+    <t>T05.01</t>
+  </si>
+  <si>
+    <t>T05.02</t>
+  </si>
+  <si>
+    <t>T05.03</t>
+  </si>
+  <si>
+    <t>T04.01</t>
+  </si>
+  <si>
+    <t>T04.02</t>
+  </si>
+  <si>
+    <t>T04.03</t>
+  </si>
+  <si>
+    <t>T06.01</t>
+  </si>
+  <si>
+    <t>T06.02</t>
+  </si>
+  <si>
+    <t>check if the husband is a male and the wife is a female</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="m/d"/>
     <numFmt numFmtId="165" formatCode="0.0"/>
   </numFmts>
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="10">
     <font>
       <sz val="10"/>
       <name val="Verdana"/>
@@ -1219,22 +1303,11 @@
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="1"/>
   <c:lang val="en-US"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
   <c:chart>
-    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
       <c:lineChart>
         <c:grouping val="standard"/>
-        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
@@ -1268,62 +1341,46 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:smooth val="0"/>
         </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
+        <c:dLbls/>
         <c:marker val="1"/>
-        <c:smooth val="0"/>
-        <c:axId val="104432000"/>
-        <c:axId val="104433536"/>
+        <c:axId val="111040768"/>
+        <c:axId val="111042560"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="104432000"/>
+        <c:axId val="111040768"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
-        <c:delete val="0"/>
         <c:axPos val="b"/>
         <c:numFmt formatCode="m/d" sourceLinked="1"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="104433536"/>
+        <c:crossAx val="111042560"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
         <c:baseTimeUnit val="days"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="104433536"/>
+        <c:axId val="111042560"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
-        <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="104432000"/>
+        <c:crossAx val="111040768"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="1" l="0.75000000000000089" r="0.75000000000000089" t="1" header="0.5" footer="0.5"/>
+    <c:pageMargins b="1" l="0.750000000000001" r="0.750000000000001" t="1" header="0.5" footer="0.5"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1683,14 +1740,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView zoomScale="150" workbookViewId="0">
       <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75"/>
   <cols>
     <col min="1" max="1" width="7.625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="6.375" customWidth="1"/>
@@ -1699,7 +1756,7 @@
     <col min="5" max="5" width="19.25" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" s="4" customFormat="1">
       <c r="A1" s="4" t="s">
         <v>22</v>
       </c>
@@ -1716,7 +1773,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5">
       <c r="A3" t="s">
         <v>72</v>
       </c>
@@ -1733,7 +1790,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5">
       <c r="A4" t="s">
         <v>135</v>
       </c>
@@ -1750,9 +1807,9 @@
         <v>139</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5">
       <c r="A5" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="B5" t="s">
         <v>140</v>
@@ -1767,7 +1824,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:5">
       <c r="D9" s="4" t="s">
         <v>69</v>
       </c>
@@ -1796,16 +1853,16 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:J1"/>
   <sheetViews>
     <sheetView zoomScale="150" workbookViewId="0">
       <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75"/>
   <sheetData>
-    <row r="1" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" ht="25.5">
       <c r="A1" s="4" t="s">
         <v>3</v>
       </c>
@@ -1849,14 +1906,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:L26"/>
   <sheetViews>
-    <sheetView zoomScale="150" workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
+    <sheetView topLeftCell="C1" zoomScale="150" workbookViewId="0">
+      <selection activeCell="F7" sqref="F7:K7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75"/>
   <cols>
     <col min="1" max="1" width="6.625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="8.875" bestFit="1" customWidth="1"/>
@@ -1872,7 +1929,7 @@
     <col min="12" max="12" width="10.75" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:12" s="4" customFormat="1">
       <c r="A1" s="4" t="s">
         <v>40</v>
       </c>
@@ -1910,7 +1967,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:12">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1948,7 +2005,7 @@
         <v>40598</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:12">
       <c r="A3">
         <v>1</v>
       </c>
@@ -1986,7 +2043,7 @@
         <v>40598</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:12">
       <c r="A4">
         <v>1</v>
       </c>
@@ -1997,7 +2054,7 @@
         <v>193</v>
       </c>
       <c r="D4" s="18" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="E4" t="s">
         <v>194</v>
@@ -2024,18 +2081,45 @@
         <v>40598</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:12">
+      <c r="A5">
+        <v>1</v>
+      </c>
       <c r="B5" t="s">
         <v>76</v>
       </c>
       <c r="C5" t="s">
         <v>118</v>
       </c>
+      <c r="D5" s="18" t="s">
+        <v>296</v>
+      </c>
+      <c r="E5" s="18" t="s">
+        <v>276</v>
+      </c>
+      <c r="F5" s="18" t="s">
+        <v>183</v>
+      </c>
+      <c r="G5">
+        <v>80</v>
+      </c>
+      <c r="H5">
+        <v>45</v>
+      </c>
+      <c r="I5">
+        <v>44</v>
+      </c>
+      <c r="J5">
+        <v>45</v>
+      </c>
+      <c r="K5" s="16">
+        <v>40601</v>
+      </c>
       <c r="L5" s="7">
         <v>40598</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:12">
       <c r="A6">
         <v>1</v>
       </c>
@@ -2046,7 +2130,7 @@
         <v>109</v>
       </c>
       <c r="D6" s="18" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="E6" t="s">
         <v>194</v>
@@ -2073,18 +2157,45 @@
         <v>40598</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:12">
+      <c r="A7">
+        <v>1</v>
+      </c>
       <c r="B7" t="s">
         <v>78</v>
       </c>
       <c r="C7" t="s">
         <v>112</v>
       </c>
+      <c r="D7" s="18" t="s">
+        <v>297</v>
+      </c>
+      <c r="E7" s="18" t="s">
+        <v>276</v>
+      </c>
+      <c r="F7" s="18" t="s">
+        <v>183</v>
+      </c>
+      <c r="G7">
+        <v>50</v>
+      </c>
+      <c r="H7">
+        <v>25</v>
+      </c>
+      <c r="I7">
+        <v>27</v>
+      </c>
+      <c r="J7">
+        <v>20</v>
+      </c>
+      <c r="K7" s="16">
+        <v>40602</v>
+      </c>
       <c r="L7" s="7">
         <v>40598</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:12">
       <c r="B8" t="s">
         <v>79</v>
       </c>
@@ -2095,7 +2206,7 @@
         <v>40598</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:12">
       <c r="B9" t="s">
         <v>80</v>
       </c>
@@ -2106,7 +2217,7 @@
         <v>40598</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:12">
       <c r="B10" t="s">
         <v>81</v>
       </c>
@@ -2117,7 +2228,7 @@
         <v>40598</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:12">
       <c r="B11" t="s">
         <v>82</v>
       </c>
@@ -2128,7 +2239,7 @@
         <v>40598</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:12">
       <c r="B12" t="s">
         <v>83</v>
       </c>
@@ -2139,7 +2250,7 @@
         <v>40598</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:12">
       <c r="B13" t="s">
         <v>84</v>
       </c>
@@ -2150,7 +2261,7 @@
         <v>40598</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:12">
       <c r="B14" t="s">
         <v>85</v>
       </c>
@@ -2161,7 +2272,7 @@
         <v>40598</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:12">
       <c r="B15" t="s">
         <v>86</v>
       </c>
@@ -2172,7 +2283,7 @@
         <v>40598</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:12">
       <c r="B16" t="s">
         <v>87</v>
       </c>
@@ -2183,7 +2294,7 @@
         <v>40598</v>
       </c>
     </row>
-    <row r="17" spans="2:12" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:12">
       <c r="B17" t="s">
         <v>88</v>
       </c>
@@ -2194,7 +2305,7 @@
         <v>40598</v>
       </c>
     </row>
-    <row r="18" spans="2:12" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:12">
       <c r="B18" t="s">
         <v>89</v>
       </c>
@@ -2205,7 +2316,7 @@
         <v>40598</v>
       </c>
     </row>
-    <row r="19" spans="2:12" x14ac:dyDescent="0.2">
+    <row r="19" spans="2:12">
       <c r="B19" t="s">
         <v>90</v>
       </c>
@@ -2216,7 +2327,7 @@
         <v>40598</v>
       </c>
     </row>
-    <row r="20" spans="2:12" x14ac:dyDescent="0.2">
+    <row r="20" spans="2:12">
       <c r="B20" t="s">
         <v>91</v>
       </c>
@@ -2227,7 +2338,7 @@
         <v>40598</v>
       </c>
     </row>
-    <row r="21" spans="2:12" x14ac:dyDescent="0.2">
+    <row r="21" spans="2:12">
       <c r="B21" t="s">
         <v>92</v>
       </c>
@@ -2238,7 +2349,7 @@
         <v>40598</v>
       </c>
     </row>
-    <row r="22" spans="2:12" x14ac:dyDescent="0.2">
+    <row r="22" spans="2:12">
       <c r="B22" t="s">
         <v>93</v>
       </c>
@@ -2249,28 +2360,28 @@
         <v>40598</v>
       </c>
     </row>
-    <row r="23" spans="2:12" x14ac:dyDescent="0.2">
+    <row r="23" spans="2:12">
       <c r="B23" t="s">
         <v>94</v>
       </c>
       <c r="C23" s="18" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="L23" s="7">
         <v>40602</v>
       </c>
     </row>
-    <row r="24" spans="2:12" x14ac:dyDescent="0.2">
+    <row r="24" spans="2:12">
       <c r="B24" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="25" spans="2:12" x14ac:dyDescent="0.2">
+    <row r="25" spans="2:12">
       <c r="B25" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="26" spans="2:12" x14ac:dyDescent="0.2">
+    <row r="26" spans="2:12">
       <c r="B26" t="s">
         <v>97</v>
       </c>
@@ -2288,14 +2399,14 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F28"/>
   <sheetViews>
     <sheetView zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75"/>
   <cols>
     <col min="1" max="1" width="8.875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="24.75" bestFit="1" customWidth="1"/>
@@ -2304,7 +2415,7 @@
     <col min="6" max="6" width="9" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6">
       <c r="A1" s="4" t="s">
         <v>28</v>
       </c>
@@ -2324,7 +2435,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" ht="25.5">
       <c r="A2" t="s">
         <v>31</v>
       </c>
@@ -2344,7 +2455,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" ht="25.5">
       <c r="A3" t="s">
         <v>32</v>
       </c>
@@ -2364,7 +2475,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6">
       <c r="A4" t="s">
         <v>34</v>
       </c>
@@ -2375,7 +2486,7 @@
         <v>128</v>
       </c>
       <c r="D4" s="18" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="E4">
         <v>80</v>
@@ -2384,7 +2495,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6">
       <c r="A5" t="s">
         <v>76</v>
       </c>
@@ -2395,7 +2506,7 @@
         <v>120</v>
       </c>
       <c r="D5" s="18" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="E5">
         <v>20</v>
@@ -2404,7 +2515,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6">
       <c r="A6" t="s">
         <v>77</v>
       </c>
@@ -2414,8 +2525,17 @@
       <c r="C6" s="1" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="D6" s="18" t="s">
+        <v>295</v>
+      </c>
+      <c r="E6">
+        <v>80</v>
+      </c>
+      <c r="F6">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
       <c r="A7" t="s">
         <v>78</v>
       </c>
@@ -2425,8 +2545,17 @@
       <c r="C7" s="1" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="D7" s="18" t="s">
+        <v>297</v>
+      </c>
+      <c r="E7">
+        <v>50</v>
+      </c>
+      <c r="F7">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
       <c r="A8" t="s">
         <v>79</v>
       </c>
@@ -2437,7 +2566,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:6">
       <c r="A9" t="s">
         <v>80</v>
       </c>
@@ -2448,7 +2577,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:6">
       <c r="A10" t="s">
         <v>81</v>
       </c>
@@ -2459,7 +2588,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:6">
       <c r="A11" t="s">
         <v>82</v>
       </c>
@@ -2470,7 +2599,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:6">
       <c r="A12" t="s">
         <v>83</v>
       </c>
@@ -2481,7 +2610,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:6">
       <c r="A13" t="s">
         <v>84</v>
       </c>
@@ -2492,7 +2621,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:6" ht="25.5">
       <c r="A14" t="s">
         <v>85</v>
       </c>
@@ -2503,7 +2632,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:6">
       <c r="A15" t="s">
         <v>86</v>
       </c>
@@ -2514,7 +2643,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:6">
       <c r="A16" t="s">
         <v>87</v>
       </c>
@@ -2525,7 +2654,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:3">
       <c r="A17" t="s">
         <v>88</v>
       </c>
@@ -2536,7 +2665,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:3">
       <c r="A18" t="s">
         <v>89</v>
       </c>
@@ -2547,7 +2676,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:3" ht="25.5">
       <c r="A19" t="s">
         <v>90</v>
       </c>
@@ -2558,7 +2687,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:3">
       <c r="A20" t="s">
         <v>91</v>
       </c>
@@ -2569,7 +2698,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:3">
       <c r="A21" t="s">
         <v>92</v>
       </c>
@@ -2580,7 +2709,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:3">
       <c r="A22" t="s">
         <v>93</v>
       </c>
@@ -2591,38 +2720,38 @@
         <v>132</v>
       </c>
     </row>
-    <row r="23" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:3" ht="25.5">
       <c r="A23" t="s">
         <v>94</v>
       </c>
       <c r="B23" s="18" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="C23" s="20" t="s">
-        <v>286</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3">
       <c r="A24" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:3">
       <c r="A25" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:3">
       <c r="A26" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:3">
       <c r="A27" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:3">
       <c r="A28" t="s">
         <v>102</v>
       </c>
@@ -2639,14 +2768,14 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F80"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" zoomScale="145" zoomScaleNormal="145" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="H23" sqref="H23"/>
+    <sheetView topLeftCell="A22" zoomScale="145" zoomScaleNormal="145" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="E29" sqref="E29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75"/>
   <cols>
     <col min="1" max="1" width="6.375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="8.875" bestFit="1" customWidth="1"/>
@@ -2656,7 +2785,7 @@
     <col min="6" max="6" width="7.25" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6">
       <c r="A1" s="4" t="s">
         <v>61</v>
       </c>
@@ -2676,7 +2805,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" ht="47.25">
       <c r="A2" t="s">
         <v>54</v>
       </c>
@@ -2696,7 +2825,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" ht="47.25">
       <c r="A3" t="s">
         <v>55</v>
       </c>
@@ -2716,7 +2845,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" ht="47.25">
       <c r="A4" t="s">
         <v>56</v>
       </c>
@@ -2736,7 +2865,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" ht="47.25">
       <c r="A5" t="s">
         <v>57</v>
       </c>
@@ -2756,7 +2885,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" ht="47.25">
       <c r="A6" t="s">
         <v>58</v>
       </c>
@@ -2776,7 +2905,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" ht="31.5">
       <c r="A7" t="s">
         <v>59</v>
       </c>
@@ -2796,7 +2925,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="63" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" ht="63">
       <c r="A8" t="s">
         <v>157</v>
       </c>
@@ -2816,7 +2945,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="63" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" ht="63">
       <c r="A9" t="s">
         <v>161</v>
       </c>
@@ -2836,7 +2965,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="78.75" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" ht="78.75">
       <c r="A10" t="s">
         <v>162</v>
       </c>
@@ -2856,7 +2985,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="63" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" ht="63">
       <c r="A11" t="s">
         <v>164</v>
       </c>
@@ -2876,7 +3005,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="63" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" ht="63">
       <c r="A12" t="s">
         <v>165</v>
       </c>
@@ -2896,7 +3025,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="78.75" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" ht="78.75">
       <c r="A13" t="s">
         <v>166</v>
       </c>
@@ -2916,7 +3045,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" ht="47.25">
       <c r="A14" t="s">
         <v>177</v>
       </c>
@@ -2936,7 +3065,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" ht="47.25">
       <c r="A15" t="s">
         <v>179</v>
       </c>
@@ -2956,7 +3085,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="16" spans="1:6" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:6" ht="38.25">
       <c r="A16" t="s">
         <v>195</v>
       </c>
@@ -2976,7 +3105,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="17" spans="1:6" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:6" ht="38.25">
       <c r="A17" t="s">
         <v>196</v>
       </c>
@@ -2996,7 +3125,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="18" spans="1:6" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:6" ht="38.25">
       <c r="A18" t="s">
         <v>197</v>
       </c>
@@ -3016,7 +3145,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="19" spans="1:6" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:6" ht="38.25">
       <c r="A19" t="s">
         <v>198</v>
       </c>
@@ -3036,7 +3165,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="20" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" ht="26.25">
       <c r="A20" t="s">
         <v>199</v>
       </c>
@@ -3056,7 +3185,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="21" spans="1:6" ht="47.25" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:6" ht="47.25">
       <c r="A21" t="s">
         <v>200</v>
       </c>
@@ -3067,16 +3196,16 @@
         <v>193</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="E21" s="17" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="F21" s="18" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="22" spans="1:6" ht="47.25" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:6" ht="47.25">
       <c r="A22" t="s">
         <v>201</v>
       </c>
@@ -3087,16 +3216,16 @@
         <v>193</v>
       </c>
       <c r="D22" s="20" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="E22" s="19" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="F22" s="18" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="23" spans="1:6" ht="37.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:6" ht="37.5" customHeight="1">
       <c r="A23" t="s">
         <v>202</v>
       </c>
@@ -3116,7 +3245,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="24" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" ht="26.25">
       <c r="A24" t="s">
         <v>203</v>
       </c>
@@ -3136,282 +3265,357 @@
         <v>53</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:6" ht="25.5">
       <c r="A25" t="s">
         <v>202</v>
       </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B25" t="s">
+        <v>76</v>
+      </c>
+      <c r="C25" t="s">
+        <v>118</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>285</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>288</v>
+      </c>
+      <c r="F25" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6">
       <c r="A26" t="s">
         <v>202</v>
       </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B26" t="s">
+        <v>76</v>
+      </c>
+      <c r="C26" t="s">
+        <v>118</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>286</v>
+      </c>
+      <c r="E26" s="1" t="s">
+        <v>289</v>
+      </c>
+      <c r="F26" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6">
       <c r="A27" t="s">
         <v>203</v>
       </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B27" t="s">
+        <v>76</v>
+      </c>
+      <c r="C27" t="s">
+        <v>118</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>287</v>
+      </c>
+      <c r="E27" s="1" t="s">
+        <v>290</v>
+      </c>
+      <c r="F27" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" ht="25.5">
       <c r="A28" t="s">
         <v>204</v>
       </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B28" t="s">
+        <v>78</v>
+      </c>
+      <c r="C28" t="s">
+        <v>112</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>293</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>291</v>
+      </c>
+      <c r="F28" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" ht="25.5">
       <c r="A29" t="s">
         <v>205</v>
       </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B29" t="s">
+        <v>78</v>
+      </c>
+      <c r="C29" t="s">
+        <v>112</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>294</v>
+      </c>
+      <c r="E29" s="1" t="s">
+        <v>292</v>
+      </c>
+      <c r="F29" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6">
       <c r="A30" t="s">
         <v>206</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:6">
       <c r="A31" t="s">
         <v>207</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:6">
       <c r="A32" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:1">
       <c r="A33" t="s">
         <v>209</v>
       </c>
     </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:1">
       <c r="A34" t="s">
         <v>210</v>
       </c>
     </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:1">
       <c r="A35" t="s">
         <v>211</v>
       </c>
     </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:1">
       <c r="A36" t="s">
         <v>212</v>
       </c>
     </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:1">
       <c r="A37" t="s">
         <v>213</v>
       </c>
     </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:1">
       <c r="A38" t="s">
         <v>214</v>
       </c>
     </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:1">
       <c r="A39" t="s">
         <v>215</v>
       </c>
     </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:1">
       <c r="A40" t="s">
         <v>216</v>
       </c>
     </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:1">
       <c r="A41" t="s">
         <v>217</v>
       </c>
     </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:1">
       <c r="A42" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:1">
       <c r="A43" t="s">
         <v>219</v>
       </c>
     </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:1">
       <c r="A44" t="s">
         <v>220</v>
       </c>
     </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:1">
       <c r="A45" t="s">
         <v>221</v>
       </c>
     </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:1">
       <c r="A46" t="s">
         <v>222</v>
       </c>
     </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:1">
       <c r="A47" t="s">
         <v>223</v>
       </c>
     </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:1">
       <c r="A48" t="s">
         <v>224</v>
       </c>
     </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:1">
       <c r="A49" t="s">
         <v>225</v>
       </c>
     </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:1">
       <c r="A50" t="s">
         <v>226</v>
       </c>
     </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:1">
       <c r="A51" t="s">
         <v>227</v>
       </c>
     </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:1">
       <c r="A52" t="s">
         <v>228</v>
       </c>
     </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:1">
       <c r="A53" t="s">
         <v>229</v>
       </c>
     </row>
-    <row r="54" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:1">
       <c r="A54" t="s">
         <v>230</v>
       </c>
     </row>
-    <row r="55" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:1">
       <c r="A55" t="s">
         <v>231</v>
       </c>
     </row>
-    <row r="56" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:1">
       <c r="A56" t="s">
         <v>232</v>
       </c>
     </row>
-    <row r="57" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:1">
       <c r="A57" t="s">
         <v>233</v>
       </c>
     </row>
-    <row r="58" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:1">
       <c r="A58" t="s">
         <v>234</v>
       </c>
     </row>
-    <row r="59" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:1">
       <c r="A59" t="s">
         <v>235</v>
       </c>
     </row>
-    <row r="60" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:1">
       <c r="A60" t="s">
         <v>236</v>
       </c>
     </row>
-    <row r="61" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:1">
       <c r="A61" t="s">
         <v>237</v>
       </c>
     </row>
-    <row r="62" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:1">
       <c r="A62" t="s">
         <v>238</v>
       </c>
     </row>
-    <row r="63" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:1">
       <c r="A63" t="s">
         <v>239</v>
       </c>
     </row>
-    <row r="64" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:1">
       <c r="A64" t="s">
         <v>240</v>
       </c>
     </row>
-    <row r="65" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:1">
       <c r="A65" t="s">
         <v>241</v>
       </c>
     </row>
-    <row r="66" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:1">
       <c r="A66" t="s">
         <v>242</v>
       </c>
     </row>
-    <row r="67" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:1">
       <c r="A67" t="s">
         <v>243</v>
       </c>
     </row>
-    <row r="68" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:1">
       <c r="A68" t="s">
         <v>244</v>
       </c>
     </row>
-    <row r="69" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:1">
       <c r="A69" t="s">
         <v>245</v>
       </c>
     </row>
-    <row r="70" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:1">
       <c r="A70" t="s">
         <v>246</v>
       </c>
     </row>
-    <row r="71" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:1">
       <c r="A71" t="s">
         <v>247</v>
       </c>
     </row>
-    <row r="72" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:1">
       <c r="A72" t="s">
         <v>248</v>
       </c>
     </row>
-    <row r="73" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:1">
       <c r="A73" t="s">
         <v>249</v>
       </c>
     </row>
-    <row r="74" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:1">
       <c r="A74" t="s">
         <v>250</v>
       </c>
     </row>
-    <row r="75" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:1">
       <c r="A75" t="s">
         <v>251</v>
       </c>
     </row>
-    <row r="76" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:1">
       <c r="A76" t="s">
         <v>252</v>
       </c>
     </row>
-    <row r="77" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:1">
       <c r="A77" t="s">
         <v>253</v>
       </c>
     </row>
-    <row r="78" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:1">
       <c r="A78" t="s">
         <v>254</v>
       </c>
     </row>
-    <row r="79" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:1">
       <c r="A79" t="s">
         <v>255</v>
       </c>
     </row>
-    <row r="80" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:1">
       <c r="A80" t="s">
         <v>256</v>
       </c>
@@ -3429,14 +3633,14 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView zoomScale="150" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75"/>
   <cols>
     <col min="1" max="1" width="10.75" style="2"/>
     <col min="2" max="2" width="18.125" bestFit="1" customWidth="1"/>
@@ -3446,7 +3650,7 @@
     <col min="6" max="6" width="13.75" style="9" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" s="4" customFormat="1">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -3466,7 +3670,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6">
       <c r="A2" s="2">
         <v>40598</v>
       </c>
@@ -3477,7 +3681,7 @@
         <v>598</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6">
       <c r="A3" s="2">
         <v>40602</v>
       </c>
@@ -3489,14 +3693,14 @@
         <v>6</v>
       </c>
       <c r="D3">
-        <v>908</v>
+        <v>1034</v>
       </c>
       <c r="E3">
-        <v>120</v>
+        <v>260</v>
       </c>
       <c r="F3" s="9">
         <f>(D3-D2)/E3*60</f>
-        <v>155</v>
+        <v>100.61538461538461</v>
       </c>
     </row>
   </sheetData>
@@ -3513,14 +3717,14 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J32"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:J40"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" zoomScale="150" workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="150" workbookViewId="0">
+      <selection activeCell="E30" sqref="E30:J30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75"/>
   <cols>
     <col min="1" max="1" width="8.875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="38.75" style="1" bestFit="1" customWidth="1"/>
@@ -3534,7 +3738,7 @@
     <col min="10" max="10" width="11" style="6" bestFit="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10">
       <c r="A1" s="4" t="s">
         <v>11</v>
       </c>
@@ -3566,7 +3770,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:10">
       <c r="A2" t="s">
         <v>31</v>
       </c>
@@ -3598,7 +3802,7 @@
         <v>40600</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:10" ht="25.5">
       <c r="A4" t="s">
         <v>192</v>
       </c>
@@ -3609,7 +3813,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:10" ht="25.5">
       <c r="A5" t="s">
         <v>41</v>
       </c>
@@ -3620,7 +3824,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="6" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:10" ht="25.5">
       <c r="A6" t="s">
         <v>42</v>
       </c>
@@ -3631,7 +3835,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="7" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:10" ht="25.5">
       <c r="A7" t="s">
         <v>187</v>
       </c>
@@ -3642,7 +3846,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:10">
       <c r="A9" t="s">
         <v>32</v>
       </c>
@@ -3674,7 +3878,7 @@
         <v>40601</v>
       </c>
     </row>
-    <row r="11" spans="1:10" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:10" ht="38.25">
       <c r="A11" t="s">
         <v>43</v>
       </c>
@@ -3685,7 +3889,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="12" spans="1:10" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:10" ht="38.25">
       <c r="A12" t="s">
         <v>44</v>
       </c>
@@ -3696,7 +3900,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:10">
       <c r="A14" t="s">
         <v>163</v>
       </c>
@@ -3704,7 +3908,7 @@
         <v>193</v>
       </c>
       <c r="C14" s="18" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="D14" t="s">
         <v>72</v>
@@ -3728,9 +3932,9 @@
         <v>40602</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:10">
       <c r="A15" t="s">
-        <v>192</v>
+        <v>302</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>269</v>
@@ -3740,47 +3944,44 @@
       </c>
       <c r="J15" s="7"/>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:10">
       <c r="A16" t="s">
+        <v>303</v>
+      </c>
+      <c r="B16" s="1" t="s">
         <v>270</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>271</v>
       </c>
       <c r="D16" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:10">
       <c r="A17" t="s">
+        <v>304</v>
+      </c>
+      <c r="B17" s="1" t="s">
         <v>272</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>274</v>
       </c>
       <c r="D17" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="18" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:10" ht="25.5">
       <c r="A18" t="s">
-        <v>187</v>
+        <v>305</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="D18" t="s">
         <v>72</v>
       </c>
       <c r="J18" s="7"/>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="D19" t="s">
-        <v>72</v>
-      </c>
+    <row r="19" spans="1:10">
       <c r="J19" s="7"/>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:10">
       <c r="A20" t="s">
         <v>77</v>
       </c>
@@ -3788,7 +3989,7 @@
         <v>109</v>
       </c>
       <c r="C20" s="20" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="D20" t="s">
         <v>72</v>
@@ -3812,71 +4013,198 @@
         <v>40602</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:10">
       <c r="A21" t="s">
-        <v>192</v>
+        <v>306</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="D21" t="s">
         <v>72</v>
       </c>
       <c r="J21" s="7"/>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:10">
       <c r="A22" t="s">
-        <v>270</v>
+        <v>307</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="D22" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:10">
       <c r="A23" t="s">
-        <v>272</v>
+        <v>308</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="J23" s="7"/>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:10">
       <c r="J24" s="7"/>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="B25" s="5" t="s">
+    <row r="25" spans="1:10">
+      <c r="A25" t="s">
+        <v>76</v>
+      </c>
+      <c r="B25" t="s">
+        <v>118</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>296</v>
+      </c>
+      <c r="D25" t="s">
+        <v>276</v>
+      </c>
+      <c r="E25" t="s">
+        <v>183</v>
+      </c>
+      <c r="F25">
+        <v>80</v>
+      </c>
+      <c r="G25">
+        <v>45</v>
+      </c>
+      <c r="H25">
+        <v>44</v>
+      </c>
+      <c r="I25">
+        <v>45</v>
+      </c>
+      <c r="J25" s="16">
+        <v>40601</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" ht="25.5">
+      <c r="A26" t="s">
+        <v>309</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>298</v>
+      </c>
+      <c r="D26" t="s">
+        <v>276</v>
+      </c>
+      <c r="J26" s="7"/>
+    </row>
+    <row r="27" spans="1:10" ht="25.5">
+      <c r="A27" t="s">
+        <v>310</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>299</v>
+      </c>
+      <c r="D27" t="s">
+        <v>276</v>
+      </c>
+      <c r="J27" s="7"/>
+    </row>
+    <row r="28" spans="1:10" ht="25.5">
+      <c r="A28" t="s">
+        <v>311</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>300</v>
+      </c>
+      <c r="D28" t="s">
+        <v>276</v>
+      </c>
+      <c r="J28" s="7"/>
+    </row>
+    <row r="29" spans="1:10">
+      <c r="J29" s="7"/>
+    </row>
+    <row r="30" spans="1:10">
+      <c r="A30" t="s">
+        <v>78</v>
+      </c>
+      <c r="B30" t="s">
+        <v>112</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>297</v>
+      </c>
+      <c r="D30" t="s">
+        <v>276</v>
+      </c>
+      <c r="E30" s="18" t="s">
+        <v>183</v>
+      </c>
+      <c r="F30">
+        <v>50</v>
+      </c>
+      <c r="G30">
+        <v>25</v>
+      </c>
+      <c r="H30">
+        <v>27</v>
+      </c>
+      <c r="I30">
+        <v>20</v>
+      </c>
+      <c r="J30" s="16">
+        <v>40602</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" ht="25.5">
+      <c r="A31" t="s">
+        <v>312</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>301</v>
+      </c>
+      <c r="D31" t="s">
+        <v>276</v>
+      </c>
+      <c r="J31" s="7"/>
+    </row>
+    <row r="32" spans="1:10" ht="25.5">
+      <c r="A32" t="s">
+        <v>313</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>314</v>
+      </c>
+      <c r="D32" t="s">
+        <v>276</v>
+      </c>
+      <c r="J32" s="7"/>
+    </row>
+    <row r="33" spans="2:2">
+      <c r="B33" s="5" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="B26" s="5"/>
-    </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="B27" s="5" t="s">
+    <row r="34" spans="2:2">
+      <c r="B34" s="5"/>
+    </row>
+    <row r="35" spans="2:2">
+      <c r="B35" s="5" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="B28" s="1" t="s">
+    <row r="36" spans="2:2">
+      <c r="B36" s="1" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="B29" s="1" t="s">
+    <row r="37" spans="2:2">
+      <c r="B37" s="1" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="B31" s="5" t="s">
+    <row r="39" spans="2:2">
+      <c r="B39" s="5" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="B32" s="1" t="s">
+    <row r="40" spans="2:2">
+      <c r="B40" s="1" t="s">
         <v>65</v>
       </c>
     </row>
@@ -3893,16 +4221,16 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:J1"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="150" workbookViewId="0">
+    <sheetView zoomScale="150" workbookViewId="0">
       <selection activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75"/>
   <sheetData>
-    <row r="1" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" ht="25.5">
       <c r="A1" s="4" t="s">
         <v>11</v>
       </c>
@@ -3947,16 +4275,16 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:J1"/>
   <sheetViews>
     <sheetView zoomScale="150" workbookViewId="0">
       <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75"/>
   <sheetData>
-    <row r="1" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" ht="25.5">
       <c r="A1" s="4" t="s">
         <v>3</v>
       </c>
@@ -4000,16 +4328,16 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:J1"/>
   <sheetViews>
     <sheetView zoomScale="150" workbookViewId="0">
       <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75"/>
   <sheetData>
-    <row r="1" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" ht="25.5">
       <c r="A1" s="4" t="s">
         <v>3</v>
       </c>

</xml_diff>

<commit_message>
add two more user stories
</commit_message>
<xml_diff>
--- a/Team05Report.xlsx
+++ b/Team05Report.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="240" windowWidth="20730" windowHeight="11760" tabRatio="500" activeTab="5"/>
+    <workbookView xWindow="240" yWindow="240" windowWidth="20730" windowHeight="11760" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Team" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
     <sheet name="Sprint4" sheetId="6" r:id="rId9"/>
     <sheet name="Sprint5" sheetId="8" r:id="rId10"/>
   </sheets>
-  <calcPr calcId="124519" concurrentCalc="0"/>
+  <calcPr calcId="125725" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -62,7 +62,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="552" uniqueCount="315">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="556" uniqueCount="317">
   <si>
     <t>Date</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -409,15 +409,6 @@
     <t>Make sure that in a family, father is a male and mother is a female</t>
   </si>
   <si>
-    <t>US26</t>
-  </si>
-  <si>
-    <t>Monogamy</t>
-  </si>
-  <si>
-    <t>US27</t>
-  </si>
-  <si>
     <t>Make sure that an individual's divorce date is &gt;= their marriage date</t>
   </si>
   <si>
@@ -428,9 +419,6 @@
   </si>
   <si>
     <t xml:space="preserve">Death before giving birth </t>
-  </si>
-  <si>
-    <t>An individual can't marry to their sibling unless they are not biologically related</t>
   </si>
   <si>
     <t>A man can't get married until 20, a woman can't get married until 18</t>
@@ -1063,6 +1051,24 @@
   </si>
   <si>
     <t>check if the husband is a male and the wife is a female</t>
+  </si>
+  <si>
+    <t>Divorce before giving birth</t>
+  </si>
+  <si>
+    <t>An individual can't marry to their sibling</t>
+  </si>
+  <si>
+    <t>Marriage to death person</t>
+  </si>
+  <si>
+    <t>Make sure that the spouses were all alive when they were married</t>
+  </si>
+  <si>
+    <t>Polygamy</t>
+  </si>
+  <si>
+    <t>If the parents were divorced in a family, make sure that all the children were born before the divorce date</t>
   </si>
 </sst>
 </file>
@@ -1238,56 +1244,56 @@
     </xf>
   </cellXfs>
   <cellStyles count="50">
-    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="30" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="32" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="34" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="36" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="38" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="40" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="44" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="46" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="48" builtinId="9" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="29" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="31" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="33" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="35" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="37" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="39" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="41" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="43" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="45" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="47" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="49" builtinId="8"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="已访问的超链接" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="20" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="22" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="24" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="26" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="28" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="30" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="32" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="34" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="36" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="38" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="40" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="42" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="44" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="46" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="48" builtinId="9" hidden="1"/>
+    <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle name="超链接" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="15" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="17" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="19" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="21" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="23" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="25" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="27" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="29" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="31" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="33" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="35" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="37" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="39" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="41" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="43" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="45" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="47" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="49" builtinId="8"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
@@ -1342,27 +1348,26 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:dLbls/>
         <c:marker val="1"/>
-        <c:axId val="111040768"/>
-        <c:axId val="111042560"/>
+        <c:axId val="223820032"/>
+        <c:axId val="223821824"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="111040768"/>
+        <c:axId val="223820032"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="m/d" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="111042560"/>
+        <c:crossAx val="223821824"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
         <c:baseTimeUnit val="days"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="111042560"/>
+        <c:axId val="223821824"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1370,7 +1375,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="111040768"/>
+        <c:crossAx val="223820032"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1380,7 +1385,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="1" l="0.750000000000001" r="0.750000000000001" t="1" header="0.5" footer="0.5"/>
+    <c:pageMargins b="1" l="0.75000000000000133" r="0.75000000000000133" t="1" header="0.5" footer="0.5"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1792,36 +1797,36 @@
     </row>
     <row r="4" spans="1:5">
       <c r="A4" t="s">
+        <v>131</v>
+      </c>
+      <c r="B4" t="s">
+        <v>132</v>
+      </c>
+      <c r="C4" t="s">
+        <v>133</v>
+      </c>
+      <c r="D4" s="14" t="s">
+        <v>134</v>
+      </c>
+      <c r="E4" t="s">
         <v>135</v>
-      </c>
-      <c r="B4" t="s">
-        <v>136</v>
-      </c>
-      <c r="C4" t="s">
-        <v>137</v>
-      </c>
-      <c r="D4" s="14" t="s">
-        <v>138</v>
-      </c>
-      <c r="E4" t="s">
-        <v>139</v>
       </c>
     </row>
     <row r="5" spans="1:5">
       <c r="A5" t="s">
-        <v>276</v>
+        <v>272</v>
       </c>
       <c r="B5" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="C5" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="D5" s="14" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="E5" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
     </row>
     <row r="9" spans="1:5">
@@ -1910,7 +1915,7 @@
   <dimension ref="A1:L26"/>
   <sheetViews>
     <sheetView topLeftCell="C1" zoomScale="150" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7:K7"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75"/>
@@ -1975,13 +1980,13 @@
         <v>31</v>
       </c>
       <c r="C2" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="D2" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="E2" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="F2" t="s">
         <v>35</v>
@@ -1993,7 +1998,7 @@
         <v>60</v>
       </c>
       <c r="I2">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="J2">
         <v>60</v>
@@ -2013,16 +2018,16 @@
         <v>32</v>
       </c>
       <c r="C3" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="D3" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
       <c r="E3" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="F3" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
       <c r="G3">
         <v>50</v>
@@ -2031,7 +2036,7 @@
         <v>40</v>
       </c>
       <c r="I3">
-        <v>72</v>
+        <v>90</v>
       </c>
       <c r="J3">
         <v>45</v>
@@ -2051,16 +2056,16 @@
         <v>34</v>
       </c>
       <c r="C4" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="D4" s="18" t="s">
-        <v>281</v>
+        <v>277</v>
       </c>
       <c r="E4" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="F4" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
       <c r="G4">
         <v>80</v>
@@ -2089,16 +2094,16 @@
         <v>76</v>
       </c>
       <c r="C5" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="D5" s="18" t="s">
-        <v>296</v>
+        <v>292</v>
       </c>
       <c r="E5" s="18" t="s">
-        <v>276</v>
+        <v>272</v>
       </c>
       <c r="F5" s="18" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
       <c r="G5">
         <v>80</v>
@@ -2127,16 +2132,16 @@
         <v>77</v>
       </c>
       <c r="C6" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="D6" s="18" t="s">
-        <v>282</v>
+        <v>278</v>
       </c>
       <c r="E6" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="F6" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
       <c r="G6">
         <v>20</v>
@@ -2165,16 +2170,16 @@
         <v>78</v>
       </c>
       <c r="C7" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="D7" s="18" t="s">
-        <v>297</v>
+        <v>293</v>
       </c>
       <c r="E7" s="18" t="s">
-        <v>276</v>
+        <v>272</v>
       </c>
       <c r="F7" s="18" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
       <c r="G7">
         <v>50</v>
@@ -2200,7 +2205,7 @@
         <v>79</v>
       </c>
       <c r="C8" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="L8" s="7">
         <v>40598</v>
@@ -2211,7 +2216,7 @@
         <v>80</v>
       </c>
       <c r="C9" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="L9" s="7">
         <v>40598</v>
@@ -2222,7 +2227,7 @@
         <v>81</v>
       </c>
       <c r="C10" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="L10" s="7">
         <v>40598</v>
@@ -2244,7 +2249,7 @@
         <v>83</v>
       </c>
       <c r="C12" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="L12" s="7">
         <v>40598</v>
@@ -2255,7 +2260,7 @@
         <v>84</v>
       </c>
       <c r="C13" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="L13" s="7">
         <v>40598</v>
@@ -2266,7 +2271,7 @@
         <v>85</v>
       </c>
       <c r="C14" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="L14" s="7">
         <v>40598</v>
@@ -2277,7 +2282,7 @@
         <v>86</v>
       </c>
       <c r="C15" t="s">
-        <v>101</v>
+        <v>315</v>
       </c>
       <c r="L15" s="7">
         <v>40598</v>
@@ -2288,7 +2293,7 @@
         <v>87</v>
       </c>
       <c r="C16" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="L16" s="7">
         <v>40598</v>
@@ -2299,7 +2304,7 @@
         <v>88</v>
       </c>
       <c r="C17" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="L17" s="7">
         <v>40598</v>
@@ -2310,7 +2315,7 @@
         <v>89</v>
       </c>
       <c r="C18" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="L18" s="7">
         <v>40598</v>
@@ -2321,7 +2326,7 @@
         <v>90</v>
       </c>
       <c r="C19" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="L19" s="7">
         <v>40598</v>
@@ -2332,7 +2337,7 @@
         <v>91</v>
       </c>
       <c r="C20" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="L20" s="7">
         <v>40598</v>
@@ -2343,7 +2348,7 @@
         <v>92</v>
       </c>
       <c r="C21" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="L21" s="7">
         <v>40598</v>
@@ -2354,7 +2359,7 @@
         <v>93</v>
       </c>
       <c r="C22" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="L22" s="7">
         <v>40598</v>
@@ -2365,7 +2370,7 @@
         <v>94</v>
       </c>
       <c r="C23" s="18" t="s">
-        <v>283</v>
+        <v>279</v>
       </c>
       <c r="L23" s="7">
         <v>40602</v>
@@ -2375,10 +2380,22 @@
       <c r="B24" t="s">
         <v>95</v>
       </c>
+      <c r="C24" s="18" t="s">
+        <v>311</v>
+      </c>
+      <c r="L24" s="7">
+        <v>40602</v>
+      </c>
     </row>
     <row r="25" spans="2:12">
       <c r="B25" t="s">
         <v>96</v>
+      </c>
+      <c r="C25" s="18" t="s">
+        <v>313</v>
+      </c>
+      <c r="L25" s="7">
+        <v>40602</v>
       </c>
     </row>
     <row r="26" spans="2:12">
@@ -2400,10 +2417,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F28"/>
+  <dimension ref="A1:F26"/>
   <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75"/>
@@ -2440,13 +2457,13 @@
         <v>31</v>
       </c>
       <c r="B2" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="D2" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="E2">
         <v>150</v>
@@ -2460,13 +2477,13 @@
         <v>32</v>
       </c>
       <c r="B3" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="D3" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
       <c r="E3">
         <v>50</v>
@@ -2480,13 +2497,13 @@
         <v>34</v>
       </c>
       <c r="B4" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="D4" s="18" t="s">
-        <v>281</v>
+        <v>277</v>
       </c>
       <c r="E4">
         <v>80</v>
@@ -2500,13 +2517,13 @@
         <v>76</v>
       </c>
       <c r="B5" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="D5" s="18" t="s">
-        <v>282</v>
+        <v>278</v>
       </c>
       <c r="E5">
         <v>20</v>
@@ -2520,13 +2537,13 @@
         <v>77</v>
       </c>
       <c r="B6" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>46</v>
       </c>
       <c r="D6" s="18" t="s">
-        <v>295</v>
+        <v>291</v>
       </c>
       <c r="E6">
         <v>80</v>
@@ -2540,13 +2557,13 @@
         <v>78</v>
       </c>
       <c r="B7" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>99</v>
       </c>
       <c r="D7" s="18" t="s">
-        <v>297</v>
+        <v>293</v>
       </c>
       <c r="E7">
         <v>50</v>
@@ -2560,7 +2577,7 @@
         <v>79</v>
       </c>
       <c r="B8" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>98</v>
@@ -2571,10 +2588,10 @@
         <v>80</v>
       </c>
       <c r="B9" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
     </row>
     <row r="10" spans="1:6">
@@ -2582,10 +2599,10 @@
         <v>81</v>
       </c>
       <c r="B10" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
     </row>
     <row r="11" spans="1:6">
@@ -2604,7 +2621,7 @@
         <v>83</v>
       </c>
       <c r="B12" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>48</v>
@@ -2615,10 +2632,10 @@
         <v>84</v>
       </c>
       <c r="B13" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="25.5">
@@ -2626,10 +2643,10 @@
         <v>85</v>
       </c>
       <c r="B14" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
     </row>
     <row r="15" spans="1:6">
@@ -2637,10 +2654,10 @@
         <v>86</v>
       </c>
       <c r="B15" t="s">
-        <v>101</v>
+        <v>315</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
     </row>
     <row r="16" spans="1:6">
@@ -2648,10 +2665,10 @@
         <v>87</v>
       </c>
       <c r="B16" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>107</v>
+        <v>312</v>
       </c>
     </row>
     <row r="17" spans="1:3">
@@ -2659,10 +2676,10 @@
         <v>88</v>
       </c>
       <c r="B17" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
     </row>
     <row r="18" spans="1:3">
@@ -2670,10 +2687,10 @@
         <v>89</v>
       </c>
       <c r="B18" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
     </row>
     <row r="19" spans="1:3" ht="25.5">
@@ -2681,10 +2698,10 @@
         <v>90</v>
       </c>
       <c r="B19" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
     </row>
     <row r="20" spans="1:3">
@@ -2692,10 +2709,10 @@
         <v>91</v>
       </c>
       <c r="B20" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
     </row>
     <row r="21" spans="1:3">
@@ -2703,10 +2720,10 @@
         <v>92</v>
       </c>
       <c r="B21" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
     </row>
     <row r="22" spans="1:3">
@@ -2714,10 +2731,10 @@
         <v>93</v>
       </c>
       <c r="B22" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
     </row>
     <row r="23" spans="1:3" ht="25.5">
@@ -2725,35 +2742,37 @@
         <v>94</v>
       </c>
       <c r="B23" s="18" t="s">
-        <v>283</v>
+        <v>279</v>
       </c>
       <c r="C23" s="20" t="s">
-        <v>284</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" ht="25.5">
       <c r="A24" t="s">
         <v>95</v>
+      </c>
+      <c r="B24" s="18" t="s">
+        <v>311</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>316</v>
       </c>
     </row>
     <row r="25" spans="1:3">
       <c r="A25" t="s">
         <v>96</v>
       </c>
+      <c r="B25" s="18" t="s">
+        <v>313</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>314</v>
+      </c>
     </row>
     <row r="26" spans="1:3">
       <c r="A26" t="s">
         <v>97</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3">
-      <c r="A27" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3">
-      <c r="A28" t="s">
-        <v>102</v>
       </c>
     </row>
   </sheetData>
@@ -2813,13 +2832,13 @@
         <v>31</v>
       </c>
       <c r="C2" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="D2" s="13" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="E2" s="13" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="F2" t="s">
         <v>53</v>
@@ -2833,13 +2852,13 @@
         <v>31</v>
       </c>
       <c r="C3" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="D3" s="13" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="E3" s="15" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="F3" t="s">
         <v>53</v>
@@ -2850,16 +2869,16 @@
         <v>56</v>
       </c>
       <c r="B4" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="C4" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="D4" s="13" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="E4" s="13" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="F4" t="s">
         <v>53</v>
@@ -2870,16 +2889,16 @@
         <v>57</v>
       </c>
       <c r="B5" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="C5" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="D5" s="13" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="E5" s="15" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="F5" t="s">
         <v>53</v>
@@ -2890,16 +2909,16 @@
         <v>58</v>
       </c>
       <c r="B6" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="C6" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="D6" s="13" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="E6" s="13" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="F6" t="s">
         <v>53</v>
@@ -2910,13 +2929,13 @@
         <v>59</v>
       </c>
       <c r="B7" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="C7" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="D7" s="13" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="E7" s="12" t="s">
         <v>51</v>
@@ -2927,16 +2946,16 @@
     </row>
     <row r="8" spans="1:6" ht="63">
       <c r="A8" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="B8" t="s">
+        <v>151</v>
+      </c>
+      <c r="C8" t="s">
+        <v>107</v>
+      </c>
+      <c r="D8" s="13" t="s">
         <v>155</v>
-      </c>
-      <c r="C8" t="s">
-        <v>111</v>
-      </c>
-      <c r="D8" s="13" t="s">
-        <v>159</v>
       </c>
       <c r="E8" s="12" t="s">
         <v>51</v>
@@ -2947,19 +2966,19 @@
     </row>
     <row r="9" spans="1:6" ht="63">
       <c r="A9" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="B9" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="C9" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="D9" s="13" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="E9" s="15" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="F9" t="s">
         <v>53</v>
@@ -2967,19 +2986,19 @@
     </row>
     <row r="10" spans="1:6" ht="78.75">
       <c r="A10" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="B10" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="C10" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="D10" s="13" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="E10" s="15" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="F10" t="s">
         <v>53</v>
@@ -2987,19 +3006,19 @@
     </row>
     <row r="11" spans="1:6" ht="63">
       <c r="A11" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="B11" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="C11" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="D11" s="13" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="E11" s="15" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="F11" t="s">
         <v>53</v>
@@ -3007,19 +3026,19 @@
     </row>
     <row r="12" spans="1:6" ht="63">
       <c r="A12" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="B12" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="C12" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="D12" s="13" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="E12" s="15" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="F12" t="s">
         <v>53</v>
@@ -3027,19 +3046,19 @@
     </row>
     <row r="13" spans="1:6" ht="78.75">
       <c r="A13" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="B13" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="C13" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="D13" s="13" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
       <c r="E13" s="15" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="F13" t="s">
         <v>53</v>
@@ -3047,16 +3066,16 @@
     </row>
     <row r="14" spans="1:6" ht="47.25">
       <c r="A14" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
       <c r="B14" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="C14" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="D14" s="13" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
       <c r="E14" s="15" t="s">
         <v>51</v>
@@ -3067,16 +3086,16 @@
     </row>
     <row r="15" spans="1:6" ht="47.25">
       <c r="A15" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="B15" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="C15" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="D15" s="13" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
       <c r="E15" s="15" t="s">
         <v>51</v>
@@ -3087,19 +3106,19 @@
     </row>
     <row r="16" spans="1:6" ht="38.25">
       <c r="A16" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
       <c r="B16" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="C16" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>258</v>
+        <v>254</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>257</v>
+        <v>253</v>
       </c>
       <c r="F16" t="s">
         <v>53</v>
@@ -3107,19 +3126,19 @@
     </row>
     <row r="17" spans="1:6" ht="38.25">
       <c r="A17" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="B17" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="C17" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>259</v>
+        <v>255</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>260</v>
+        <v>256</v>
       </c>
       <c r="F17" t="s">
         <v>53</v>
@@ -3127,19 +3146,19 @@
     </row>
     <row r="18" spans="1:6" ht="38.25">
       <c r="A18" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
       <c r="B18" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="C18" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>262</v>
+        <v>258</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>261</v>
+        <v>257</v>
       </c>
       <c r="F18" t="s">
         <v>53</v>
@@ -3147,19 +3166,19 @@
     </row>
     <row r="19" spans="1:6" ht="38.25">
       <c r="A19" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
       <c r="B19" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="C19" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>264</v>
+        <v>260</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>263</v>
+        <v>259</v>
       </c>
       <c r="F19" t="s">
         <v>53</v>
@@ -3167,16 +3186,16 @@
     </row>
     <row r="20" spans="1:6" ht="26.25">
       <c r="A20" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
       <c r="B20" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="C20" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>265</v>
+        <v>261</v>
       </c>
       <c r="E20" s="12" t="s">
         <v>51</v>
@@ -3187,19 +3206,19 @@
     </row>
     <row r="21" spans="1:6" ht="47.25">
       <c r="A21" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
       <c r="B21" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="C21" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>277</v>
+        <v>273</v>
       </c>
       <c r="E21" s="17" t="s">
-        <v>278</v>
+        <v>274</v>
       </c>
       <c r="F21" s="18" t="s">
         <v>53</v>
@@ -3207,19 +3226,19 @@
     </row>
     <row r="22" spans="1:6" ht="47.25">
       <c r="A22" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
       <c r="B22" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="C22" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="D22" s="20" t="s">
-        <v>280</v>
+        <v>276</v>
       </c>
       <c r="E22" s="19" t="s">
-        <v>279</v>
+        <v>275</v>
       </c>
       <c r="F22" s="18" t="s">
         <v>53</v>
@@ -3227,19 +3246,19 @@
     </row>
     <row r="23" spans="1:6" ht="37.5" customHeight="1">
       <c r="A23" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
       <c r="B23" t="s">
         <v>77</v>
       </c>
       <c r="C23" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>266</v>
+        <v>262</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>267</v>
+        <v>263</v>
       </c>
       <c r="F23" t="s">
         <v>53</v>
@@ -3247,16 +3266,16 @@
     </row>
     <row r="24" spans="1:6" ht="26.25">
       <c r="A24" t="s">
-        <v>203</v>
+        <v>199</v>
       </c>
       <c r="B24" t="s">
         <v>77</v>
       </c>
       <c r="C24" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>268</v>
+        <v>264</v>
       </c>
       <c r="E24" s="12" t="s">
         <v>51</v>
@@ -3267,19 +3286,19 @@
     </row>
     <row r="25" spans="1:6" ht="25.5">
       <c r="A25" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
       <c r="B25" t="s">
         <v>76</v>
       </c>
       <c r="C25" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>285</v>
+        <v>281</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>288</v>
+        <v>284</v>
       </c>
       <c r="F25" t="s">
         <v>53</v>
@@ -3287,39 +3306,39 @@
     </row>
     <row r="26" spans="1:6">
       <c r="A26" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
       <c r="B26" t="s">
         <v>76</v>
       </c>
       <c r="C26" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>286</v>
+        <v>282</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>289</v>
+        <v>285</v>
       </c>
       <c r="F26" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="27" spans="1:6">
+    <row r="27" spans="1:6" ht="25.5">
       <c r="A27" t="s">
-        <v>203</v>
+        <v>199</v>
       </c>
       <c r="B27" t="s">
         <v>76</v>
       </c>
       <c r="C27" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>287</v>
+        <v>283</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>290</v>
+        <v>286</v>
       </c>
       <c r="F27" t="s">
         <v>53</v>
@@ -3327,19 +3346,19 @@
     </row>
     <row r="28" spans="1:6" ht="25.5">
       <c r="A28" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
       <c r="B28" t="s">
         <v>78</v>
       </c>
       <c r="C28" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>293</v>
+        <v>289</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>291</v>
+        <v>287</v>
       </c>
       <c r="F28" t="s">
         <v>53</v>
@@ -3347,19 +3366,19 @@
     </row>
     <row r="29" spans="1:6" ht="25.5">
       <c r="A29" t="s">
-        <v>205</v>
+        <v>201</v>
       </c>
       <c r="B29" t="s">
         <v>78</v>
       </c>
       <c r="C29" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>294</v>
+        <v>290</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>292</v>
+        <v>288</v>
       </c>
       <c r="F29" t="s">
         <v>53</v>
@@ -3367,257 +3386,257 @@
     </row>
     <row r="30" spans="1:6">
       <c r="A30" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
     </row>
     <row r="31" spans="1:6">
       <c r="A31" t="s">
-        <v>207</v>
+        <v>203</v>
       </c>
     </row>
     <row r="32" spans="1:6">
       <c r="A32" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
     </row>
     <row r="33" spans="1:1">
       <c r="A33" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
     </row>
     <row r="34" spans="1:1">
       <c r="A34" t="s">
-        <v>210</v>
+        <v>206</v>
       </c>
     </row>
     <row r="35" spans="1:1">
       <c r="A35" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
     </row>
     <row r="36" spans="1:1">
       <c r="A36" t="s">
-        <v>212</v>
+        <v>208</v>
       </c>
     </row>
     <row r="37" spans="1:1">
       <c r="A37" t="s">
-        <v>213</v>
+        <v>209</v>
       </c>
     </row>
     <row r="38" spans="1:1">
       <c r="A38" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
     </row>
     <row r="39" spans="1:1">
       <c r="A39" t="s">
-        <v>215</v>
+        <v>211</v>
       </c>
     </row>
     <row r="40" spans="1:1">
       <c r="A40" t="s">
-        <v>216</v>
+        <v>212</v>
       </c>
     </row>
     <row r="41" spans="1:1">
       <c r="A41" t="s">
-        <v>217</v>
+        <v>213</v>
       </c>
     </row>
     <row r="42" spans="1:1">
       <c r="A42" t="s">
-        <v>218</v>
+        <v>214</v>
       </c>
     </row>
     <row r="43" spans="1:1">
       <c r="A43" t="s">
-        <v>219</v>
+        <v>215</v>
       </c>
     </row>
     <row r="44" spans="1:1">
       <c r="A44" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
     </row>
     <row r="45" spans="1:1">
       <c r="A45" t="s">
-        <v>221</v>
+        <v>217</v>
       </c>
     </row>
     <row r="46" spans="1:1">
       <c r="A46" t="s">
-        <v>222</v>
+        <v>218</v>
       </c>
     </row>
     <row r="47" spans="1:1">
       <c r="A47" t="s">
-        <v>223</v>
+        <v>219</v>
       </c>
     </row>
     <row r="48" spans="1:1">
       <c r="A48" t="s">
-        <v>224</v>
+        <v>220</v>
       </c>
     </row>
     <row r="49" spans="1:1">
       <c r="A49" t="s">
-        <v>225</v>
+        <v>221</v>
       </c>
     </row>
     <row r="50" spans="1:1">
       <c r="A50" t="s">
-        <v>226</v>
+        <v>222</v>
       </c>
     </row>
     <row r="51" spans="1:1">
       <c r="A51" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
     </row>
     <row r="52" spans="1:1">
       <c r="A52" t="s">
-        <v>228</v>
+        <v>224</v>
       </c>
     </row>
     <row r="53" spans="1:1">
       <c r="A53" t="s">
-        <v>229</v>
+        <v>225</v>
       </c>
     </row>
     <row r="54" spans="1:1">
       <c r="A54" t="s">
-        <v>230</v>
+        <v>226</v>
       </c>
     </row>
     <row r="55" spans="1:1">
       <c r="A55" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
     </row>
     <row r="56" spans="1:1">
       <c r="A56" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
     </row>
     <row r="57" spans="1:1">
       <c r="A57" t="s">
-        <v>233</v>
+        <v>229</v>
       </c>
     </row>
     <row r="58" spans="1:1">
       <c r="A58" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
     </row>
     <row r="59" spans="1:1">
       <c r="A59" t="s">
-        <v>235</v>
+        <v>231</v>
       </c>
     </row>
     <row r="60" spans="1:1">
       <c r="A60" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
     </row>
     <row r="61" spans="1:1">
       <c r="A61" t="s">
-        <v>237</v>
+        <v>233</v>
       </c>
     </row>
     <row r="62" spans="1:1">
       <c r="A62" t="s">
-        <v>238</v>
+        <v>234</v>
       </c>
     </row>
     <row r="63" spans="1:1">
       <c r="A63" t="s">
-        <v>239</v>
+        <v>235</v>
       </c>
     </row>
     <row r="64" spans="1:1">
       <c r="A64" t="s">
-        <v>240</v>
+        <v>236</v>
       </c>
     </row>
     <row r="65" spans="1:1">
       <c r="A65" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
     </row>
     <row r="66" spans="1:1">
       <c r="A66" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
     </row>
     <row r="67" spans="1:1">
       <c r="A67" t="s">
-        <v>243</v>
+        <v>239</v>
       </c>
     </row>
     <row r="68" spans="1:1">
       <c r="A68" t="s">
-        <v>244</v>
+        <v>240</v>
       </c>
     </row>
     <row r="69" spans="1:1">
       <c r="A69" t="s">
-        <v>245</v>
+        <v>241</v>
       </c>
     </row>
     <row r="70" spans="1:1">
       <c r="A70" t="s">
-        <v>246</v>
+        <v>242</v>
       </c>
     </row>
     <row r="71" spans="1:1">
       <c r="A71" t="s">
-        <v>247</v>
+        <v>243</v>
       </c>
     </row>
     <row r="72" spans="1:1">
       <c r="A72" t="s">
-        <v>248</v>
+        <v>244</v>
       </c>
     </row>
     <row r="73" spans="1:1">
       <c r="A73" t="s">
-        <v>249</v>
+        <v>245</v>
       </c>
     </row>
     <row r="74" spans="1:1">
       <c r="A74" t="s">
-        <v>250</v>
+        <v>246</v>
       </c>
     </row>
     <row r="75" spans="1:1">
       <c r="A75" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
     </row>
     <row r="76" spans="1:1">
       <c r="A76" t="s">
-        <v>252</v>
+        <v>248</v>
       </c>
     </row>
     <row r="77" spans="1:1">
       <c r="A77" t="s">
-        <v>253</v>
+        <v>249</v>
       </c>
     </row>
     <row r="78" spans="1:1">
       <c r="A78" t="s">
-        <v>254</v>
+        <v>250</v>
       </c>
     </row>
     <row r="79" spans="1:1">
       <c r="A79" t="s">
-        <v>255</v>
+        <v>251</v>
       </c>
     </row>
     <row r="80" spans="1:1">
       <c r="A80" t="s">
-        <v>256</v>
+        <v>252</v>
       </c>
     </row>
   </sheetData>
@@ -3667,7 +3686,7 @@
         <v>27</v>
       </c>
       <c r="F1" s="8" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
     </row>
     <row r="2" spans="1:6">
@@ -3720,7 +3739,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:J40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="150" workbookViewId="0">
+    <sheetView topLeftCell="A16" zoomScale="150" workbookViewId="0">
       <selection activeCell="E30" sqref="E30:J30"/>
     </sheetView>
   </sheetViews>
@@ -3775,13 +3794,13 @@
         <v>31</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="C2" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="D2" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="E2" t="s">
         <v>35</v>
@@ -3804,13 +3823,13 @@
     </row>
     <row r="4" spans="1:10" ht="25.5">
       <c r="A4" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
       <c r="D4" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
     </row>
     <row r="5" spans="1:10" ht="25.5">
@@ -3818,10 +3837,10 @@
         <v>41</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="D5" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
     </row>
     <row r="6" spans="1:10" ht="25.5">
@@ -3829,21 +3848,21 @@
         <v>42</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="D6" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
     </row>
     <row r="7" spans="1:10" ht="25.5">
       <c r="A7" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
       <c r="D7" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -3851,16 +3870,16 @@
         <v>32</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="C9" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
       <c r="D9" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="E9" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
       <c r="F9">
         <v>50</v>
@@ -3883,10 +3902,10 @@
         <v>43</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
       <c r="D11" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
     </row>
     <row r="12" spans="1:10" ht="38.25">
@@ -3894,27 +3913,27 @@
         <v>44</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="D12" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
     </row>
     <row r="14" spans="1:10">
       <c r="A14" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="B14" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="C14" s="18" t="s">
-        <v>281</v>
+        <v>277</v>
       </c>
       <c r="D14" t="s">
         <v>72</v>
       </c>
       <c r="E14" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
       <c r="F14">
         <v>80</v>
@@ -3934,10 +3953,10 @@
     </row>
     <row r="15" spans="1:10">
       <c r="A15" t="s">
-        <v>302</v>
+        <v>298</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
       <c r="D15" t="s">
         <v>72</v>
@@ -3946,10 +3965,10 @@
     </row>
     <row r="16" spans="1:10">
       <c r="A16" t="s">
-        <v>303</v>
+        <v>299</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>270</v>
+        <v>266</v>
       </c>
       <c r="D16" t="s">
         <v>72</v>
@@ -3957,10 +3976,10 @@
     </row>
     <row r="17" spans="1:10">
       <c r="A17" t="s">
-        <v>304</v>
+        <v>300</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>272</v>
+        <v>268</v>
       </c>
       <c r="D17" t="s">
         <v>72</v>
@@ -3968,10 +3987,10 @@
     </row>
     <row r="18" spans="1:10" ht="25.5">
       <c r="A18" t="s">
-        <v>305</v>
+        <v>301</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>271</v>
+        <v>267</v>
       </c>
       <c r="D18" t="s">
         <v>72</v>
@@ -3986,16 +4005,16 @@
         <v>77</v>
       </c>
       <c r="B20" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="C20" s="20" t="s">
-        <v>282</v>
+        <v>278</v>
       </c>
       <c r="D20" t="s">
         <v>72</v>
       </c>
       <c r="E20" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
       <c r="F20">
         <v>20</v>
@@ -4015,10 +4034,10 @@
     </row>
     <row r="21" spans="1:10">
       <c r="A21" t="s">
-        <v>306</v>
+        <v>302</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>273</v>
+        <v>269</v>
       </c>
       <c r="D21" t="s">
         <v>72</v>
@@ -4027,10 +4046,10 @@
     </row>
     <row r="22" spans="1:10">
       <c r="A22" t="s">
-        <v>307</v>
+        <v>303</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>274</v>
+        <v>270</v>
       </c>
       <c r="D22" t="s">
         <v>72</v>
@@ -4038,10 +4057,10 @@
     </row>
     <row r="23" spans="1:10">
       <c r="A23" t="s">
-        <v>308</v>
+        <v>304</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>275</v>
+        <v>271</v>
       </c>
       <c r="J23" s="7"/>
     </row>
@@ -4053,16 +4072,16 @@
         <v>76</v>
       </c>
       <c r="B25" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>296</v>
+        <v>292</v>
       </c>
       <c r="D25" t="s">
-        <v>276</v>
+        <v>272</v>
       </c>
       <c r="E25" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
       <c r="F25">
         <v>80</v>
@@ -4082,37 +4101,37 @@
     </row>
     <row r="26" spans="1:10" ht="25.5">
       <c r="A26" t="s">
-        <v>309</v>
+        <v>305</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>298</v>
+        <v>294</v>
       </c>
       <c r="D26" t="s">
-        <v>276</v>
+        <v>272</v>
       </c>
       <c r="J26" s="7"/>
     </row>
     <row r="27" spans="1:10" ht="25.5">
       <c r="A27" t="s">
-        <v>310</v>
+        <v>306</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>299</v>
+        <v>295</v>
       </c>
       <c r="D27" t="s">
-        <v>276</v>
+        <v>272</v>
       </c>
       <c r="J27" s="7"/>
     </row>
     <row r="28" spans="1:10" ht="25.5">
       <c r="A28" t="s">
-        <v>311</v>
+        <v>307</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>300</v>
+        <v>296</v>
       </c>
       <c r="D28" t="s">
-        <v>276</v>
+        <v>272</v>
       </c>
       <c r="J28" s="7"/>
     </row>
@@ -4124,16 +4143,16 @@
         <v>78</v>
       </c>
       <c r="B30" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>297</v>
+        <v>293</v>
       </c>
       <c r="D30" t="s">
-        <v>276</v>
+        <v>272</v>
       </c>
       <c r="E30" s="18" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
       <c r="F30">
         <v>50</v>
@@ -4153,25 +4172,25 @@
     </row>
     <row r="31" spans="1:10" ht="25.5">
       <c r="A31" t="s">
-        <v>312</v>
+        <v>308</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>301</v>
+        <v>297</v>
       </c>
       <c r="D31" t="s">
-        <v>276</v>
+        <v>272</v>
       </c>
       <c r="J31" s="7"/>
     </row>
     <row r="32" spans="1:10" ht="25.5">
       <c r="A32" t="s">
-        <v>313</v>
+        <v>309</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>314</v>
+        <v>310</v>
       </c>
       <c r="D32" t="s">
-        <v>276</v>
+        <v>272</v>
       </c>
       <c r="J32" s="7"/>
     </row>

</xml_diff>

<commit_message>
Planning for sprint 2
</commit_message>
<xml_diff>
--- a/Team05Report.xlsx
+++ b/Team05Report.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="240" windowWidth="20730" windowHeight="11760" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="240" yWindow="240" windowWidth="20730" windowHeight="11760" tabRatio="500" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Team" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
     <sheet name="Sprint4" sheetId="6" r:id="rId9"/>
     <sheet name="Sprint5" sheetId="8" r:id="rId10"/>
   </sheets>
-  <calcPr calcId="125725" concurrentCalc="0"/>
+  <calcPr calcId="145621" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -62,7 +62,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="556" uniqueCount="317">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="573" uniqueCount="321">
   <si>
     <t>Date</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -295,12 +295,6 @@
     <t>AT ID</t>
   </si>
   <si>
-    <t>Meet twice a week</t>
-  </si>
-  <si>
-    <t>Text everyone when you discover a problem</t>
-  </si>
-  <si>
     <t>Review Results</t>
   </si>
   <si>
@@ -1069,17 +1063,35 @@
   </si>
   <si>
     <t>If the parents were divorced in a family, make sure that all the children were born before the divorce date</t>
+  </si>
+  <si>
+    <t>Unique information</t>
+  </si>
+  <si>
+    <t>An individual can only have one tag of sex, name, birthdate, etc.</t>
+  </si>
+  <si>
+    <t>Inform everyone when you discover a problem</t>
+  </si>
+  <si>
+    <t>Meet at least twice a week</t>
+  </si>
+  <si>
+    <t>Add more user stories if you come up new one</t>
+  </si>
+  <si>
+    <t>Modify the user stories we are about to implement next sprint to more proper and completed</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="m/d"/>
     <numFmt numFmtId="165" formatCode="0.0"/>
   </numFmts>
-  <fonts count="10">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Verdana"/>
@@ -1244,56 +1256,56 @@
     </xf>
   </cellXfs>
   <cellStyles count="50">
-    <cellStyle name="已访问的超链接" xfId="2" builtinId="9" hidden="1"/>
-    <cellStyle name="已访问的超链接" xfId="4" builtinId="9" hidden="1"/>
-    <cellStyle name="已访问的超链接" xfId="6" builtinId="9" hidden="1"/>
-    <cellStyle name="已访问的超链接" xfId="8" builtinId="9" hidden="1"/>
-    <cellStyle name="已访问的超链接" xfId="10" builtinId="9" hidden="1"/>
-    <cellStyle name="已访问的超链接" xfId="12" builtinId="9" hidden="1"/>
-    <cellStyle name="已访问的超链接" xfId="14" builtinId="9" hidden="1"/>
-    <cellStyle name="已访问的超链接" xfId="16" builtinId="9" hidden="1"/>
-    <cellStyle name="已访问的超链接" xfId="18" builtinId="9" hidden="1"/>
-    <cellStyle name="已访问的超链接" xfId="20" builtinId="9" hidden="1"/>
-    <cellStyle name="已访问的超链接" xfId="22" builtinId="9" hidden="1"/>
-    <cellStyle name="已访问的超链接" xfId="24" builtinId="9" hidden="1"/>
-    <cellStyle name="已访问的超链接" xfId="26" builtinId="9" hidden="1"/>
-    <cellStyle name="已访问的超链接" xfId="28" builtinId="9" hidden="1"/>
-    <cellStyle name="已访问的超链接" xfId="30" builtinId="9" hidden="1"/>
-    <cellStyle name="已访问的超链接" xfId="32" builtinId="9" hidden="1"/>
-    <cellStyle name="已访问的超链接" xfId="34" builtinId="9" hidden="1"/>
-    <cellStyle name="已访问的超链接" xfId="36" builtinId="9" hidden="1"/>
-    <cellStyle name="已访问的超链接" xfId="38" builtinId="9" hidden="1"/>
-    <cellStyle name="已访问的超链接" xfId="40" builtinId="9" hidden="1"/>
-    <cellStyle name="已访问的超链接" xfId="42" builtinId="9" hidden="1"/>
-    <cellStyle name="已访问的超链接" xfId="44" builtinId="9" hidden="1"/>
-    <cellStyle name="已访问的超链接" xfId="46" builtinId="9" hidden="1"/>
-    <cellStyle name="已访问的超链接" xfId="48" builtinId="9" hidden="1"/>
-    <cellStyle name="常规" xfId="0" builtinId="0"/>
-    <cellStyle name="超链接" xfId="1" builtinId="8" hidden="1"/>
-    <cellStyle name="超链接" xfId="3" builtinId="8" hidden="1"/>
-    <cellStyle name="超链接" xfId="5" builtinId="8" hidden="1"/>
-    <cellStyle name="超链接" xfId="7" builtinId="8" hidden="1"/>
-    <cellStyle name="超链接" xfId="9" builtinId="8" hidden="1"/>
-    <cellStyle name="超链接" xfId="11" builtinId="8" hidden="1"/>
-    <cellStyle name="超链接" xfId="13" builtinId="8" hidden="1"/>
-    <cellStyle name="超链接" xfId="15" builtinId="8" hidden="1"/>
-    <cellStyle name="超链接" xfId="17" builtinId="8" hidden="1"/>
-    <cellStyle name="超链接" xfId="19" builtinId="8" hidden="1"/>
-    <cellStyle name="超链接" xfId="21" builtinId="8" hidden="1"/>
-    <cellStyle name="超链接" xfId="23" builtinId="8" hidden="1"/>
-    <cellStyle name="超链接" xfId="25" builtinId="8" hidden="1"/>
-    <cellStyle name="超链接" xfId="27" builtinId="8" hidden="1"/>
-    <cellStyle name="超链接" xfId="29" builtinId="8" hidden="1"/>
-    <cellStyle name="超链接" xfId="31" builtinId="8" hidden="1"/>
-    <cellStyle name="超链接" xfId="33" builtinId="8" hidden="1"/>
-    <cellStyle name="超链接" xfId="35" builtinId="8" hidden="1"/>
-    <cellStyle name="超链接" xfId="37" builtinId="8" hidden="1"/>
-    <cellStyle name="超链接" xfId="39" builtinId="8" hidden="1"/>
-    <cellStyle name="超链接" xfId="41" builtinId="8" hidden="1"/>
-    <cellStyle name="超链接" xfId="43" builtinId="8" hidden="1"/>
-    <cellStyle name="超链接" xfId="45" builtinId="8" hidden="1"/>
-    <cellStyle name="超链接" xfId="47" builtinId="8" hidden="1"/>
-    <cellStyle name="超链接" xfId="49" builtinId="8"/>
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="30" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="32" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="34" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="36" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="38" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="40" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="44" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="46" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="48" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="29" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="31" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="33" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="35" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="37" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="39" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="41" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="43" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="45" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="47" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="49" builtinId="8"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
@@ -1309,11 +1321,22 @@
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="1"/>
   <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
   <c:chart>
+    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
       <c:lineChart>
         <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
@@ -1347,41 +1370,58 @@
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:smooth val="0"/>
         </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
         <c:marker val="1"/>
-        <c:axId val="223820032"/>
-        <c:axId val="223821824"/>
+        <c:smooth val="0"/>
+        <c:axId val="105415040"/>
+        <c:axId val="105416576"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="223820032"/>
+        <c:axId val="105415040"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="b"/>
         <c:numFmt formatCode="m/d" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="223821824"/>
+        <c:crossAx val="105416576"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
         <c:baseTimeUnit val="days"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="223821824"/>
+        <c:axId val="105416576"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="223820032"/>
+        <c:crossAx val="105415040"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
@@ -1745,14 +1785,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView zoomScale="150" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="7.625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="6.375" customWidth="1"/>
@@ -1761,7 +1801,7 @@
     <col min="5" max="5" width="19.25" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="4" customFormat="1">
+    <row r="1" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>22</v>
       </c>
@@ -1775,66 +1815,66 @@
         <v>25</v>
       </c>
       <c r="E1" s="4" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>70</v>
+      </c>
+      <c r="B3" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="3" spans="1:5">
-      <c r="A3" t="s">
+      <c r="C3" t="s">
+        <v>69</v>
+      </c>
+      <c r="D3" s="14" t="s">
+        <v>71</v>
+      </c>
+      <c r="E3" t="s">
         <v>72</v>
       </c>
-      <c r="B3" t="s">
-        <v>70</v>
-      </c>
-      <c r="C3" t="s">
-        <v>71</v>
-      </c>
-      <c r="D3" s="14" t="s">
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>129</v>
+      </c>
+      <c r="B4" t="s">
+        <v>130</v>
+      </c>
+      <c r="C4" t="s">
+        <v>131</v>
+      </c>
+      <c r="D4" s="14" t="s">
+        <v>132</v>
+      </c>
+      <c r="E4" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>270</v>
+      </c>
+      <c r="B5" t="s">
+        <v>134</v>
+      </c>
+      <c r="C5" t="s">
+        <v>135</v>
+      </c>
+      <c r="D5" s="14" t="s">
+        <v>136</v>
+      </c>
+      <c r="E5" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D9" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="E9" t="s">
         <v>73</v>
-      </c>
-      <c r="E3" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5">
-      <c r="A4" t="s">
-        <v>131</v>
-      </c>
-      <c r="B4" t="s">
-        <v>132</v>
-      </c>
-      <c r="C4" t="s">
-        <v>133</v>
-      </c>
-      <c r="D4" s="14" t="s">
-        <v>134</v>
-      </c>
-      <c r="E4" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5">
-      <c r="A5" t="s">
-        <v>272</v>
-      </c>
-      <c r="B5" t="s">
-        <v>136</v>
-      </c>
-      <c r="C5" t="s">
-        <v>137</v>
-      </c>
-      <c r="D5" s="14" t="s">
-        <v>138</v>
-      </c>
-      <c r="E5" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5">
-      <c r="D9" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="E9" t="s">
-        <v>75</v>
       </c>
     </row>
   </sheetData>
@@ -1858,16 +1898,16 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J1"/>
   <sheetViews>
     <sheetView zoomScale="150" workbookViewId="0">
       <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:10" ht="25.5">
+    <row r="1" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>3</v>
       </c>
@@ -1911,14 +1951,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L26"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" zoomScale="150" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+    <sheetView zoomScale="150" workbookViewId="0">
+      <selection activeCell="G8" sqref="G8:H13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="6.625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="8.875" bestFit="1" customWidth="1"/>
@@ -1934,7 +1974,7 @@
     <col min="12" max="12" width="10.75" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="4" customFormat="1">
+    <row r="1" spans="1:12" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>40</v>
       </c>
@@ -1972,7 +2012,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:12">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1980,13 +2020,13 @@
         <v>31</v>
       </c>
       <c r="C2" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="D2" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="E2" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="F2" t="s">
         <v>35</v>
@@ -2010,7 +2050,7 @@
         <v>40598</v>
       </c>
     </row>
-    <row r="3" spans="1:12">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>1</v>
       </c>
@@ -2018,16 +2058,16 @@
         <v>32</v>
       </c>
       <c r="C3" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="D3" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="E3" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="F3" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="G3">
         <v>50</v>
@@ -2048,7 +2088,7 @@
         <v>40598</v>
       </c>
     </row>
-    <row r="4" spans="1:12">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>1</v>
       </c>
@@ -2056,16 +2096,16 @@
         <v>34</v>
       </c>
       <c r="C4" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="D4" s="18" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="E4" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="F4" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="G4">
         <v>80</v>
@@ -2086,24 +2126,24 @@
         <v>40598</v>
       </c>
     </row>
-    <row r="5" spans="1:12">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>1</v>
       </c>
       <c r="B5" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C5" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="D5" s="18" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="E5" s="18" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="F5" s="18" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="G5">
         <v>80</v>
@@ -2124,24 +2164,24 @@
         <v>40598</v>
       </c>
     </row>
-    <row r="6" spans="1:12">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>1</v>
       </c>
       <c r="B6" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C6" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="D6" s="18" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="E6" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="F6" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="G6">
         <v>20</v>
@@ -2162,24 +2202,24 @@
         <v>40598</v>
       </c>
     </row>
-    <row r="7" spans="1:12">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>1</v>
       </c>
       <c r="B7" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C7" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="D7" s="18" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="E7" s="18" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="F7" s="18" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="G7">
         <v>50</v>
@@ -2200,207 +2240,267 @@
         <v>40598</v>
       </c>
     </row>
-    <row r="8" spans="1:12">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>2</v>
+      </c>
       <c r="B8" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C8" t="s">
-        <v>109</v>
+        <v>107</v>
+      </c>
+      <c r="G8">
+        <v>20</v>
+      </c>
+      <c r="H8">
+        <v>10</v>
       </c>
       <c r="L8" s="7">
         <v>40598</v>
       </c>
     </row>
-    <row r="9" spans="1:12">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>2</v>
+      </c>
       <c r="B9" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C9" t="s">
-        <v>117</v>
+        <v>115</v>
+      </c>
+      <c r="G9">
+        <v>50</v>
+      </c>
+      <c r="H9">
+        <v>30</v>
       </c>
       <c r="L9" s="7">
         <v>40598</v>
       </c>
     </row>
-    <row r="10" spans="1:12">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>2</v>
+      </c>
       <c r="B10" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C10" t="s">
-        <v>110</v>
+        <v>108</v>
+      </c>
+      <c r="G10">
+        <v>50</v>
+      </c>
+      <c r="H10">
+        <v>45</v>
       </c>
       <c r="L10" s="7">
         <v>40598</v>
       </c>
     </row>
-    <row r="11" spans="1:12">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>2</v>
+      </c>
       <c r="B11" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C11" t="s">
         <v>33</v>
       </c>
+      <c r="G11">
+        <v>30</v>
+      </c>
+      <c r="H11">
+        <v>10</v>
+      </c>
       <c r="L11" s="7">
         <v>40598</v>
       </c>
     </row>
-    <row r="12" spans="1:12">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <v>2</v>
+      </c>
       <c r="B12" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C12" t="s">
-        <v>101</v>
+        <v>99</v>
+      </c>
+      <c r="G12">
+        <v>30</v>
+      </c>
+      <c r="H12">
+        <v>10</v>
       </c>
       <c r="L12" s="7">
         <v>40598</v>
       </c>
     </row>
-    <row r="13" spans="1:12">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <v>2</v>
+      </c>
       <c r="B13" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C13" t="s">
-        <v>102</v>
+        <v>100</v>
+      </c>
+      <c r="G13">
+        <v>30</v>
+      </c>
+      <c r="H13">
+        <v>10</v>
       </c>
       <c r="L13" s="7">
         <v>40598</v>
       </c>
     </row>
-    <row r="14" spans="1:12">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B14" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C14" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="L14" s="7">
         <v>40598</v>
       </c>
     </row>
-    <row r="15" spans="1:12">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B15" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C15" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="L15" s="7">
         <v>40598</v>
       </c>
     </row>
-    <row r="16" spans="1:12">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B16" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C16" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="L16" s="7">
         <v>40598</v>
       </c>
     </row>
-    <row r="17" spans="2:12">
+    <row r="17" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B17" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="C17" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="L17" s="7">
         <v>40598</v>
       </c>
     </row>
-    <row r="18" spans="2:12">
+    <row r="18" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B18" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C18" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="L18" s="7">
         <v>40598</v>
       </c>
     </row>
-    <row r="19" spans="2:12">
+    <row r="19" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B19" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C19" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="L19" s="7">
         <v>40598</v>
       </c>
     </row>
-    <row r="20" spans="2:12">
+    <row r="20" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B20" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="C20" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="L20" s="7">
         <v>40598</v>
       </c>
     </row>
-    <row r="21" spans="2:12">
+    <row r="21" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B21" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="C21" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="L21" s="7">
         <v>40598</v>
       </c>
     </row>
-    <row r="22" spans="2:12">
+    <row r="22" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B22" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C22" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="L22" s="7">
         <v>40598</v>
       </c>
     </row>
-    <row r="23" spans="2:12">
+    <row r="23" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B23" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="C23" s="18" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="L23" s="7">
         <v>40602</v>
       </c>
     </row>
-    <row r="24" spans="2:12">
+    <row r="24" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B24" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="C24" s="18" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="L24" s="7">
         <v>40602</v>
       </c>
     </row>
-    <row r="25" spans="2:12">
+    <row r="25" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B25" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="C25" s="18" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="L25" s="7">
         <v>40602</v>
       </c>
     </row>
-    <row r="26" spans="2:12">
+    <row r="26" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B26" t="s">
-        <v>97</v>
+        <v>95</v>
+      </c>
+      <c r="C26" s="18" t="s">
+        <v>315</v>
+      </c>
+      <c r="L26" s="7">
+        <v>40602</v>
       </c>
     </row>
   </sheetData>
@@ -2416,14 +2516,14 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="D26" sqref="D26"/>
+    <sheetView zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="E8" sqref="E8:F13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="8.875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="24.75" bestFit="1" customWidth="1"/>
@@ -2432,7 +2532,7 @@
     <col min="6" max="6" width="9" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>28</v>
       </c>
@@ -2452,18 +2552,18 @@
         <v>38</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="25.5">
+    <row r="2" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>31</v>
       </c>
       <c r="B2" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="D2" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="E2">
         <v>150</v>
@@ -2472,18 +2572,18 @@
         <v>60</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="25.5">
+    <row r="3" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>32</v>
       </c>
       <c r="B3" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="D3" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="E3">
         <v>50</v>
@@ -2492,18 +2592,18 @@
         <v>40</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>34</v>
       </c>
       <c r="B4" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="D4" s="18" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="E4">
         <v>80</v>
@@ -2512,18 +2612,18 @@
         <v>45</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B5" t="s">
+        <v>112</v>
+      </c>
+      <c r="C5" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="C5" s="1" t="s">
-        <v>116</v>
-      </c>
       <c r="D5" s="18" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="E5">
         <v>20</v>
@@ -2532,18 +2632,18 @@
         <v>30</v>
       </c>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B6" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>46</v>
       </c>
       <c r="D6" s="18" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="E6">
         <v>80</v>
@@ -2552,18 +2652,18 @@
         <v>45</v>
       </c>
     </row>
-    <row r="7" spans="1:6">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B7" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="D7" s="18" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="E7">
         <v>50</v>
@@ -2572,42 +2672,60 @@
         <v>25</v>
       </c>
     </row>
-    <row r="8" spans="1:6">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
+        <v>77</v>
+      </c>
+      <c r="B8" t="s">
+        <v>107</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="E8">
+        <v>20</v>
+      </c>
+      <c r="F8">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>78</v>
+      </c>
+      <c r="B9" t="s">
+        <v>115</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="E9">
+        <v>50</v>
+      </c>
+      <c r="F9">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
         <v>79</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B10" t="s">
+        <v>108</v>
+      </c>
+      <c r="C10" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="C8" s="1" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6">
-      <c r="A9" t="s">
+      <c r="E10">
+        <v>50</v>
+      </c>
+      <c r="F10">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
         <v>80</v>
-      </c>
-      <c r="B9" t="s">
-        <v>117</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6">
-      <c r="A10" t="s">
-        <v>81</v>
-      </c>
-      <c r="B10" t="s">
-        <v>110</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6">
-      <c r="A11" t="s">
-        <v>82</v>
       </c>
       <c r="B11" t="s">
         <v>33</v>
@@ -2615,164 +2733,188 @@
       <c r="C11" s="1" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="12" spans="1:6">
+      <c r="E11">
+        <v>30</v>
+      </c>
+      <c r="F11">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B12" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="13" spans="1:6">
+      <c r="E12">
+        <v>30</v>
+      </c>
+      <c r="F12">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
+        <v>82</v>
+      </c>
+      <c r="B13" t="s">
+        <v>100</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="E13">
+        <v>30</v>
+      </c>
+      <c r="F13">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>83</v>
+      </c>
+      <c r="B14" t="s">
+        <v>101</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
         <v>84</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B15" t="s">
+        <v>313</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>85</v>
+      </c>
+      <c r="B16" t="s">
+        <v>110</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>86</v>
+      </c>
+      <c r="B17" t="s">
+        <v>111</v>
+      </c>
+      <c r="C17" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="C13" s="1" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" ht="25.5">
-      <c r="A14" t="s">
-        <v>85</v>
-      </c>
-      <c r="B14" t="s">
-        <v>103</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6">
-      <c r="A15" t="s">
-        <v>86</v>
-      </c>
-      <c r="B15" t="s">
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>87</v>
+      </c>
+      <c r="B18" t="s">
+        <v>118</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>88</v>
+      </c>
+      <c r="B19" t="s">
+        <v>120</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>89</v>
+      </c>
+      <c r="B20" t="s">
+        <v>123</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>90</v>
+      </c>
+      <c r="B21" t="s">
+        <v>127</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>91</v>
+      </c>
+      <c r="B22" t="s">
+        <v>128</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>92</v>
+      </c>
+      <c r="B23" s="18" t="s">
+        <v>277</v>
+      </c>
+      <c r="C23" s="20" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>93</v>
+      </c>
+      <c r="B24" s="18" t="s">
+        <v>309</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>94</v>
+      </c>
+      <c r="B25" s="18" t="s">
+        <v>311</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>95</v>
+      </c>
+      <c r="B26" s="18" t="s">
         <v>315</v>
       </c>
-      <c r="C15" s="1" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6">
-      <c r="A16" t="s">
-        <v>87</v>
-      </c>
-      <c r="B16" t="s">
-        <v>112</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>312</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3">
-      <c r="A17" t="s">
-        <v>88</v>
-      </c>
-      <c r="B17" t="s">
-        <v>113</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3">
-      <c r="A18" t="s">
-        <v>89</v>
-      </c>
-      <c r="B18" t="s">
-        <v>120</v>
-      </c>
-      <c r="C18" s="1" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" ht="25.5">
-      <c r="A19" t="s">
-        <v>90</v>
-      </c>
-      <c r="B19" t="s">
-        <v>122</v>
-      </c>
-      <c r="C19" s="1" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3">
-      <c r="A20" t="s">
-        <v>91</v>
-      </c>
-      <c r="B20" t="s">
-        <v>125</v>
-      </c>
-      <c r="C20" s="1" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3">
-      <c r="A21" t="s">
-        <v>92</v>
-      </c>
-      <c r="B21" t="s">
-        <v>129</v>
-      </c>
-      <c r="C21" s="1" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3">
-      <c r="A22" t="s">
-        <v>93</v>
-      </c>
-      <c r="B22" t="s">
-        <v>130</v>
-      </c>
-      <c r="C22" s="1" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" ht="25.5">
-      <c r="A23" t="s">
-        <v>94</v>
-      </c>
-      <c r="B23" s="18" t="s">
-        <v>279</v>
-      </c>
-      <c r="C23" s="20" t="s">
-        <v>280</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" ht="25.5">
-      <c r="A24" t="s">
-        <v>95</v>
-      </c>
-      <c r="B24" s="18" t="s">
-        <v>311</v>
-      </c>
-      <c r="C24" s="1" t="s">
+      <c r="C26" s="1" t="s">
         <v>316</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3">
-      <c r="A25" t="s">
-        <v>96</v>
-      </c>
-      <c r="B25" s="18" t="s">
-        <v>313</v>
-      </c>
-      <c r="C25" s="1" t="s">
-        <v>314</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3">
-      <c r="A26" t="s">
-        <v>97</v>
       </c>
     </row>
   </sheetData>
@@ -2787,14 +2929,14 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F80"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" zoomScale="145" zoomScaleNormal="145" zoomScalePageLayoutView="150" workbookViewId="0">
+    <sheetView zoomScale="145" zoomScaleNormal="145" zoomScalePageLayoutView="150" workbookViewId="0">
       <selection activeCell="E29" sqref="E29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="6.375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="8.875" bestFit="1" customWidth="1"/>
@@ -2804,7 +2946,7 @@
     <col min="6" max="6" width="7.25" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>61</v>
       </c>
@@ -2824,7 +2966,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="47.25">
+    <row r="2" spans="1:6" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>54</v>
       </c>
@@ -2832,19 +2974,19 @@
         <v>31</v>
       </c>
       <c r="C2" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="D2" s="13" t="s">
+        <v>140</v>
+      </c>
+      <c r="E2" s="13" t="s">
         <v>142</v>
-      </c>
-      <c r="E2" s="13" t="s">
-        <v>144</v>
       </c>
       <c r="F2" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="47.25">
+    <row r="3" spans="1:6" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>55</v>
       </c>
@@ -2852,90 +2994,90 @@
         <v>31</v>
       </c>
       <c r="C3" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="D3" s="13" t="s">
+        <v>141</v>
+      </c>
+      <c r="E3" s="15" t="s">
         <v>143</v>
-      </c>
-      <c r="E3" s="15" t="s">
-        <v>145</v>
       </c>
       <c r="F3" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="47.25">
+    <row r="4" spans="1:6" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>56</v>
       </c>
       <c r="B4" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="C4" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="D4" s="13" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="E4" s="13" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="F4" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="47.25">
+    <row r="5" spans="1:6" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>57</v>
       </c>
       <c r="B5" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="C5" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="D5" s="13" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="E5" s="15" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="F5" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="47.25">
+    <row r="6" spans="1:6" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>58</v>
       </c>
       <c r="B6" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="C6" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="D6" s="13" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="E6" s="13" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="F6" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="31.5">
+    <row r="7" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>59</v>
       </c>
       <c r="B7" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="C7" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="D7" s="13" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="E7" s="12" t="s">
         <v>51</v>
@@ -2944,18 +3086,18 @@
         <v>53</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="63">
+    <row r="8" spans="1:6" ht="63" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
+        <v>151</v>
+      </c>
+      <c r="B8" t="s">
+        <v>149</v>
+      </c>
+      <c r="C8" t="s">
+        <v>105</v>
+      </c>
+      <c r="D8" s="13" t="s">
         <v>153</v>
-      </c>
-      <c r="B8" t="s">
-        <v>151</v>
-      </c>
-      <c r="C8" t="s">
-        <v>107</v>
-      </c>
-      <c r="D8" s="13" t="s">
-        <v>155</v>
       </c>
       <c r="E8" s="12" t="s">
         <v>51</v>
@@ -2964,118 +3106,118 @@
         <v>53</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="63">
+    <row r="9" spans="1:6" ht="63" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="B9" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="C9" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="D9" s="13" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="E9" s="15" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="F9" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="78.75">
+    <row r="10" spans="1:6" ht="78.75" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="B10" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="C10" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="D10" s="13" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="E10" s="15" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="F10" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="63">
+    <row r="11" spans="1:6" ht="63" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="B11" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="C11" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="D11" s="13" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="E11" s="15" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="F11" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="63">
+    <row r="12" spans="1:6" ht="63" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="B12" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="C12" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="D12" s="13" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="E12" s="15" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="F12" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="78.75">
+    <row r="13" spans="1:6" ht="78.75" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="B13" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="C13" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="D13" s="13" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="E13" s="15" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="F13" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="47.25">
+    <row r="14" spans="1:6" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="B14" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="C14" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="D14" s="13" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="E14" s="15" t="s">
         <v>51</v>
@@ -3084,18 +3226,18 @@
         <v>53</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="47.25">
+    <row r="15" spans="1:6" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
+        <v>173</v>
+      </c>
+      <c r="B15" t="s">
+        <v>152</v>
+      </c>
+      <c r="C15" t="s">
+        <v>117</v>
+      </c>
+      <c r="D15" s="13" t="s">
         <v>175</v>
-      </c>
-      <c r="B15" t="s">
-        <v>154</v>
-      </c>
-      <c r="C15" t="s">
-        <v>119</v>
-      </c>
-      <c r="D15" s="13" t="s">
-        <v>177</v>
       </c>
       <c r="E15" s="15" t="s">
         <v>51</v>
@@ -3104,98 +3246,98 @@
         <v>53</v>
       </c>
     </row>
-    <row r="16" spans="1:6" ht="38.25">
+    <row r="16" spans="1:6" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="B16" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="C16" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="F16" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="17" spans="1:6" ht="38.25">
+    <row r="17" spans="1:6" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="B17" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="C17" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="F17" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="18" spans="1:6" ht="38.25">
+    <row r="18" spans="1:6" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="B18" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="C18" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="F18" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="19" spans="1:6" ht="38.25">
+    <row r="19" spans="1:6" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="B19" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="C19" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="F19" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="20" spans="1:6" ht="26.25">
+    <row r="20" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="B20" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="C20" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="E20" s="12" t="s">
         <v>51</v>
@@ -3204,78 +3346,78 @@
         <v>53</v>
       </c>
     </row>
-    <row r="21" spans="1:6" ht="47.25">
+    <row r="21" spans="1:6" ht="47.25" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="B21" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="C21" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="E21" s="17" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="F21" s="18" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="22" spans="1:6" ht="47.25">
+    <row r="22" spans="1:6" ht="47.25" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="B22" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="C22" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="D22" s="20" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="E22" s="19" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="F22" s="18" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="23" spans="1:6" ht="37.5" customHeight="1">
+    <row r="23" spans="1:6" ht="37.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="B23" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C23" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="F23" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="24" spans="1:6" ht="26.25">
+    <row r="24" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="B24" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C24" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="E24" s="12" t="s">
         <v>51</v>
@@ -3284,359 +3426,359 @@
         <v>53</v>
       </c>
     </row>
-    <row r="25" spans="1:6" ht="25.5">
+    <row r="25" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="B25" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C25" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="F25" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="26" spans="1:6">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="B26" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C26" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="F26" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="27" spans="1:6" ht="25.5">
+    <row r="27" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="B27" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C27" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="F27" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="28" spans="1:6" ht="25.5">
+    <row r="28" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="B28" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C28" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="F28" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="29" spans="1:6" ht="25.5">
+    <row r="29" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="B29" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C29" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="F29" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="30" spans="1:6">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
         <v>202</v>
       </c>
     </row>
-    <row r="31" spans="1:6">
-      <c r="A31" t="s">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
         <v>203</v>
       </c>
     </row>
-    <row r="32" spans="1:6">
-      <c r="A32" t="s">
+    <row r="34" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
         <v>204</v>
       </c>
     </row>
-    <row r="33" spans="1:1">
-      <c r="A33" t="s">
+    <row r="35" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
         <v>205</v>
       </c>
     </row>
-    <row r="34" spans="1:1">
-      <c r="A34" t="s">
+    <row r="36" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
         <v>206</v>
       </c>
     </row>
-    <row r="35" spans="1:1">
-      <c r="A35" t="s">
+    <row r="37" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
         <v>207</v>
       </c>
     </row>
-    <row r="36" spans="1:1">
-      <c r="A36" t="s">
+    <row r="38" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="37" spans="1:1">
-      <c r="A37" t="s">
+    <row r="39" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
         <v>209</v>
       </c>
     </row>
-    <row r="38" spans="1:1">
-      <c r="A38" t="s">
+    <row r="40" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
         <v>210</v>
       </c>
     </row>
-    <row r="39" spans="1:1">
-      <c r="A39" t="s">
+    <row r="41" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
         <v>211</v>
       </c>
     </row>
-    <row r="40" spans="1:1">
-      <c r="A40" t="s">
+    <row r="42" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A42" t="s">
         <v>212</v>
       </c>
     </row>
-    <row r="41" spans="1:1">
-      <c r="A41" t="s">
+    <row r="43" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A43" t="s">
         <v>213</v>
       </c>
     </row>
-    <row r="42" spans="1:1">
-      <c r="A42" t="s">
+    <row r="44" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A44" t="s">
         <v>214</v>
       </c>
     </row>
-    <row r="43" spans="1:1">
-      <c r="A43" t="s">
+    <row r="45" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A45" t="s">
         <v>215</v>
       </c>
     </row>
-    <row r="44" spans="1:1">
-      <c r="A44" t="s">
+    <row r="46" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A46" t="s">
         <v>216</v>
       </c>
     </row>
-    <row r="45" spans="1:1">
-      <c r="A45" t="s">
+    <row r="47" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A47" t="s">
         <v>217</v>
       </c>
     </row>
-    <row r="46" spans="1:1">
-      <c r="A46" t="s">
+    <row r="48" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A48" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="47" spans="1:1">
-      <c r="A47" t="s">
+    <row r="49" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A49" t="s">
         <v>219</v>
       </c>
     </row>
-    <row r="48" spans="1:1">
-      <c r="A48" t="s">
+    <row r="50" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A50" t="s">
         <v>220</v>
       </c>
     </row>
-    <row r="49" spans="1:1">
-      <c r="A49" t="s">
+    <row r="51" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A51" t="s">
         <v>221</v>
       </c>
     </row>
-    <row r="50" spans="1:1">
-      <c r="A50" t="s">
+    <row r="52" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A52" t="s">
         <v>222</v>
       </c>
     </row>
-    <row r="51" spans="1:1">
-      <c r="A51" t="s">
+    <row r="53" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A53" t="s">
         <v>223</v>
       </c>
     </row>
-    <row r="52" spans="1:1">
-      <c r="A52" t="s">
+    <row r="54" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A54" t="s">
         <v>224</v>
       </c>
     </row>
-    <row r="53" spans="1:1">
-      <c r="A53" t="s">
+    <row r="55" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A55" t="s">
         <v>225</v>
       </c>
     </row>
-    <row r="54" spans="1:1">
-      <c r="A54" t="s">
+    <row r="56" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A56" t="s">
         <v>226</v>
       </c>
     </row>
-    <row r="55" spans="1:1">
-      <c r="A55" t="s">
+    <row r="57" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A57" t="s">
         <v>227</v>
       </c>
     </row>
-    <row r="56" spans="1:1">
-      <c r="A56" t="s">
+    <row r="58" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A58" t="s">
         <v>228</v>
       </c>
     </row>
-    <row r="57" spans="1:1">
-      <c r="A57" t="s">
+    <row r="59" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A59" t="s">
         <v>229</v>
       </c>
     </row>
-    <row r="58" spans="1:1">
-      <c r="A58" t="s">
+    <row r="60" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A60" t="s">
         <v>230</v>
       </c>
     </row>
-    <row r="59" spans="1:1">
-      <c r="A59" t="s">
+    <row r="61" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A61" t="s">
         <v>231</v>
       </c>
     </row>
-    <row r="60" spans="1:1">
-      <c r="A60" t="s">
+    <row r="62" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A62" t="s">
         <v>232</v>
       </c>
     </row>
-    <row r="61" spans="1:1">
-      <c r="A61" t="s">
+    <row r="63" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A63" t="s">
         <v>233</v>
       </c>
     </row>
-    <row r="62" spans="1:1">
-      <c r="A62" t="s">
+    <row r="64" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A64" t="s">
         <v>234</v>
       </c>
     </row>
-    <row r="63" spans="1:1">
-      <c r="A63" t="s">
+    <row r="65" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A65" t="s">
         <v>235</v>
       </c>
     </row>
-    <row r="64" spans="1:1">
-      <c r="A64" t="s">
+    <row r="66" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A66" t="s">
         <v>236</v>
       </c>
     </row>
-    <row r="65" spans="1:1">
-      <c r="A65" t="s">
+    <row r="67" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A67" t="s">
         <v>237</v>
       </c>
     </row>
-    <row r="66" spans="1:1">
-      <c r="A66" t="s">
+    <row r="68" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A68" t="s">
         <v>238</v>
       </c>
     </row>
-    <row r="67" spans="1:1">
-      <c r="A67" t="s">
+    <row r="69" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A69" t="s">
         <v>239</v>
       </c>
     </row>
-    <row r="68" spans="1:1">
-      <c r="A68" t="s">
+    <row r="70" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A70" t="s">
         <v>240</v>
       </c>
     </row>
-    <row r="69" spans="1:1">
-      <c r="A69" t="s">
+    <row r="71" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A71" t="s">
         <v>241</v>
       </c>
     </row>
-    <row r="70" spans="1:1">
-      <c r="A70" t="s">
+    <row r="72" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A72" t="s">
         <v>242</v>
       </c>
     </row>
-    <row r="71" spans="1:1">
-      <c r="A71" t="s">
+    <row r="73" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A73" t="s">
         <v>243</v>
       </c>
     </row>
-    <row r="72" spans="1:1">
-      <c r="A72" t="s">
+    <row r="74" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A74" t="s">
         <v>244</v>
       </c>
     </row>
-    <row r="73" spans="1:1">
-      <c r="A73" t="s">
+    <row r="75" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A75" t="s">
         <v>245</v>
       </c>
     </row>
-    <row r="74" spans="1:1">
-      <c r="A74" t="s">
+    <row r="76" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A76" t="s">
         <v>246</v>
       </c>
     </row>
-    <row r="75" spans="1:1">
-      <c r="A75" t="s">
+    <row r="77" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A77" t="s">
         <v>247</v>
       </c>
     </row>
-    <row r="76" spans="1:1">
-      <c r="A76" t="s">
+    <row r="78" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A78" t="s">
         <v>248</v>
       </c>
     </row>
-    <row r="77" spans="1:1">
-      <c r="A77" t="s">
+    <row r="79" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A79" t="s">
         <v>249</v>
       </c>
     </row>
-    <row r="78" spans="1:1">
-      <c r="A78" t="s">
+    <row r="80" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A80" t="s">
         <v>250</v>
-      </c>
-    </row>
-    <row r="79" spans="1:1">
-      <c r="A79" t="s">
-        <v>251</v>
-      </c>
-    </row>
-    <row r="80" spans="1:1">
-      <c r="A80" t="s">
-        <v>252</v>
       </c>
     </row>
   </sheetData>
@@ -3652,14 +3794,14 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView zoomScale="150" workbookViewId="0">
       <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="10.75" style="2"/>
     <col min="2" max="2" width="18.125" bestFit="1" customWidth="1"/>
@@ -3669,7 +3811,7 @@
     <col min="6" max="6" width="13.75" style="9" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="4" customFormat="1">
+    <row r="1" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -3686,10 +3828,10 @@
         <v>27</v>
       </c>
       <c r="F1" s="8" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="2">
         <v>40598</v>
       </c>
@@ -3700,7 +3842,7 @@
         <v>598</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="2">
         <v>40602</v>
       </c>
@@ -3736,14 +3878,14 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J40"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:J42"/>
   <sheetViews>
     <sheetView topLeftCell="A16" zoomScale="150" workbookViewId="0">
-      <selection activeCell="E30" sqref="E30:J30"/>
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="8.875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="38.75" style="1" bestFit="1" customWidth="1"/>
@@ -3757,7 +3899,7 @@
     <col min="10" max="10" width="11" style="6" bestFit="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>11</v>
       </c>
@@ -3789,18 +3931,18 @@
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:10">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>31</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="C2" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="D2" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="E2" t="s">
         <v>35</v>
@@ -3821,65 +3963,65 @@
         <v>40600</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="25.5">
+    <row r="4" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="D4" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" ht="25.5">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>41</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="D5" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" ht="25.5">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>42</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="D6" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" ht="25.5">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="D7" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>32</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="C9" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="D9" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="E9" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="F9">
         <v>50</v>
@@ -3897,43 +4039,43 @@
         <v>40601</v>
       </c>
     </row>
-    <row r="11" spans="1:10" ht="38.25">
+    <row r="11" spans="1:10" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>43</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="D11" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" ht="38.25">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>44</v>
       </c>
       <c r="B12" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="D12" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>157</v>
+      </c>
+      <c r="B14" t="s">
         <v>187</v>
       </c>
-      <c r="D12" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10">
-      <c r="A14" t="s">
-        <v>159</v>
-      </c>
-      <c r="B14" t="s">
-        <v>189</v>
-      </c>
       <c r="C14" s="18" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="D14" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="E14" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="F14">
         <v>80</v>
@@ -3951,70 +4093,70 @@
         <v>40602</v>
       </c>
     </row>
-    <row r="15" spans="1:10">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
+        <v>296</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>263</v>
+      </c>
+      <c r="D15" t="s">
+        <v>70</v>
+      </c>
+      <c r="J15" s="7"/>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>297</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>264</v>
+      </c>
+      <c r="D16" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
         <v>298</v>
       </c>
-      <c r="B15" s="1" t="s">
+      <c r="B17" s="1" t="s">
+        <v>266</v>
+      </c>
+      <c r="D17" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>299</v>
+      </c>
+      <c r="B18" s="1" t="s">
         <v>265</v>
       </c>
-      <c r="D15" t="s">
-        <v>72</v>
-      </c>
-      <c r="J15" s="7"/>
-    </row>
-    <row r="16" spans="1:10">
-      <c r="A16" t="s">
-        <v>299</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>266</v>
-      </c>
-      <c r="D16" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="17" spans="1:10">
-      <c r="A17" t="s">
-        <v>300</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>268</v>
-      </c>
-      <c r="D17" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10" ht="25.5">
-      <c r="A18" t="s">
-        <v>301</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>267</v>
-      </c>
       <c r="D18" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="J18" s="7"/>
     </row>
-    <row r="19" spans="1:10">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
       <c r="J19" s="7"/>
     </row>
-    <row r="20" spans="1:10">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B20" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="C20" s="20" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="D20" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="E20" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="F20">
         <v>20</v>
@@ -4032,56 +4174,56 @@
         <v>40602</v>
       </c>
     </row>
-    <row r="21" spans="1:10">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
+        <v>300</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>267</v>
+      </c>
+      <c r="D21" t="s">
+        <v>70</v>
+      </c>
+      <c r="J21" s="7"/>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>301</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>268</v>
+      </c>
+      <c r="D22" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
         <v>302</v>
       </c>
-      <c r="B21" s="1" t="s">
+      <c r="B23" s="1" t="s">
         <v>269</v>
       </c>
-      <c r="D21" t="s">
-        <v>72</v>
-      </c>
-      <c r="J21" s="7"/>
-    </row>
-    <row r="22" spans="1:10">
-      <c r="A22" t="s">
-        <v>303</v>
-      </c>
-      <c r="B22" s="1" t="s">
+      <c r="J23" s="7"/>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="J24" s="7"/>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>74</v>
+      </c>
+      <c r="B25" t="s">
+        <v>112</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>290</v>
+      </c>
+      <c r="D25" t="s">
         <v>270</v>
       </c>
-      <c r="D22" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="23" spans="1:10">
-      <c r="A23" t="s">
-        <v>304</v>
-      </c>
-      <c r="B23" s="1" t="s">
-        <v>271</v>
-      </c>
-      <c r="J23" s="7"/>
-    </row>
-    <row r="24" spans="1:10">
-      <c r="J24" s="7"/>
-    </row>
-    <row r="25" spans="1:10">
-      <c r="A25" t="s">
-        <v>76</v>
-      </c>
-      <c r="B25" t="s">
-        <v>114</v>
-      </c>
-      <c r="C25" s="1" t="s">
-        <v>292</v>
-      </c>
-      <c r="D25" t="s">
-        <v>272</v>
-      </c>
       <c r="E25" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="F25">
         <v>80</v>
@@ -4099,60 +4241,60 @@
         <v>40601</v>
       </c>
     </row>
-    <row r="26" spans="1:10" ht="25.5">
+    <row r="26" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
+        <v>303</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>292</v>
+      </c>
+      <c r="D26" t="s">
+        <v>270</v>
+      </c>
+      <c r="J26" s="7"/>
+    </row>
+    <row r="27" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>304</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>293</v>
+      </c>
+      <c r="D27" t="s">
+        <v>270</v>
+      </c>
+      <c r="J27" s="7"/>
+    </row>
+    <row r="28" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
         <v>305</v>
       </c>
-      <c r="B26" s="1" t="s">
+      <c r="B28" s="1" t="s">
         <v>294</v>
       </c>
-      <c r="D26" t="s">
-        <v>272</v>
-      </c>
-      <c r="J26" s="7"/>
-    </row>
-    <row r="27" spans="1:10" ht="25.5">
-      <c r="A27" t="s">
-        <v>306</v>
-      </c>
-      <c r="B27" s="1" t="s">
-        <v>295</v>
-      </c>
-      <c r="D27" t="s">
-        <v>272</v>
-      </c>
-      <c r="J27" s="7"/>
-    </row>
-    <row r="28" spans="1:10" ht="25.5">
-      <c r="A28" t="s">
-        <v>307</v>
-      </c>
-      <c r="B28" s="1" t="s">
-        <v>296</v>
-      </c>
       <c r="D28" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="J28" s="7"/>
     </row>
-    <row r="29" spans="1:10">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.2">
       <c r="J29" s="7"/>
     </row>
-    <row r="30" spans="1:10">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B30" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="D30" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="E30" s="18" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="F30">
         <v>50</v>
@@ -4170,61 +4312,75 @@
         <v>40602</v>
       </c>
     </row>
-    <row r="31" spans="1:10" ht="25.5">
+    <row r="31" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
+        <v>306</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>295</v>
+      </c>
+      <c r="D31" t="s">
+        <v>270</v>
+      </c>
+      <c r="J31" s="7"/>
+    </row>
+    <row r="32" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>307</v>
+      </c>
+      <c r="B32" s="1" t="s">
         <v>308</v>
       </c>
-      <c r="B31" s="1" t="s">
-        <v>297</v>
-      </c>
-      <c r="D31" t="s">
-        <v>272</v>
-      </c>
-      <c r="J31" s="7"/>
-    </row>
-    <row r="32" spans="1:10" ht="25.5">
-      <c r="A32" t="s">
-        <v>309</v>
-      </c>
-      <c r="B32" s="1" t="s">
-        <v>310</v>
-      </c>
       <c r="D32" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="J32" s="7"/>
     </row>
-    <row r="33" spans="2:2">
-      <c r="B33" s="5" t="s">
+    <row r="33" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="J33" s="7"/>
+    </row>
+    <row r="34" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B34" s="5" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="35" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B35" s="5"/>
+    </row>
+    <row r="36" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B36" s="5" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="34" spans="2:2">
-      <c r="B34" s="5"/>
-    </row>
-    <row r="35" spans="2:2">
-      <c r="B35" s="5" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="36" spans="2:2">
-      <c r="B36" s="1" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="37" spans="2:2">
+    <row r="37" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B37" s="1" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="38" spans="2:10" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="B38" s="1" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="39" spans="2:10" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="B39" s="1" t="s">
+        <v>320</v>
+      </c>
+      <c r="J39" s="7"/>
+    </row>
+    <row r="40" spans="2:10" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="B40" s="1" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="41" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B41" s="5" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="42" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B42" s="1" t="s">
         <v>63</v>
-      </c>
-    </row>
-    <row r="39" spans="2:2">
-      <c r="B39" s="5" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="40" spans="2:2">
-      <c r="B40" s="1" t="s">
-        <v>65</v>
       </c>
     </row>
   </sheetData>
@@ -4240,16 +4396,20 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:J7"/>
   <sheetViews>
-    <sheetView zoomScale="150" workbookViewId="0">
-      <selection activeCell="F23" sqref="F23"/>
+    <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="8.875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="25.5">
+    <row r="1" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>11</v>
       </c>
@@ -4279,6 +4439,90 @@
       </c>
       <c r="J1" s="10" t="s">
         <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>77</v>
+      </c>
+      <c r="B2" t="s">
+        <v>107</v>
+      </c>
+      <c r="F2">
+        <v>20</v>
+      </c>
+      <c r="G2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>78</v>
+      </c>
+      <c r="B3" t="s">
+        <v>115</v>
+      </c>
+      <c r="F3">
+        <v>50</v>
+      </c>
+      <c r="G3">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>79</v>
+      </c>
+      <c r="B4" t="s">
+        <v>108</v>
+      </c>
+      <c r="F4">
+        <v>50</v>
+      </c>
+      <c r="G4">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>80</v>
+      </c>
+      <c r="B5" t="s">
+        <v>33</v>
+      </c>
+      <c r="F5">
+        <v>30</v>
+      </c>
+      <c r="G5">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>81</v>
+      </c>
+      <c r="B6" t="s">
+        <v>99</v>
+      </c>
+      <c r="F6">
+        <v>30</v>
+      </c>
+      <c r="G6">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>82</v>
+      </c>
+      <c r="B7" t="s">
+        <v>100</v>
+      </c>
+      <c r="F7">
+        <v>30</v>
+      </c>
+      <c r="G7">
+        <v>10</v>
       </c>
     </row>
   </sheetData>
@@ -4294,16 +4538,16 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J1"/>
   <sheetViews>
     <sheetView zoomScale="150" workbookViewId="0">
       <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:10" ht="25.5">
+    <row r="1" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>3</v>
       </c>
@@ -4347,16 +4591,16 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J1"/>
   <sheetViews>
     <sheetView zoomScale="150" workbookViewId="0">
       <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:10" ht="25.5">
+    <row r="1" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>3</v>
       </c>

</xml_diff>

<commit_message>
add two more user stories for sprint 2
</commit_message>
<xml_diff>
--- a/Team05Report.xlsx
+++ b/Team05Report.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="240" windowWidth="20730" windowHeight="11760" tabRatio="500" activeTab="6"/>
@@ -18,7 +18,7 @@
     <sheet name="Sprint4" sheetId="6" r:id="rId9"/>
     <sheet name="Sprint5" sheetId="8" r:id="rId10"/>
   </sheets>
-  <calcPr calcId="145621" concurrentCalc="0"/>
+  <calcPr calcId="125725" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -62,7 +62,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="573" uniqueCount="321">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="625" uniqueCount="340">
   <si>
     <t>Date</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -1081,17 +1081,74 @@
   </si>
   <si>
     <t>Modify the user stories we are about to implement next sprint to more proper and completed</t>
+  </si>
+  <si>
+    <t>Individual I1(Jacky /Mao/) is older than 150 years old. Birt date(27 JAN 1848), not dead.</t>
+  </si>
+  <si>
+    <t>Individual I1(Jacky /Mao/)'s birth date is 27 JAN 1848, and he is not dead.</t>
+  </si>
+  <si>
+    <t>Individual I8(Kevin /Brown/) was older than 150 years old. Birt date(1 NOV 1848), deat date(11 SEP 2001).</t>
+  </si>
+  <si>
+    <t>Individual I8(Kevin /Brown/)'s birth date is 1 NOV 1848, and death date is 11 SEP 2001.</t>
+  </si>
+  <si>
+    <t>Individual I6(Lisabella /Taylor/)'s birth date is 6 JUN 2014, she is not dead.</t>
+  </si>
+  <si>
+    <t>AT26~28</t>
+  </si>
+  <si>
+    <t>Get the birth date of the individual</t>
+  </si>
+  <si>
+    <t>Get the death date of the individual(if exist)</t>
+  </si>
+  <si>
+    <t>Check the age of the individual</t>
+  </si>
+  <si>
+    <t>US26</t>
+  </si>
+  <si>
+    <t>Duplicate children</t>
+  </si>
+  <si>
+    <t>A family cannot have more than one children record of the same person.</t>
+  </si>
+  <si>
+    <t>Individual I3(Katie /Brown/) plays multiple roles in Family F2: child, wife</t>
+  </si>
+  <si>
+    <t>Individual I3(Katie /Brown/) is the wife and the child of Family F2.</t>
+  </si>
+  <si>
+    <t>Individual I2(Jianguo /Mao/) is the husband of Family F2.</t>
+  </si>
+  <si>
+    <t>AT29~30</t>
+  </si>
+  <si>
+    <t>Get all the individuals of the family</t>
+  </si>
+  <si>
+    <t>Sort the individuals by ID</t>
+  </si>
+  <si>
+    <t>Check if some individuals play multiple roles in the family</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="m/d"/>
     <numFmt numFmtId="165" formatCode="0.0"/>
   </numFmts>
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="10">
     <font>
       <sz val="10"/>
       <name val="Verdana"/>
@@ -1256,56 +1313,56 @@
     </xf>
   </cellXfs>
   <cellStyles count="50">
-    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="30" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="32" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="34" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="36" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="38" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="40" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="44" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="46" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="48" builtinId="9" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="29" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="31" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="33" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="35" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="37" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="39" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="41" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="43" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="45" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="47" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="49" builtinId="8"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="已访问的超链接" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="20" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="22" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="24" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="26" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="28" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="30" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="32" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="34" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="36" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="38" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="40" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="42" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="44" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="46" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="48" builtinId="9" hidden="1"/>
+    <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle name="超链接" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="15" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="17" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="19" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="21" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="23" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="25" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="27" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="29" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="31" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="33" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="35" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="37" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="39" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="41" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="43" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="45" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="47" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="49" builtinId="8"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
@@ -1321,22 +1378,11 @@
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="1"/>
   <c:lang val="en-US"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
   <c:chart>
-    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
       <c:lineChart>
         <c:grouping val="standard"/>
-        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
@@ -1370,62 +1416,46 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:smooth val="0"/>
         </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
+        <c:dLbls/>
         <c:marker val="1"/>
-        <c:smooth val="0"/>
-        <c:axId val="105415040"/>
-        <c:axId val="105416576"/>
+        <c:axId val="128936960"/>
+        <c:axId val="128938752"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="105415040"/>
+        <c:axId val="128936960"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
-        <c:delete val="0"/>
         <c:axPos val="b"/>
         <c:numFmt formatCode="m/d" sourceLinked="1"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="105416576"/>
+        <c:crossAx val="128938752"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
         <c:baseTimeUnit val="days"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="105416576"/>
+        <c:axId val="128938752"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
-        <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="105415040"/>
+        <c:crossAx val="128936960"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="1" l="0.75000000000000133" r="0.75000000000000133" t="1" header="0.5" footer="0.5"/>
+    <c:pageMargins b="1" l="0.75000000000000144" r="0.75000000000000144" t="1" header="0.5" footer="0.5"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1785,14 +1815,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView zoomScale="150" workbookViewId="0">
       <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75"/>
   <cols>
     <col min="1" max="1" width="7.625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="6.375" customWidth="1"/>
@@ -1801,7 +1831,7 @@
     <col min="5" max="5" width="19.25" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" s="4" customFormat="1">
       <c r="A1" s="4" t="s">
         <v>22</v>
       </c>
@@ -1818,7 +1848,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5">
       <c r="A3" t="s">
         <v>70</v>
       </c>
@@ -1835,7 +1865,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5">
       <c r="A4" t="s">
         <v>129</v>
       </c>
@@ -1852,7 +1882,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5">
       <c r="A5" t="s">
         <v>270</v>
       </c>
@@ -1869,7 +1899,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:5">
       <c r="D9" s="4" t="s">
         <v>67</v>
       </c>
@@ -1898,16 +1928,16 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:J1"/>
   <sheetViews>
     <sheetView zoomScale="150" workbookViewId="0">
       <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75"/>
   <sheetData>
-    <row r="1" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" ht="25.5">
       <c r="A1" s="4" t="s">
         <v>3</v>
       </c>
@@ -1951,14 +1981,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:L26"/>
   <sheetViews>
     <sheetView zoomScale="150" workbookViewId="0">
       <selection activeCell="G8" sqref="G8:H13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75"/>
   <cols>
     <col min="1" max="1" width="6.625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="8.875" bestFit="1" customWidth="1"/>
@@ -1974,7 +2004,7 @@
     <col min="12" max="12" width="10.75" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:12" s="4" customFormat="1">
       <c r="A1" s="4" t="s">
         <v>40</v>
       </c>
@@ -2012,7 +2042,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:12">
       <c r="A2">
         <v>1</v>
       </c>
@@ -2050,7 +2080,7 @@
         <v>40598</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:12">
       <c r="A3">
         <v>1</v>
       </c>
@@ -2088,7 +2118,7 @@
         <v>40598</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:12">
       <c r="A4">
         <v>1</v>
       </c>
@@ -2126,7 +2156,7 @@
         <v>40598</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:12">
       <c r="A5">
         <v>1</v>
       </c>
@@ -2164,7 +2194,7 @@
         <v>40598</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:12">
       <c r="A6">
         <v>1</v>
       </c>
@@ -2202,7 +2232,7 @@
         <v>40598</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:12">
       <c r="A7">
         <v>1</v>
       </c>
@@ -2240,7 +2270,7 @@
         <v>40598</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:12">
       <c r="A8">
         <v>2</v>
       </c>
@@ -2260,7 +2290,7 @@
         <v>40598</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:12">
       <c r="A9">
         <v>2</v>
       </c>
@@ -2280,7 +2310,7 @@
         <v>40598</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:12">
       <c r="A10">
         <v>2</v>
       </c>
@@ -2300,7 +2330,7 @@
         <v>40598</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:12">
       <c r="A11">
         <v>2</v>
       </c>
@@ -2320,7 +2350,7 @@
         <v>40598</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:12">
       <c r="A12">
         <v>2</v>
       </c>
@@ -2340,7 +2370,7 @@
         <v>40598</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:12">
       <c r="A13">
         <v>2</v>
       </c>
@@ -2360,7 +2390,7 @@
         <v>40598</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:12">
       <c r="B14" t="s">
         <v>83</v>
       </c>
@@ -2371,7 +2401,7 @@
         <v>40598</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:12">
       <c r="B15" t="s">
         <v>84</v>
       </c>
@@ -2382,7 +2412,7 @@
         <v>40598</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:12">
       <c r="B16" t="s">
         <v>85</v>
       </c>
@@ -2393,7 +2423,7 @@
         <v>40598</v>
       </c>
     </row>
-    <row r="17" spans="2:12" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:12">
       <c r="B17" t="s">
         <v>86</v>
       </c>
@@ -2404,7 +2434,7 @@
         <v>40598</v>
       </c>
     </row>
-    <row r="18" spans="2:12" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:12">
       <c r="B18" t="s">
         <v>87</v>
       </c>
@@ -2415,7 +2445,7 @@
         <v>40598</v>
       </c>
     </row>
-    <row r="19" spans="2:12" x14ac:dyDescent="0.2">
+    <row r="19" spans="2:12">
       <c r="B19" t="s">
         <v>88</v>
       </c>
@@ -2426,7 +2456,7 @@
         <v>40598</v>
       </c>
     </row>
-    <row r="20" spans="2:12" x14ac:dyDescent="0.2">
+    <row r="20" spans="2:12">
       <c r="B20" t="s">
         <v>89</v>
       </c>
@@ -2437,7 +2467,7 @@
         <v>40598</v>
       </c>
     </row>
-    <row r="21" spans="2:12" x14ac:dyDescent="0.2">
+    <row r="21" spans="2:12">
       <c r="B21" t="s">
         <v>90</v>
       </c>
@@ -2448,7 +2478,7 @@
         <v>40598</v>
       </c>
     </row>
-    <row r="22" spans="2:12" x14ac:dyDescent="0.2">
+    <row r="22" spans="2:12">
       <c r="B22" t="s">
         <v>91</v>
       </c>
@@ -2459,7 +2489,7 @@
         <v>40598</v>
       </c>
     </row>
-    <row r="23" spans="2:12" x14ac:dyDescent="0.2">
+    <row r="23" spans="2:12">
       <c r="B23" t="s">
         <v>92</v>
       </c>
@@ -2470,7 +2500,7 @@
         <v>40602</v>
       </c>
     </row>
-    <row r="24" spans="2:12" x14ac:dyDescent="0.2">
+    <row r="24" spans="2:12">
       <c r="B24" t="s">
         <v>93</v>
       </c>
@@ -2481,7 +2511,7 @@
         <v>40602</v>
       </c>
     </row>
-    <row r="25" spans="2:12" x14ac:dyDescent="0.2">
+    <row r="25" spans="2:12">
       <c r="B25" t="s">
         <v>94</v>
       </c>
@@ -2492,7 +2522,7 @@
         <v>40602</v>
       </c>
     </row>
-    <row r="26" spans="2:12" x14ac:dyDescent="0.2">
+    <row r="26" spans="2:12">
       <c r="B26" t="s">
         <v>95</v>
       </c>
@@ -2516,14 +2546,14 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F26"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:F27"/>
   <sheetViews>
     <sheetView zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8:F13"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75"/>
   <cols>
     <col min="1" max="1" width="8.875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="24.75" bestFit="1" customWidth="1"/>
@@ -2532,7 +2562,7 @@
     <col min="6" max="6" width="9" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6">
       <c r="A1" s="4" t="s">
         <v>28</v>
       </c>
@@ -2552,7 +2582,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" ht="25.5">
       <c r="A2" t="s">
         <v>31</v>
       </c>
@@ -2572,7 +2602,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" ht="25.5">
       <c r="A3" t="s">
         <v>32</v>
       </c>
@@ -2592,7 +2622,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6">
       <c r="A4" t="s">
         <v>34</v>
       </c>
@@ -2612,7 +2642,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6">
       <c r="A5" t="s">
         <v>74</v>
       </c>
@@ -2632,7 +2662,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6">
       <c r="A6" t="s">
         <v>75</v>
       </c>
@@ -2652,7 +2682,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:6">
       <c r="A7" t="s">
         <v>76</v>
       </c>
@@ -2672,7 +2702,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:6">
       <c r="A8" t="s">
         <v>77</v>
       </c>
@@ -2689,7 +2719,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:6">
       <c r="A9" t="s">
         <v>78</v>
       </c>
@@ -2706,7 +2736,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:6">
       <c r="A10" t="s">
         <v>79</v>
       </c>
@@ -2723,7 +2753,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:6">
       <c r="A11" t="s">
         <v>80</v>
       </c>
@@ -2740,7 +2770,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:6">
       <c r="A12" t="s">
         <v>81</v>
       </c>
@@ -2757,7 +2787,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:6">
       <c r="A13" t="s">
         <v>82</v>
       </c>
@@ -2774,7 +2804,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:6" ht="25.5">
       <c r="A14" t="s">
         <v>83</v>
       </c>
@@ -2785,7 +2815,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:6">
       <c r="A15" t="s">
         <v>84</v>
       </c>
@@ -2796,7 +2826,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:6">
       <c r="A16" t="s">
         <v>85</v>
       </c>
@@ -2807,7 +2837,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:3">
       <c r="A17" t="s">
         <v>86</v>
       </c>
@@ -2818,7 +2848,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:3">
       <c r="A18" t="s">
         <v>87</v>
       </c>
@@ -2829,7 +2859,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:3" ht="25.5">
       <c r="A19" t="s">
         <v>88</v>
       </c>
@@ -2840,7 +2870,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:3">
       <c r="A20" t="s">
         <v>89</v>
       </c>
@@ -2851,7 +2881,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:3">
       <c r="A21" t="s">
         <v>90</v>
       </c>
@@ -2862,7 +2892,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:3">
       <c r="A22" t="s">
         <v>91</v>
       </c>
@@ -2873,7 +2903,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="23" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:3" ht="25.5">
       <c r="A23" t="s">
         <v>92</v>
       </c>
@@ -2884,7 +2914,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="24" spans="1:3" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:3" ht="25.5">
       <c r="A24" t="s">
         <v>93</v>
       </c>
@@ -2895,7 +2925,7 @@
         <v>314</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:3">
       <c r="A25" t="s">
         <v>94</v>
       </c>
@@ -2906,7 +2936,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:3">
       <c r="A26" t="s">
         <v>95</v>
       </c>
@@ -2915,6 +2945,17 @@
       </c>
       <c r="C26" s="1" t="s">
         <v>316</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3">
+      <c r="A27" t="s">
+        <v>330</v>
+      </c>
+      <c r="B27" s="18" t="s">
+        <v>331</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>332</v>
       </c>
     </row>
   </sheetData>
@@ -2929,24 +2970,24 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F80"/>
   <sheetViews>
-    <sheetView zoomScale="145" zoomScaleNormal="145" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="E29" sqref="E29"/>
+    <sheetView topLeftCell="A28" zoomScale="145" zoomScaleNormal="145" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="E34" sqref="E34:F34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75"/>
   <cols>
     <col min="1" max="1" width="6.375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="8.875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="20.25" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="23.875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="40" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="36" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="7.25" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6">
       <c r="A1" s="4" t="s">
         <v>61</v>
       </c>
@@ -2966,7 +3007,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" ht="47.25">
       <c r="A2" t="s">
         <v>54</v>
       </c>
@@ -2986,7 +3027,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" ht="47.25">
       <c r="A3" t="s">
         <v>55</v>
       </c>
@@ -3006,7 +3047,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" ht="47.25">
       <c r="A4" t="s">
         <v>56</v>
       </c>
@@ -3026,7 +3067,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" ht="47.25">
       <c r="A5" t="s">
         <v>57</v>
       </c>
@@ -3046,7 +3087,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" ht="47.25">
       <c r="A6" t="s">
         <v>58</v>
       </c>
@@ -3066,7 +3107,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" ht="31.5">
       <c r="A7" t="s">
         <v>59</v>
       </c>
@@ -3086,7 +3127,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="63" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" ht="63">
       <c r="A8" t="s">
         <v>151</v>
       </c>
@@ -3106,7 +3147,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="63" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" ht="63">
       <c r="A9" t="s">
         <v>155</v>
       </c>
@@ -3126,7 +3167,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="78.75" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" ht="78.75">
       <c r="A10" t="s">
         <v>156</v>
       </c>
@@ -3146,7 +3187,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="63" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" ht="63">
       <c r="A11" t="s">
         <v>158</v>
       </c>
@@ -3166,7 +3207,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="63" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" ht="63">
       <c r="A12" t="s">
         <v>159</v>
       </c>
@@ -3186,7 +3227,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="78.75" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" ht="78.75">
       <c r="A13" t="s">
         <v>160</v>
       </c>
@@ -3206,7 +3247,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" ht="47.25">
       <c r="A14" t="s">
         <v>171</v>
       </c>
@@ -3226,7 +3267,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" ht="47.25">
       <c r="A15" t="s">
         <v>173</v>
       </c>
@@ -3246,7 +3287,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="16" spans="1:6" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:6" ht="38.25">
       <c r="A16" t="s">
         <v>189</v>
       </c>
@@ -3266,7 +3307,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="17" spans="1:6" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:6" ht="38.25">
       <c r="A17" t="s">
         <v>190</v>
       </c>
@@ -3286,7 +3327,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="18" spans="1:6" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:6" ht="38.25">
       <c r="A18" t="s">
         <v>191</v>
       </c>
@@ -3306,7 +3347,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="19" spans="1:6" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:6" ht="38.25">
       <c r="A19" t="s">
         <v>192</v>
       </c>
@@ -3326,7 +3367,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="20" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" ht="26.25">
       <c r="A20" t="s">
         <v>193</v>
       </c>
@@ -3346,7 +3387,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="21" spans="1:6" ht="47.25" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:6" ht="47.25">
       <c r="A21" t="s">
         <v>194</v>
       </c>
@@ -3366,7 +3407,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="22" spans="1:6" ht="47.25" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:6" ht="47.25">
       <c r="A22" t="s">
         <v>195</v>
       </c>
@@ -3386,7 +3427,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="23" spans="1:6" ht="37.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:6" ht="37.5" customHeight="1">
       <c r="A23" t="s">
         <v>196</v>
       </c>
@@ -3406,7 +3447,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="24" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" ht="26.25">
       <c r="A24" t="s">
         <v>197</v>
       </c>
@@ -3426,7 +3467,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="25" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:6" ht="25.5">
       <c r="A25" t="s">
         <v>196</v>
       </c>
@@ -3446,7 +3487,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:6">
       <c r="A26" t="s">
         <v>196</v>
       </c>
@@ -3466,7 +3507,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="27" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:6" ht="25.5">
       <c r="A27" t="s">
         <v>197</v>
       </c>
@@ -3486,7 +3527,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="28" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:6" ht="25.5">
       <c r="A28" t="s">
         <v>198</v>
       </c>
@@ -3506,7 +3547,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="29" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:6" ht="25.5">
       <c r="A29" t="s">
         <v>199</v>
       </c>
@@ -3526,257 +3567,332 @@
         <v>53</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:6" ht="38.25">
       <c r="A30" t="s">
         <v>200</v>
       </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B30" t="s">
+        <v>77</v>
+      </c>
+      <c r="C30" t="s">
+        <v>107</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>322</v>
+      </c>
+      <c r="E30" s="1" t="s">
+        <v>321</v>
+      </c>
+      <c r="F30" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" ht="38.25">
       <c r="A31" t="s">
         <v>201</v>
       </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B31" t="s">
+        <v>77</v>
+      </c>
+      <c r="C31" t="s">
+        <v>107</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>324</v>
+      </c>
+      <c r="E31" s="1" t="s">
+        <v>323</v>
+      </c>
+      <c r="F31" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" ht="26.25">
       <c r="A32" t="s">
         <v>202</v>
       </c>
-    </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B32" t="s">
+        <v>77</v>
+      </c>
+      <c r="C32" t="s">
+        <v>107</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>325</v>
+      </c>
+      <c r="E32" s="12" t="s">
+        <v>51</v>
+      </c>
+      <c r="F32" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" ht="25.5">
       <c r="A33" t="s">
         <v>203</v>
       </c>
-    </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B33" t="s">
+        <v>78</v>
+      </c>
+      <c r="C33" t="s">
+        <v>115</v>
+      </c>
+      <c r="D33" s="1" t="s">
+        <v>334</v>
+      </c>
+      <c r="E33" s="1" t="s">
+        <v>333</v>
+      </c>
+      <c r="F33" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" ht="26.25">
       <c r="A34" t="s">
         <v>204</v>
       </c>
-    </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B34" t="s">
+        <v>78</v>
+      </c>
+      <c r="C34" t="s">
+        <v>115</v>
+      </c>
+      <c r="D34" s="1" t="s">
+        <v>335</v>
+      </c>
+      <c r="E34" s="12" t="s">
+        <v>51</v>
+      </c>
+      <c r="F34" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6">
       <c r="A35" t="s">
         <v>205</v>
       </c>
     </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:6">
       <c r="A36" t="s">
         <v>206</v>
       </c>
     </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:6">
       <c r="A37" t="s">
         <v>207</v>
       </c>
     </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:6">
       <c r="A38" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:6">
       <c r="A39" t="s">
         <v>209</v>
       </c>
     </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:6">
       <c r="A40" t="s">
         <v>210</v>
       </c>
     </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:6">
       <c r="A41" t="s">
         <v>211</v>
       </c>
     </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:6">
       <c r="A42" t="s">
         <v>212</v>
       </c>
     </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:6">
       <c r="A43" t="s">
         <v>213</v>
       </c>
     </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:6">
       <c r="A44" t="s">
         <v>214</v>
       </c>
     </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:6">
       <c r="A45" t="s">
         <v>215</v>
       </c>
     </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:6">
       <c r="A46" t="s">
         <v>216</v>
       </c>
     </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:6">
       <c r="A47" t="s">
         <v>217</v>
       </c>
     </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:6">
       <c r="A48" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:1">
       <c r="A49" t="s">
         <v>219</v>
       </c>
     </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:1">
       <c r="A50" t="s">
         <v>220</v>
       </c>
     </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:1">
       <c r="A51" t="s">
         <v>221</v>
       </c>
     </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:1">
       <c r="A52" t="s">
         <v>222</v>
       </c>
     </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:1">
       <c r="A53" t="s">
         <v>223</v>
       </c>
     </row>
-    <row r="54" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:1">
       <c r="A54" t="s">
         <v>224</v>
       </c>
     </row>
-    <row r="55" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:1">
       <c r="A55" t="s">
         <v>225</v>
       </c>
     </row>
-    <row r="56" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:1">
       <c r="A56" t="s">
         <v>226</v>
       </c>
     </row>
-    <row r="57" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:1">
       <c r="A57" t="s">
         <v>227</v>
       </c>
     </row>
-    <row r="58" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:1">
       <c r="A58" t="s">
         <v>228</v>
       </c>
     </row>
-    <row r="59" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:1">
       <c r="A59" t="s">
         <v>229</v>
       </c>
     </row>
-    <row r="60" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:1">
       <c r="A60" t="s">
         <v>230</v>
       </c>
     </row>
-    <row r="61" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:1">
       <c r="A61" t="s">
         <v>231</v>
       </c>
     </row>
-    <row r="62" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:1">
       <c r="A62" t="s">
         <v>232</v>
       </c>
     </row>
-    <row r="63" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:1">
       <c r="A63" t="s">
         <v>233</v>
       </c>
     </row>
-    <row r="64" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:1">
       <c r="A64" t="s">
         <v>234</v>
       </c>
     </row>
-    <row r="65" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:1">
       <c r="A65" t="s">
         <v>235</v>
       </c>
     </row>
-    <row r="66" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:1">
       <c r="A66" t="s">
         <v>236</v>
       </c>
     </row>
-    <row r="67" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:1">
       <c r="A67" t="s">
         <v>237</v>
       </c>
     </row>
-    <row r="68" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:1">
       <c r="A68" t="s">
         <v>238</v>
       </c>
     </row>
-    <row r="69" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:1">
       <c r="A69" t="s">
         <v>239</v>
       </c>
     </row>
-    <row r="70" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:1">
       <c r="A70" t="s">
         <v>240</v>
       </c>
     </row>
-    <row r="71" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:1">
       <c r="A71" t="s">
         <v>241</v>
       </c>
     </row>
-    <row r="72" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:1">
       <c r="A72" t="s">
         <v>242</v>
       </c>
     </row>
-    <row r="73" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:1">
       <c r="A73" t="s">
         <v>243</v>
       </c>
     </row>
-    <row r="74" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:1">
       <c r="A74" t="s">
         <v>244</v>
       </c>
     </row>
-    <row r="75" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:1">
       <c r="A75" t="s">
         <v>245</v>
       </c>
     </row>
-    <row r="76" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:1">
       <c r="A76" t="s">
         <v>246</v>
       </c>
     </row>
-    <row r="77" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:1">
       <c r="A77" t="s">
         <v>247</v>
       </c>
     </row>
-    <row r="78" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:1">
       <c r="A78" t="s">
         <v>248</v>
       </c>
     </row>
-    <row r="79" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:1">
       <c r="A79" t="s">
         <v>249</v>
       </c>
     </row>
-    <row r="80" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:1">
       <c r="A80" t="s">
         <v>250</v>
       </c>
@@ -3794,14 +3910,14 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView zoomScale="150" workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75"/>
   <cols>
     <col min="1" max="1" width="10.75" style="2"/>
     <col min="2" max="2" width="18.125" bestFit="1" customWidth="1"/>
@@ -3811,7 +3927,7 @@
     <col min="6" max="6" width="13.75" style="9" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" s="4" customFormat="1">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -3831,7 +3947,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6">
       <c r="A2" s="2">
         <v>40598</v>
       </c>
@@ -3842,7 +3958,7 @@
         <v>598</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6">
       <c r="A3" s="2">
         <v>40602</v>
       </c>
@@ -3878,14 +3994,14 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:J42"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" zoomScale="150" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+    <sheetView zoomScale="150" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75"/>
   <cols>
     <col min="1" max="1" width="8.875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="38.75" style="1" bestFit="1" customWidth="1"/>
@@ -3899,7 +4015,7 @@
     <col min="10" max="10" width="11" style="6" bestFit="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10">
       <c r="A1" s="4" t="s">
         <v>11</v>
       </c>
@@ -3931,7 +4047,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:10">
       <c r="A2" t="s">
         <v>31</v>
       </c>
@@ -3963,7 +4079,7 @@
         <v>40600</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:10" ht="25.5">
       <c r="A4" t="s">
         <v>186</v>
       </c>
@@ -3974,7 +4090,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:10" ht="25.5">
       <c r="A5" t="s">
         <v>41</v>
       </c>
@@ -3985,7 +4101,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="6" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:10" ht="25.5">
       <c r="A6" t="s">
         <v>42</v>
       </c>
@@ -3996,7 +4112,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="7" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:10" ht="25.5">
       <c r="A7" t="s">
         <v>181</v>
       </c>
@@ -4007,7 +4123,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:10">
       <c r="A9" t="s">
         <v>32</v>
       </c>
@@ -4039,7 +4155,7 @@
         <v>40601</v>
       </c>
     </row>
-    <row r="11" spans="1:10" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:10" ht="38.25">
       <c r="A11" t="s">
         <v>43</v>
       </c>
@@ -4050,7 +4166,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="12" spans="1:10" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:10" ht="38.25">
       <c r="A12" t="s">
         <v>44</v>
       </c>
@@ -4061,7 +4177,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:10">
       <c r="A14" t="s">
         <v>157</v>
       </c>
@@ -4093,7 +4209,7 @@
         <v>40602</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:10">
       <c r="A15" t="s">
         <v>296</v>
       </c>
@@ -4105,7 +4221,7 @@
       </c>
       <c r="J15" s="7"/>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:10">
       <c r="A16" t="s">
         <v>297</v>
       </c>
@@ -4116,7 +4232,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:10">
       <c r="A17" t="s">
         <v>298</v>
       </c>
@@ -4127,7 +4243,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="18" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:10" ht="25.5">
       <c r="A18" t="s">
         <v>299</v>
       </c>
@@ -4139,10 +4255,10 @@
       </c>
       <c r="J18" s="7"/>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:10">
       <c r="J19" s="7"/>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:10">
       <c r="A20" t="s">
         <v>75</v>
       </c>
@@ -4174,7 +4290,7 @@
         <v>40602</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:10">
       <c r="A21" t="s">
         <v>300</v>
       </c>
@@ -4186,7 +4302,7 @@
       </c>
       <c r="J21" s="7"/>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:10">
       <c r="A22" t="s">
         <v>301</v>
       </c>
@@ -4197,7 +4313,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:10">
       <c r="A23" t="s">
         <v>302</v>
       </c>
@@ -4206,10 +4322,10 @@
       </c>
       <c r="J23" s="7"/>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:10">
       <c r="J24" s="7"/>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:10">
       <c r="A25" t="s">
         <v>74</v>
       </c>
@@ -4241,7 +4357,7 @@
         <v>40601</v>
       </c>
     </row>
-    <row r="26" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:10" ht="25.5">
       <c r="A26" t="s">
         <v>303</v>
       </c>
@@ -4253,7 +4369,7 @@
       </c>
       <c r="J26" s="7"/>
     </row>
-    <row r="27" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:10" ht="25.5">
       <c r="A27" t="s">
         <v>304</v>
       </c>
@@ -4265,7 +4381,7 @@
       </c>
       <c r="J27" s="7"/>
     </row>
-    <row r="28" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:10" ht="25.5">
       <c r="A28" t="s">
         <v>305</v>
       </c>
@@ -4277,10 +4393,10 @@
       </c>
       <c r="J28" s="7"/>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:10">
       <c r="J29" s="7"/>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:10">
       <c r="A30" t="s">
         <v>76</v>
       </c>
@@ -4312,7 +4428,7 @@
         <v>40602</v>
       </c>
     </row>
-    <row r="31" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:10" ht="25.5">
       <c r="A31" t="s">
         <v>306</v>
       </c>
@@ -4324,7 +4440,7 @@
       </c>
       <c r="J31" s="7"/>
     </row>
-    <row r="32" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:10" ht="25.5">
       <c r="A32" t="s">
         <v>307</v>
       </c>
@@ -4336,49 +4452,49 @@
       </c>
       <c r="J32" s="7"/>
     </row>
-    <row r="33" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="33" spans="2:10">
       <c r="J33" s="7"/>
     </row>
-    <row r="34" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="34" spans="2:10">
       <c r="B34" s="5" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="35" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="35" spans="2:10">
       <c r="B35" s="5"/>
     </row>
-    <row r="36" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="36" spans="2:10">
       <c r="B36" s="5" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="37" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="37" spans="2:10">
       <c r="B37" s="1" t="s">
         <v>318</v>
       </c>
     </row>
-    <row r="38" spans="2:10" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="38" spans="2:10" ht="25.5">
       <c r="B38" s="1" t="s">
         <v>317</v>
       </c>
     </row>
-    <row r="39" spans="2:10" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="39" spans="2:10" ht="38.25">
       <c r="B39" s="1" t="s">
         <v>320</v>
       </c>
       <c r="J39" s="7"/>
     </row>
-    <row r="40" spans="2:10" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="40" spans="2:10" ht="25.5">
       <c r="B40" s="1" t="s">
         <v>319</v>
       </c>
     </row>
-    <row r="41" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="41" spans="2:10">
       <c r="B41" s="5" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="42" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="42" spans="2:10">
       <c r="B42" s="1" t="s">
         <v>63</v>
       </c>
@@ -4396,20 +4512,20 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J7"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:J20"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
       <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75"/>
   <cols>
     <col min="1" max="1" width="8.875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="24.125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10">
       <c r="A1" s="4" t="s">
         <v>11</v>
       </c>
@@ -4441,87 +4557,199 @@
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:10">
       <c r="A2" t="s">
         <v>77</v>
       </c>
       <c r="B2" t="s">
         <v>107</v>
       </c>
+      <c r="C2" t="s">
+        <v>326</v>
+      </c>
+      <c r="D2" t="s">
+        <v>129</v>
+      </c>
+      <c r="E2" t="s">
+        <v>177</v>
+      </c>
       <c r="F2">
         <v>20</v>
       </c>
       <c r="G2">
         <v>10</v>
       </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
+      <c r="H2">
+        <v>20</v>
+      </c>
+      <c r="I2">
+        <v>30</v>
+      </c>
+      <c r="J2" s="16">
+        <v>40608</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" ht="25.5">
+      <c r="A4" t="s">
+        <v>186</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>327</v>
+      </c>
+      <c r="C4" s="1"/>
+      <c r="D4" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" ht="25.5">
+      <c r="A5" t="s">
+        <v>41</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>328</v>
+      </c>
+      <c r="C5" s="1"/>
+      <c r="D5" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" ht="25.5">
+      <c r="A6" t="s">
+        <v>42</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>329</v>
+      </c>
+      <c r="C6" s="1"/>
+      <c r="D6" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10">
+      <c r="B7" s="1"/>
+      <c r="C7" s="1"/>
+    </row>
+    <row r="8" spans="1:10">
+      <c r="A8" t="s">
         <v>78</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B8" t="s">
         <v>115</v>
       </c>
-      <c r="F3">
+      <c r="C8" t="s">
+        <v>336</v>
+      </c>
+      <c r="D8" t="s">
+        <v>129</v>
+      </c>
+      <c r="E8" t="s">
+        <v>177</v>
+      </c>
+      <c r="F8">
         <v>50</v>
       </c>
-      <c r="G3">
+      <c r="G8">
         <v>30</v>
       </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
+      <c r="H8">
+        <v>72</v>
+      </c>
+      <c r="I8">
+        <v>30</v>
+      </c>
+      <c r="J8" s="16">
+        <v>40608</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" ht="25.5">
+      <c r="A10" t="s">
+        <v>186</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>337</v>
+      </c>
+      <c r="C10" s="1"/>
+      <c r="D10" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10">
+      <c r="A11" t="s">
+        <v>41</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>338</v>
+      </c>
+      <c r="C11" s="1"/>
+      <c r="D11" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" ht="38.25">
+      <c r="A12" t="s">
+        <v>42</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>339</v>
+      </c>
+      <c r="C12" s="1"/>
+      <c r="D12" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7">
+      <c r="A17" t="s">
         <v>79</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B17" t="s">
         <v>108</v>
       </c>
-      <c r="F4">
+      <c r="F17">
         <v>50</v>
       </c>
-      <c r="G4">
+      <c r="G17">
         <v>45</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
+    <row r="18" spans="1:7">
+      <c r="A18" t="s">
         <v>80</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B18" t="s">
         <v>33</v>
       </c>
-      <c r="F5">
+      <c r="F18">
         <v>30</v>
       </c>
-      <c r="G5">
+      <c r="G18">
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
+    <row r="19" spans="1:7">
+      <c r="A19" t="s">
         <v>81</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B19" t="s">
         <v>99</v>
       </c>
-      <c r="F6">
+      <c r="F19">
         <v>30</v>
       </c>
-      <c r="G6">
+      <c r="G19">
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
+    <row r="20" spans="1:7">
+      <c r="A20" t="s">
         <v>82</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B20" t="s">
         <v>100</v>
       </c>
-      <c r="F7">
+      <c r="F20">
         <v>30</v>
       </c>
-      <c r="G7">
+      <c r="G20">
         <v>10</v>
       </c>
     </row>
@@ -4538,16 +4766,16 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:J1"/>
   <sheetViews>
     <sheetView zoomScale="150" workbookViewId="0">
       <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75"/>
   <sheetData>
-    <row r="1" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" ht="25.5">
       <c r="A1" s="4" t="s">
         <v>3</v>
       </c>
@@ -4591,16 +4819,16 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:J1"/>
   <sheetViews>
     <sheetView zoomScale="150" workbookViewId="0">
       <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75"/>
   <sheetData>
-    <row r="1" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" ht="25.5">
       <c r="A1" s="4" t="s">
         <v>3</v>
       </c>

</xml_diff>

<commit_message>
implemented user story 13
</commit_message>
<xml_diff>
--- a/Team05Report.xlsx
+++ b/Team05Report.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="240" windowWidth="20730" windowHeight="11760" tabRatio="500" activeTab="6"/>
+    <workbookView xWindow="240" yWindow="240" windowWidth="20730" windowHeight="11760" tabRatio="500" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="Team" sheetId="1" r:id="rId1"/>
@@ -62,7 +62,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="796" uniqueCount="414">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="833" uniqueCount="434">
   <si>
     <t>Date</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -1361,6 +1361,66 @@
   </si>
   <si>
     <t>AT37~AT38</t>
+  </si>
+  <si>
+    <t>In Family F5, wife I5(Emily /Mao/)'s death date(5 JUN 2014) is &lt; her child I6(Lisabella /Taylor/)'s birth date(6 JUN 2014)</t>
+  </si>
+  <si>
+    <t>In Family F5, husband I7(Chris /Taylor/)'s death date(6 JUN 2013) + 10 months is &lt; his child I6(Lisabella /Taylor/)'s birth date(6 JUN 2014)</t>
+  </si>
+  <si>
+    <t>In Family F5, wife I5(Emily /Mao/) died on 5 JUN 2014, and child I6(Lisabella /Taylor/) was born on 6 JUN 2014</t>
+  </si>
+  <si>
+    <t>In Family F5, husband I7(Chris /Taylor/) died on 6 JUN 2013, and child I6(Lisabella /Taylor/) was born on 6 JUN 2014</t>
+  </si>
+  <si>
+    <t>In Family F6, husband I8(Kevin /Brown/) died on 11 SEP 2001, wife I10(Jen /Brown/) not dead, child I11(James /Brown/) was born on 1 MAY 1962</t>
+  </si>
+  <si>
+    <t>AT44~46</t>
+  </si>
+  <si>
+    <t>T13.01</t>
+  </si>
+  <si>
+    <t>T13.02</t>
+  </si>
+  <si>
+    <t>T13.03</t>
+  </si>
+  <si>
+    <t>Get the death date of the wife(if exists) in each family</t>
+  </si>
+  <si>
+    <t>Compare the death date of the wife with the birth date of her each child</t>
+  </si>
+  <si>
+    <t>Check if the wife died before she giving birth to some child</t>
+  </si>
+  <si>
+    <t>T13.04</t>
+  </si>
+  <si>
+    <t>T13.05</t>
+  </si>
+  <si>
+    <t>T13.06</t>
+  </si>
+  <si>
+    <t>Get the death date of the husband(if exists) in each family</t>
+  </si>
+  <si>
+    <t>T13.07</t>
+  </si>
+  <si>
+    <t>Add 10 months to the death date</t>
+  </si>
+  <si>
+    <t>Compare the fixed death date of the husband with the birth date of her each child</t>
+  </si>
+  <si>
+    <t>Check if the husband died more than 10 months before his child was born</t>
   </si>
 </sst>
 </file>
@@ -1647,25 +1707,25 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="209016704"/>
-        <c:axId val="209018240"/>
+        <c:axId val="104298368"/>
+        <c:axId val="104299904"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="209016704"/>
+        <c:axId val="104298368"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="m/d" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="209018240"/>
+        <c:crossAx val="104299904"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
         <c:baseTimeUnit val="days"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="209018240"/>
+        <c:axId val="104299904"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1673,7 +1733,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="209016704"/>
+        <c:crossAx val="104298368"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1683,7 +1743,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="1" l="0.75000000000000189" r="0.75000000000000189" t="1" header="0.5" footer="0.5"/>
+    <c:pageMargins b="1" l="0.750000000000002" r="0.750000000000002" t="1" header="0.5" footer="0.5"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -2940,8 +3000,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F31"/>
   <sheetViews>
-    <sheetView topLeftCell="A5" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+    <sheetView topLeftCell="A4" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="A14" sqref="A14:B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75"/>
@@ -3462,8 +3522,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F77"/>
   <sheetViews>
-    <sheetView topLeftCell="A30" zoomScale="145" zoomScaleNormal="145" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="A35" sqref="A35:A37"/>
+    <sheetView topLeftCell="A39" zoomScale="145" zoomScaleNormal="145" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="D51" sqref="D51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75"/>
@@ -4356,19 +4416,64 @@
         <v>53</v>
       </c>
     </row>
-    <row r="45" spans="1:6">
+    <row r="45" spans="1:6" ht="51">
       <c r="A45" t="s">
         <v>218</v>
       </c>
-    </row>
-    <row r="46" spans="1:6">
+      <c r="B45" s="18" t="s">
+        <v>83</v>
+      </c>
+      <c r="C45" t="s">
+        <v>101</v>
+      </c>
+      <c r="D45" s="1" t="s">
+        <v>416</v>
+      </c>
+      <c r="E45" s="1" t="s">
+        <v>414</v>
+      </c>
+      <c r="F45" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" ht="51">
       <c r="A46" t="s">
         <v>219</v>
       </c>
-    </row>
-    <row r="47" spans="1:6">
+      <c r="B46" s="18" t="s">
+        <v>83</v>
+      </c>
+      <c r="C46" t="s">
+        <v>101</v>
+      </c>
+      <c r="D46" s="1" t="s">
+        <v>417</v>
+      </c>
+      <c r="E46" s="1" t="s">
+        <v>415</v>
+      </c>
+      <c r="F46" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" ht="51">
       <c r="A47" t="s">
         <v>220</v>
+      </c>
+      <c r="B47" s="18" t="s">
+        <v>83</v>
+      </c>
+      <c r="C47" t="s">
+        <v>101</v>
+      </c>
+      <c r="D47" s="1" t="s">
+        <v>418</v>
+      </c>
+      <c r="E47" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="F47" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="48" spans="1:6">
@@ -5159,8 +5264,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:J45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="150" workbookViewId="0">
-      <selection activeCell="E24" sqref="E24"/>
+    <sheetView zoomScale="150" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4:D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75"/>
@@ -5687,10 +5792,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J7"/>
+  <dimension ref="A1:J16"/>
   <sheetViews>
-    <sheetView zoomScale="150" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75"/>
@@ -5737,98 +5842,193 @@
       <c r="B2" t="s">
         <v>101</v>
       </c>
+      <c r="C2" t="s">
+        <v>419</v>
+      </c>
       <c r="D2" s="18" t="s">
         <v>129</v>
       </c>
+      <c r="E2" s="18" t="s">
+        <v>331</v>
+      </c>
       <c r="F2">
         <v>70</v>
       </c>
       <c r="G2">
         <v>30</v>
       </c>
-    </row>
-    <row r="3" spans="1:10">
-      <c r="A3" t="s">
+      <c r="H2">
+        <v>115</v>
+      </c>
+      <c r="I2">
+        <v>40</v>
+      </c>
+      <c r="J2" s="16">
+        <v>40625</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" ht="25.5">
+      <c r="A4" t="s">
+        <v>420</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>423</v>
+      </c>
+      <c r="C4" s="1"/>
+      <c r="D4" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" ht="38.25">
+      <c r="A5" t="s">
+        <v>421</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>424</v>
+      </c>
+      <c r="C5" s="1"/>
+      <c r="D5" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" ht="38.25">
+      <c r="A6" t="s">
+        <v>422</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>425</v>
+      </c>
+      <c r="C6" s="1"/>
+      <c r="D6" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" ht="38.25">
+      <c r="A7" t="s">
+        <v>426</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>429</v>
+      </c>
+      <c r="C7" s="1"/>
+      <c r="D7" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" ht="25.5">
+      <c r="A8" t="s">
+        <v>427</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>431</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" ht="51">
+      <c r="A9" t="s">
+        <v>428</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>432</v>
+      </c>
+      <c r="C9" s="1"/>
+      <c r="D9" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" ht="38.25">
+      <c r="A10" t="s">
+        <v>430</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>433</v>
+      </c>
+      <c r="C10" s="1"/>
+      <c r="D10" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10">
+      <c r="A12" t="s">
         <v>84</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B12" t="s">
         <v>296</v>
       </c>
-      <c r="D3" s="18" t="s">
+      <c r="D12" s="18" t="s">
         <v>129</v>
       </c>
-      <c r="F3">
+      <c r="F12">
         <v>50</v>
       </c>
-      <c r="G3">
+      <c r="G12">
         <v>20</v>
       </c>
     </row>
-    <row r="4" spans="1:10">
-      <c r="A4" t="s">
+    <row r="13" spans="1:10">
+      <c r="A13" t="s">
         <v>85</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B13" t="s">
         <v>110</v>
       </c>
-      <c r="D4" s="18" t="s">
+      <c r="D13" s="18" t="s">
         <v>70</v>
       </c>
-      <c r="F4">
+      <c r="F13">
         <v>100</v>
       </c>
-      <c r="G4">
+      <c r="G13">
         <v>45</v>
       </c>
     </row>
-    <row r="5" spans="1:10">
-      <c r="A5" t="s">
+    <row r="14" spans="1:10">
+      <c r="A14" t="s">
         <v>86</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B14" t="s">
         <v>111</v>
       </c>
-      <c r="D5" s="18" t="s">
+      <c r="D14" s="18" t="s">
         <v>70</v>
       </c>
-      <c r="F5">
+      <c r="F14">
         <v>30</v>
       </c>
-      <c r="G5">
+      <c r="G14">
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:10">
-      <c r="A6" t="s">
+    <row r="15" spans="1:10">
+      <c r="A15" t="s">
         <v>87</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B15" t="s">
         <v>118</v>
       </c>
-      <c r="D6" s="18" t="s">
+      <c r="D15" s="18" t="s">
         <v>255</v>
       </c>
-      <c r="F6">
+      <c r="F15">
         <v>20</v>
       </c>
-      <c r="G6">
+      <c r="G15">
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:10">
-      <c r="A7" t="s">
+    <row r="16" spans="1:10">
+      <c r="A16" t="s">
         <v>88</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B16" t="s">
         <v>120</v>
       </c>
-      <c r="D7" s="18" t="s">
+      <c r="D16" s="18" t="s">
         <v>255</v>
       </c>
-      <c r="F7">
+      <c r="F16">
         <v>50</v>
       </c>
-      <c r="G7">
+      <c r="G16">
         <v>20</v>
       </c>
     </row>

</xml_diff>

<commit_message>
user story 14 implemented
</commit_message>
<xml_diff>
--- a/Team05Report.xlsx
+++ b/Team05Report.xlsx
@@ -62,7 +62,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="833" uniqueCount="434">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="869" uniqueCount="444">
   <si>
     <t>Date</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -448,9 +448,6 @@
     <t>Invalid family members</t>
   </si>
   <si>
-    <t>An individual can have at most one spouse</t>
-  </si>
-  <si>
     <t>A family must contain a husband and a wife</t>
   </si>
   <si>
@@ -1421,6 +1418,39 @@
   </si>
   <si>
     <t>Check if the husband died more than 10 months before his child was born</t>
+  </si>
+  <si>
+    <t>An individual can have at most one spouse currently</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Individual I8(Kevin /Brown/) has more than one spouse currently: I9(Elena /Wilson/) in Family F4, I10(Jen /Brown/) in Family F6. </t>
+  </si>
+  <si>
+    <t>Individual I8(Kevin /Brown/) is the husband of Family F4 and Family F6 currently</t>
+  </si>
+  <si>
+    <t>Individual I10(Jen /Brown/) is the wife of Family F6 only</t>
+  </si>
+  <si>
+    <t>AT47~48</t>
+  </si>
+  <si>
+    <t>T14.01</t>
+  </si>
+  <si>
+    <t>T14.02</t>
+  </si>
+  <si>
+    <t>T14.03</t>
+  </si>
+  <si>
+    <t>Get the FAMS of each Individual</t>
+  </si>
+  <si>
+    <t>Store the other spouse of each family if they do not divorce currently</t>
+  </si>
+  <si>
+    <t>Check if the number of the stored spouses is greater than 1</t>
   </si>
 </sst>
 </file>
@@ -1707,25 +1737,25 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="104298368"/>
-        <c:axId val="104299904"/>
+        <c:axId val="64055168"/>
+        <c:axId val="64056704"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="104298368"/>
+        <c:axId val="64055168"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="m/d" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="104299904"/>
+        <c:crossAx val="64056704"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
         <c:baseTimeUnit val="days"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="104299904"/>
+        <c:axId val="64056704"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1733,7 +1763,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="104298368"/>
+        <c:crossAx val="64055168"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1743,7 +1773,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="1" l="0.750000000000002" r="0.750000000000002" t="1" header="0.5" footer="0.5"/>
+    <c:pageMargins b="1" l="0.75000000000000211" r="0.75000000000000211" t="1" header="0.5" footer="0.5"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -2155,36 +2185,36 @@
     </row>
     <row r="4" spans="1:5">
       <c r="A4" t="s">
+        <v>128</v>
+      </c>
+      <c r="B4" t="s">
         <v>129</v>
       </c>
-      <c r="B4" t="s">
+      <c r="C4" t="s">
         <v>130</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D4" s="14" t="s">
         <v>131</v>
       </c>
-      <c r="D4" s="14" t="s">
+      <c r="E4" t="s">
         <v>132</v>
-      </c>
-      <c r="E4" t="s">
-        <v>133</v>
       </c>
     </row>
     <row r="5" spans="1:5">
       <c r="A5" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="B5" t="s">
+        <v>133</v>
+      </c>
+      <c r="C5" t="s">
         <v>134</v>
       </c>
-      <c r="C5" t="s">
+      <c r="D5" s="14" t="s">
         <v>135</v>
       </c>
-      <c r="D5" s="14" t="s">
+      <c r="E5" t="s">
         <v>136</v>
-      </c>
-      <c r="E5" t="s">
-        <v>137</v>
       </c>
     </row>
     <row r="9" spans="1:5">
@@ -2273,7 +2303,7 @@
   <dimension ref="A1:L31"/>
   <sheetViews>
     <sheetView zoomScale="150" workbookViewId="0">
-      <selection activeCell="K13" sqref="K13"/>
+      <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75"/>
@@ -2341,10 +2371,10 @@
         <v>105</v>
       </c>
       <c r="D2" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="E2" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="F2" t="s">
         <v>35</v>
@@ -2376,16 +2406,16 @@
         <v>32</v>
       </c>
       <c r="C3" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D3" t="s">
+        <v>175</v>
+      </c>
+      <c r="E3" t="s">
+        <v>128</v>
+      </c>
+      <c r="F3" t="s">
         <v>176</v>
-      </c>
-      <c r="E3" t="s">
-        <v>129</v>
-      </c>
-      <c r="F3" t="s">
-        <v>177</v>
       </c>
       <c r="G3">
         <v>50</v>
@@ -2414,16 +2444,16 @@
         <v>34</v>
       </c>
       <c r="C4" t="s">
+        <v>186</v>
+      </c>
+      <c r="D4" s="18" t="s">
+        <v>259</v>
+      </c>
+      <c r="E4" t="s">
         <v>187</v>
       </c>
-      <c r="D4" s="18" t="s">
-        <v>260</v>
-      </c>
-      <c r="E4" t="s">
-        <v>188</v>
-      </c>
       <c r="F4" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="G4">
         <v>80</v>
@@ -2455,13 +2485,13 @@
         <v>112</v>
       </c>
       <c r="D5" s="18" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="E5" s="18" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="F5" s="18" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="G5">
         <v>80</v>
@@ -2493,13 +2523,13 @@
         <v>103</v>
       </c>
       <c r="D6" s="18" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="E6" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="F6" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="G6">
         <v>20</v>
@@ -2531,13 +2561,13 @@
         <v>106</v>
       </c>
       <c r="D7" s="18" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="E7" s="18" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="F7" s="18" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="G7">
         <v>50</v>
@@ -2569,13 +2599,13 @@
         <v>107</v>
       </c>
       <c r="D8" s="18" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="E8" s="18" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="F8" s="18" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="G8">
         <v>20</v>
@@ -2604,16 +2634,16 @@
         <v>78</v>
       </c>
       <c r="C9" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="D9" s="18" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="E9" s="18" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="F9" s="18" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="G9">
         <v>50</v>
@@ -2645,13 +2675,13 @@
         <v>108</v>
       </c>
       <c r="D10" s="18" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="E10" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="F10" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="G10">
         <v>50</v>
@@ -2683,13 +2713,13 @@
         <v>33</v>
       </c>
       <c r="D11" s="18" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="E11" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="F11" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="G11">
         <v>30</v>
@@ -2721,13 +2751,13 @@
         <v>99</v>
       </c>
       <c r="D12" s="18" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="E12" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="F12" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="G12">
         <v>30</v>
@@ -2759,13 +2789,13 @@
         <v>100</v>
       </c>
       <c r="D13" s="18" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="E13" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="F13" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="G13">
         <v>30</v>
@@ -2787,28 +2817,85 @@
       </c>
     </row>
     <row r="14" spans="1:12">
+      <c r="A14">
+        <v>3</v>
+      </c>
       <c r="B14" t="s">
         <v>83</v>
       </c>
       <c r="C14" t="s">
         <v>101</v>
       </c>
+      <c r="D14" t="s">
+        <v>418</v>
+      </c>
+      <c r="E14" s="18" t="s">
+        <v>128</v>
+      </c>
+      <c r="F14" s="18" t="s">
+        <v>176</v>
+      </c>
+      <c r="G14">
+        <v>70</v>
+      </c>
+      <c r="H14">
+        <v>30</v>
+      </c>
+      <c r="I14">
+        <v>115</v>
+      </c>
+      <c r="J14">
+        <v>40</v>
+      </c>
+      <c r="K14" s="16">
+        <v>40625</v>
+      </c>
       <c r="L14" s="7">
         <v>40598</v>
       </c>
     </row>
     <row r="15" spans="1:12">
+      <c r="A15">
+        <v>3</v>
+      </c>
       <c r="B15" t="s">
         <v>84</v>
       </c>
       <c r="C15" t="s">
-        <v>296</v>
+        <v>295</v>
+      </c>
+      <c r="D15" t="s">
+        <v>437</v>
+      </c>
+      <c r="E15" s="18" t="s">
+        <v>128</v>
+      </c>
+      <c r="F15" s="18" t="s">
+        <v>176</v>
+      </c>
+      <c r="G15">
+        <v>50</v>
+      </c>
+      <c r="H15">
+        <v>20</v>
+      </c>
+      <c r="I15">
+        <v>45</v>
+      </c>
+      <c r="J15">
+        <v>30</v>
+      </c>
+      <c r="K15" s="16">
+        <v>40625</v>
       </c>
       <c r="L15" s="7">
         <v>40598</v>
       </c>
     </row>
     <row r="16" spans="1:12">
+      <c r="A16">
+        <v>3</v>
+      </c>
       <c r="B16" t="s">
         <v>85</v>
       </c>
@@ -2819,7 +2906,10 @@
         <v>40598</v>
       </c>
     </row>
-    <row r="17" spans="2:12">
+    <row r="17" spans="1:12">
+      <c r="A17">
+        <v>3</v>
+      </c>
       <c r="B17" t="s">
         <v>86</v>
       </c>
@@ -2830,155 +2920,161 @@
         <v>40598</v>
       </c>
     </row>
-    <row r="18" spans="2:12">
+    <row r="18" spans="1:12">
+      <c r="A18">
+        <v>3</v>
+      </c>
       <c r="B18" t="s">
         <v>87</v>
       </c>
       <c r="C18" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="L18" s="7">
         <v>40598</v>
       </c>
     </row>
-    <row r="19" spans="2:12">
+    <row r="19" spans="1:12">
+      <c r="A19">
+        <v>3</v>
+      </c>
       <c r="B19" t="s">
         <v>88</v>
       </c>
       <c r="C19" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="L19" s="7">
         <v>40598</v>
       </c>
     </row>
-    <row r="20" spans="2:12">
+    <row r="20" spans="1:12">
       <c r="B20" t="s">
         <v>89</v>
       </c>
       <c r="C20" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="L20" s="7">
         <v>40598</v>
       </c>
     </row>
-    <row r="21" spans="2:12">
+    <row r="21" spans="1:12">
       <c r="B21" t="s">
         <v>90</v>
       </c>
       <c r="C21" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="L21" s="7">
         <v>40598</v>
       </c>
     </row>
-    <row r="22" spans="2:12">
+    <row r="22" spans="1:12">
       <c r="B22" t="s">
         <v>91</v>
       </c>
       <c r="C22" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="L22" s="7">
         <v>40598</v>
       </c>
     </row>
-    <row r="23" spans="2:12">
+    <row r="23" spans="1:12">
       <c r="B23" t="s">
         <v>92</v>
       </c>
       <c r="C23" s="18" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="L23" s="7">
         <v>40602</v>
       </c>
     </row>
-    <row r="24" spans="2:12">
+    <row r="24" spans="1:12">
       <c r="B24" t="s">
         <v>93</v>
       </c>
       <c r="C24" s="18" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="L24" s="7">
         <v>40602</v>
       </c>
     </row>
-    <row r="25" spans="2:12">
+    <row r="25" spans="1:12">
       <c r="B25" t="s">
         <v>94</v>
       </c>
       <c r="C25" s="18" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="L25" s="7">
         <v>40602</v>
       </c>
     </row>
-    <row r="26" spans="2:12">
+    <row r="26" spans="1:12">
       <c r="B26" t="s">
         <v>95</v>
       </c>
       <c r="C26" s="18" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="L26" s="7">
         <v>40610</v>
       </c>
     </row>
-    <row r="27" spans="2:12">
+    <row r="27" spans="1:12">
       <c r="B27" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="C27" s="18" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="L27" s="7">
         <v>40610</v>
       </c>
     </row>
-    <row r="28" spans="2:12">
+    <row r="28" spans="1:12">
       <c r="B28" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="C28" s="18" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="L28" s="7">
         <v>40610</v>
       </c>
     </row>
-    <row r="29" spans="2:12">
+    <row r="29" spans="1:12">
       <c r="B29" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="C29" s="18" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="L29" s="7">
         <v>40610</v>
       </c>
     </row>
-    <row r="30" spans="2:12">
+    <row r="30" spans="1:12">
       <c r="B30" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="C30" s="18" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="L30" s="7">
         <v>40610</v>
       </c>
     </row>
-    <row r="31" spans="2:12">
+    <row r="31" spans="1:12">
       <c r="B31" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="C31" s="18" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="L31" s="7">
         <v>40610</v>
@@ -3001,7 +3097,7 @@
   <dimension ref="A1:F31"/>
   <sheetViews>
     <sheetView topLeftCell="A4" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14:B14"/>
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75"/>
@@ -3044,7 +3140,7 @@
         <v>104</v>
       </c>
       <c r="D2" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="E2">
         <v>150</v>
@@ -3058,13 +3154,13 @@
         <v>32</v>
       </c>
       <c r="B3" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="D3" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="E3">
         <v>50</v>
@@ -3078,13 +3174,13 @@
         <v>34</v>
       </c>
       <c r="B4" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="D4" s="18" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="E4">
         <v>80</v>
@@ -3101,10 +3197,10 @@
         <v>112</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D5" s="18" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="E5">
         <v>20</v>
@@ -3124,7 +3220,7 @@
         <v>46</v>
       </c>
       <c r="D6" s="18" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="E6">
         <v>80</v>
@@ -3144,7 +3240,7 @@
         <v>97</v>
       </c>
       <c r="D7" s="18" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="E7">
         <v>50</v>
@@ -3164,7 +3260,7 @@
         <v>96</v>
       </c>
       <c r="D8" s="18" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="E8">
         <v>20</v>
@@ -3178,13 +3274,13 @@
         <v>78</v>
       </c>
       <c r="B9" t="s">
+        <v>114</v>
+      </c>
+      <c r="C9" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="C9" s="1" t="s">
-        <v>116</v>
-      </c>
       <c r="D9" s="18" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="E9">
         <v>50</v>
@@ -3204,7 +3300,7 @@
         <v>109</v>
       </c>
       <c r="D10" s="18" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="E10">
         <v>50</v>
@@ -3224,7 +3320,7 @@
         <v>47</v>
       </c>
       <c r="D11" s="18" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="E11">
         <v>30</v>
@@ -3244,7 +3340,7 @@
         <v>48</v>
       </c>
       <c r="D12" s="18" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="E12">
         <v>30</v>
@@ -3264,7 +3360,7 @@
         <v>98</v>
       </c>
       <c r="D13" s="18" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="E13">
         <v>30</v>
@@ -3281,7 +3377,10 @@
         <v>101</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>139</v>
+        <v>138</v>
+      </c>
+      <c r="D14" t="s">
+        <v>418</v>
       </c>
       <c r="E14">
         <v>70</v>
@@ -3295,10 +3394,13 @@
         <v>84</v>
       </c>
       <c r="B15" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>113</v>
+        <v>433</v>
+      </c>
+      <c r="D15" t="s">
+        <v>437</v>
       </c>
       <c r="E15">
         <v>50</v>
@@ -3315,7 +3417,7 @@
         <v>110</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="E16">
         <v>100</v>
@@ -3329,7 +3431,7 @@
         <v>86</v>
       </c>
       <c r="B17" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="C17" s="1" t="s">
         <v>102</v>
@@ -3346,10 +3448,10 @@
         <v>87</v>
       </c>
       <c r="B18" t="s">
+        <v>117</v>
+      </c>
+      <c r="C18" s="1" t="s">
         <v>118</v>
-      </c>
-      <c r="C18" s="1" t="s">
-        <v>119</v>
       </c>
       <c r="E18">
         <v>20</v>
@@ -3363,10 +3465,10 @@
         <v>88</v>
       </c>
       <c r="B19" t="s">
+        <v>119</v>
+      </c>
+      <c r="C19" s="1" t="s">
         <v>120</v>
-      </c>
-      <c r="C19" s="1" t="s">
-        <v>121</v>
       </c>
       <c r="E19">
         <v>50</v>
@@ -3380,10 +3482,10 @@
         <v>89</v>
       </c>
       <c r="B20" t="s">
+        <v>122</v>
+      </c>
+      <c r="C20" s="1" t="s">
         <v>123</v>
-      </c>
-      <c r="C20" s="1" t="s">
-        <v>124</v>
       </c>
     </row>
     <row r="21" spans="1:6">
@@ -3391,10 +3493,10 @@
         <v>90</v>
       </c>
       <c r="B21" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="22" spans="1:6">
@@ -3402,10 +3504,10 @@
         <v>91</v>
       </c>
       <c r="B22" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="23" spans="1:6" ht="25.5">
@@ -3413,10 +3515,10 @@
         <v>92</v>
       </c>
       <c r="B23" s="18" t="s">
+        <v>261</v>
+      </c>
+      <c r="C23" s="20" t="s">
         <v>262</v>
-      </c>
-      <c r="C23" s="20" t="s">
-        <v>263</v>
       </c>
     </row>
     <row r="24" spans="1:6" ht="25.5">
@@ -3424,10 +3526,10 @@
         <v>93</v>
       </c>
       <c r="B24" s="18" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
     </row>
     <row r="25" spans="1:6">
@@ -3435,10 +3537,10 @@
         <v>94</v>
       </c>
       <c r="B25" s="18" t="s">
+        <v>297</v>
+      </c>
+      <c r="C25" s="1" t="s">
         <v>298</v>
-      </c>
-      <c r="C25" s="1" t="s">
-        <v>299</v>
       </c>
     </row>
     <row r="26" spans="1:6">
@@ -3446,65 +3548,65 @@
         <v>95</v>
       </c>
       <c r="B26" s="18" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
     </row>
     <row r="27" spans="1:6" ht="25.5">
       <c r="A27" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="B27" s="18" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
     </row>
     <row r="28" spans="1:6">
       <c r="A28" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="B28" s="18" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
     </row>
     <row r="29" spans="1:6">
       <c r="A29" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="B29" s="18" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
     </row>
     <row r="30" spans="1:6">
       <c r="A30" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="B30" s="18" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
     </row>
     <row r="31" spans="1:6">
       <c r="A31" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="B31" s="18" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
     </row>
   </sheetData>
@@ -3522,8 +3624,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F77"/>
   <sheetViews>
-    <sheetView topLeftCell="A39" zoomScale="145" zoomScaleNormal="145" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="D51" sqref="D51"/>
+    <sheetView topLeftCell="A42" zoomScale="145" zoomScaleNormal="145" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="D52" sqref="D52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75"/>
@@ -3567,10 +3669,10 @@
         <v>105</v>
       </c>
       <c r="D2" s="13" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="E2" s="13" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="F2" t="s">
         <v>53</v>
@@ -3587,10 +3689,10 @@
         <v>105</v>
       </c>
       <c r="D3" s="13" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="E3" s="15" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="F3" t="s">
         <v>53</v>
@@ -3601,16 +3703,16 @@
         <v>56</v>
       </c>
       <c r="B4" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C4" t="s">
         <v>105</v>
       </c>
       <c r="D4" s="13" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="E4" s="13" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="F4" t="s">
         <v>53</v>
@@ -3621,16 +3723,16 @@
         <v>57</v>
       </c>
       <c r="B5" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C5" t="s">
         <v>105</v>
       </c>
       <c r="D5" s="13" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="E5" s="15" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="F5" t="s">
         <v>53</v>
@@ -3641,16 +3743,16 @@
         <v>58</v>
       </c>
       <c r="B6" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C6" t="s">
         <v>105</v>
       </c>
       <c r="D6" s="13" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="E6" s="13" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="F6" t="s">
         <v>53</v>
@@ -3661,13 +3763,13 @@
         <v>59</v>
       </c>
       <c r="B7" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C7" t="s">
         <v>105</v>
       </c>
       <c r="D7" s="13" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="E7" s="12" t="s">
         <v>51</v>
@@ -3678,16 +3780,16 @@
     </row>
     <row r="8" spans="1:6" ht="63">
       <c r="A8" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B8" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C8" t="s">
         <v>105</v>
       </c>
       <c r="D8" s="13" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="E8" s="12" t="s">
         <v>51</v>
@@ -3698,19 +3800,19 @@
     </row>
     <row r="9" spans="1:6" ht="63">
       <c r="A9" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B9" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C9" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D9" s="13" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="E9" s="15" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="F9" t="s">
         <v>53</v>
@@ -3718,19 +3820,19 @@
     </row>
     <row r="10" spans="1:6" ht="78.75">
       <c r="A10" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B10" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C10" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D10" s="13" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="E10" s="15" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="F10" t="s">
         <v>53</v>
@@ -3738,19 +3840,19 @@
     </row>
     <row r="11" spans="1:6" ht="63">
       <c r="A11" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B11" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C11" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D11" s="13" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="E11" s="15" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="F11" t="s">
         <v>53</v>
@@ -3758,19 +3860,19 @@
     </row>
     <row r="12" spans="1:6" ht="63">
       <c r="A12" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B12" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C12" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D12" s="13" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="E12" s="15" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="F12" t="s">
         <v>53</v>
@@ -3778,19 +3880,19 @@
     </row>
     <row r="13" spans="1:6" ht="78.75">
       <c r="A13" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B13" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C13" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D13" s="13" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="E13" s="15" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="F13" t="s">
         <v>53</v>
@@ -3798,16 +3900,16 @@
     </row>
     <row r="14" spans="1:6" ht="47.25">
       <c r="A14" t="s">
+        <v>170</v>
+      </c>
+      <c r="B14" t="s">
+        <v>151</v>
+      </c>
+      <c r="C14" t="s">
+        <v>116</v>
+      </c>
+      <c r="D14" s="13" t="s">
         <v>171</v>
-      </c>
-      <c r="B14" t="s">
-        <v>152</v>
-      </c>
-      <c r="C14" t="s">
-        <v>117</v>
-      </c>
-      <c r="D14" s="13" t="s">
-        <v>172</v>
       </c>
       <c r="E14" s="15" t="s">
         <v>51</v>
@@ -3818,16 +3920,16 @@
     </row>
     <row r="15" spans="1:6" ht="47.25">
       <c r="A15" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B15" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C15" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D15" s="13" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="E15" s="15" t="s">
         <v>51</v>
@@ -3838,19 +3940,19 @@
     </row>
     <row r="16" spans="1:6" ht="38.25">
       <c r="A16" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B16" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C16" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="F16" t="s">
         <v>53</v>
@@ -3858,19 +3960,19 @@
     </row>
     <row r="17" spans="1:6" ht="38.25">
       <c r="A17" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B17" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C17" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="D17" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="E17" s="1" t="s">
         <v>238</v>
-      </c>
-      <c r="E17" s="1" t="s">
-        <v>239</v>
       </c>
       <c r="F17" t="s">
         <v>53</v>
@@ -3878,19 +3980,19 @@
     </row>
     <row r="18" spans="1:6" ht="38.25">
       <c r="A18" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B18" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C18" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="F18" t="s">
         <v>53</v>
@@ -3898,19 +4000,19 @@
     </row>
     <row r="19" spans="1:6" ht="38.25">
       <c r="A19" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="B19" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C19" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="F19" t="s">
         <v>53</v>
@@ -3918,16 +4020,16 @@
     </row>
     <row r="20" spans="1:6" ht="26.25">
       <c r="A20" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="B20" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C20" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="E20" s="12" t="s">
         <v>51</v>
@@ -3938,19 +4040,19 @@
     </row>
     <row r="21" spans="1:6" ht="47.25">
       <c r="A21" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B21" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C21" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="D21" s="1" t="s">
+        <v>255</v>
+      </c>
+      <c r="E21" s="17" t="s">
         <v>256</v>
-      </c>
-      <c r="E21" s="17" t="s">
-        <v>257</v>
       </c>
       <c r="F21" s="18" t="s">
         <v>53</v>
@@ -3958,19 +4060,19 @@
     </row>
     <row r="22" spans="1:6" ht="47.25">
       <c r="A22" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="B22" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C22" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="D22" s="20" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="E22" s="19" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="F22" s="18" t="s">
         <v>53</v>
@@ -3978,7 +4080,7 @@
     </row>
     <row r="23" spans="1:6" ht="37.5" customHeight="1">
       <c r="A23" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="B23" t="s">
         <v>75</v>
@@ -3987,10 +4089,10 @@
         <v>103</v>
       </c>
       <c r="D23" s="1" t="s">
+        <v>244</v>
+      </c>
+      <c r="E23" s="1" t="s">
         <v>245</v>
-      </c>
-      <c r="E23" s="1" t="s">
-        <v>246</v>
       </c>
       <c r="F23" t="s">
         <v>53</v>
@@ -3998,7 +4100,7 @@
     </row>
     <row r="24" spans="1:6" ht="26.25">
       <c r="A24" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="B24" t="s">
         <v>75</v>
@@ -4007,7 +4109,7 @@
         <v>103</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="E24" s="12" t="s">
         <v>51</v>
@@ -4018,7 +4120,7 @@
     </row>
     <row r="25" spans="1:6" ht="25.5">
       <c r="A25" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="B25" t="s">
         <v>74</v>
@@ -4027,10 +4129,10 @@
         <v>112</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="F25" t="s">
         <v>53</v>
@@ -4038,7 +4140,7 @@
     </row>
     <row r="26" spans="1:6">
       <c r="A26" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="B26" t="s">
         <v>74</v>
@@ -4047,10 +4149,10 @@
         <v>112</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="F26" t="s">
         <v>53</v>
@@ -4058,7 +4160,7 @@
     </row>
     <row r="27" spans="1:6" ht="25.5">
       <c r="A27" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="B27" t="s">
         <v>74</v>
@@ -4067,10 +4169,10 @@
         <v>112</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="F27" t="s">
         <v>53</v>
@@ -4078,7 +4180,7 @@
     </row>
     <row r="28" spans="1:6" ht="25.5">
       <c r="A28" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B28" t="s">
         <v>76</v>
@@ -4087,10 +4189,10 @@
         <v>106</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="F28" t="s">
         <v>53</v>
@@ -4098,7 +4200,7 @@
     </row>
     <row r="29" spans="1:6" ht="25.5">
       <c r="A29" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B29" t="s">
         <v>76</v>
@@ -4107,10 +4209,10 @@
         <v>106</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="F29" t="s">
         <v>53</v>
@@ -4118,7 +4220,7 @@
     </row>
     <row r="30" spans="1:6" ht="38.25">
       <c r="A30" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B30" t="s">
         <v>77</v>
@@ -4127,10 +4229,10 @@
         <v>107</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="F30" t="s">
         <v>53</v>
@@ -4138,7 +4240,7 @@
     </row>
     <row r="31" spans="1:6" ht="51">
       <c r="A31" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B31" t="s">
         <v>77</v>
@@ -4147,10 +4249,10 @@
         <v>107</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="F31" t="s">
         <v>53</v>
@@ -4158,7 +4260,7 @@
     </row>
     <row r="32" spans="1:6" ht="26.25">
       <c r="A32" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B32" t="s">
         <v>77</v>
@@ -4167,7 +4269,7 @@
         <v>107</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="E32" s="12" t="s">
         <v>51</v>
@@ -4178,19 +4280,19 @@
     </row>
     <row r="33" spans="1:6" ht="25.5">
       <c r="A33" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B33" t="s">
         <v>78</v>
       </c>
       <c r="C33" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="F33" t="s">
         <v>53</v>
@@ -4198,16 +4300,16 @@
     </row>
     <row r="34" spans="1:6" ht="26.25">
       <c r="A34" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B34" t="s">
         <v>78</v>
       </c>
       <c r="C34" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="E34" s="12" t="s">
         <v>51</v>
@@ -4218,7 +4320,7 @@
     </row>
     <row r="35" spans="1:6" ht="25.5">
       <c r="A35" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B35" t="s">
         <v>79</v>
@@ -4227,7 +4329,7 @@
         <v>108</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="E35" s="1" t="s">
         <v>51</v>
@@ -4238,7 +4340,7 @@
     </row>
     <row r="36" spans="1:6" ht="38.25">
       <c r="A36" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B36" t="s">
         <v>79</v>
@@ -4247,10 +4349,10 @@
         <v>108</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="E36" s="1" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="F36" t="s">
         <v>53</v>
@@ -4258,7 +4360,7 @@
     </row>
     <row r="37" spans="1:6" ht="38.25">
       <c r="A37" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B37" t="s">
         <v>79</v>
@@ -4267,10 +4369,10 @@
         <v>108</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="E37" s="1" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="F37" t="s">
         <v>53</v>
@@ -4278,7 +4380,7 @@
     </row>
     <row r="38" spans="1:6" ht="38.25">
       <c r="A38" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B38" t="s">
         <v>80</v>
@@ -4287,10 +4389,10 @@
         <v>33</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="E38" s="1" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="F38" t="s">
         <v>53</v>
@@ -4298,7 +4400,7 @@
     </row>
     <row r="39" spans="1:6" ht="25.5">
       <c r="A39" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B39" t="s">
         <v>80</v>
@@ -4307,7 +4409,7 @@
         <v>33</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="E39" s="1" t="s">
         <v>51</v>
@@ -4318,7 +4420,7 @@
     </row>
     <row r="40" spans="1:6" ht="38.25">
       <c r="A40" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B40" t="s">
         <v>81</v>
@@ -4327,18 +4429,18 @@
         <v>99</v>
       </c>
       <c r="D40" s="1" t="s">
+        <v>398</v>
+      </c>
+      <c r="E40" s="1" t="s">
         <v>399</v>
       </c>
-      <c r="E40" s="1" t="s">
-        <v>400</v>
-      </c>
       <c r="F40" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
     </row>
     <row r="41" spans="1:6" ht="25.5">
       <c r="A41" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B41" t="s">
         <v>81</v>
@@ -4347,10 +4449,10 @@
         <v>99</v>
       </c>
       <c r="D41" s="1" t="s">
+        <v>400</v>
+      </c>
+      <c r="E41" s="1" t="s">
         <v>401</v>
-      </c>
-      <c r="E41" s="1" t="s">
-        <v>402</v>
       </c>
       <c r="F41" t="s">
         <v>53</v>
@@ -4358,7 +4460,7 @@
     </row>
     <row r="42" spans="1:6" ht="38.25">
       <c r="A42" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="B42" t="s">
         <v>81</v>
@@ -4367,7 +4469,7 @@
         <v>99</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="E42" s="1" t="s">
         <v>51</v>
@@ -4378,7 +4480,7 @@
     </row>
     <row r="43" spans="1:6" ht="25.5">
       <c r="A43" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="B43" t="s">
         <v>82</v>
@@ -4387,10 +4489,10 @@
         <v>100</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="E43" s="1" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="F43" t="s">
         <v>53</v>
@@ -4398,7 +4500,7 @@
     </row>
     <row r="44" spans="1:6" ht="25.5">
       <c r="A44" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="B44" t="s">
         <v>82</v>
@@ -4407,7 +4509,7 @@
         <v>100</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="E44" s="1" t="s">
         <v>51</v>
@@ -4418,7 +4520,7 @@
     </row>
     <row r="45" spans="1:6" ht="51">
       <c r="A45" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B45" s="18" t="s">
         <v>83</v>
@@ -4427,10 +4529,10 @@
         <v>101</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="E45" s="1" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="F45" t="s">
         <v>53</v>
@@ -4438,7 +4540,7 @@
     </row>
     <row r="46" spans="1:6" ht="51">
       <c r="A46" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="B46" s="18" t="s">
         <v>83</v>
@@ -4447,10 +4549,10 @@
         <v>101</v>
       </c>
       <c r="D46" s="1" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="E46" s="1" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="F46" t="s">
         <v>53</v>
@@ -4458,7 +4560,7 @@
     </row>
     <row r="47" spans="1:6" ht="51">
       <c r="A47" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="B47" s="18" t="s">
         <v>83</v>
@@ -4467,7 +4569,7 @@
         <v>101</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="E47" s="1" t="s">
         <v>51</v>
@@ -4476,154 +4578,184 @@
         <v>53</v>
       </c>
     </row>
-    <row r="48" spans="1:6">
+    <row r="48" spans="1:6" ht="51">
       <c r="A48" t="s">
+        <v>220</v>
+      </c>
+      <c r="B48" s="18" t="s">
+        <v>84</v>
+      </c>
+      <c r="C48" t="s">
+        <v>295</v>
+      </c>
+      <c r="D48" s="1" t="s">
+        <v>435</v>
+      </c>
+      <c r="E48" s="1" t="s">
+        <v>434</v>
+      </c>
+      <c r="F48" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" ht="25.5">
+      <c r="A49" t="s">
         <v>221</v>
       </c>
-    </row>
-    <row r="49" spans="1:1">
-      <c r="A49" t="s">
+      <c r="B49" s="18" t="s">
+        <v>84</v>
+      </c>
+      <c r="C49" t="s">
+        <v>295</v>
+      </c>
+      <c r="D49" s="1" t="s">
+        <v>436</v>
+      </c>
+      <c r="E49" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="F49" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6">
+      <c r="A50" t="s">
         <v>222</v>
       </c>
     </row>
-    <row r="50" spans="1:1">
-      <c r="A50" t="s">
+    <row r="51" spans="1:6">
+      <c r="A51" t="s">
         <v>223</v>
       </c>
     </row>
-    <row r="51" spans="1:1">
-      <c r="A51" t="s">
+    <row r="52" spans="1:6">
+      <c r="A52" t="s">
         <v>224</v>
       </c>
     </row>
-    <row r="52" spans="1:1">
-      <c r="A52" t="s">
+    <row r="53" spans="1:6">
+      <c r="A53" t="s">
         <v>225</v>
       </c>
     </row>
-    <row r="53" spans="1:1">
-      <c r="A53" t="s">
+    <row r="54" spans="1:6">
+      <c r="A54" t="s">
         <v>226</v>
       </c>
     </row>
-    <row r="54" spans="1:1">
-      <c r="A54" t="s">
+    <row r="55" spans="1:6">
+      <c r="A55" t="s">
         <v>227</v>
       </c>
     </row>
-    <row r="55" spans="1:1">
-      <c r="A55" t="s">
+    <row r="56" spans="1:6">
+      <c r="A56" t="s">
         <v>228</v>
       </c>
     </row>
-    <row r="56" spans="1:1">
-      <c r="A56" t="s">
+    <row r="57" spans="1:6">
+      <c r="A57" t="s">
         <v>229</v>
       </c>
     </row>
-    <row r="57" spans="1:1">
-      <c r="A57" t="s">
+    <row r="58" spans="1:6">
+      <c r="A58" t="s">
         <v>230</v>
       </c>
     </row>
-    <row r="58" spans="1:1">
-      <c r="A58" t="s">
+    <row r="59" spans="1:6">
+      <c r="A59" t="s">
         <v>231</v>
       </c>
     </row>
-    <row r="59" spans="1:1">
-      <c r="A59" t="s">
+    <row r="60" spans="1:6">
+      <c r="A60" t="s">
         <v>232</v>
       </c>
     </row>
-    <row r="60" spans="1:1">
-      <c r="A60" t="s">
+    <row r="61" spans="1:6">
+      <c r="A61" t="s">
         <v>233</v>
       </c>
     </row>
-    <row r="61" spans="1:1">
-      <c r="A61" t="s">
+    <row r="62" spans="1:6">
+      <c r="A62" t="s">
         <v>234</v>
       </c>
     </row>
-    <row r="62" spans="1:1">
-      <c r="A62" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="63" spans="1:1">
+    <row r="63" spans="1:6">
       <c r="A63" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6">
+      <c r="A64" t="s">
         <v>371</v>
-      </c>
-    </row>
-    <row r="64" spans="1:1">
-      <c r="A64" t="s">
-        <v>372</v>
       </c>
     </row>
     <row r="65" spans="1:1">
       <c r="A65" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
     </row>
     <row r="66" spans="1:1">
       <c r="A66" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
     </row>
     <row r="67" spans="1:1">
       <c r="A67" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
     </row>
     <row r="68" spans="1:1">
       <c r="A68" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
     </row>
     <row r="69" spans="1:1">
       <c r="A69" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
     </row>
     <row r="70" spans="1:1">
       <c r="A70" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
     </row>
     <row r="71" spans="1:1">
       <c r="A71" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
     </row>
     <row r="72" spans="1:1">
       <c r="A72" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
     </row>
     <row r="73" spans="1:1">
       <c r="A73" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
     </row>
     <row r="74" spans="1:1">
       <c r="A74" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
     </row>
     <row r="75" spans="1:1">
       <c r="A75" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
     </row>
     <row r="76" spans="1:1">
       <c r="A76" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
     </row>
     <row r="77" spans="1:1">
       <c r="A77" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
     </row>
   </sheetData>
@@ -4673,7 +4805,7 @@
         <v>27</v>
       </c>
       <c r="F1" s="8" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="2" spans="1:6">
@@ -4746,7 +4878,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:J42"/>
   <sheetViews>
-    <sheetView topLeftCell="A28" zoomScale="150" workbookViewId="0">
+    <sheetView topLeftCell="A22" zoomScale="150" workbookViewId="0">
       <selection activeCell="B34" sqref="B34:B42"/>
     </sheetView>
   </sheetViews>
@@ -4804,10 +4936,10 @@
         <v>105</v>
       </c>
       <c r="C2" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="D2" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="E2" t="s">
         <v>35</v>
@@ -4830,13 +4962,13 @@
     </row>
     <row r="4" spans="1:10" ht="25.5">
       <c r="A4" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="D4" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="5" spans="1:10" ht="25.5">
@@ -4844,10 +4976,10 @@
         <v>41</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="D5" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="6" spans="1:10" ht="25.5">
@@ -4855,21 +4987,21 @@
         <v>42</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="D6" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="7" spans="1:10" ht="25.5">
       <c r="A7" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="D7" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="9" spans="1:10">
@@ -4877,16 +5009,16 @@
         <v>32</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C9" t="s">
+        <v>175</v>
+      </c>
+      <c r="D9" t="s">
+        <v>128</v>
+      </c>
+      <c r="E9" t="s">
         <v>176</v>
-      </c>
-      <c r="D9" t="s">
-        <v>129</v>
-      </c>
-      <c r="E9" t="s">
-        <v>177</v>
       </c>
       <c r="F9">
         <v>50</v>
@@ -4909,10 +5041,10 @@
         <v>43</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="D11" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="12" spans="1:10" ht="38.25">
@@ -4920,27 +5052,27 @@
         <v>44</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="D12" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="14" spans="1:10">
       <c r="A14" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B14" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C14" s="18" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="D14" t="s">
         <v>70</v>
       </c>
       <c r="E14" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="F14">
         <v>80</v>
@@ -4960,10 +5092,10 @@
     </row>
     <row r="15" spans="1:10">
       <c r="A15" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="D15" t="s">
         <v>70</v>
@@ -4972,10 +5104,10 @@
     </row>
     <row r="16" spans="1:10">
       <c r="A16" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="D16" t="s">
         <v>70</v>
@@ -4983,10 +5115,10 @@
     </row>
     <row r="17" spans="1:10">
       <c r="A17" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="D17" t="s">
         <v>70</v>
@@ -4994,10 +5126,10 @@
     </row>
     <row r="18" spans="1:10" ht="25.5">
       <c r="A18" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="D18" t="s">
         <v>70</v>
@@ -5015,13 +5147,13 @@
         <v>103</v>
       </c>
       <c r="C20" s="20" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="D20" t="s">
         <v>70</v>
       </c>
       <c r="E20" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="F20">
         <v>20</v>
@@ -5041,10 +5173,10 @@
     </row>
     <row r="21" spans="1:10">
       <c r="A21" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="D21" t="s">
         <v>70</v>
@@ -5053,10 +5185,10 @@
     </row>
     <row r="22" spans="1:10">
       <c r="A22" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="D22" t="s">
         <v>70</v>
@@ -5064,10 +5196,10 @@
     </row>
     <row r="23" spans="1:10">
       <c r="A23" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="J23" s="7"/>
     </row>
@@ -5082,13 +5214,13 @@
         <v>112</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="D25" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="E25" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="F25">
         <v>80</v>
@@ -5108,37 +5240,37 @@
     </row>
     <row r="26" spans="1:10" ht="25.5">
       <c r="A26" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="D26" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="J26" s="7"/>
     </row>
     <row r="27" spans="1:10" ht="25.5">
       <c r="A27" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="D27" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="J27" s="7"/>
     </row>
     <row r="28" spans="1:10" ht="25.5">
       <c r="A28" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="D28" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="J28" s="7"/>
     </row>
@@ -5153,13 +5285,13 @@
         <v>106</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="D30" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="E30" s="18" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="F30">
         <v>50</v>
@@ -5179,25 +5311,25 @@
     </row>
     <row r="31" spans="1:10" ht="25.5">
       <c r="A31" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="D31" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="J31" s="7"/>
     </row>
     <row r="32" spans="1:10" ht="25.5">
       <c r="A32" t="s">
+        <v>291</v>
+      </c>
+      <c r="B32" s="1" t="s">
         <v>292</v>
       </c>
-      <c r="B32" s="1" t="s">
-        <v>293</v>
-      </c>
       <c r="D32" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="J32" s="7"/>
     </row>
@@ -5219,23 +5351,23 @@
     </row>
     <row r="37" spans="2:10">
       <c r="B37" s="1" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
     </row>
     <row r="38" spans="2:10" ht="25.5">
       <c r="B38" s="1" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
     </row>
     <row r="39" spans="2:10" ht="38.25">
       <c r="B39" s="1" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="J39" s="7"/>
     </row>
     <row r="40" spans="2:10" ht="25.5">
       <c r="B40" s="1" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
     </row>
     <row r="41" spans="2:10">
@@ -5264,8 +5396,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:J45"/>
   <sheetViews>
-    <sheetView zoomScale="150" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:D6"/>
+    <sheetView topLeftCell="A34" zoomScale="150" workbookViewId="0">
+      <selection activeCell="B37" sqref="B37:B45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75"/>
@@ -5314,13 +5446,13 @@
         <v>107</v>
       </c>
       <c r="C2" s="18" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="D2" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="E2" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="F2">
         <v>20</v>
@@ -5340,38 +5472,38 @@
     </row>
     <row r="4" spans="1:10" ht="25.5">
       <c r="A4" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="C4" s="1"/>
       <c r="D4" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="5" spans="1:10" ht="25.5">
       <c r="A5" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="C5" s="1"/>
       <c r="D5" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="6" spans="1:10" ht="25.5">
       <c r="A6" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="C6" s="1"/>
       <c r="D6" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="7" spans="1:10">
@@ -5383,16 +5515,16 @@
         <v>78</v>
       </c>
       <c r="B8" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C8" s="18" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="D8" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="E8" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="F8">
         <v>50</v>
@@ -5412,38 +5544,38 @@
     </row>
     <row r="10" spans="1:10" ht="25.5">
       <c r="A10" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="C10" s="1"/>
       <c r="D10" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="11" spans="1:10">
       <c r="A11" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="C11" s="1"/>
       <c r="D11" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="12" spans="1:10" ht="38.25">
       <c r="A12" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="C12" s="1"/>
       <c r="D12" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="14" spans="1:10">
@@ -5454,13 +5586,13 @@
         <v>108</v>
       </c>
       <c r="C14" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="D14" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="E14" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="F14">
         <v>50</v>
@@ -5480,46 +5612,46 @@
     </row>
     <row r="15" spans="1:10" ht="25.5">
       <c r="A15" t="s">
+        <v>322</v>
+      </c>
+      <c r="B15" s="1" t="s">
         <v>323</v>
       </c>
-      <c r="B15" s="1" t="s">
-        <v>324</v>
-      </c>
       <c r="D15" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="16" spans="1:10" ht="25.5">
       <c r="A16" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="D16" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="17" spans="1:10">
       <c r="A17" t="s">
+        <v>325</v>
+      </c>
+      <c r="B17" s="1" t="s">
         <v>326</v>
       </c>
-      <c r="B17" s="1" t="s">
-        <v>327</v>
-      </c>
       <c r="D17" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="18" spans="1:10" ht="38.25">
       <c r="A18" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="D18" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="J18" s="16"/>
     </row>
@@ -5534,13 +5666,13 @@
         <v>33</v>
       </c>
       <c r="C20" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="D20" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="E20" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="F20">
         <v>30</v>
@@ -5560,57 +5692,57 @@
     </row>
     <row r="21" spans="1:10" ht="25.5">
       <c r="A21" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="D21" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="22" spans="1:10" ht="38.25">
       <c r="A22" t="s">
+        <v>332</v>
+      </c>
+      <c r="B22" s="1" t="s">
         <v>333</v>
       </c>
-      <c r="B22" s="1" t="s">
-        <v>334</v>
-      </c>
       <c r="D22" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="23" spans="1:10" ht="25.5">
       <c r="A23" t="s">
+        <v>334</v>
+      </c>
+      <c r="B23" s="1" t="s">
         <v>335</v>
       </c>
-      <c r="B23" s="1" t="s">
-        <v>336</v>
-      </c>
       <c r="D23" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="24" spans="1:10" ht="25.5">
       <c r="A24" t="s">
+        <v>336</v>
+      </c>
+      <c r="B24" s="1" t="s">
         <v>337</v>
       </c>
-      <c r="B24" s="1" t="s">
-        <v>338</v>
-      </c>
       <c r="D24" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="25" spans="1:10" ht="25.5">
       <c r="A25" t="s">
+        <v>338</v>
+      </c>
+      <c r="B25" s="1" t="s">
         <v>339</v>
       </c>
-      <c r="B25" s="1" t="s">
-        <v>340</v>
-      </c>
       <c r="D25" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="27" spans="1:10">
@@ -5621,13 +5753,13 @@
         <v>99</v>
       </c>
       <c r="C27" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="D27" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="E27" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="F27">
         <v>30</v>
@@ -5647,37 +5779,37 @@
     </row>
     <row r="28" spans="1:10" ht="25.5">
       <c r="A28" t="s">
+        <v>385</v>
+      </c>
+      <c r="B28" s="1" t="s">
         <v>386</v>
-      </c>
-      <c r="B28" s="1" t="s">
-        <v>387</v>
       </c>
       <c r="J28" s="16"/>
     </row>
     <row r="29" spans="1:10" ht="38.25">
       <c r="A29" t="s">
+        <v>387</v>
+      </c>
+      <c r="B29" s="1" t="s">
         <v>388</v>
-      </c>
-      <c r="B29" s="1" t="s">
-        <v>389</v>
       </c>
       <c r="J29" s="16"/>
     </row>
     <row r="30" spans="1:10" ht="25.5">
       <c r="A30" t="s">
+        <v>389</v>
+      </c>
+      <c r="B30" s="1" t="s">
         <v>390</v>
-      </c>
-      <c r="B30" s="1" t="s">
-        <v>391</v>
       </c>
       <c r="J30" s="16"/>
     </row>
     <row r="31" spans="1:10" ht="25.5">
       <c r="A31" t="s">
+        <v>391</v>
+      </c>
+      <c r="B31" s="1" t="s">
         <v>392</v>
-      </c>
-      <c r="B31" s="1" t="s">
-        <v>393</v>
       </c>
       <c r="J31" s="16"/>
     </row>
@@ -5689,13 +5821,13 @@
         <v>100</v>
       </c>
       <c r="C32" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="D32" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="E32" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="F32">
         <v>30</v>
@@ -5715,26 +5847,26 @@
     </row>
     <row r="33" spans="1:2" ht="25.5">
       <c r="A33" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
     </row>
     <row r="34" spans="1:2" ht="51">
       <c r="A34" t="s">
+        <v>394</v>
+      </c>
+      <c r="B34" s="1" t="s">
         <v>395</v>
-      </c>
-      <c r="B34" s="1" t="s">
-        <v>396</v>
       </c>
     </row>
     <row r="35" spans="1:2" ht="25.5">
       <c r="A35" t="s">
+        <v>396</v>
+      </c>
+      <c r="B35" s="1" t="s">
         <v>397</v>
-      </c>
-      <c r="B35" s="1" t="s">
-        <v>398</v>
       </c>
     </row>
     <row r="37" spans="1:2">
@@ -5752,17 +5884,17 @@
     </row>
     <row r="40" spans="1:2">
       <c r="B40" s="1" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
     </row>
     <row r="41" spans="1:2" ht="25.5">
       <c r="B41" s="1" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
     </row>
     <row r="42" spans="1:2" ht="51">
       <c r="B42" s="1" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
     </row>
     <row r="43" spans="1:2">
@@ -5792,10 +5924,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J16"/>
+  <dimension ref="A1:J31"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="150" workbookViewId="0">
+      <selection activeCell="D31" sqref="D31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75"/>
@@ -5843,13 +5975,13 @@
         <v>101</v>
       </c>
       <c r="C2" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="D2" s="18" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="E2" s="18" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="F2">
         <v>70</v>
@@ -5869,82 +6001,82 @@
     </row>
     <row r="4" spans="1:10" ht="25.5">
       <c r="A4" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="C4" s="1"/>
       <c r="D4" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="5" spans="1:10" ht="38.25">
       <c r="A5" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="C5" s="1"/>
       <c r="D5" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="6" spans="1:10" ht="38.25">
       <c r="A6" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="C6" s="1"/>
       <c r="D6" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="7" spans="1:10" ht="38.25">
       <c r="A7" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="C7" s="1"/>
       <c r="D7" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="8" spans="1:10" ht="25.5">
       <c r="A8" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
     </row>
     <row r="9" spans="1:10" ht="51">
       <c r="A9" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="C9" s="1"/>
       <c r="D9" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="10" spans="1:10" ht="38.25">
       <c r="A10" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="C10" s="1"/>
       <c r="D10" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="12" spans="1:10">
@@ -5952,10 +6084,16 @@
         <v>84</v>
       </c>
       <c r="B12" t="s">
-        <v>296</v>
+        <v>295</v>
+      </c>
+      <c r="C12" t="s">
+        <v>437</v>
       </c>
       <c r="D12" s="18" t="s">
-        <v>129</v>
+        <v>128</v>
+      </c>
+      <c r="E12" s="18" t="s">
+        <v>330</v>
       </c>
       <c r="F12">
         <v>50</v>
@@ -5963,73 +6101,163 @@
       <c r="G12">
         <v>20</v>
       </c>
-    </row>
-    <row r="13" spans="1:10">
-      <c r="A13" t="s">
+      <c r="H12">
+        <v>45</v>
+      </c>
+      <c r="I12">
+        <v>30</v>
+      </c>
+      <c r="J12" s="16">
+        <v>40625</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" ht="25.5">
+      <c r="A14" t="s">
+        <v>438</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>441</v>
+      </c>
+      <c r="C14" s="1"/>
+      <c r="D14" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" ht="38.25">
+      <c r="A15" t="s">
+        <v>439</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>442</v>
+      </c>
+      <c r="C15" s="1"/>
+      <c r="D15" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" ht="38.25">
+      <c r="A16" t="s">
+        <v>440</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>443</v>
+      </c>
+      <c r="C16" s="1"/>
+      <c r="D16" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7">
+      <c r="B17" s="1"/>
+      <c r="C17" s="1"/>
+    </row>
+    <row r="18" spans="1:7">
+      <c r="A18" t="s">
         <v>85</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B18" t="s">
         <v>110</v>
       </c>
-      <c r="D13" s="18" t="s">
+      <c r="D18" s="18" t="s">
         <v>70</v>
       </c>
-      <c r="F13">
+      <c r="F18">
         <v>100</v>
       </c>
-      <c r="G13">
+      <c r="G18">
         <v>45</v>
       </c>
     </row>
-    <row r="14" spans="1:10">
-      <c r="A14" t="s">
+    <row r="19" spans="1:7">
+      <c r="A19" t="s">
         <v>86</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B19" t="s">
         <v>111</v>
       </c>
-      <c r="D14" s="18" t="s">
+      <c r="D19" s="18" t="s">
         <v>70</v>
       </c>
-      <c r="F14">
+      <c r="F19">
         <v>30</v>
       </c>
-      <c r="G14">
+      <c r="G19">
         <v>10</v>
       </c>
     </row>
-    <row r="15" spans="1:10">
-      <c r="A15" t="s">
+    <row r="20" spans="1:7">
+      <c r="A20" t="s">
         <v>87</v>
       </c>
-      <c r="B15" t="s">
-        <v>118</v>
-      </c>
-      <c r="D15" s="18" t="s">
-        <v>255</v>
-      </c>
-      <c r="F15">
+      <c r="B20" t="s">
+        <v>117</v>
+      </c>
+      <c r="D20" s="18" t="s">
+        <v>254</v>
+      </c>
+      <c r="F20">
         <v>20</v>
       </c>
-      <c r="G15">
+      <c r="G20">
         <v>10</v>
       </c>
     </row>
-    <row r="16" spans="1:10">
-      <c r="A16" t="s">
+    <row r="21" spans="1:7">
+      <c r="A21" t="s">
         <v>88</v>
       </c>
-      <c r="B16" t="s">
-        <v>120</v>
-      </c>
-      <c r="D16" s="18" t="s">
-        <v>255</v>
-      </c>
-      <c r="F16">
+      <c r="B21" t="s">
+        <v>119</v>
+      </c>
+      <c r="D21" s="18" t="s">
+        <v>254</v>
+      </c>
+      <c r="F21">
         <v>50</v>
       </c>
-      <c r="G16">
+      <c r="G21">
         <v>20</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7">
+      <c r="B23" s="5" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7">
+      <c r="B24" s="5"/>
+    </row>
+    <row r="25" spans="1:7">
+      <c r="B25" s="5" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7">
+      <c r="B26" s="1" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" ht="25.5">
+      <c r="B27" s="1" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" ht="51">
+      <c r="B28" s="1" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7">
+      <c r="B29" s="1"/>
+    </row>
+    <row r="30" spans="1:7">
+      <c r="B30" s="5" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" ht="25.5">
+      <c r="B31" s="1" t="s">
+        <v>63</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Revert "Revert "Report Completed""
This reverts commit 9c67546d0c85e152dd0008f5654ec898a90d1f3a.

Conflicts:
	SSW555.sdf
	SSW555.v12.suo
</commit_message>
<xml_diff>
--- a/Team05Report.xlsx
+++ b/Team05Report.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="240" windowWidth="20730" windowHeight="11760" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="240" windowWidth="20730" windowHeight="11760" tabRatio="500" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="Team" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
     <sheet name="Sprint4" sheetId="6" r:id="rId9"/>
     <sheet name="Sprint5" sheetId="8" r:id="rId10"/>
   </sheets>
-  <calcPr calcId="145621" concurrentCalc="0"/>
+  <calcPr calcId="124519" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -62,7 +62,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="963" uniqueCount="477">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1005" uniqueCount="493">
   <si>
     <t>Date</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -1550,17 +1550,66 @@
   </si>
   <si>
     <t>It is not allowed if the husband gets married under 20 nor wife gets married under 18</t>
+  </si>
+  <si>
+    <t>Family F2 has more than 8 members (9).</t>
+  </si>
+  <si>
+    <t xml:space="preserve">In Family F2, child I5(Emily /Mao/) and child I1(Jacky /Mao/) are not twins but born within one year.
+</t>
+  </si>
+  <si>
+    <t>T17.01</t>
+  </si>
+  <si>
+    <t>Get each family record</t>
+  </si>
+  <si>
+    <t>T17.02</t>
+  </si>
+  <si>
+    <t>In family record get the count of husband , wife and child</t>
+  </si>
+  <si>
+    <t>T18.01</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Compare their birth date </t>
+  </si>
+  <si>
+    <t>T18.02</t>
+  </si>
+  <si>
+    <t>T18.03</t>
+  </si>
+  <si>
+    <t>Individual I5 was born on 11 SEP 1970 and Individual I1 born on 27 JAN 1970</t>
+  </si>
+  <si>
+    <t>Individual I2 and I3 have 7 children</t>
+  </si>
+  <si>
+    <t>Individual I8 and I9 have two children</t>
+  </si>
+  <si>
+    <t>Individual I3 was born on 14 FEB 1965 and Individual I4 born on 1 OCT 1960</t>
+  </si>
+  <si>
+    <t>AT55~56</t>
+  </si>
+  <si>
+    <t>AT57~58</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="m/d"/>
     <numFmt numFmtId="165" formatCode="0.0"/>
   </numFmts>
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="10">
     <font>
       <sz val="10"/>
       <name val="Verdana"/>
@@ -1790,22 +1839,11 @@
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="1"/>
   <c:lang val="en-US"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
   <c:chart>
-    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
       <c:lineChart>
         <c:grouping val="standard"/>
-        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
@@ -1851,62 +1889,45 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:smooth val="0"/>
         </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
         <c:marker val="1"/>
-        <c:smooth val="0"/>
-        <c:axId val="92316032"/>
-        <c:axId val="92317568"/>
+        <c:axId val="68999808"/>
+        <c:axId val="69001600"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="92316032"/>
+        <c:axId val="68999808"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
-        <c:delete val="0"/>
         <c:axPos val="b"/>
         <c:numFmt formatCode="m/d" sourceLinked="1"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="92317568"/>
+        <c:crossAx val="69001600"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
         <c:baseTimeUnit val="days"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="92317568"/>
+        <c:axId val="69001600"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
-        <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="92316032"/>
+        <c:crossAx val="68999808"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="1" l="0.75000000000000211" r="0.75000000000000211" t="1" header="0.5" footer="0.5"/>
+    <c:pageMargins b="1" l="0.75000000000000233" r="0.75000000000000233" t="1" header="0.5" footer="0.5"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -2266,14 +2287,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView zoomScale="150" workbookViewId="0">
       <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75"/>
   <cols>
     <col min="1" max="1" width="7.625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="6.375" customWidth="1"/>
@@ -2282,7 +2303,7 @@
     <col min="5" max="5" width="19.25" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" s="4" customFormat="1">
       <c r="A1" s="4" t="s">
         <v>22</v>
       </c>
@@ -2299,7 +2320,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5">
       <c r="A3" t="s">
         <v>70</v>
       </c>
@@ -2316,7 +2337,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5">
       <c r="A4" t="s">
         <v>128</v>
       </c>
@@ -2333,7 +2354,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5">
       <c r="A5" t="s">
         <v>254</v>
       </c>
@@ -2350,7 +2371,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:5">
       <c r="D9" s="4" t="s">
         <v>67</v>
       </c>
@@ -2379,16 +2400,16 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:J1"/>
   <sheetViews>
     <sheetView zoomScale="150" workbookViewId="0">
       <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75"/>
   <sheetData>
-    <row r="1" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" ht="25.5">
       <c r="A1" s="4" t="s">
         <v>3</v>
       </c>
@@ -2432,14 +2453,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:L31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B7" zoomScale="150" workbookViewId="0">
-      <selection activeCell="G24" sqref="G24"/>
+    <sheetView topLeftCell="B9" zoomScale="150" workbookViewId="0">
+      <selection activeCell="K19" sqref="K19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75"/>
   <cols>
     <col min="1" max="1" width="6.625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="8.875" bestFit="1" customWidth="1"/>
@@ -2455,7 +2476,7 @@
     <col min="12" max="12" width="10.75" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:12" s="4" customFormat="1">
       <c r="A1" s="4" t="s">
         <v>40</v>
       </c>
@@ -2493,7 +2514,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:12">
       <c r="A2">
         <v>1</v>
       </c>
@@ -2531,7 +2552,7 @@
         <v>40598</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:12">
       <c r="A3">
         <v>1</v>
       </c>
@@ -2569,7 +2590,7 @@
         <v>40598</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:12">
       <c r="A4">
         <v>1</v>
       </c>
@@ -2607,7 +2628,7 @@
         <v>40598</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:12">
       <c r="A5">
         <v>1</v>
       </c>
@@ -2645,7 +2666,7 @@
         <v>40598</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:12">
       <c r="A6">
         <v>1</v>
       </c>
@@ -2683,7 +2704,7 @@
         <v>40598</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:12">
       <c r="A7">
         <v>1</v>
       </c>
@@ -2721,7 +2742,7 @@
         <v>40598</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:12">
       <c r="A8">
         <v>2</v>
       </c>
@@ -2759,7 +2780,7 @@
         <v>40598</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:12">
       <c r="A9">
         <v>2</v>
       </c>
@@ -2797,7 +2818,7 @@
         <v>40598</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:12">
       <c r="A10">
         <v>2</v>
       </c>
@@ -2835,7 +2856,7 @@
         <v>40598</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:12">
       <c r="A11">
         <v>2</v>
       </c>
@@ -2873,7 +2894,7 @@
         <v>40598</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:12">
       <c r="A12">
         <v>2</v>
       </c>
@@ -2911,7 +2932,7 @@
         <v>40598</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:12">
       <c r="A13">
         <v>2</v>
       </c>
@@ -2949,7 +2970,7 @@
         <v>40598</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:12">
       <c r="A14">
         <v>3</v>
       </c>
@@ -2987,7 +3008,7 @@
         <v>40598</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:12">
       <c r="A15">
         <v>3</v>
       </c>
@@ -3025,7 +3046,7 @@
         <v>40598</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:12">
       <c r="A16">
         <v>3</v>
       </c>
@@ -3063,7 +3084,7 @@
         <v>40598</v>
       </c>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:12">
       <c r="A17">
         <v>3</v>
       </c>
@@ -3101,7 +3122,7 @@
         <v>40598</v>
       </c>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:12">
       <c r="A18">
         <v>3</v>
       </c>
@@ -3111,11 +3132,35 @@
       <c r="C18" t="s">
         <v>117</v>
       </c>
+      <c r="D18" t="s">
+        <v>491</v>
+      </c>
+      <c r="E18" s="18" t="s">
+        <v>254</v>
+      </c>
+      <c r="F18" s="18" t="s">
+        <v>176</v>
+      </c>
+      <c r="G18">
+        <v>20</v>
+      </c>
+      <c r="H18">
+        <v>10</v>
+      </c>
+      <c r="I18">
+        <v>20</v>
+      </c>
+      <c r="J18">
+        <v>10</v>
+      </c>
+      <c r="K18" s="16">
+        <v>40630</v>
+      </c>
       <c r="L18" s="7">
         <v>40598</v>
       </c>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:12">
       <c r="A19">
         <v>3</v>
       </c>
@@ -3125,11 +3170,35 @@
       <c r="C19" t="s">
         <v>119</v>
       </c>
+      <c r="D19" t="s">
+        <v>492</v>
+      </c>
+      <c r="E19" s="18" t="s">
+        <v>254</v>
+      </c>
+      <c r="F19" s="18" t="s">
+        <v>176</v>
+      </c>
+      <c r="G19">
+        <v>50</v>
+      </c>
+      <c r="H19">
+        <v>20</v>
+      </c>
+      <c r="I19">
+        <v>50</v>
+      </c>
+      <c r="J19">
+        <v>25</v>
+      </c>
+      <c r="K19" s="16">
+        <v>40630</v>
+      </c>
       <c r="L19" s="7">
         <v>40598</v>
       </c>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:12">
       <c r="B20" t="s">
         <v>89</v>
       </c>
@@ -3149,7 +3218,7 @@
         <v>40598</v>
       </c>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:12">
       <c r="B21" t="s">
         <v>90</v>
       </c>
@@ -3169,7 +3238,7 @@
         <v>40598</v>
       </c>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:12">
       <c r="B22" t="s">
         <v>91</v>
       </c>
@@ -3189,7 +3258,7 @@
         <v>40598</v>
       </c>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:12">
       <c r="B23" t="s">
         <v>92</v>
       </c>
@@ -3209,7 +3278,7 @@
         <v>40602</v>
       </c>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:12">
       <c r="B24" t="s">
         <v>93</v>
       </c>
@@ -3229,7 +3298,7 @@
         <v>40602</v>
       </c>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:12">
       <c r="B25" t="s">
         <v>94</v>
       </c>
@@ -3249,7 +3318,7 @@
         <v>40602</v>
       </c>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:12">
       <c r="B26" t="s">
         <v>95</v>
       </c>
@@ -3260,7 +3329,7 @@
         <v>40610</v>
       </c>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:12">
       <c r="B27" t="s">
         <v>308</v>
       </c>
@@ -3271,7 +3340,7 @@
         <v>40610</v>
       </c>
     </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:12">
       <c r="B28" t="s">
         <v>341</v>
       </c>
@@ -3282,7 +3351,7 @@
         <v>40610</v>
       </c>
     </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:12">
       <c r="B29" t="s">
         <v>343</v>
       </c>
@@ -3293,7 +3362,7 @@
         <v>40610</v>
       </c>
     </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:12">
       <c r="B30" t="s">
         <v>344</v>
       </c>
@@ -3304,7 +3373,7 @@
         <v>40610</v>
       </c>
     </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:12">
       <c r="B31" t="s">
         <v>345</v>
       </c>
@@ -3328,14 +3397,14 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F31"/>
   <sheetViews>
-    <sheetView topLeftCell="C16" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+    <sheetView topLeftCell="C12" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75"/>
   <cols>
     <col min="1" max="1" width="8.875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="24.75" bestFit="1" customWidth="1"/>
@@ -3344,7 +3413,7 @@
     <col min="6" max="6" width="9" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6">
       <c r="A1" s="4" t="s">
         <v>28</v>
       </c>
@@ -3364,7 +3433,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" ht="25.5">
       <c r="A2" t="s">
         <v>31</v>
       </c>
@@ -3384,7 +3453,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" ht="25.5">
       <c r="A3" t="s">
         <v>32</v>
       </c>
@@ -3404,7 +3473,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6">
       <c r="A4" t="s">
         <v>34</v>
       </c>
@@ -3424,7 +3493,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6">
       <c r="A5" t="s">
         <v>74</v>
       </c>
@@ -3444,7 +3513,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6">
       <c r="A6" t="s">
         <v>75</v>
       </c>
@@ -3464,7 +3533,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:6">
       <c r="A7" t="s">
         <v>76</v>
       </c>
@@ -3484,7 +3553,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:6">
       <c r="A8" t="s">
         <v>77</v>
       </c>
@@ -3504,7 +3573,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:6">
       <c r="A9" t="s">
         <v>78</v>
       </c>
@@ -3524,7 +3593,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:6">
       <c r="A10" t="s">
         <v>79</v>
       </c>
@@ -3544,7 +3613,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:6">
       <c r="A11" t="s">
         <v>80</v>
       </c>
@@ -3564,7 +3633,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:6">
       <c r="A12" t="s">
         <v>81</v>
       </c>
@@ -3584,7 +3653,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:6">
       <c r="A13" t="s">
         <v>82</v>
       </c>
@@ -3604,7 +3673,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:6" ht="25.5">
       <c r="A14" s="18" t="s">
         <v>83</v>
       </c>
@@ -3624,7 +3693,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:6">
       <c r="A15" t="s">
         <v>84</v>
       </c>
@@ -3644,7 +3713,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:6">
       <c r="A16" t="s">
         <v>85</v>
       </c>
@@ -3664,7 +3733,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:6">
       <c r="A17" t="s">
         <v>86</v>
       </c>
@@ -3684,7 +3753,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:6">
       <c r="A18" t="s">
         <v>87</v>
       </c>
@@ -3694,6 +3763,9 @@
       <c r="C18" s="1" t="s">
         <v>118</v>
       </c>
+      <c r="D18" t="s">
+        <v>491</v>
+      </c>
       <c r="E18">
         <v>20</v>
       </c>
@@ -3701,7 +3773,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="19" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:6" ht="25.5">
       <c r="A19" t="s">
         <v>88</v>
       </c>
@@ -3711,6 +3783,9 @@
       <c r="C19" s="1" t="s">
         <v>120</v>
       </c>
+      <c r="D19" t="s">
+        <v>492</v>
+      </c>
       <c r="E19">
         <v>50</v>
       </c>
@@ -3718,7 +3793,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:6">
       <c r="A20" t="s">
         <v>89</v>
       </c>
@@ -3735,7 +3810,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:6">
       <c r="A21" t="s">
         <v>90</v>
       </c>
@@ -3752,7 +3827,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:6">
       <c r="A22" t="s">
         <v>91</v>
       </c>
@@ -3769,7 +3844,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="23" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:6" ht="25.5">
       <c r="A23" t="s">
         <v>92</v>
       </c>
@@ -3786,7 +3861,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="24" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:6" ht="25.5">
       <c r="A24" t="s">
         <v>93</v>
       </c>
@@ -3803,7 +3878,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:6">
       <c r="A25" t="s">
         <v>94</v>
       </c>
@@ -3820,7 +3895,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:6">
       <c r="A26" t="s">
         <v>95</v>
       </c>
@@ -3831,7 +3906,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="27" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:6" ht="25.5">
       <c r="A27" t="s">
         <v>308</v>
       </c>
@@ -3842,7 +3917,7 @@
         <v>351</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:6">
       <c r="A28" t="s">
         <v>341</v>
       </c>
@@ -3853,7 +3928,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:6">
       <c r="A29" t="s">
         <v>343</v>
       </c>
@@ -3864,7 +3939,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:6">
       <c r="A30" t="s">
         <v>344</v>
       </c>
@@ -3875,7 +3950,7 @@
         <v>355</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:6">
       <c r="A31" t="s">
         <v>345</v>
       </c>
@@ -3898,14 +3973,14 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F77"/>
   <sheetViews>
-    <sheetView topLeftCell="A51" zoomScale="145" zoomScaleNormal="145" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="E55" sqref="E55"/>
+    <sheetView topLeftCell="A54" zoomScale="145" zoomScaleNormal="145" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="A61" sqref="A61:A77"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75"/>
   <cols>
     <col min="1" max="1" width="6.375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="8.875" bestFit="1" customWidth="1"/>
@@ -3915,7 +3990,7 @@
     <col min="6" max="6" width="7.25" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6">
       <c r="A1" s="4" t="s">
         <v>61</v>
       </c>
@@ -3935,7 +4010,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" ht="47.25">
       <c r="A2" t="s">
         <v>54</v>
       </c>
@@ -3955,7 +4030,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" ht="47.25">
       <c r="A3" t="s">
         <v>55</v>
       </c>
@@ -3975,7 +4050,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" ht="47.25">
       <c r="A4" t="s">
         <v>56</v>
       </c>
@@ -3995,7 +4070,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" ht="47.25">
       <c r="A5" t="s">
         <v>57</v>
       </c>
@@ -4015,7 +4090,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" ht="47.25">
       <c r="A6" t="s">
         <v>58</v>
       </c>
@@ -4035,7 +4110,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" ht="31.5">
       <c r="A7" t="s">
         <v>59</v>
       </c>
@@ -4055,7 +4130,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="63" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" ht="63">
       <c r="A8" t="s">
         <v>150</v>
       </c>
@@ -4075,7 +4150,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="63" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" ht="63">
       <c r="A9" t="s">
         <v>154</v>
       </c>
@@ -4095,7 +4170,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="78.75" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" ht="78.75">
       <c r="A10" t="s">
         <v>155</v>
       </c>
@@ -4115,7 +4190,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="63" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" ht="63">
       <c r="A11" t="s">
         <v>157</v>
       </c>
@@ -4135,7 +4210,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="63" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" ht="63">
       <c r="A12" t="s">
         <v>158</v>
       </c>
@@ -4155,7 +4230,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="78.75" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" ht="78.75">
       <c r="A13" t="s">
         <v>159</v>
       </c>
@@ -4175,7 +4250,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" ht="47.25">
       <c r="A14" t="s">
         <v>170</v>
       </c>
@@ -4195,7 +4270,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" ht="47.25">
       <c r="A15" t="s">
         <v>172</v>
       </c>
@@ -4215,7 +4290,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="16" spans="1:6" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:6" ht="38.25">
       <c r="A16" t="s">
         <v>188</v>
       </c>
@@ -4235,7 +4310,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="17" spans="1:6" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:6" ht="38.25">
       <c r="A17" t="s">
         <v>189</v>
       </c>
@@ -4255,7 +4330,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="18" spans="1:6" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:6" ht="38.25">
       <c r="A18" t="s">
         <v>190</v>
       </c>
@@ -4275,7 +4350,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="19" spans="1:6" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:6" ht="38.25">
       <c r="A19" t="s">
         <v>191</v>
       </c>
@@ -4295,7 +4370,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="20" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" ht="26.25">
       <c r="A20" t="s">
         <v>192</v>
       </c>
@@ -4315,7 +4390,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="21" spans="1:6" ht="47.25" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:6" ht="47.25">
       <c r="A21" t="s">
         <v>193</v>
       </c>
@@ -4335,7 +4410,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="22" spans="1:6" ht="47.25" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:6" ht="47.25">
       <c r="A22" t="s">
         <v>194</v>
       </c>
@@ -4355,7 +4430,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="23" spans="1:6" ht="37.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:6" ht="37.5" customHeight="1">
       <c r="A23" t="s">
         <v>195</v>
       </c>
@@ -4375,7 +4450,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="24" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" ht="26.25">
       <c r="A24" t="s">
         <v>196</v>
       </c>
@@ -4395,7 +4470,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="25" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:6" ht="25.5">
       <c r="A25" t="s">
         <v>197</v>
       </c>
@@ -4415,7 +4490,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:6">
       <c r="A26" t="s">
         <v>198</v>
       </c>
@@ -4435,7 +4510,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="27" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:6" ht="25.5">
       <c r="A27" t="s">
         <v>199</v>
       </c>
@@ -4455,7 +4530,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="28" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:6" ht="25.5">
       <c r="A28" t="s">
         <v>200</v>
       </c>
@@ -4475,7 +4550,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="29" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:6" ht="25.5">
       <c r="A29" t="s">
         <v>201</v>
       </c>
@@ -4495,7 +4570,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="30" spans="1:6" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:6" ht="38.25">
       <c r="A30" t="s">
         <v>202</v>
       </c>
@@ -4515,7 +4590,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="31" spans="1:6" ht="51" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:6" ht="51">
       <c r="A31" t="s">
         <v>203</v>
       </c>
@@ -4535,7 +4610,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="32" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:6" ht="26.25">
       <c r="A32" t="s">
         <v>204</v>
       </c>
@@ -4555,7 +4630,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="33" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:6" ht="25.5">
       <c r="A33" t="s">
         <v>205</v>
       </c>
@@ -4575,7 +4650,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="34" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:6" ht="26.25">
       <c r="A34" t="s">
         <v>206</v>
       </c>
@@ -4595,7 +4670,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="35" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:6" ht="25.5">
       <c r="A35" t="s">
         <v>207</v>
       </c>
@@ -4615,7 +4690,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="36" spans="1:6" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:6" ht="38.25">
       <c r="A36" t="s">
         <v>208</v>
       </c>
@@ -4635,7 +4710,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="37" spans="1:6" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:6" ht="38.25">
       <c r="A37" t="s">
         <v>209</v>
       </c>
@@ -4655,7 +4730,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="38" spans="1:6" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:6" ht="38.25">
       <c r="A38" t="s">
         <v>210</v>
       </c>
@@ -4675,7 +4750,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="39" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:6" ht="25.5">
       <c r="A39" t="s">
         <v>211</v>
       </c>
@@ -4695,7 +4770,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="40" spans="1:6" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:6" ht="38.25">
       <c r="A40" t="s">
         <v>212</v>
       </c>
@@ -4715,7 +4790,7 @@
         <v>403</v>
       </c>
     </row>
-    <row r="41" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:6" ht="25.5">
       <c r="A41" t="s">
         <v>213</v>
       </c>
@@ -4735,7 +4810,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="42" spans="1:6" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:6" ht="38.25">
       <c r="A42" t="s">
         <v>214</v>
       </c>
@@ -4755,7 +4830,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="43" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:6" ht="25.5">
       <c r="A43" t="s">
         <v>215</v>
       </c>
@@ -4775,7 +4850,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="44" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:6" ht="25.5">
       <c r="A44" t="s">
         <v>216</v>
       </c>
@@ -4795,7 +4870,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="45" spans="1:6" ht="51" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:6" ht="51">
       <c r="A45" t="s">
         <v>217</v>
       </c>
@@ -4815,7 +4890,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="46" spans="1:6" ht="51" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:6" ht="51">
       <c r="A46" t="s">
         <v>218</v>
       </c>
@@ -4835,7 +4910,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="47" spans="1:6" ht="51" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:6" ht="51">
       <c r="A47" t="s">
         <v>219</v>
       </c>
@@ -4855,7 +4930,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="48" spans="1:6" ht="51" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:6" ht="51">
       <c r="A48" t="s">
         <v>220</v>
       </c>
@@ -4875,7 +4950,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="49" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:6" ht="25.5">
       <c r="A49" t="s">
         <v>221</v>
       </c>
@@ -4895,7 +4970,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="50" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:6" ht="51">
       <c r="A50" t="s">
         <v>222</v>
       </c>
@@ -4915,7 +4990,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="51" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:6" ht="25.5">
       <c r="A51" t="s">
         <v>223</v>
       </c>
@@ -4935,7 +5010,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="52" spans="1:6" ht="51" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:6" ht="51">
       <c r="A52" t="s">
         <v>224</v>
       </c>
@@ -4955,7 +5030,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="53" spans="1:6" ht="51" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:6" ht="51">
       <c r="A53" t="s">
         <v>225</v>
       </c>
@@ -4975,7 +5050,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="54" spans="1:6" ht="51" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:6" ht="51">
       <c r="A54" t="s">
         <v>226</v>
       </c>
@@ -4995,7 +5070,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="55" spans="1:6" ht="51" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:6" ht="51">
       <c r="A55" t="s">
         <v>227</v>
       </c>
@@ -5015,112 +5090,172 @@
         <v>53</v>
       </c>
     </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:6">
       <c r="A56" t="s">
         <v>228</v>
       </c>
-    </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B56" s="18" t="s">
+        <v>87</v>
+      </c>
+      <c r="C56" t="s">
+        <v>117</v>
+      </c>
+      <c r="D56" s="1" t="s">
+        <v>488</v>
+      </c>
+      <c r="E56" s="1" t="s">
+        <v>477</v>
+      </c>
+      <c r="F56" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6">
       <c r="A57" t="s">
         <v>229</v>
       </c>
-    </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B57" s="18" t="s">
+        <v>87</v>
+      </c>
+      <c r="C57" t="s">
+        <v>117</v>
+      </c>
+      <c r="D57" s="1" t="s">
+        <v>489</v>
+      </c>
+      <c r="E57" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="F57" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" ht="51">
       <c r="A58" t="s">
         <v>230</v>
       </c>
-    </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B58" s="18" t="s">
+        <v>88</v>
+      </c>
+      <c r="C58" t="s">
+        <v>119</v>
+      </c>
+      <c r="D58" s="1" t="s">
+        <v>487</v>
+      </c>
+      <c r="E58" s="1" t="s">
+        <v>478</v>
+      </c>
+      <c r="F58" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" ht="25.5">
       <c r="A59" t="s">
         <v>231</v>
       </c>
-    </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B59" s="18" t="s">
+        <v>88</v>
+      </c>
+      <c r="C59" t="s">
+        <v>119</v>
+      </c>
+      <c r="D59" s="1" t="s">
+        <v>490</v>
+      </c>
+      <c r="E59" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="F59" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6">
       <c r="A60" t="s">
         <v>232</v>
       </c>
     </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:6">
       <c r="A61" t="s">
         <v>233</v>
       </c>
     </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:6">
       <c r="A62" t="s">
         <v>234</v>
       </c>
     </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:6">
       <c r="A63" t="s">
         <v>370</v>
       </c>
     </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:6">
       <c r="A64" t="s">
         <v>371</v>
       </c>
     </row>
-    <row r="65" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:1">
       <c r="A65" t="s">
         <v>372</v>
       </c>
     </row>
-    <row r="66" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:1">
       <c r="A66" t="s">
         <v>373</v>
       </c>
     </row>
-    <row r="67" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:1">
       <c r="A67" t="s">
         <v>374</v>
       </c>
     </row>
-    <row r="68" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:1">
       <c r="A68" t="s">
         <v>375</v>
       </c>
     </row>
-    <row r="69" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:1">
       <c r="A69" t="s">
         <v>376</v>
       </c>
     </row>
-    <row r="70" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:1">
       <c r="A70" t="s">
         <v>377</v>
       </c>
     </row>
-    <row r="71" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:1">
       <c r="A71" t="s">
         <v>378</v>
       </c>
     </row>
-    <row r="72" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:1">
       <c r="A72" t="s">
         <v>379</v>
       </c>
     </row>
-    <row r="73" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:1">
       <c r="A73" t="s">
         <v>380</v>
       </c>
     </row>
-    <row r="74" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:1">
       <c r="A74" t="s">
         <v>381</v>
       </c>
     </row>
-    <row r="75" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:1">
       <c r="A75" t="s">
         <v>382</v>
       </c>
     </row>
-    <row r="76" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:1">
       <c r="A76" t="s">
         <v>383</v>
       </c>
     </row>
-    <row r="77" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:1">
       <c r="A77" t="s">
         <v>384</v>
       </c>
@@ -5138,14 +5273,14 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView zoomScale="150" workbookViewId="0">
       <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75"/>
   <cols>
     <col min="1" max="1" width="10.75" style="2"/>
     <col min="2" max="2" width="18.125" bestFit="1" customWidth="1"/>
@@ -5155,7 +5290,7 @@
     <col min="6" max="6" width="13.75" style="9" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" s="4" customFormat="1">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -5175,7 +5310,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6">
       <c r="A2" s="2">
         <v>40598</v>
       </c>
@@ -5186,7 +5321,7 @@
         <v>598</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6">
       <c r="A3" s="2">
         <v>40602</v>
       </c>
@@ -5207,7 +5342,7 @@
         <v>100.61538461538461</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6">
       <c r="A4" s="2">
         <v>40611</v>
       </c>
@@ -5228,7 +5363,7 @@
         <v>129.12</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6">
       <c r="A5" s="2">
         <v>40630</v>
       </c>
@@ -5249,13 +5384,13 @@
         <v>142.56</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6">
       <c r="F6" s="9" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:6">
       <c r="F7" s="9" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
@@ -5275,14 +5410,14 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:J42"/>
   <sheetViews>
     <sheetView topLeftCell="A22" zoomScale="150" workbookViewId="0">
       <selection activeCell="B34" sqref="B34:B42"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75"/>
   <cols>
     <col min="1" max="1" width="8.875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="38.75" style="1" bestFit="1" customWidth="1"/>
@@ -5296,7 +5431,7 @@
     <col min="10" max="10" width="11" style="6" bestFit="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10">
       <c r="A1" s="4" t="s">
         <v>11</v>
       </c>
@@ -5328,7 +5463,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:10">
       <c r="A2" t="s">
         <v>31</v>
       </c>
@@ -5360,7 +5495,7 @@
         <v>40600</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:10" ht="25.5">
       <c r="A4" t="s">
         <v>185</v>
       </c>
@@ -5371,7 +5506,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:10" ht="25.5">
       <c r="A5" t="s">
         <v>41</v>
       </c>
@@ -5382,7 +5517,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="6" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:10" ht="25.5">
       <c r="A6" t="s">
         <v>42</v>
       </c>
@@ -5393,7 +5528,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="7" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:10" ht="25.5">
       <c r="A7" t="s">
         <v>180</v>
       </c>
@@ -5404,7 +5539,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:10">
       <c r="A9" t="s">
         <v>32</v>
       </c>
@@ -5436,7 +5571,7 @@
         <v>40601</v>
       </c>
     </row>
-    <row r="11" spans="1:10" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:10" ht="38.25">
       <c r="A11" t="s">
         <v>43</v>
       </c>
@@ -5447,7 +5582,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="12" spans="1:10" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:10" ht="38.25">
       <c r="A12" t="s">
         <v>44</v>
       </c>
@@ -5458,7 +5593,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:10">
       <c r="A14" t="s">
         <v>156</v>
       </c>
@@ -5490,7 +5625,7 @@
         <v>40602</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:10">
       <c r="A15" t="s">
         <v>280</v>
       </c>
@@ -5502,7 +5637,7 @@
       </c>
       <c r="J15" s="7"/>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:10">
       <c r="A16" t="s">
         <v>281</v>
       </c>
@@ -5513,7 +5648,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:10">
       <c r="A17" t="s">
         <v>282</v>
       </c>
@@ -5524,7 +5659,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="18" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:10" ht="25.5">
       <c r="A18" t="s">
         <v>283</v>
       </c>
@@ -5536,10 +5671,10 @@
       </c>
       <c r="J18" s="7"/>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:10">
       <c r="J19" s="7"/>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:10">
       <c r="A20" t="s">
         <v>75</v>
       </c>
@@ -5571,7 +5706,7 @@
         <v>40602</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:10">
       <c r="A21" t="s">
         <v>284</v>
       </c>
@@ -5583,7 +5718,7 @@
       </c>
       <c r="J21" s="7"/>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:10">
       <c r="A22" t="s">
         <v>285</v>
       </c>
@@ -5594,7 +5729,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:10">
       <c r="A23" t="s">
         <v>286</v>
       </c>
@@ -5603,10 +5738,10 @@
       </c>
       <c r="J23" s="7"/>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:10">
       <c r="J24" s="7"/>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:10">
       <c r="A25" t="s">
         <v>74</v>
       </c>
@@ -5638,7 +5773,7 @@
         <v>40601</v>
       </c>
     </row>
-    <row r="26" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:10" ht="25.5">
       <c r="A26" t="s">
         <v>287</v>
       </c>
@@ -5650,7 +5785,7 @@
       </c>
       <c r="J26" s="7"/>
     </row>
-    <row r="27" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:10" ht="25.5">
       <c r="A27" t="s">
         <v>288</v>
       </c>
@@ -5662,7 +5797,7 @@
       </c>
       <c r="J27" s="7"/>
     </row>
-    <row r="28" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:10" ht="25.5">
       <c r="A28" t="s">
         <v>289</v>
       </c>
@@ -5674,10 +5809,10 @@
       </c>
       <c r="J28" s="7"/>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:10">
       <c r="J29" s="7"/>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:10">
       <c r="A30" t="s">
         <v>76</v>
       </c>
@@ -5709,7 +5844,7 @@
         <v>40602</v>
       </c>
     </row>
-    <row r="31" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:10" ht="25.5">
       <c r="A31" t="s">
         <v>290</v>
       </c>
@@ -5721,7 +5856,7 @@
       </c>
       <c r="J31" s="7"/>
     </row>
-    <row r="32" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:10" ht="25.5">
       <c r="A32" t="s">
         <v>291</v>
       </c>
@@ -5733,49 +5868,49 @@
       </c>
       <c r="J32" s="7"/>
     </row>
-    <row r="33" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="33" spans="2:10">
       <c r="J33" s="7"/>
     </row>
-    <row r="34" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="34" spans="2:10">
       <c r="B34" s="5" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="35" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="35" spans="2:10">
       <c r="B35" s="5"/>
     </row>
-    <row r="36" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="36" spans="2:10">
       <c r="B36" s="5" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="37" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="37" spans="2:10">
       <c r="B37" s="1" t="s">
         <v>300</v>
       </c>
     </row>
-    <row r="38" spans="2:10" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="38" spans="2:10" ht="25.5">
       <c r="B38" s="1" t="s">
         <v>299</v>
       </c>
     </row>
-    <row r="39" spans="2:10" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="39" spans="2:10" ht="38.25">
       <c r="B39" s="1" t="s">
         <v>302</v>
       </c>
       <c r="J39" s="7"/>
     </row>
-    <row r="40" spans="2:10" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="40" spans="2:10" ht="25.5">
       <c r="B40" s="1" t="s">
         <v>301</v>
       </c>
     </row>
-    <row r="41" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="41" spans="2:10">
       <c r="B41" s="5" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="42" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="42" spans="2:10">
       <c r="B42" s="1" t="s">
         <v>63</v>
       </c>
@@ -5793,20 +5928,20 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:J45"/>
   <sheetViews>
-    <sheetView topLeftCell="A34" zoomScale="150" workbookViewId="0">
+    <sheetView topLeftCell="A30" zoomScale="150" workbookViewId="0">
       <selection activeCell="B37" sqref="B37:B45"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75"/>
   <cols>
     <col min="1" max="1" width="8.875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="24.125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10">
       <c r="A1" s="4" t="s">
         <v>11</v>
       </c>
@@ -5838,7 +5973,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:10">
       <c r="A2" t="s">
         <v>77</v>
       </c>
@@ -5870,7 +6005,7 @@
         <v>40608</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:10" ht="25.5">
       <c r="A4" t="s">
         <v>316</v>
       </c>
@@ -5882,7 +6017,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:10" ht="25.5">
       <c r="A5" t="s">
         <v>317</v>
       </c>
@@ -5894,7 +6029,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="6" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:10" ht="25.5">
       <c r="A6" t="s">
         <v>318</v>
       </c>
@@ -5906,11 +6041,11 @@
         <v>128</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:10">
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:10">
       <c r="A8" t="s">
         <v>78</v>
       </c>
@@ -5942,7 +6077,7 @@
         <v>40608</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:10" ht="25.5">
       <c r="A10" t="s">
         <v>319</v>
       </c>
@@ -5954,7 +6089,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:10">
       <c r="A11" t="s">
         <v>320</v>
       </c>
@@ -5966,7 +6101,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="12" spans="1:10" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:10" ht="38.25">
       <c r="A12" t="s">
         <v>321</v>
       </c>
@@ -5978,7 +6113,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:10">
       <c r="A14" t="s">
         <v>79</v>
       </c>
@@ -6010,7 +6145,7 @@
         <v>40610</v>
       </c>
     </row>
-    <row r="15" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:10" ht="25.5">
       <c r="A15" t="s">
         <v>322</v>
       </c>
@@ -6021,7 +6156,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="16" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:10" ht="25.5">
       <c r="A16" t="s">
         <v>324</v>
       </c>
@@ -6032,7 +6167,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:10">
       <c r="A17" t="s">
         <v>325</v>
       </c>
@@ -6043,7 +6178,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="18" spans="1:10" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:10" ht="38.25">
       <c r="A18" t="s">
         <v>327</v>
       </c>
@@ -6055,10 +6190,10 @@
       </c>
       <c r="J18" s="16"/>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:10">
       <c r="J19" s="16"/>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:10">
       <c r="A20" t="s">
         <v>80</v>
       </c>
@@ -6090,7 +6225,7 @@
         <v>40610</v>
       </c>
     </row>
-    <row r="21" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:10" ht="25.5">
       <c r="A21" t="s">
         <v>331</v>
       </c>
@@ -6101,7 +6236,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="22" spans="1:10" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:10" ht="38.25">
       <c r="A22" t="s">
         <v>332</v>
       </c>
@@ -6112,7 +6247,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="23" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:10" ht="25.5">
       <c r="A23" t="s">
         <v>334</v>
       </c>
@@ -6123,7 +6258,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="24" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:10" ht="25.5">
       <c r="A24" t="s">
         <v>336</v>
       </c>
@@ -6134,7 +6269,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="25" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:10" ht="25.5">
       <c r="A25" t="s">
         <v>338</v>
       </c>
@@ -6145,7 +6280,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:10">
       <c r="A27" t="s">
         <v>81</v>
       </c>
@@ -6177,7 +6312,7 @@
         <v>40612</v>
       </c>
     </row>
-    <row r="28" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:10" ht="25.5">
       <c r="A28" t="s">
         <v>385</v>
       </c>
@@ -6186,7 +6321,7 @@
       </c>
       <c r="J28" s="16"/>
     </row>
-    <row r="29" spans="1:10" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:10" ht="38.25">
       <c r="A29" t="s">
         <v>387</v>
       </c>
@@ -6195,7 +6330,7 @@
       </c>
       <c r="J29" s="16"/>
     </row>
-    <row r="30" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:10" ht="25.5">
       <c r="A30" t="s">
         <v>389</v>
       </c>
@@ -6204,7 +6339,7 @@
       </c>
       <c r="J30" s="16"/>
     </row>
-    <row r="31" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:10" ht="25.5">
       <c r="A31" t="s">
         <v>391</v>
       </c>
@@ -6213,7 +6348,7 @@
       </c>
       <c r="J31" s="16"/>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:10">
       <c r="A32" t="s">
         <v>82</v>
       </c>
@@ -6245,7 +6380,7 @@
         <v>40612</v>
       </c>
     </row>
-    <row r="33" spans="1:2" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:2" ht="25.5">
       <c r="A33" t="s">
         <v>393</v>
       </c>
@@ -6253,7 +6388,7 @@
         <v>386</v>
       </c>
     </row>
-    <row r="34" spans="1:2" ht="51" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:2" ht="51">
       <c r="A34" t="s">
         <v>394</v>
       </c>
@@ -6261,7 +6396,7 @@
         <v>395</v>
       </c>
     </row>
-    <row r="35" spans="1:2" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:2" ht="25.5">
       <c r="A35" t="s">
         <v>396</v>
       </c>
@@ -6269,43 +6404,43 @@
         <v>397</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:2">
       <c r="B37" s="5" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:2">
       <c r="B38" s="5"/>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:2">
       <c r="B39" s="5" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:2">
       <c r="B40" s="1" t="s">
         <v>300</v>
       </c>
     </row>
-    <row r="41" spans="1:2" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:2" ht="25.5">
       <c r="B41" s="1" t="s">
         <v>299</v>
       </c>
     </row>
-    <row r="42" spans="1:2" ht="51" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:2" ht="51">
       <c r="B42" s="1" t="s">
         <v>302</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:2">
       <c r="B43" s="1"/>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:2">
       <c r="B44" s="5" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="45" spans="1:2" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:2" ht="25.5">
       <c r="B45" s="1" t="s">
         <v>63</v>
       </c>
@@ -6323,19 +6458,19 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J43"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:J47"/>
   <sheetViews>
-    <sheetView topLeftCell="A28" zoomScale="150" workbookViewId="0">
-      <selection activeCell="E25" sqref="E25"/>
+    <sheetView tabSelected="1" topLeftCell="A30" zoomScale="150" workbookViewId="0">
+      <selection activeCell="C30" sqref="C30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75"/>
   <cols>
     <col min="2" max="2" width="24.875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10">
       <c r="A1" s="4" t="s">
         <v>3</v>
       </c>
@@ -6367,7 +6502,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:10">
       <c r="A2" s="18" t="s">
         <v>83</v>
       </c>
@@ -6399,7 +6534,7 @@
         <v>40625</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:10" ht="25.5">
       <c r="A4" t="s">
         <v>419</v>
       </c>
@@ -6411,7 +6546,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:10" ht="38.25">
       <c r="A5" t="s">
         <v>420</v>
       </c>
@@ -6423,7 +6558,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="6" spans="1:10" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:10" ht="38.25">
       <c r="A6" t="s">
         <v>421</v>
       </c>
@@ -6435,7 +6570,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="7" spans="1:10" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:10" ht="38.25">
       <c r="A7" t="s">
         <v>425</v>
       </c>
@@ -6447,7 +6582,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="8" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:10" ht="25.5">
       <c r="A8" t="s">
         <v>426</v>
       </c>
@@ -6455,7 +6590,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="9" spans="1:10" ht="51" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:10" ht="51">
       <c r="A9" t="s">
         <v>427</v>
       </c>
@@ -6467,7 +6602,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:10" ht="38.25">
       <c r="A10" t="s">
         <v>429</v>
       </c>
@@ -6479,7 +6614,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:10">
       <c r="A12" t="s">
         <v>84</v>
       </c>
@@ -6511,7 +6646,7 @@
         <v>40625</v>
       </c>
     </row>
-    <row r="14" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:10" ht="25.5">
       <c r="A14" t="s">
         <v>438</v>
       </c>
@@ -6523,7 +6658,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="15" spans="1:10" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:10" ht="38.25">
       <c r="A15" t="s">
         <v>439</v>
       </c>
@@ -6535,7 +6670,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="16" spans="1:10" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:10" ht="38.25">
       <c r="A16" t="s">
         <v>440</v>
       </c>
@@ -6547,11 +6682,11 @@
         <v>128</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:10">
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:10">
       <c r="A18" t="s">
         <v>85</v>
       </c>
@@ -6580,7 +6715,7 @@
         <v>40628</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:10">
       <c r="A19" t="s">
         <v>458</v>
       </c>
@@ -6591,7 +6726,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="20" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:10" ht="25.5">
       <c r="A20" t="s">
         <v>460</v>
       </c>
@@ -6602,7 +6737,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="21" spans="1:10" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:10" ht="38.25">
       <c r="A21" t="s">
         <v>462</v>
       </c>
@@ -6613,7 +6748,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="22" spans="1:10" ht="51" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:10" ht="51">
       <c r="A22" t="s">
         <v>463</v>
       </c>
@@ -6624,7 +6759,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="23" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:10" ht="25.5">
       <c r="A23" t="s">
         <v>466</v>
       </c>
@@ -6635,10 +6770,10 @@
         <v>70</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:10">
       <c r="D24" s="18"/>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:10">
       <c r="A25" t="s">
         <v>86</v>
       </c>
@@ -6667,7 +6802,7 @@
         <v>40628</v>
       </c>
     </row>
-    <row r="26" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:10" ht="25.5">
       <c r="A26" t="s">
         <v>468</v>
       </c>
@@ -6678,7 +6813,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="27" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:10" ht="25.5">
       <c r="A27" t="s">
         <v>469</v>
       </c>
@@ -6689,7 +6824,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="28" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:10" ht="25.5">
       <c r="A28" t="s">
         <v>470</v>
       </c>
@@ -6700,7 +6835,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="29" spans="1:10" ht="51" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:10" ht="51">
       <c r="A29" t="s">
         <v>471</v>
       </c>
@@ -6711,7 +6846,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="30" spans="1:10" ht="51" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:10" ht="51">
       <c r="A30" t="s">
         <v>474</v>
       </c>
@@ -6722,81 +6857,145 @@
         <v>70</v>
       </c>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:10">
       <c r="D31" s="18"/>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:10">
       <c r="A32" t="s">
         <v>87</v>
       </c>
       <c r="B32" t="s">
         <v>117</v>
       </c>
+      <c r="C32" t="s">
+        <v>491</v>
+      </c>
       <c r="D32" s="18" t="s">
         <v>254</v>
       </c>
+      <c r="E32" s="18" t="s">
+        <v>330</v>
+      </c>
       <c r="F32">
         <v>20</v>
       </c>
       <c r="G32">
         <v>10</v>
       </c>
-    </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H32">
+        <v>20</v>
+      </c>
+      <c r="I32">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9">
       <c r="A33" t="s">
+        <v>479</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" ht="38.25">
+      <c r="A34" t="s">
+        <v>481</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>482</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9">
+      <c r="A35" t="s">
         <v>88</v>
       </c>
-      <c r="B33" t="s">
+      <c r="B35" t="s">
         <v>119</v>
       </c>
-      <c r="D33" s="18" t="s">
+      <c r="C35" t="s">
+        <v>492</v>
+      </c>
+      <c r="D35" s="18" t="s">
         <v>254</v>
       </c>
-      <c r="F33">
+      <c r="E35" s="18" t="s">
+        <v>330</v>
+      </c>
+      <c r="F35">
         <v>50</v>
       </c>
-      <c r="G33">
+      <c r="G35">
         <v>20</v>
       </c>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="B35" s="5" t="s">
+      <c r="H35">
+        <v>50</v>
+      </c>
+      <c r="I35">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9">
+      <c r="A36" t="s">
+        <v>483</v>
+      </c>
+      <c r="B36" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9">
+      <c r="A37" t="s">
+        <v>485</v>
+      </c>
+      <c r="B37" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9">
+      <c r="A38" t="s">
+        <v>486</v>
+      </c>
+      <c r="B38" t="s">
+        <v>484</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9">
+      <c r="B39" s="5" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="B36" s="5"/>
-    </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="B37" s="5" t="s">
+    <row r="40" spans="1:9">
+      <c r="B40" s="5"/>
+    </row>
+    <row r="41" spans="1:9">
+      <c r="B41" s="5" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="B38" s="1" t="s">
+    <row r="42" spans="1:9">
+      <c r="B42" s="1" t="s">
         <v>300</v>
       </c>
     </row>
-    <row r="39" spans="1:7" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="B39" s="1" t="s">
+    <row r="43" spans="1:9" ht="25.5">
+      <c r="B43" s="1" t="s">
         <v>299</v>
       </c>
     </row>
-    <row r="40" spans="1:7" ht="51" x14ac:dyDescent="0.2">
-      <c r="B40" s="1" t="s">
+    <row r="44" spans="1:9" ht="51">
+      <c r="B44" s="1" t="s">
         <v>302</v>
       </c>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="B41" s="1"/>
-    </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="B42" s="5" t="s">
+    <row r="45" spans="1:9">
+      <c r="B45" s="1"/>
+    </row>
+    <row r="46" spans="1:9">
+      <c r="B46" s="5" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="43" spans="1:7" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="B43" s="1" t="s">
+    <row r="47" spans="1:9" ht="25.5">
+      <c r="B47" s="1" t="s">
         <v>63</v>
       </c>
     </row>
@@ -6812,19 +7011,19 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:J7"/>
   <sheetViews>
     <sheetView zoomScale="150" workbookViewId="0">
       <selection activeCell="D2" sqref="D2:G7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75"/>
   <cols>
     <col min="2" max="2" width="23.75" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10">
       <c r="A1" s="4" t="s">
         <v>3</v>
       </c>
@@ -6856,7 +7055,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:10">
       <c r="A2" t="s">
         <v>89</v>
       </c>
@@ -6873,7 +7072,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:10">
       <c r="A3" t="s">
         <v>90</v>
       </c>
@@ -6890,7 +7089,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:10">
       <c r="A4" t="s">
         <v>91</v>
       </c>
@@ -6907,7 +7106,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:10">
       <c r="A5" t="s">
         <v>92</v>
       </c>
@@ -6924,7 +7123,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:10">
       <c r="A6" t="s">
         <v>93</v>
       </c>
@@ -6941,7 +7140,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:10">
       <c r="A7" t="s">
         <v>94</v>
       </c>

</xml_diff>

<commit_message>
two user stories implemented
create the new test file;
user story 20 and 24 are implemented;
fixed some bugs.
</commit_message>
<xml_diff>
--- a/Team05Report.xlsx
+++ b/Team05Report.xlsx
@@ -62,7 +62,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1007" uniqueCount="493">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1108" uniqueCount="534">
   <si>
     <t>Date</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -1014,9 +1014,6 @@
     <t>Unique information</t>
   </si>
   <si>
-    <t>An individual can only have one tag of sex, name, birthdate, etc.</t>
-  </si>
-  <si>
     <t>Inform everyone when you discover a problem</t>
   </si>
   <si>
@@ -1599,6 +1596,132 @@
   <si>
     <t xml:space="preserve">In Family F2, child I5(Emily /Mao/) and child I1(Jacky /Mao/) are not multiple births but born within one year.
 </t>
+  </si>
+  <si>
+    <t>Individual I1(Jacky /Mao/) is the child of multiple families: Family F2, Family F3.</t>
+  </si>
+  <si>
+    <t>Individual I1 is the child of both Family F2 and Family F3</t>
+  </si>
+  <si>
+    <t>Individual I3 is the child of only Family F4</t>
+  </si>
+  <si>
+    <t>AT59~60</t>
+  </si>
+  <si>
+    <t>T20.01</t>
+  </si>
+  <si>
+    <t>T20.02</t>
+  </si>
+  <si>
+    <t>Get the pointers of famc for each individual</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Check if the size of pointers is greater than 1 </t>
+  </si>
+  <si>
+    <t>An individual should only have one tag of sex, name, birthdate, and at most one tag of death date; a family should only have one tag of marriage date and at most one tag of divorce date.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Individual I1 has more than one name : Jacky /Mao/, Jackie /Mao/. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Individual I1 has more than one sex : F, M. </t>
+  </si>
+  <si>
+    <t>Individual I1 has more than one birthday : 27 JAN 1960, 27 JAN 1970.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Individual I1 has more than one death date : 1 JAN 2014, 1 FEB 2014. </t>
+  </si>
+  <si>
+    <t>Individual I2 does not have a name.</t>
+  </si>
+  <si>
+    <t>Individual I2 does not have a sex.</t>
+  </si>
+  <si>
+    <t>Individual I2 does not have a birthday.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Family F4 does not have a marriage date. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Family F5 has more than one marriage date : 2 JAN 2000, 1 JAN 2000. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Family F5 has more than one divorce date : 5 JAN 2014, 5 JAN 2014. </t>
+  </si>
+  <si>
+    <t>Individual I1 has two names: Jacky /Mao/ and Jackie /Mao/</t>
+  </si>
+  <si>
+    <t>Individual I1 has two sexes: F, M</t>
+  </si>
+  <si>
+    <t>Individual I1 has two birthdays: 27 JAN 1960 and 27 JAN 1970</t>
+  </si>
+  <si>
+    <t>Individual I1 has two death dates: 1 JAN 2014 and 1 FEB 2014</t>
+  </si>
+  <si>
+    <t>Individual I2 does not have a name</t>
+  </si>
+  <si>
+    <t>Individual I2 does not have a sex</t>
+  </si>
+  <si>
+    <t>Individual I2 does not have a birthday</t>
+  </si>
+  <si>
+    <t>Individual I3 has one name, one sex, one birthday and zero death date</t>
+  </si>
+  <si>
+    <t>Family F4 does not have a marriage date</t>
+  </si>
+  <si>
+    <t>Family F5 has two marriage date: 2 JAN 2000 and 1 JAN 2000</t>
+  </si>
+  <si>
+    <t>Family F5 has two divorce date: 5 JAN 2014 and 5 JAN 2014</t>
+  </si>
+  <si>
+    <t>Family F6 has one marriage date and zero divorce date</t>
+  </si>
+  <si>
+    <t>AT61~72</t>
+  </si>
+  <si>
+    <t>T24.01</t>
+  </si>
+  <si>
+    <t>T24.02</t>
+  </si>
+  <si>
+    <t>Scan all the tags in the file</t>
+  </si>
+  <si>
+    <t>For the tags within each INDI tag, count the numbers of NAME, SEX, BIRT DATE and DEAT DATE</t>
+  </si>
+  <si>
+    <t>For the tags within each FAM tag, count the numbers of MARR DATE and DIV DATE</t>
+  </si>
+  <si>
+    <t>T24.03</t>
+  </si>
+  <si>
+    <t>T24.04</t>
+  </si>
+  <si>
+    <t>For each individual, check if the numbers of NAME, SEX and BIRT DATE are all 1, and if the number of DEAT DATE is 0 or 1</t>
+  </si>
+  <si>
+    <t>T24.05</t>
+  </si>
+  <si>
+    <t>For each family, check if the number of MARR DATE is 1, and if the number of DIV DATE is 0 or 1</t>
   </si>
 </sst>
 </file>
@@ -1896,25 +2019,25 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="177294720"/>
-        <c:axId val="262890624"/>
+        <c:axId val="356019200"/>
+        <c:axId val="376402688"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="177294720"/>
+        <c:axId val="356019200"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="m/d" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="262890624"/>
+        <c:crossAx val="376402688"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
         <c:baseTimeUnit val="days"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="262890624"/>
+        <c:axId val="376402688"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1922,7 +2045,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="177294720"/>
+        <c:crossAx val="356019200"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1932,7 +2055,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="1" l="0.75000000000000244" r="0.75000000000000244" t="1" header="0.5" footer="0.5"/>
+    <c:pageMargins b="1" l="0.75000000000000266" r="0.75000000000000266" t="1" header="0.5" footer="0.5"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -2461,8 +2584,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:L31"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" zoomScale="150" workbookViewId="0">
-      <selection activeCell="K19" sqref="K19"/>
+    <sheetView topLeftCell="B4" zoomScale="150" workbookViewId="0">
+      <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75"/>
@@ -2758,7 +2881,7 @@
         <v>107</v>
       </c>
       <c r="D8" s="18" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="E8" s="18" t="s">
         <v>128</v>
@@ -2796,7 +2919,7 @@
         <v>114</v>
       </c>
       <c r="D9" s="18" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="E9" s="18" t="s">
         <v>128</v>
@@ -2834,7 +2957,7 @@
         <v>108</v>
       </c>
       <c r="D10" s="18" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="E10" t="s">
         <v>187</v>
@@ -2872,7 +2995,7 @@
         <v>33</v>
       </c>
       <c r="D11" s="18" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="E11" t="s">
         <v>187</v>
@@ -2910,13 +3033,13 @@
         <v>99</v>
       </c>
       <c r="D12" s="18" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="E12" t="s">
         <v>254</v>
       </c>
       <c r="F12" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="G12">
         <v>30</v>
@@ -2948,13 +3071,13 @@
         <v>100</v>
       </c>
       <c r="D13" s="18" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="E13" t="s">
         <v>254</v>
       </c>
       <c r="F13" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="G13">
         <v>30</v>
@@ -2986,7 +3109,7 @@
         <v>101</v>
       </c>
       <c r="D14" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="E14" s="18" t="s">
         <v>128</v>
@@ -3024,7 +3147,7 @@
         <v>295</v>
       </c>
       <c r="D15" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="E15" s="18" t="s">
         <v>128</v>
@@ -3062,7 +3185,7 @@
         <v>110</v>
       </c>
       <c r="D16" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="E16" s="18" t="s">
         <v>187</v>
@@ -3100,7 +3223,7 @@
         <v>111</v>
       </c>
       <c r="D17" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="E17" s="18" t="s">
         <v>187</v>
@@ -3138,7 +3261,7 @@
         <v>117</v>
       </c>
       <c r="D18" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="E18" s="18" t="s">
         <v>254</v>
@@ -3176,7 +3299,7 @@
         <v>119</v>
       </c>
       <c r="D19" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="E19" s="18" t="s">
         <v>254</v>
@@ -3230,14 +3353,29 @@
       <c r="C21" t="s">
         <v>126</v>
       </c>
+      <c r="D21" s="18" t="s">
+        <v>495</v>
+      </c>
       <c r="E21" t="s">
         <v>128</v>
       </c>
+      <c r="F21" s="18" t="s">
+        <v>176</v>
+      </c>
       <c r="G21">
         <v>75</v>
       </c>
       <c r="H21">
         <v>30</v>
+      </c>
+      <c r="I21">
+        <v>15</v>
+      </c>
+      <c r="J21">
+        <v>30</v>
+      </c>
+      <c r="K21" s="16">
+        <v>40638</v>
       </c>
       <c r="L21" s="7">
         <v>40598</v>
@@ -3310,14 +3448,29 @@
       <c r="C25" s="18" t="s">
         <v>297</v>
       </c>
+      <c r="D25" s="18" t="s">
+        <v>523</v>
+      </c>
       <c r="E25" t="s">
         <v>128</v>
       </c>
+      <c r="F25" s="18" t="s">
+        <v>329</v>
+      </c>
       <c r="G25">
         <v>100</v>
       </c>
       <c r="H25">
         <v>45</v>
+      </c>
+      <c r="I25">
+        <v>226</v>
+      </c>
+      <c r="J25">
+        <v>90</v>
+      </c>
+      <c r="K25" s="16">
+        <v>40638</v>
       </c>
       <c r="L25" s="7">
         <v>40602</v>
@@ -3328,7 +3481,7 @@
         <v>95</v>
       </c>
       <c r="C26" s="18" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="L26" s="7">
         <v>40610</v>
@@ -3336,10 +3489,10 @@
     </row>
     <row r="27" spans="1:12">
       <c r="B27" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="C27" s="18" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="L27" s="7">
         <v>40610</v>
@@ -3347,10 +3500,10 @@
     </row>
     <row r="28" spans="1:12">
       <c r="B28" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="C28" s="18" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="L28" s="7">
         <v>40610</v>
@@ -3358,10 +3511,10 @@
     </row>
     <row r="29" spans="1:12">
       <c r="B29" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="C29" s="18" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="L29" s="7">
         <v>40610</v>
@@ -3369,10 +3522,10 @@
     </row>
     <row r="30" spans="1:12">
       <c r="B30" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="C30" s="18" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="L30" s="7">
         <v>40610</v>
@@ -3380,10 +3533,10 @@
     </row>
     <row r="31" spans="1:12">
       <c r="B31" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="C31" s="18" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="L31" s="7">
         <v>40610</v>
@@ -3405,8 +3558,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75"/>
@@ -3569,7 +3722,7 @@
         <v>96</v>
       </c>
       <c r="D8" s="18" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="E8">
         <v>20</v>
@@ -3589,7 +3742,7 @@
         <v>115</v>
       </c>
       <c r="D9" s="18" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="E9">
         <v>50</v>
@@ -3609,7 +3762,7 @@
         <v>109</v>
       </c>
       <c r="D10" s="18" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="E10">
         <v>50</v>
@@ -3629,7 +3782,7 @@
         <v>47</v>
       </c>
       <c r="D11" s="18" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="E11">
         <v>30</v>
@@ -3649,7 +3802,7 @@
         <v>48</v>
       </c>
       <c r="D12" s="18" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="E12">
         <v>30</v>
@@ -3669,7 +3822,7 @@
         <v>98</v>
       </c>
       <c r="D13" s="18" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="E13">
         <v>30</v>
@@ -3689,7 +3842,7 @@
         <v>138</v>
       </c>
       <c r="D14" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="E14">
         <v>70</v>
@@ -3706,10 +3859,10 @@
         <v>295</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="D15" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="E15">
         <v>50</v>
@@ -3729,7 +3882,7 @@
         <v>294</v>
       </c>
       <c r="D16" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="E16">
         <v>100</v>
@@ -3743,13 +3896,13 @@
         <v>86</v>
       </c>
       <c r="B17" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="C17" s="1" t="s">
         <v>102</v>
       </c>
       <c r="D17" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="E17">
         <v>30</v>
@@ -3769,7 +3922,7 @@
         <v>118</v>
       </c>
       <c r="D18" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="E18">
         <v>20</v>
@@ -3789,7 +3942,7 @@
         <v>120</v>
       </c>
       <c r="D19" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="E19">
         <v>50</v>
@@ -3825,6 +3978,9 @@
       <c r="C21" s="1" t="s">
         <v>124</v>
       </c>
+      <c r="D21" s="18" t="s">
+        <v>495</v>
+      </c>
       <c r="E21">
         <v>75</v>
       </c>
@@ -3883,15 +4039,18 @@
         <v>30</v>
       </c>
     </row>
-    <row r="25" spans="1:6">
+    <row r="25" spans="1:6" ht="38.25">
       <c r="A25" t="s">
         <v>94</v>
       </c>
       <c r="B25" s="18" t="s">
         <v>297</v>
       </c>
-      <c r="C25" s="1" t="s">
-        <v>298</v>
+      <c r="C25" s="20" t="s">
+        <v>500</v>
+      </c>
+      <c r="D25" s="18" t="s">
+        <v>523</v>
       </c>
       <c r="E25">
         <v>100</v>
@@ -3905,65 +4064,65 @@
         <v>95</v>
       </c>
       <c r="B26" s="18" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="27" spans="1:6" ht="25.5">
       <c r="A27" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="B27" s="18" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
     </row>
     <row r="28" spans="1:6">
       <c r="A28" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="B28" s="18" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
     </row>
     <row r="29" spans="1:6">
       <c r="A29" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="B29" s="18" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
     </row>
     <row r="30" spans="1:6">
       <c r="A30" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="B30" s="18" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
     </row>
     <row r="31" spans="1:6">
       <c r="A31" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="B31" s="18" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
     </row>
   </sheetData>
@@ -3981,8 +4140,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F77"/>
   <sheetViews>
-    <sheetView topLeftCell="A48" zoomScale="145" zoomScaleNormal="145" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="E63" sqref="E63"/>
+    <sheetView topLeftCell="A61" zoomScale="145" zoomScaleNormal="145" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="A73" sqref="A73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75"/>
@@ -4586,10 +4745,10 @@
         <v>107</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="F30" t="s">
         <v>53</v>
@@ -4606,10 +4765,10 @@
         <v>107</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="F31" t="s">
         <v>53</v>
@@ -4626,7 +4785,7 @@
         <v>107</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="E32" s="12" t="s">
         <v>51</v>
@@ -4646,10 +4805,10 @@
         <v>114</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="F33" t="s">
         <v>53</v>
@@ -4666,7 +4825,7 @@
         <v>114</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="E34" s="12" t="s">
         <v>51</v>
@@ -4686,7 +4845,7 @@
         <v>108</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="E35" s="1" t="s">
         <v>51</v>
@@ -4706,10 +4865,10 @@
         <v>108</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="E36" s="1" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="F36" t="s">
         <v>53</v>
@@ -4726,10 +4885,10 @@
         <v>108</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="E37" s="1" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="F37" t="s">
         <v>53</v>
@@ -4746,10 +4905,10 @@
         <v>33</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="E38" s="1" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="F38" t="s">
         <v>53</v>
@@ -4766,7 +4925,7 @@
         <v>33</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="E39" s="1" t="s">
         <v>51</v>
@@ -4786,13 +4945,13 @@
         <v>99</v>
       </c>
       <c r="D40" s="1" t="s">
+        <v>397</v>
+      </c>
+      <c r="E40" s="1" t="s">
         <v>398</v>
       </c>
-      <c r="E40" s="1" t="s">
-        <v>399</v>
-      </c>
       <c r="F40" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
     </row>
     <row r="41" spans="1:6" ht="25.5">
@@ -4806,10 +4965,10 @@
         <v>99</v>
       </c>
       <c r="D41" s="1" t="s">
+        <v>399</v>
+      </c>
+      <c r="E41" s="1" t="s">
         <v>400</v>
-      </c>
-      <c r="E41" s="1" t="s">
-        <v>401</v>
       </c>
       <c r="F41" t="s">
         <v>53</v>
@@ -4826,7 +4985,7 @@
         <v>99</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="E42" s="1" t="s">
         <v>51</v>
@@ -4846,10 +5005,10 @@
         <v>100</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="E43" s="1" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="F43" t="s">
         <v>53</v>
@@ -4866,7 +5025,7 @@
         <v>100</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="E44" s="1" t="s">
         <v>51</v>
@@ -4886,10 +5045,10 @@
         <v>101</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="E45" s="1" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="F45" t="s">
         <v>53</v>
@@ -4906,10 +5065,10 @@
         <v>101</v>
       </c>
       <c r="D46" s="1" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="E46" s="1" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="F46" t="s">
         <v>53</v>
@@ -4926,7 +5085,7 @@
         <v>101</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="E47" s="1" t="s">
         <v>51</v>
@@ -4946,10 +5105,10 @@
         <v>295</v>
       </c>
       <c r="D48" s="1" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="E48" s="1" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="F48" t="s">
         <v>53</v>
@@ -4966,7 +5125,7 @@
         <v>295</v>
       </c>
       <c r="D49" s="1" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="E49" s="1" t="s">
         <v>51</v>
@@ -4986,10 +5145,10 @@
         <v>110</v>
       </c>
       <c r="D50" s="1" t="s">
+        <v>443</v>
+      </c>
+      <c r="E50" s="1" t="s">
         <v>444</v>
-      </c>
-      <c r="E50" s="1" t="s">
-        <v>445</v>
       </c>
       <c r="F50" t="s">
         <v>53</v>
@@ -5000,13 +5159,13 @@
         <v>223</v>
       </c>
       <c r="B51" s="18" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="C51" t="s">
         <v>110</v>
       </c>
       <c r="D51" s="1" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="E51" s="1" t="s">
         <v>51</v>
@@ -5023,13 +5182,13 @@
         <v>86</v>
       </c>
       <c r="C52" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="D52" s="1" t="s">
+        <v>447</v>
+      </c>
+      <c r="E52" s="1" t="s">
         <v>448</v>
-      </c>
-      <c r="E52" s="1" t="s">
-        <v>449</v>
       </c>
       <c r="F52" t="s">
         <v>53</v>
@@ -5043,13 +5202,13 @@
         <v>86</v>
       </c>
       <c r="C53" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="D53" s="1" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="E53" s="1" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="F53" t="s">
         <v>53</v>
@@ -5063,13 +5222,13 @@
         <v>86</v>
       </c>
       <c r="C54" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="D54" s="1" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="E54" s="1" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="F54" t="s">
         <v>53</v>
@@ -5083,13 +5242,13 @@
         <v>86</v>
       </c>
       <c r="C55" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="D55" s="1" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="E55" s="1" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="F55" t="s">
         <v>53</v>
@@ -5106,10 +5265,10 @@
         <v>117</v>
       </c>
       <c r="D56" s="1" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="E56" s="1" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="F56" t="s">
         <v>53</v>
@@ -5126,7 +5285,7 @@
         <v>117</v>
       </c>
       <c r="D57" s="1" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="E57" s="1" t="s">
         <v>51</v>
@@ -5146,10 +5305,10 @@
         <v>119</v>
       </c>
       <c r="D58" s="1" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="E58" s="20" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="F58" t="s">
         <v>53</v>
@@ -5166,7 +5325,7 @@
         <v>119</v>
       </c>
       <c r="D59" s="1" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="E59" s="1" t="s">
         <v>51</v>
@@ -5175,94 +5334,304 @@
         <v>53</v>
       </c>
     </row>
-    <row r="60" spans="1:6">
+    <row r="60" spans="1:6" ht="25.5">
       <c r="A60" t="s">
         <v>232</v>
+      </c>
+      <c r="B60" s="18" t="s">
+        <v>90</v>
+      </c>
+      <c r="C60" t="s">
+        <v>126</v>
+      </c>
+      <c r="D60" s="20" t="s">
+        <v>493</v>
+      </c>
+      <c r="E60" s="20" t="s">
+        <v>492</v>
+      </c>
+      <c r="F60" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="61" spans="1:6">
       <c r="A61" t="s">
         <v>233</v>
       </c>
-    </row>
-    <row r="62" spans="1:6">
+      <c r="B61" s="18" t="s">
+        <v>90</v>
+      </c>
+      <c r="C61" t="s">
+        <v>126</v>
+      </c>
+      <c r="D61" s="20" t="s">
+        <v>494</v>
+      </c>
+      <c r="E61" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="F61" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" ht="25.5">
       <c r="A62" t="s">
         <v>234</v>
       </c>
-    </row>
-    <row r="63" spans="1:6">
+      <c r="B62" s="18" t="s">
+        <v>94</v>
+      </c>
+      <c r="C62" s="18" t="s">
+        <v>297</v>
+      </c>
+      <c r="D62" s="20" t="s">
+        <v>511</v>
+      </c>
+      <c r="E62" s="20" t="s">
+        <v>501</v>
+      </c>
+      <c r="F62" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" ht="25.5">
       <c r="A63" t="s">
+        <v>369</v>
+      </c>
+      <c r="B63" s="18" t="s">
+        <v>94</v>
+      </c>
+      <c r="C63" s="18" t="s">
+        <v>297</v>
+      </c>
+      <c r="D63" s="20" t="s">
+        <v>512</v>
+      </c>
+      <c r="E63" s="20" t="s">
+        <v>502</v>
+      </c>
+      <c r="F63" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" ht="25.5">
+      <c r="A64" t="s">
         <v>370</v>
       </c>
-    </row>
-    <row r="64" spans="1:6">
-      <c r="A64" t="s">
+      <c r="B64" s="18" t="s">
+        <v>94</v>
+      </c>
+      <c r="C64" s="18" t="s">
+        <v>297</v>
+      </c>
+      <c r="D64" s="20" t="s">
+        <v>513</v>
+      </c>
+      <c r="E64" s="20" t="s">
+        <v>503</v>
+      </c>
+      <c r="F64" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" ht="25.5">
+      <c r="A65" t="s">
         <v>371</v>
       </c>
-    </row>
-    <row r="65" spans="1:1">
-      <c r="A65" t="s">
+      <c r="B65" s="18" t="s">
+        <v>94</v>
+      </c>
+      <c r="C65" s="18" t="s">
+        <v>297</v>
+      </c>
+      <c r="D65" s="20" t="s">
+        <v>514</v>
+      </c>
+      <c r="E65" s="20" t="s">
+        <v>504</v>
+      </c>
+      <c r="F65" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6">
+      <c r="A66" t="s">
         <v>372</v>
       </c>
-    </row>
-    <row r="66" spans="1:1">
-      <c r="A66" t="s">
+      <c r="B66" s="18" t="s">
+        <v>94</v>
+      </c>
+      <c r="C66" s="18" t="s">
+        <v>297</v>
+      </c>
+      <c r="D66" s="20" t="s">
+        <v>515</v>
+      </c>
+      <c r="E66" s="20" t="s">
+        <v>505</v>
+      </c>
+      <c r="F66" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6">
+      <c r="A67" t="s">
         <v>373</v>
       </c>
-    </row>
-    <row r="67" spans="1:1">
-      <c r="A67" t="s">
+      <c r="B67" s="18" t="s">
+        <v>94</v>
+      </c>
+      <c r="C67" s="18" t="s">
+        <v>297</v>
+      </c>
+      <c r="D67" s="20" t="s">
+        <v>516</v>
+      </c>
+      <c r="E67" s="20" t="s">
+        <v>506</v>
+      </c>
+      <c r="F67" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6">
+      <c r="A68" t="s">
         <v>374</v>
       </c>
-    </row>
-    <row r="68" spans="1:1">
-      <c r="A68" t="s">
+      <c r="B68" s="18" t="s">
+        <v>94</v>
+      </c>
+      <c r="C68" s="18" t="s">
+        <v>297</v>
+      </c>
+      <c r="D68" s="20" t="s">
+        <v>517</v>
+      </c>
+      <c r="E68" s="20" t="s">
+        <v>507</v>
+      </c>
+      <c r="F68" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6" ht="25.5">
+      <c r="A69" t="s">
         <v>375</v>
       </c>
-    </row>
-    <row r="69" spans="1:1">
-      <c r="A69" t="s">
+      <c r="B69" s="18" t="s">
+        <v>94</v>
+      </c>
+      <c r="C69" s="18" t="s">
+        <v>297</v>
+      </c>
+      <c r="D69" s="20" t="s">
+        <v>518</v>
+      </c>
+      <c r="E69" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="F69" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6">
+      <c r="A70" t="s">
         <v>376</v>
       </c>
-    </row>
-    <row r="70" spans="1:1">
-      <c r="A70" t="s">
+      <c r="B70" s="18" t="s">
+        <v>94</v>
+      </c>
+      <c r="C70" s="18" t="s">
+        <v>297</v>
+      </c>
+      <c r="D70" s="20" t="s">
+        <v>519</v>
+      </c>
+      <c r="E70" s="20" t="s">
+        <v>508</v>
+      </c>
+      <c r="F70" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6" ht="25.5">
+      <c r="A71" t="s">
         <v>377</v>
       </c>
-    </row>
-    <row r="71" spans="1:1">
-      <c r="A71" t="s">
+      <c r="B71" s="18" t="s">
+        <v>94</v>
+      </c>
+      <c r="C71" s="18" t="s">
+        <v>297</v>
+      </c>
+      <c r="D71" s="20" t="s">
+        <v>520</v>
+      </c>
+      <c r="E71" s="20" t="s">
+        <v>509</v>
+      </c>
+      <c r="F71" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="72" spans="1:6" ht="25.5">
+      <c r="A72" t="s">
         <v>378</v>
       </c>
-    </row>
-    <row r="72" spans="1:1">
-      <c r="A72" t="s">
+      <c r="B72" s="18" t="s">
+        <v>94</v>
+      </c>
+      <c r="C72" s="18" t="s">
+        <v>297</v>
+      </c>
+      <c r="D72" s="20" t="s">
+        <v>521</v>
+      </c>
+      <c r="E72" s="20" t="s">
+        <v>510</v>
+      </c>
+      <c r="F72" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="73" spans="1:6" ht="25.5">
+      <c r="A73" t="s">
         <v>379</v>
       </c>
-    </row>
-    <row r="73" spans="1:1">
-      <c r="A73" t="s">
+      <c r="B73" s="18" t="s">
+        <v>94</v>
+      </c>
+      <c r="C73" s="18" t="s">
+        <v>297</v>
+      </c>
+      <c r="D73" s="20" t="s">
+        <v>522</v>
+      </c>
+      <c r="E73" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="F73" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="74" spans="1:6">
+      <c r="A74" t="s">
         <v>380</v>
       </c>
     </row>
-    <row r="74" spans="1:1">
-      <c r="A74" t="s">
+    <row r="75" spans="1:6">
+      <c r="A75" t="s">
         <v>381</v>
       </c>
     </row>
-    <row r="75" spans="1:1">
-      <c r="A75" t="s">
+    <row r="76" spans="1:6">
+      <c r="A76" t="s">
         <v>382</v>
       </c>
     </row>
-    <row r="76" spans="1:1">
-      <c r="A76" t="s">
+    <row r="77" spans="1:6">
+      <c r="A77" t="s">
         <v>383</v>
-      </c>
-    </row>
-    <row r="77" spans="1:1">
-      <c r="A77" t="s">
-        <v>384</v>
       </c>
     </row>
   </sheetData>
@@ -5891,23 +6260,23 @@
     </row>
     <row r="37" spans="2:10">
       <c r="B37" s="1" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
     </row>
     <row r="38" spans="2:10" ht="25.5">
       <c r="B38" s="1" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
     </row>
     <row r="39" spans="2:10" ht="38.25">
       <c r="B39" s="1" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="J39" s="7"/>
     </row>
     <row r="40" spans="2:10" ht="25.5">
       <c r="B40" s="1" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
     </row>
     <row r="41" spans="2:10">
@@ -5986,7 +6355,7 @@
         <v>107</v>
       </c>
       <c r="C2" s="18" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="D2" t="s">
         <v>128</v>
@@ -6012,10 +6381,10 @@
     </row>
     <row r="4" spans="1:10" ht="25.5">
       <c r="A4" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="C4" s="1"/>
       <c r="D4" t="s">
@@ -6024,10 +6393,10 @@
     </row>
     <row r="5" spans="1:10" ht="25.5">
       <c r="A5" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="C5" s="1"/>
       <c r="D5" t="s">
@@ -6036,10 +6405,10 @@
     </row>
     <row r="6" spans="1:10" ht="25.5">
       <c r="A6" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="C6" s="1"/>
       <c r="D6" t="s">
@@ -6058,7 +6427,7 @@
         <v>114</v>
       </c>
       <c r="C8" s="18" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="D8" t="s">
         <v>128</v>
@@ -6084,10 +6453,10 @@
     </row>
     <row r="10" spans="1:10" ht="25.5">
       <c r="A10" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="C10" s="1"/>
       <c r="D10" t="s">
@@ -6096,10 +6465,10 @@
     </row>
     <row r="11" spans="1:10">
       <c r="A11" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="C11" s="1"/>
       <c r="D11" t="s">
@@ -6108,10 +6477,10 @@
     </row>
     <row r="12" spans="1:10" ht="38.25">
       <c r="A12" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="C12" s="1"/>
       <c r="D12" t="s">
@@ -6126,13 +6495,13 @@
         <v>108</v>
       </c>
       <c r="C14" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="D14" t="s">
         <v>187</v>
       </c>
       <c r="E14" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="F14">
         <v>50</v>
@@ -6152,10 +6521,10 @@
     </row>
     <row r="15" spans="1:10" ht="25.5">
       <c r="A15" t="s">
+        <v>321</v>
+      </c>
+      <c r="B15" s="1" t="s">
         <v>322</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>323</v>
       </c>
       <c r="D15" t="s">
         <v>187</v>
@@ -6163,10 +6532,10 @@
     </row>
     <row r="16" spans="1:10" ht="25.5">
       <c r="A16" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="D16" t="s">
         <v>187</v>
@@ -6174,10 +6543,10 @@
     </row>
     <row r="17" spans="1:10">
       <c r="A17" t="s">
+        <v>324</v>
+      </c>
+      <c r="B17" s="1" t="s">
         <v>325</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>326</v>
       </c>
       <c r="D17" t="s">
         <v>187</v>
@@ -6185,10 +6554,10 @@
     </row>
     <row r="18" spans="1:10" ht="38.25">
       <c r="A18" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="D18" t="s">
         <v>187</v>
@@ -6206,13 +6575,13 @@
         <v>33</v>
       </c>
       <c r="C20" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="D20" t="s">
         <v>187</v>
       </c>
       <c r="E20" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="F20">
         <v>30</v>
@@ -6232,10 +6601,10 @@
     </row>
     <row r="21" spans="1:10" ht="25.5">
       <c r="A21" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="D21" t="s">
         <v>187</v>
@@ -6243,10 +6612,10 @@
     </row>
     <row r="22" spans="1:10" ht="38.25">
       <c r="A22" t="s">
+        <v>331</v>
+      </c>
+      <c r="B22" s="1" t="s">
         <v>332</v>
-      </c>
-      <c r="B22" s="1" t="s">
-        <v>333</v>
       </c>
       <c r="D22" t="s">
         <v>187</v>
@@ -6254,10 +6623,10 @@
     </row>
     <row r="23" spans="1:10" ht="25.5">
       <c r="A23" t="s">
+        <v>333</v>
+      </c>
+      <c r="B23" s="1" t="s">
         <v>334</v>
-      </c>
-      <c r="B23" s="1" t="s">
-        <v>335</v>
       </c>
       <c r="D23" t="s">
         <v>187</v>
@@ -6265,10 +6634,10 @@
     </row>
     <row r="24" spans="1:10" ht="25.5">
       <c r="A24" t="s">
+        <v>335</v>
+      </c>
+      <c r="B24" s="1" t="s">
         <v>336</v>
-      </c>
-      <c r="B24" s="1" t="s">
-        <v>337</v>
       </c>
       <c r="D24" t="s">
         <v>187</v>
@@ -6276,10 +6645,10 @@
     </row>
     <row r="25" spans="1:10" ht="25.5">
       <c r="A25" t="s">
+        <v>337</v>
+      </c>
+      <c r="B25" s="1" t="s">
         <v>338</v>
-      </c>
-      <c r="B25" s="1" t="s">
-        <v>339</v>
       </c>
       <c r="D25" t="s">
         <v>187</v>
@@ -6293,13 +6662,13 @@
         <v>99</v>
       </c>
       <c r="C27" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="D27" t="s">
         <v>254</v>
       </c>
       <c r="E27" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="F27">
         <v>30</v>
@@ -6319,37 +6688,37 @@
     </row>
     <row r="28" spans="1:10" ht="25.5">
       <c r="A28" t="s">
+        <v>384</v>
+      </c>
+      <c r="B28" s="1" t="s">
         <v>385</v>
-      </c>
-      <c r="B28" s="1" t="s">
-        <v>386</v>
       </c>
       <c r="J28" s="16"/>
     </row>
     <row r="29" spans="1:10" ht="38.25">
       <c r="A29" t="s">
+        <v>386</v>
+      </c>
+      <c r="B29" s="1" t="s">
         <v>387</v>
-      </c>
-      <c r="B29" s="1" t="s">
-        <v>388</v>
       </c>
       <c r="J29" s="16"/>
     </row>
     <row r="30" spans="1:10" ht="25.5">
       <c r="A30" t="s">
+        <v>388</v>
+      </c>
+      <c r="B30" s="1" t="s">
         <v>389</v>
-      </c>
-      <c r="B30" s="1" t="s">
-        <v>390</v>
       </c>
       <c r="J30" s="16"/>
     </row>
     <row r="31" spans="1:10" ht="25.5">
       <c r="A31" t="s">
+        <v>390</v>
+      </c>
+      <c r="B31" s="1" t="s">
         <v>391</v>
-      </c>
-      <c r="B31" s="1" t="s">
-        <v>392</v>
       </c>
       <c r="J31" s="16"/>
     </row>
@@ -6361,13 +6730,13 @@
         <v>100</v>
       </c>
       <c r="C32" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="D32" t="s">
         <v>254</v>
       </c>
       <c r="E32" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="F32">
         <v>30</v>
@@ -6387,26 +6756,26 @@
     </row>
     <row r="33" spans="1:2" ht="25.5">
       <c r="A33" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
     </row>
     <row r="34" spans="1:2" ht="51">
       <c r="A34" t="s">
+        <v>393</v>
+      </c>
+      <c r="B34" s="1" t="s">
         <v>394</v>
-      </c>
-      <c r="B34" s="1" t="s">
-        <v>395</v>
       </c>
     </row>
     <row r="35" spans="1:2" ht="25.5">
       <c r="A35" t="s">
+        <v>395</v>
+      </c>
+      <c r="B35" s="1" t="s">
         <v>396</v>
-      </c>
-      <c r="B35" s="1" t="s">
-        <v>397</v>
       </c>
     </row>
     <row r="37" spans="1:2">
@@ -6424,17 +6793,17 @@
     </row>
     <row r="40" spans="1:2">
       <c r="B40" s="1" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
     </row>
     <row r="41" spans="1:2" ht="25.5">
       <c r="B41" s="1" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
     </row>
     <row r="42" spans="1:2" ht="51">
       <c r="B42" s="1" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
     </row>
     <row r="43" spans="1:2">
@@ -6466,8 +6835,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:J48"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" zoomScale="150" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+    <sheetView zoomScale="150" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75"/>
@@ -6515,13 +6884,13 @@
         <v>101</v>
       </c>
       <c r="C2" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="D2" s="18" t="s">
         <v>128</v>
       </c>
       <c r="E2" s="18" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="F2">
         <v>70</v>
@@ -6541,10 +6910,10 @@
     </row>
     <row r="4" spans="1:10" ht="25.5">
       <c r="A4" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="C4" s="1"/>
       <c r="D4" t="s">
@@ -6553,10 +6922,10 @@
     </row>
     <row r="5" spans="1:10" ht="38.25">
       <c r="A5" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="C5" s="1"/>
       <c r="D5" t="s">
@@ -6565,10 +6934,10 @@
     </row>
     <row r="6" spans="1:10" ht="38.25">
       <c r="A6" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="C6" s="1"/>
       <c r="D6" t="s">
@@ -6577,10 +6946,10 @@
     </row>
     <row r="7" spans="1:10" ht="38.25">
       <c r="A7" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="C7" s="1"/>
       <c r="D7" t="s">
@@ -6589,18 +6958,18 @@
     </row>
     <row r="8" spans="1:10" ht="25.5">
       <c r="A8" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
     </row>
     <row r="9" spans="1:10" ht="51">
       <c r="A9" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="C9" s="1"/>
       <c r="D9" t="s">
@@ -6609,10 +6978,10 @@
     </row>
     <row r="10" spans="1:10" ht="38.25">
       <c r="A10" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="C10" s="1"/>
       <c r="D10" t="s">
@@ -6627,13 +6996,13 @@
         <v>295</v>
       </c>
       <c r="C12" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="D12" s="18" t="s">
         <v>128</v>
       </c>
       <c r="E12" s="18" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="F12">
         <v>50</v>
@@ -6653,10 +7022,10 @@
     </row>
     <row r="14" spans="1:10" ht="25.5">
       <c r="A14" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="C14" s="1"/>
       <c r="D14" t="s">
@@ -6665,10 +7034,10 @@
     </row>
     <row r="15" spans="1:10" ht="38.25">
       <c r="A15" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="C15" s="1"/>
       <c r="D15" t="s">
@@ -6677,10 +7046,10 @@
     </row>
     <row r="16" spans="1:10" ht="38.25">
       <c r="A16" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="C16" s="1"/>
       <c r="D16" t="s">
@@ -6699,13 +7068,13 @@
         <v>110</v>
       </c>
       <c r="C18" s="18" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="D18" s="18" t="s">
         <v>70</v>
       </c>
       <c r="E18" s="18" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="F18">
         <v>100</v>
@@ -6725,10 +7094,10 @@
     </row>
     <row r="19" spans="1:10">
       <c r="A19" t="s">
+        <v>457</v>
+      </c>
+      <c r="B19" s="1" t="s">
         <v>458</v>
-      </c>
-      <c r="B19" s="1" t="s">
-        <v>459</v>
       </c>
       <c r="D19" s="18" t="s">
         <v>70</v>
@@ -6736,10 +7105,10 @@
     </row>
     <row r="20" spans="1:10" ht="25.5">
       <c r="A20" t="s">
+        <v>459</v>
+      </c>
+      <c r="B20" s="1" t="s">
         <v>460</v>
-      </c>
-      <c r="B20" s="1" t="s">
-        <v>461</v>
       </c>
       <c r="D20" s="18" t="s">
         <v>70</v>
@@ -6747,10 +7116,10 @@
     </row>
     <row r="21" spans="1:10" ht="38.25">
       <c r="A21" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="D21" s="18" t="s">
         <v>70</v>
@@ -6758,10 +7127,10 @@
     </row>
     <row r="22" spans="1:10" ht="51">
       <c r="A22" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="D22" s="18" t="s">
         <v>70</v>
@@ -6769,10 +7138,10 @@
     </row>
     <row r="23" spans="1:10" ht="25.5">
       <c r="A23" t="s">
+        <v>465</v>
+      </c>
+      <c r="B23" s="1" t="s">
         <v>466</v>
-      </c>
-      <c r="B23" s="1" t="s">
-        <v>467</v>
       </c>
       <c r="D23" s="18" t="s">
         <v>70</v>
@@ -6789,13 +7158,13 @@
         <v>111</v>
       </c>
       <c r="C25" s="18" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="D25" s="18" t="s">
         <v>70</v>
       </c>
       <c r="E25" s="18" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="F25">
         <v>30</v>
@@ -6815,10 +7184,10 @@
     </row>
     <row r="26" spans="1:10" ht="25.5">
       <c r="A26" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="D26" s="18" t="s">
         <v>70</v>
@@ -6826,10 +7195,10 @@
     </row>
     <row r="27" spans="1:10" ht="25.5">
       <c r="A27" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="D27" s="18" t="s">
         <v>70</v>
@@ -6837,10 +7206,10 @@
     </row>
     <row r="28" spans="1:10" ht="25.5">
       <c r="A28" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="D28" s="18" t="s">
         <v>70</v>
@@ -6848,10 +7217,10 @@
     </row>
     <row r="29" spans="1:10" ht="51">
       <c r="A29" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="D29" s="18" t="s">
         <v>70</v>
@@ -6859,10 +7228,10 @@
     </row>
     <row r="30" spans="1:10" ht="51">
       <c r="A30" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="D30" s="18" t="s">
         <v>70</v>
@@ -6879,13 +7248,13 @@
         <v>117</v>
       </c>
       <c r="C32" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="D32" s="18" t="s">
         <v>254</v>
       </c>
       <c r="E32" s="18" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="F32">
         <v>20</v>
@@ -6905,18 +7274,18 @@
     </row>
     <row r="33" spans="1:10">
       <c r="A33" t="s">
+        <v>477</v>
+      </c>
+      <c r="B33" s="1" t="s">
         <v>478</v>
-      </c>
-      <c r="B33" s="1" t="s">
-        <v>479</v>
       </c>
     </row>
     <row r="34" spans="1:10" ht="38.25">
       <c r="A34" t="s">
+        <v>479</v>
+      </c>
+      <c r="B34" s="1" t="s">
         <v>480</v>
-      </c>
-      <c r="B34" s="1" t="s">
-        <v>481</v>
       </c>
     </row>
     <row r="36" spans="1:10">
@@ -6927,13 +7296,13 @@
         <v>119</v>
       </c>
       <c r="C36" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="D36" s="18" t="s">
         <v>254</v>
       </c>
       <c r="E36" s="18" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="F36">
         <v>50</v>
@@ -6953,26 +7322,26 @@
     </row>
     <row r="37" spans="1:10">
       <c r="A37" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="B37" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
     </row>
     <row r="38" spans="1:10">
       <c r="A38" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="B38" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
     </row>
     <row r="39" spans="1:10">
       <c r="A39" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="B39" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
     </row>
     <row r="41" spans="1:10">
@@ -6990,17 +7359,17 @@
     </row>
     <row r="44" spans="1:10">
       <c r="B44" s="1" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
     </row>
     <row r="45" spans="1:10" ht="25.5">
       <c r="B45" s="1" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
     </row>
     <row r="46" spans="1:10" ht="51">
       <c r="B46" s="1" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
     </row>
     <row r="47" spans="1:10">
@@ -7026,10 +7395,10 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J7"/>
+  <dimension ref="A1:J19"/>
   <sheetViews>
-    <sheetView zoomScale="150" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+    <sheetView topLeftCell="A4" zoomScale="150" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13:J13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75"/>
@@ -7086,89 +7455,200 @@
         <v>25</v>
       </c>
     </row>
-    <row r="3" spans="1:10">
-      <c r="A3" t="s">
-        <v>90</v>
-      </c>
-      <c r="B3" t="s">
-        <v>126</v>
-      </c>
-      <c r="D3" t="s">
-        <v>128</v>
-      </c>
-      <c r="F3">
-        <v>75</v>
-      </c>
-      <c r="G3">
-        <v>30</v>
-      </c>
-    </row>
     <row r="4" spans="1:10">
       <c r="A4" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B4" t="s">
-        <v>127</v>
+        <v>126</v>
+      </c>
+      <c r="C4" s="18" t="s">
+        <v>495</v>
       </c>
       <c r="D4" t="s">
-        <v>70</v>
+        <v>128</v>
+      </c>
+      <c r="E4" s="18" t="s">
+        <v>329</v>
       </c>
       <c r="F4">
-        <v>100</v>
+        <v>75</v>
       </c>
       <c r="G4">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10">
-      <c r="A5" t="s">
-        <v>92</v>
-      </c>
-      <c r="B5" s="18" t="s">
-        <v>261</v>
-      </c>
-      <c r="D5" t="s">
-        <v>70</v>
-      </c>
-      <c r="F5">
-        <v>70</v>
-      </c>
-      <c r="G5">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10">
-      <c r="A6" t="s">
-        <v>93</v>
-      </c>
-      <c r="B6" s="18" t="s">
-        <v>293</v>
+        <v>30</v>
+      </c>
+      <c r="H4">
+        <v>15</v>
+      </c>
+      <c r="I4">
+        <v>30</v>
+      </c>
+      <c r="J4" s="16">
+        <v>40638</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" ht="25.5">
+      <c r="A6" s="18" t="s">
+        <v>496</v>
+      </c>
+      <c r="B6" s="20" t="s">
+        <v>498</v>
       </c>
       <c r="D6" t="s">
-        <v>254</v>
-      </c>
-      <c r="F6">
-        <v>75</v>
-      </c>
-      <c r="G6">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10">
-      <c r="A7" t="s">
-        <v>94</v>
-      </c>
-      <c r="B7" s="18" t="s">
-        <v>297</v>
+        <v>128</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" ht="25.5">
+      <c r="A7" s="18" t="s">
+        <v>497</v>
+      </c>
+      <c r="B7" s="20" t="s">
+        <v>499</v>
       </c>
       <c r="D7" t="s">
         <v>128</v>
       </c>
-      <c r="F7">
+    </row>
+    <row r="8" spans="1:10">
+      <c r="A8" s="18"/>
+      <c r="B8" s="20"/>
+    </row>
+    <row r="9" spans="1:10">
+      <c r="A9" t="s">
+        <v>91</v>
+      </c>
+      <c r="B9" t="s">
+        <v>127</v>
+      </c>
+      <c r="D9" t="s">
+        <v>70</v>
+      </c>
+      <c r="F9">
         <v>100</v>
       </c>
-      <c r="G7">
+      <c r="G9">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10">
+      <c r="A10" t="s">
+        <v>92</v>
+      </c>
+      <c r="B10" s="18" t="s">
+        <v>261</v>
+      </c>
+      <c r="D10" t="s">
+        <v>70</v>
+      </c>
+      <c r="F10">
+        <v>70</v>
+      </c>
+      <c r="G10">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10">
+      <c r="A11" t="s">
+        <v>93</v>
+      </c>
+      <c r="B11" s="18" t="s">
+        <v>293</v>
+      </c>
+      <c r="D11" t="s">
+        <v>254</v>
+      </c>
+      <c r="F11">
+        <v>75</v>
+      </c>
+      <c r="G11">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10">
+      <c r="A13" t="s">
+        <v>94</v>
+      </c>
+      <c r="B13" s="18" t="s">
+        <v>297</v>
+      </c>
+      <c r="C13" s="18" t="s">
+        <v>523</v>
+      </c>
+      <c r="D13" t="s">
+        <v>128</v>
+      </c>
+      <c r="E13" s="18" t="s">
+        <v>329</v>
+      </c>
+      <c r="F13">
+        <v>100</v>
+      </c>
+      <c r="G13">
         <v>45</v>
+      </c>
+      <c r="H13">
+        <v>226</v>
+      </c>
+      <c r="I13">
+        <v>90</v>
+      </c>
+      <c r="J13" s="16">
+        <v>40638</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10">
+      <c r="A15" s="18" t="s">
+        <v>524</v>
+      </c>
+      <c r="B15" s="20" t="s">
+        <v>526</v>
+      </c>
+      <c r="D15" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" ht="51">
+      <c r="A16" s="18" t="s">
+        <v>525</v>
+      </c>
+      <c r="B16" s="20" t="s">
+        <v>527</v>
+      </c>
+      <c r="D16" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="63.75">
+      <c r="A17" s="18" t="s">
+        <v>529</v>
+      </c>
+      <c r="B17" s="20" t="s">
+        <v>531</v>
+      </c>
+      <c r="D17" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="51">
+      <c r="A18" s="18" t="s">
+        <v>530</v>
+      </c>
+      <c r="B18" s="20" t="s">
+        <v>528</v>
+      </c>
+      <c r="D18" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="51">
+      <c r="A19" s="18" t="s">
+        <v>532</v>
+      </c>
+      <c r="B19" s="20" t="s">
+        <v>533</v>
+      </c>
+      <c r="D19" t="s">
+        <v>128</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fix of sprint 4
</commit_message>
<xml_diff>
--- a/Team05Report.xlsx
+++ b/Team05Report.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="240" windowWidth="20730" windowHeight="11760" tabRatio="500" firstSheet="1" activeTab="8"/>
+    <workbookView xWindow="240" yWindow="240" windowWidth="20730" windowHeight="11760" tabRatio="500" firstSheet="1" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Team" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
     <sheet name="Sprint4" sheetId="6" r:id="rId9"/>
     <sheet name="Sprint5" sheetId="8" r:id="rId10"/>
   </sheets>
-  <calcPr calcId="145621" concurrentCalc="0"/>
+  <calcPr calcId="125725" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -1167,9 +1167,6 @@
     <t>The children should have the same last name as their father</t>
   </si>
   <si>
-    <t>There should be no more than 4 children that are born on the same day</t>
-  </si>
-  <si>
     <t>All the individuals should be born after the year of 1900. We do not record ancient people</t>
   </si>
   <si>
@@ -1727,173 +1724,176 @@
     <t xml:space="preserve">  If threr is no divorce date continue to the next family</t>
   </si>
   <si>
-    <t>Individual I10 cannot give birth, her birth date is 1 NOV 1935</t>
-  </si>
-  <si>
-    <t xml:space="preserve">I10(Jen /Brown/) is not in pregnancy age limit. Her present age is 95
+    <t>Individaul I9 is in pregnency age, Her birth date is 1991</t>
+  </si>
+  <si>
+    <t>Family F3 divorce Date is(31 DEC 1972) and child's birth Date is (27 JAN 1974).</t>
+  </si>
+  <si>
+    <t>In family F3, Divorce date is 31 DEC 1972, Child birth date is  27 JAN 1974, born after Divorce</t>
+  </si>
+  <si>
+    <t>In Family F5, Divorce date is 5 JAN 2014, Child birth date is 6 JUN 2011, Born before divorce</t>
+  </si>
+  <si>
+    <t>AT73~74</t>
+  </si>
+  <si>
+    <t>AT75~76</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Individual I1 has more than one name tag: Jacky /Mao/, Jackie /Mao/. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Individual I1 has more than one sex tag: F, M. </t>
+  </si>
+  <si>
+    <t>Individual I1 has more than one birthday tag: 27 JAN 1960, 27 JAN 1970.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Individual I1 has more than one death date tag: 1 JAN 2014, 1 FEB 2014. </t>
+  </si>
+  <si>
+    <t>Individual I2 does not have a name tag.</t>
+  </si>
+  <si>
+    <t>Individual I2 does not have a sex tag.</t>
+  </si>
+  <si>
+    <t>Individual I2 does not have a birthday tag.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Family F4 does not have a marriage date tag. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Family F5 has more than one marriage date tag: 2 JAN 2000, 1 JAN 2000. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Family F5 has more than one divorce date tag: 5 JAN 2014, 5 JAN 2014. </t>
+  </si>
+  <si>
+    <t>T21.01</t>
+  </si>
+  <si>
+    <t>get access to each individual record</t>
+  </si>
+  <si>
+    <t>T21.02</t>
+  </si>
+  <si>
+    <t>read every individual's famc and fams record</t>
+  </si>
+  <si>
+    <t>T21.03</t>
+  </si>
+  <si>
+    <t>if an individual doesn't have a famc nor a fams record, then he/she doesn't belong to any family</t>
+  </si>
+  <si>
+    <t>T22.01</t>
+  </si>
+  <si>
+    <t>T22.02</t>
+  </si>
+  <si>
+    <t>if an individual's name, sex or birthday record is null, then he/she doesn't complete his/her information</t>
+  </si>
+  <si>
+    <t>T22.03</t>
+  </si>
+  <si>
+    <t>T22.04</t>
+  </si>
+  <si>
+    <t>if a family doesn't have a marriage record, then this family doesn't complete its information</t>
+  </si>
+  <si>
+    <t>AT77</t>
+  </si>
+  <si>
+    <t>AT78</t>
+  </si>
+  <si>
+    <t>AT79</t>
+  </si>
+  <si>
+    <t>AT80</t>
+  </si>
+  <si>
+    <t>AT81</t>
+  </si>
+  <si>
+    <t>AT82</t>
+  </si>
+  <si>
+    <t>AT83</t>
+  </si>
+  <si>
+    <t>AT84</t>
+  </si>
+  <si>
+    <t>AT85</t>
+  </si>
+  <si>
+    <t>Individual I11(James /Brown/) doesn't have a fams nor a famc record</t>
+  </si>
+  <si>
+    <t>Individual I11 (James /Brown/) doesn't belong to any family.</t>
+  </si>
+  <si>
+    <t>Individual I12(Grace /Li/) is a wife in family F1, she has a fams record</t>
+  </si>
+  <si>
+    <t>Individual I2 doesn't complete information(missing name).</t>
+  </si>
+  <si>
+    <t>Individual I2 doesn't have a name tag nor a name</t>
+  </si>
+  <si>
+    <t>Individual I6 has a name tag but doesn't have a name record</t>
+  </si>
+  <si>
+    <t>Individual I6 doesn't complete information(missing name).</t>
+  </si>
+  <si>
+    <t>Individual I7 (Chris /Taylor/)  doesn't complete information(missing gender).</t>
+  </si>
+  <si>
+    <t>Individual I7 has a sex tag but doesn't have a gender record</t>
+  </si>
+  <si>
+    <t>Individual I8 has a birt tag but doesn't have a birthday record</t>
+  </si>
+  <si>
+    <t>Individual I8 (Kevin /Brown/)  doesn't complete information(missing birth date).</t>
+  </si>
+  <si>
+    <t>Individual I9 complete the information of name, sex and birthday</t>
+  </si>
+  <si>
+    <t>Family F4 doesn't complete information(missing marriage date).</t>
+  </si>
+  <si>
+    <t>family F4 has a marr tag but doesn't have a marriage date record</t>
+  </si>
+  <si>
+    <t>family F1 complete the information of marriage date</t>
+  </si>
+  <si>
+    <t>AT77~78</t>
+  </si>
+  <si>
+    <t>AT79~85</t>
+  </si>
+  <si>
+    <t>There should be no more than 4 children that are born on the same day in one family</t>
+  </si>
+  <si>
+    <t xml:space="preserve">In Family F4, wife I9(Elena /Wilson/) gave birth to child I3(Katie /Brown/) when she was 9(not between 18 and 50)
 </t>
   </si>
   <si>
-    <t>Individaul I9 is in pregnency age, Her birth date is 1991</t>
-  </si>
-  <si>
-    <t>Family F3 divorce Date is(31 DEC 1972) and child's birth Date is (27 JAN 1974).</t>
-  </si>
-  <si>
-    <t>In family F3, Divorce date is 31 DEC 1972, Child birth date is  27 JAN 1974, born after Divorce</t>
-  </si>
-  <si>
-    <t>In Family F5, Divorce date is 5 JAN 2014, Child birth date is 6 JUN 2011, Born before divorce</t>
-  </si>
-  <si>
-    <t>AT73~74</t>
-  </si>
-  <si>
-    <t>AT75~76</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Individual I1 has more than one name tag: Jacky /Mao/, Jackie /Mao/. </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Individual I1 has more than one sex tag: F, M. </t>
-  </si>
-  <si>
-    <t>Individual I1 has more than one birthday tag: 27 JAN 1960, 27 JAN 1970.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Individual I1 has more than one death date tag: 1 JAN 2014, 1 FEB 2014. </t>
-  </si>
-  <si>
-    <t>Individual I2 does not have a name tag.</t>
-  </si>
-  <si>
-    <t>Individual I2 does not have a sex tag.</t>
-  </si>
-  <si>
-    <t>Individual I2 does not have a birthday tag.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Family F4 does not have a marriage date tag. </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Family F5 has more than one marriage date tag: 2 JAN 2000, 1 JAN 2000. </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Family F5 has more than one divorce date tag: 5 JAN 2014, 5 JAN 2014. </t>
-  </si>
-  <si>
-    <t>T21.01</t>
-  </si>
-  <si>
-    <t>get access to each individual record</t>
-  </si>
-  <si>
-    <t>T21.02</t>
-  </si>
-  <si>
-    <t>read every individual's famc and fams record</t>
-  </si>
-  <si>
-    <t>T21.03</t>
-  </si>
-  <si>
-    <t>if an individual doesn't have a famc nor a fams record, then he/she doesn't belong to any family</t>
-  </si>
-  <si>
-    <t>T22.01</t>
-  </si>
-  <si>
-    <t>T22.02</t>
-  </si>
-  <si>
-    <t>if an individual's name, sex or birthday record is null, then he/she doesn't complete his/her information</t>
-  </si>
-  <si>
-    <t>T22.03</t>
-  </si>
-  <si>
-    <t>T22.04</t>
-  </si>
-  <si>
-    <t>if a family doesn't have a marriage record, then this family doesn't complete its information</t>
-  </si>
-  <si>
-    <t>AT77</t>
-  </si>
-  <si>
-    <t>AT78</t>
-  </si>
-  <si>
-    <t>AT79</t>
-  </si>
-  <si>
-    <t>AT80</t>
-  </si>
-  <si>
-    <t>AT81</t>
-  </si>
-  <si>
-    <t>AT82</t>
-  </si>
-  <si>
-    <t>AT83</t>
-  </si>
-  <si>
-    <t>AT84</t>
-  </si>
-  <si>
-    <t>AT85</t>
-  </si>
-  <si>
-    <t>Individual I11(James /Brown/) doesn't have a fams nor a famc record</t>
-  </si>
-  <si>
-    <t>Individual I11 (James /Brown/) doesn't belong to any family.</t>
-  </si>
-  <si>
-    <t>Individual I12(Grace /Li/) is a wife in family F1, she has a fams record</t>
-  </si>
-  <si>
-    <t>Individual I2 doesn't complete information(missing name).</t>
-  </si>
-  <si>
-    <t>Individual I2 doesn't have a name tag nor a name</t>
-  </si>
-  <si>
-    <t>Individual I6 has a name tag but doesn't have a name record</t>
-  </si>
-  <si>
-    <t>Individual I6 doesn't complete information(missing name).</t>
-  </si>
-  <si>
-    <t>Individual I7 (Chris /Taylor/)  doesn't complete information(missing gender).</t>
-  </si>
-  <si>
-    <t>Individual I7 has a sex tag but doesn't have a gender record</t>
-  </si>
-  <si>
-    <t>Individual I8 has a birt tag but doesn't have a birthday record</t>
-  </si>
-  <si>
-    <t>Individual I8 (Kevin /Brown/)  doesn't complete information(missing birth date).</t>
-  </si>
-  <si>
-    <t>Individual I9 complete the information of name, sex and birthday</t>
-  </si>
-  <si>
-    <t>Family F4 doesn't complete information(missing marriage date).</t>
-  </si>
-  <si>
-    <t>family F4 has a marr tag but doesn't have a marriage date record</t>
-  </si>
-  <si>
-    <t>family F1 complete the information of marriage date</t>
-  </si>
-  <si>
-    <t>AT77~78</t>
-  </si>
-  <si>
-    <t>AT79~85</t>
+    <t>In Family F4, wife I9(Elena /Wilson/) was born on 1 NOV 1941 while child I3(Katie /Brown/) was born on 14 FEB 1950</t>
   </si>
 </sst>
 </file>
@@ -2199,27 +2199,26 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:dLbls/>
         <c:marker val="1"/>
-        <c:axId val="348155904"/>
-        <c:axId val="348157440"/>
+        <c:axId val="226254848"/>
+        <c:axId val="226256384"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="348155904"/>
+        <c:axId val="226254848"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="m/d" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="348157440"/>
+        <c:crossAx val="226256384"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
         <c:baseTimeUnit val="days"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="348157440"/>
+        <c:axId val="226256384"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2227,7 +2226,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="348155904"/>
+        <c:crossAx val="226254848"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2237,7 +2236,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="1" l="0.75000000000000289" r="0.75000000000000289" t="1" header="0.5" footer="0.5"/>
+    <c:pageMargins b="1" l="0.750000000000003" r="0.750000000000003" t="1" header="0.5" footer="0.5"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -2810,7 +2809,7 @@
         <v>342</v>
       </c>
       <c r="B5" s="18" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="D5" s="18" t="s">
         <v>254</v>
@@ -2827,7 +2826,7 @@
         <v>343</v>
       </c>
       <c r="B6" s="18" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="D6" s="18" t="s">
         <v>70</v>
@@ -2844,7 +2843,7 @@
         <v>344</v>
       </c>
       <c r="B7" s="18" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="D7" s="18" t="s">
         <v>70</v>
@@ -3244,7 +3243,7 @@
         <v>108</v>
       </c>
       <c r="D10" s="18" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="E10" t="s">
         <v>187</v>
@@ -3282,7 +3281,7 @@
         <v>33</v>
       </c>
       <c r="D11" s="18" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="E11" t="s">
         <v>187</v>
@@ -3320,7 +3319,7 @@
         <v>99</v>
       </c>
       <c r="D12" s="18" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="E12" t="s">
         <v>254</v>
@@ -3358,7 +3357,7 @@
         <v>100</v>
       </c>
       <c r="D13" s="18" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="E13" t="s">
         <v>254</v>
@@ -3396,7 +3395,7 @@
         <v>101</v>
       </c>
       <c r="D14" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="E14" s="18" t="s">
         <v>128</v>
@@ -3434,7 +3433,7 @@
         <v>295</v>
       </c>
       <c r="D15" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="E15" s="18" t="s">
         <v>128</v>
@@ -3472,7 +3471,7 @@
         <v>110</v>
       </c>
       <c r="D16" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="E16" s="18" t="s">
         <v>187</v>
@@ -3510,7 +3509,7 @@
         <v>111</v>
       </c>
       <c r="D17" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="E17" s="18" t="s">
         <v>187</v>
@@ -3548,7 +3547,7 @@
         <v>117</v>
       </c>
       <c r="D18" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="E18" s="18" t="s">
         <v>254</v>
@@ -3586,7 +3585,7 @@
         <v>119</v>
       </c>
       <c r="D19" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="E19" s="18" t="s">
         <v>254</v>
@@ -3621,7 +3620,7 @@
         <v>122</v>
       </c>
       <c r="D20" t="s">
-        <v>541</v>
+        <v>538</v>
       </c>
       <c r="E20" t="s">
         <v>254</v>
@@ -3656,7 +3655,7 @@
         <v>126</v>
       </c>
       <c r="D21" s="18" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="E21" t="s">
         <v>128</v>
@@ -3691,7 +3690,7 @@
         <v>127</v>
       </c>
       <c r="D22" s="18" t="s">
-        <v>589</v>
+        <v>586</v>
       </c>
       <c r="E22" t="s">
         <v>70</v>
@@ -3726,7 +3725,7 @@
         <v>261</v>
       </c>
       <c r="D23" s="18" t="s">
-        <v>590</v>
+        <v>587</v>
       </c>
       <c r="E23" t="s">
         <v>70</v>
@@ -3761,7 +3760,7 @@
         <v>293</v>
       </c>
       <c r="D24" t="s">
-        <v>542</v>
+        <v>539</v>
       </c>
       <c r="E24" t="s">
         <v>254</v>
@@ -3796,7 +3795,7 @@
         <v>297</v>
       </c>
       <c r="D25" s="18" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="E25" t="s">
         <v>128</v>
@@ -3861,7 +3860,7 @@
         <v>342</v>
       </c>
       <c r="C29" s="18" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="L29" s="7">
         <v>40610</v>
@@ -3872,7 +3871,7 @@
         <v>343</v>
       </c>
       <c r="C30" s="18" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="L30" s="7">
         <v>40610</v>
@@ -3883,7 +3882,7 @@
         <v>344</v>
       </c>
       <c r="C31" s="18" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="L31" s="7">
         <v>40610</v>
@@ -3906,7 +3905,7 @@
   <dimension ref="A1:F31"/>
   <sheetViews>
     <sheetView topLeftCell="A14" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="D23" sqref="D23"/>
+      <selection activeCell="C33" sqref="C33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75"/>
@@ -4109,7 +4108,7 @@
         <v>109</v>
       </c>
       <c r="D10" s="18" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="E10">
         <v>50</v>
@@ -4129,7 +4128,7 @@
         <v>47</v>
       </c>
       <c r="D11" s="18" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="E11">
         <v>30</v>
@@ -4149,7 +4148,7 @@
         <v>48</v>
       </c>
       <c r="D12" s="18" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="E12">
         <v>30</v>
@@ -4169,7 +4168,7 @@
         <v>98</v>
       </c>
       <c r="D13" s="18" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="E13">
         <v>30</v>
@@ -4189,7 +4188,7 @@
         <v>138</v>
       </c>
       <c r="D14" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="E14">
         <v>70</v>
@@ -4206,10 +4205,10 @@
         <v>295</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="D15" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="E15">
         <v>50</v>
@@ -4229,7 +4228,7 @@
         <v>294</v>
       </c>
       <c r="D16" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="E16">
         <v>100</v>
@@ -4243,13 +4242,13 @@
         <v>86</v>
       </c>
       <c r="B17" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="C17" s="1" t="s">
         <v>102</v>
       </c>
       <c r="D17" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="E17">
         <v>30</v>
@@ -4269,7 +4268,7 @@
         <v>118</v>
       </c>
       <c r="D18" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="E18">
         <v>20</v>
@@ -4289,7 +4288,7 @@
         <v>120</v>
       </c>
       <c r="D19" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="E19">
         <v>50</v>
@@ -4309,7 +4308,7 @@
         <v>123</v>
       </c>
       <c r="D20" t="s">
-        <v>541</v>
+        <v>538</v>
       </c>
       <c r="E20">
         <v>50</v>
@@ -4329,7 +4328,7 @@
         <v>124</v>
       </c>
       <c r="D21" s="18" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="E21">
         <v>75</v>
@@ -4349,7 +4348,7 @@
         <v>125</v>
       </c>
       <c r="D22" s="18" t="s">
-        <v>589</v>
+        <v>586</v>
       </c>
       <c r="E22">
         <v>100</v>
@@ -4369,7 +4368,7 @@
         <v>262</v>
       </c>
       <c r="D23" s="18" t="s">
-        <v>590</v>
+        <v>587</v>
       </c>
       <c r="E23">
         <v>70</v>
@@ -4389,7 +4388,7 @@
         <v>296</v>
       </c>
       <c r="D24" t="s">
-        <v>542</v>
+        <v>539</v>
       </c>
       <c r="E24">
         <v>75</v>
@@ -4406,10 +4405,10 @@
         <v>297</v>
       </c>
       <c r="C25" s="20" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="D25" s="18" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="E25">
         <v>100</v>
@@ -4443,7 +4442,7 @@
         <v>341</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="E27">
         <v>15</v>
@@ -4452,15 +4451,15 @@
         <v>30</v>
       </c>
     </row>
-    <row r="28" spans="1:6">
+    <row r="28" spans="1:6" ht="25.5">
       <c r="A28" t="s">
         <v>340</v>
       </c>
       <c r="B28" s="18" t="s">
         <v>347</v>
       </c>
-      <c r="C28" s="1" t="s">
-        <v>349</v>
+      <c r="C28" s="20" t="s">
+        <v>588</v>
       </c>
       <c r="E28">
         <v>35</v>
@@ -4474,10 +4473,10 @@
         <v>342</v>
       </c>
       <c r="B29" s="18" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="E29">
         <v>20</v>
@@ -4491,10 +4490,10 @@
         <v>343</v>
       </c>
       <c r="B30" s="18" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="E30">
         <v>35</v>
@@ -4508,10 +4507,10 @@
         <v>344</v>
       </c>
       <c r="B31" s="18" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="E31">
         <v>30</v>
@@ -4535,8 +4534,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F100"/>
   <sheetViews>
-    <sheetView topLeftCell="A74" zoomScale="145" zoomScaleNormal="145" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="B79" sqref="B79"/>
+    <sheetView tabSelected="1" topLeftCell="A71" zoomScale="145" zoomScaleNormal="145" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="D77" sqref="D77"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75"/>
@@ -5160,10 +5159,10 @@
         <v>107</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="F31" t="s">
         <v>53</v>
@@ -5240,7 +5239,7 @@
         <v>108</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="E35" s="1" t="s">
         <v>51</v>
@@ -5260,10 +5259,10 @@
         <v>108</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="E36" s="1" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="F36" t="s">
         <v>53</v>
@@ -5280,10 +5279,10 @@
         <v>108</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="E37" s="1" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="F37" t="s">
         <v>53</v>
@@ -5300,10 +5299,10 @@
         <v>33</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="E38" s="1" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="F38" t="s">
         <v>53</v>
@@ -5320,7 +5319,7 @@
         <v>33</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="E39" s="1" t="s">
         <v>51</v>
@@ -5340,13 +5339,13 @@
         <v>99</v>
       </c>
       <c r="D40" s="1" t="s">
+        <v>396</v>
+      </c>
+      <c r="E40" s="1" t="s">
         <v>397</v>
       </c>
-      <c r="E40" s="1" t="s">
-        <v>398</v>
-      </c>
       <c r="F40" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
     </row>
     <row r="41" spans="1:6" ht="25.5">
@@ -5360,10 +5359,10 @@
         <v>99</v>
       </c>
       <c r="D41" s="1" t="s">
+        <v>398</v>
+      </c>
+      <c r="E41" s="1" t="s">
         <v>399</v>
-      </c>
-      <c r="E41" s="1" t="s">
-        <v>400</v>
       </c>
       <c r="F41" t="s">
         <v>53</v>
@@ -5380,7 +5379,7 @@
         <v>99</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="E42" s="1" t="s">
         <v>51</v>
@@ -5400,10 +5399,10 @@
         <v>100</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="E43" s="1" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="F43" t="s">
         <v>53</v>
@@ -5420,7 +5419,7 @@
         <v>100</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="E44" s="1" t="s">
         <v>51</v>
@@ -5440,10 +5439,10 @@
         <v>101</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="E45" s="1" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="F45" t="s">
         <v>53</v>
@@ -5460,10 +5459,10 @@
         <v>101</v>
       </c>
       <c r="D46" s="1" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="E46" s="1" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="F46" t="s">
         <v>53</v>
@@ -5480,7 +5479,7 @@
         <v>101</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="E47" s="1" t="s">
         <v>51</v>
@@ -5500,10 +5499,10 @@
         <v>295</v>
       </c>
       <c r="D48" s="1" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="E48" s="1" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="F48" t="s">
         <v>53</v>
@@ -5520,7 +5519,7 @@
         <v>295</v>
       </c>
       <c r="D49" s="1" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="E49" s="1" t="s">
         <v>51</v>
@@ -5540,10 +5539,10 @@
         <v>110</v>
       </c>
       <c r="D50" s="1" t="s">
+        <v>442</v>
+      </c>
+      <c r="E50" s="1" t="s">
         <v>443</v>
-      </c>
-      <c r="E50" s="1" t="s">
-        <v>444</v>
       </c>
       <c r="F50" t="s">
         <v>53</v>
@@ -5554,13 +5553,13 @@
         <v>223</v>
       </c>
       <c r="B51" s="18" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="C51" t="s">
         <v>110</v>
       </c>
       <c r="D51" s="1" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="E51" s="1" t="s">
         <v>51</v>
@@ -5577,13 +5576,13 @@
         <v>86</v>
       </c>
       <c r="C52" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="D52" s="1" t="s">
+        <v>446</v>
+      </c>
+      <c r="E52" s="1" t="s">
         <v>447</v>
-      </c>
-      <c r="E52" s="1" t="s">
-        <v>448</v>
       </c>
       <c r="F52" t="s">
         <v>53</v>
@@ -5597,13 +5596,13 @@
         <v>86</v>
       </c>
       <c r="C53" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="D53" s="1" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="E53" s="1" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="F53" t="s">
         <v>53</v>
@@ -5617,13 +5616,13 @@
         <v>86</v>
       </c>
       <c r="C54" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="D54" s="1" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="E54" s="1" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="F54" t="s">
         <v>53</v>
@@ -5637,13 +5636,13 @@
         <v>86</v>
       </c>
       <c r="C55" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="D55" s="1" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="E55" s="1" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="F55" t="s">
         <v>53</v>
@@ -5660,10 +5659,10 @@
         <v>117</v>
       </c>
       <c r="D56" s="1" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="E56" s="1" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="F56" t="s">
         <v>53</v>
@@ -5680,7 +5679,7 @@
         <v>117</v>
       </c>
       <c r="D57" s="1" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="E57" s="1" t="s">
         <v>51</v>
@@ -5700,10 +5699,10 @@
         <v>119</v>
       </c>
       <c r="D58" s="1" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="E58" s="20" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="F58" t="s">
         <v>53</v>
@@ -5720,7 +5719,7 @@
         <v>119</v>
       </c>
       <c r="D59" s="1" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="E59" s="1" t="s">
         <v>51</v>
@@ -5740,10 +5739,10 @@
         <v>126</v>
       </c>
       <c r="D60" s="20" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
       <c r="E60" s="20" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="F60" t="s">
         <v>53</v>
@@ -5760,7 +5759,7 @@
         <v>126</v>
       </c>
       <c r="D61" s="20" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="E61" s="1" t="s">
         <v>51</v>
@@ -5780,10 +5779,10 @@
         <v>297</v>
       </c>
       <c r="D62" s="20" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="E62" s="20" t="s">
-        <v>543</v>
+        <v>540</v>
       </c>
       <c r="F62" t="s">
         <v>53</v>
@@ -5791,7 +5790,7 @@
     </row>
     <row r="63" spans="1:6" ht="25.5">
       <c r="A63" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="B63" s="18" t="s">
         <v>94</v>
@@ -5800,10 +5799,10 @@
         <v>297</v>
       </c>
       <c r="D63" s="20" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="E63" s="20" t="s">
-        <v>544</v>
+        <v>541</v>
       </c>
       <c r="F63" t="s">
         <v>53</v>
@@ -5811,7 +5810,7 @@
     </row>
     <row r="64" spans="1:6" ht="25.5">
       <c r="A64" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="B64" s="18" t="s">
         <v>94</v>
@@ -5820,10 +5819,10 @@
         <v>297</v>
       </c>
       <c r="D64" s="20" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="E64" s="20" t="s">
-        <v>545</v>
+        <v>542</v>
       </c>
       <c r="F64" t="s">
         <v>53</v>
@@ -5831,7 +5830,7 @@
     </row>
     <row r="65" spans="1:6" ht="25.5">
       <c r="A65" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="B65" s="18" t="s">
         <v>94</v>
@@ -5840,10 +5839,10 @@
         <v>297</v>
       </c>
       <c r="D65" s="20" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="E65" s="20" t="s">
-        <v>546</v>
+        <v>543</v>
       </c>
       <c r="F65" t="s">
         <v>53</v>
@@ -5851,7 +5850,7 @@
     </row>
     <row r="66" spans="1:6">
       <c r="A66" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="B66" s="18" t="s">
         <v>94</v>
@@ -5860,10 +5859,10 @@
         <v>297</v>
       </c>
       <c r="D66" s="20" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="E66" s="20" t="s">
-        <v>547</v>
+        <v>544</v>
       </c>
       <c r="F66" t="s">
         <v>53</v>
@@ -5871,7 +5870,7 @@
     </row>
     <row r="67" spans="1:6">
       <c r="A67" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="B67" s="18" t="s">
         <v>94</v>
@@ -5880,10 +5879,10 @@
         <v>297</v>
       </c>
       <c r="D67" s="20" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="E67" s="20" t="s">
-        <v>548</v>
+        <v>545</v>
       </c>
       <c r="F67" t="s">
         <v>53</v>
@@ -5891,7 +5890,7 @@
     </row>
     <row r="68" spans="1:6" ht="25.5">
       <c r="A68" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="B68" s="18" t="s">
         <v>94</v>
@@ -5900,10 +5899,10 @@
         <v>297</v>
       </c>
       <c r="D68" s="20" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="E68" s="20" t="s">
-        <v>549</v>
+        <v>546</v>
       </c>
       <c r="F68" t="s">
         <v>53</v>
@@ -5911,7 +5910,7 @@
     </row>
     <row r="69" spans="1:6" ht="25.5">
       <c r="A69" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="B69" s="18" t="s">
         <v>94</v>
@@ -5920,7 +5919,7 @@
         <v>297</v>
       </c>
       <c r="D69" s="20" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="E69" s="1" t="s">
         <v>51</v>
@@ -5931,7 +5930,7 @@
     </row>
     <row r="70" spans="1:6" ht="25.5">
       <c r="A70" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="B70" s="18" t="s">
         <v>94</v>
@@ -5940,10 +5939,10 @@
         <v>297</v>
       </c>
       <c r="D70" s="20" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="E70" s="20" t="s">
-        <v>550</v>
+        <v>547</v>
       </c>
       <c r="F70" t="s">
         <v>53</v>
@@ -5951,7 +5950,7 @@
     </row>
     <row r="71" spans="1:6" ht="25.5">
       <c r="A71" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="B71" s="18" t="s">
         <v>94</v>
@@ -5960,10 +5959,10 @@
         <v>297</v>
       </c>
       <c r="D71" s="20" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="E71" s="20" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="F71" t="s">
         <v>53</v>
@@ -5971,7 +5970,7 @@
     </row>
     <row r="72" spans="1:6" ht="25.5">
       <c r="A72" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="B72" s="18" t="s">
         <v>94</v>
@@ -5980,10 +5979,10 @@
         <v>297</v>
       </c>
       <c r="D72" s="20" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="E72" s="20" t="s">
-        <v>552</v>
+        <v>549</v>
       </c>
       <c r="F72" t="s">
         <v>53</v>
@@ -5991,7 +5990,7 @@
     </row>
     <row r="73" spans="1:6" ht="25.5">
       <c r="A73" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="B73" s="18" t="s">
         <v>94</v>
@@ -6000,7 +5999,7 @@
         <v>297</v>
       </c>
       <c r="D73" s="20" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="E73" s="1" t="s">
         <v>51</v>
@@ -6009,9 +6008,9 @@
         <v>53</v>
       </c>
     </row>
-    <row r="74" spans="1:6" ht="38.25">
+    <row r="74" spans="1:6" ht="51">
       <c r="A74" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="B74" s="18" t="s">
         <v>89</v>
@@ -6019,11 +6018,11 @@
       <c r="C74" s="18" t="s">
         <v>122</v>
       </c>
-      <c r="D74" s="1" t="s">
-        <v>535</v>
-      </c>
-      <c r="E74" s="1" t="s">
-        <v>536</v>
+      <c r="D74" s="20" t="s">
+        <v>590</v>
+      </c>
+      <c r="E74" s="20" t="s">
+        <v>589</v>
       </c>
       <c r="F74" s="18" t="s">
         <v>53</v>
@@ -6031,7 +6030,7 @@
     </row>
     <row r="75" spans="1:6" ht="25.5">
       <c r="A75" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="B75" s="18" t="s">
         <v>89</v>
@@ -6040,7 +6039,7 @@
         <v>122</v>
       </c>
       <c r="D75" s="1" t="s">
-        <v>537</v>
+        <v>534</v>
       </c>
       <c r="E75" s="1" t="s">
         <v>51</v>
@@ -6051,7 +6050,7 @@
     </row>
     <row r="76" spans="1:6" ht="25.5">
       <c r="A76" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="B76" t="s">
         <v>93</v>
@@ -6060,10 +6059,10 @@
         <v>293</v>
       </c>
       <c r="D76" s="1" t="s">
-        <v>539</v>
+        <v>536</v>
       </c>
       <c r="E76" s="1" t="s">
-        <v>538</v>
+        <v>535</v>
       </c>
       <c r="F76" s="18" t="s">
         <v>53</v>
@@ -6071,7 +6070,7 @@
     </row>
     <row r="77" spans="1:6" ht="25.5">
       <c r="A77" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="B77" t="s">
         <v>93</v>
@@ -6080,7 +6079,7 @@
         <v>293</v>
       </c>
       <c r="D77" s="1" t="s">
-        <v>540</v>
+        <v>537</v>
       </c>
       <c r="E77" s="1" t="s">
         <v>51</v>
@@ -6091,7 +6090,7 @@
     </row>
     <row r="78" spans="1:6" ht="25.5">
       <c r="A78" s="18" t="s">
-        <v>565</v>
+        <v>562</v>
       </c>
       <c r="B78" s="18" t="s">
         <v>91</v>
@@ -6100,10 +6099,10 @@
         <v>127</v>
       </c>
       <c r="D78" s="20" t="s">
-        <v>574</v>
+        <v>571</v>
       </c>
       <c r="E78" s="1" t="s">
-        <v>575</v>
+        <v>572</v>
       </c>
       <c r="F78" s="18" t="s">
         <v>53</v>
@@ -6111,7 +6110,7 @@
     </row>
     <row r="79" spans="1:6" ht="25.5">
       <c r="A79" t="s">
-        <v>566</v>
+        <v>563</v>
       </c>
       <c r="B79" s="18" t="s">
         <v>91</v>
@@ -6120,7 +6119,7 @@
         <v>127</v>
       </c>
       <c r="D79" s="20" t="s">
-        <v>576</v>
+        <v>573</v>
       </c>
       <c r="E79" s="1" t="s">
         <v>51</v>
@@ -6131,7 +6130,7 @@
     </row>
     <row r="80" spans="1:6" ht="25.5">
       <c r="A80" s="18" t="s">
-        <v>567</v>
+        <v>564</v>
       </c>
       <c r="B80" t="s">
         <v>92</v>
@@ -6140,10 +6139,10 @@
         <v>261</v>
       </c>
       <c r="D80" s="20" t="s">
-        <v>578</v>
+        <v>575</v>
       </c>
       <c r="E80" s="1" t="s">
-        <v>577</v>
+        <v>574</v>
       </c>
       <c r="F80" s="18" t="s">
         <v>53</v>
@@ -6151,7 +6150,7 @@
     </row>
     <row r="81" spans="1:6" ht="25.5">
       <c r="A81" t="s">
-        <v>568</v>
+        <v>565</v>
       </c>
       <c r="B81" s="18" t="s">
         <v>92</v>
@@ -6160,10 +6159,10 @@
         <v>261</v>
       </c>
       <c r="D81" s="20" t="s">
-        <v>579</v>
+        <v>576</v>
       </c>
       <c r="E81" s="1" t="s">
-        <v>580</v>
+        <v>577</v>
       </c>
       <c r="F81" s="18" t="s">
         <v>53</v>
@@ -6171,7 +6170,7 @@
     </row>
     <row r="82" spans="1:6" ht="25.5">
       <c r="A82" s="18" t="s">
-        <v>569</v>
+        <v>566</v>
       </c>
       <c r="B82" s="18" t="s">
         <v>92</v>
@@ -6180,10 +6179,10 @@
         <v>261</v>
       </c>
       <c r="D82" s="20" t="s">
-        <v>582</v>
+        <v>579</v>
       </c>
       <c r="E82" s="20" t="s">
-        <v>581</v>
+        <v>578</v>
       </c>
       <c r="F82" s="18" t="s">
         <v>53</v>
@@ -6191,7 +6190,7 @@
     </row>
     <row r="83" spans="1:6" ht="25.5">
       <c r="A83" t="s">
-        <v>570</v>
+        <v>567</v>
       </c>
       <c r="B83" s="18" t="s">
         <v>92</v>
@@ -6200,10 +6199,10 @@
         <v>261</v>
       </c>
       <c r="D83" s="20" t="s">
-        <v>583</v>
+        <v>580</v>
       </c>
       <c r="E83" s="20" t="s">
-        <v>584</v>
+        <v>581</v>
       </c>
       <c r="F83" s="18" t="s">
         <v>53</v>
@@ -6211,7 +6210,7 @@
     </row>
     <row r="84" spans="1:6" ht="25.5">
       <c r="A84" s="18" t="s">
-        <v>571</v>
+        <v>568</v>
       </c>
       <c r="B84" s="18" t="s">
         <v>92</v>
@@ -6220,7 +6219,7 @@
         <v>261</v>
       </c>
       <c r="D84" s="20" t="s">
-        <v>585</v>
+        <v>582</v>
       </c>
       <c r="E84" s="20" t="s">
         <v>51</v>
@@ -6231,7 +6230,7 @@
     </row>
     <row r="85" spans="1:6" ht="25.5">
       <c r="A85" t="s">
-        <v>572</v>
+        <v>569</v>
       </c>
       <c r="B85" s="18" t="s">
         <v>92</v>
@@ -6240,10 +6239,10 @@
         <v>261</v>
       </c>
       <c r="D85" s="20" t="s">
-        <v>587</v>
+        <v>584</v>
       </c>
       <c r="E85" s="20" t="s">
-        <v>586</v>
+        <v>583</v>
       </c>
       <c r="F85" s="18" t="s">
         <v>53</v>
@@ -6251,7 +6250,7 @@
     </row>
     <row r="86" spans="1:6" ht="25.5">
       <c r="A86" s="18" t="s">
-        <v>573</v>
+        <v>570</v>
       </c>
       <c r="B86" s="18" t="s">
         <v>92</v>
@@ -6260,7 +6259,7 @@
         <v>261</v>
       </c>
       <c r="D86" s="20" t="s">
-        <v>588</v>
+        <v>585</v>
       </c>
       <c r="E86" s="20" t="s">
         <v>51</v>
@@ -7170,7 +7169,7 @@
         <v>108</v>
       </c>
       <c r="C14" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="D14" t="s">
         <v>187</v>
@@ -7250,7 +7249,7 @@
         <v>33</v>
       </c>
       <c r="C20" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="D20" t="s">
         <v>187</v>
@@ -7337,7 +7336,7 @@
         <v>99</v>
       </c>
       <c r="C27" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="D27" t="s">
         <v>254</v>
@@ -7363,37 +7362,37 @@
     </row>
     <row r="28" spans="1:10" ht="25.5">
       <c r="A28" t="s">
+        <v>383</v>
+      </c>
+      <c r="B28" s="1" t="s">
         <v>384</v>
-      </c>
-      <c r="B28" s="1" t="s">
-        <v>385</v>
       </c>
       <c r="J28" s="16"/>
     </row>
     <row r="29" spans="1:10" ht="38.25">
       <c r="A29" t="s">
+        <v>385</v>
+      </c>
+      <c r="B29" s="1" t="s">
         <v>386</v>
-      </c>
-      <c r="B29" s="1" t="s">
-        <v>387</v>
       </c>
       <c r="J29" s="16"/>
     </row>
     <row r="30" spans="1:10" ht="25.5">
       <c r="A30" t="s">
+        <v>387</v>
+      </c>
+      <c r="B30" s="1" t="s">
         <v>388</v>
-      </c>
-      <c r="B30" s="1" t="s">
-        <v>389</v>
       </c>
       <c r="J30" s="16"/>
     </row>
     <row r="31" spans="1:10" ht="25.5">
       <c r="A31" t="s">
+        <v>389</v>
+      </c>
+      <c r="B31" s="1" t="s">
         <v>390</v>
-      </c>
-      <c r="B31" s="1" t="s">
-        <v>391</v>
       </c>
       <c r="J31" s="16"/>
     </row>
@@ -7405,7 +7404,7 @@
         <v>100</v>
       </c>
       <c r="C32" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="D32" t="s">
         <v>254</v>
@@ -7431,26 +7430,26 @@
     </row>
     <row r="33" spans="1:2" ht="25.5">
       <c r="A33" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
     </row>
     <row r="34" spans="1:2" ht="51">
       <c r="A34" t="s">
+        <v>392</v>
+      </c>
+      <c r="B34" s="1" t="s">
         <v>393</v>
-      </c>
-      <c r="B34" s="1" t="s">
-        <v>394</v>
       </c>
     </row>
     <row r="35" spans="1:2" ht="25.5">
       <c r="A35" t="s">
+        <v>394</v>
+      </c>
+      <c r="B35" s="1" t="s">
         <v>395</v>
-      </c>
-      <c r="B35" s="1" t="s">
-        <v>396</v>
       </c>
     </row>
     <row r="37" spans="1:2">
@@ -7559,7 +7558,7 @@
         <v>101</v>
       </c>
       <c r="C2" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="D2" s="18" t="s">
         <v>128</v>
@@ -7585,10 +7584,10 @@
     </row>
     <row r="4" spans="1:10" ht="25.5">
       <c r="A4" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="C4" s="1"/>
       <c r="D4" t="s">
@@ -7597,10 +7596,10 @@
     </row>
     <row r="5" spans="1:10" ht="38.25">
       <c r="A5" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="C5" s="1"/>
       <c r="D5" t="s">
@@ -7609,10 +7608,10 @@
     </row>
     <row r="6" spans="1:10" ht="38.25">
       <c r="A6" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="C6" s="1"/>
       <c r="D6" t="s">
@@ -7621,10 +7620,10 @@
     </row>
     <row r="7" spans="1:10" ht="38.25">
       <c r="A7" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="C7" s="1"/>
       <c r="D7" t="s">
@@ -7633,18 +7632,18 @@
     </row>
     <row r="8" spans="1:10" ht="25.5">
       <c r="A8" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
     </row>
     <row r="9" spans="1:10" ht="51">
       <c r="A9" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="C9" s="1"/>
       <c r="D9" t="s">
@@ -7653,10 +7652,10 @@
     </row>
     <row r="10" spans="1:10" ht="38.25">
       <c r="A10" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="C10" s="1"/>
       <c r="D10" t="s">
@@ -7671,7 +7670,7 @@
         <v>295</v>
       </c>
       <c r="C12" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="D12" s="18" t="s">
         <v>128</v>
@@ -7697,10 +7696,10 @@
     </row>
     <row r="14" spans="1:10" ht="25.5">
       <c r="A14" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="C14" s="1"/>
       <c r="D14" t="s">
@@ -7709,10 +7708,10 @@
     </row>
     <row r="15" spans="1:10" ht="38.25">
       <c r="A15" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="C15" s="1"/>
       <c r="D15" t="s">
@@ -7721,10 +7720,10 @@
     </row>
     <row r="16" spans="1:10" ht="38.25">
       <c r="A16" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="C16" s="1"/>
       <c r="D16" t="s">
@@ -7743,7 +7742,7 @@
         <v>110</v>
       </c>
       <c r="C18" s="18" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="D18" s="18" t="s">
         <v>70</v>
@@ -7769,10 +7768,10 @@
     </row>
     <row r="19" spans="1:10">
       <c r="A19" t="s">
+        <v>456</v>
+      </c>
+      <c r="B19" s="1" t="s">
         <v>457</v>
-      </c>
-      <c r="B19" s="1" t="s">
-        <v>458</v>
       </c>
       <c r="D19" s="18" t="s">
         <v>70</v>
@@ -7780,10 +7779,10 @@
     </row>
     <row r="20" spans="1:10" ht="25.5">
       <c r="A20" t="s">
+        <v>458</v>
+      </c>
+      <c r="B20" s="1" t="s">
         <v>459</v>
-      </c>
-      <c r="B20" s="1" t="s">
-        <v>460</v>
       </c>
       <c r="D20" s="18" t="s">
         <v>70</v>
@@ -7791,10 +7790,10 @@
     </row>
     <row r="21" spans="1:10" ht="38.25">
       <c r="A21" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="D21" s="18" t="s">
         <v>70</v>
@@ -7802,10 +7801,10 @@
     </row>
     <row r="22" spans="1:10" ht="51">
       <c r="A22" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="D22" s="18" t="s">
         <v>70</v>
@@ -7813,10 +7812,10 @@
     </row>
     <row r="23" spans="1:10" ht="25.5">
       <c r="A23" t="s">
+        <v>464</v>
+      </c>
+      <c r="B23" s="1" t="s">
         <v>465</v>
-      </c>
-      <c r="B23" s="1" t="s">
-        <v>466</v>
       </c>
       <c r="D23" s="18" t="s">
         <v>70</v>
@@ -7833,7 +7832,7 @@
         <v>111</v>
       </c>
       <c r="C25" s="18" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="D25" s="18" t="s">
         <v>70</v>
@@ -7859,7 +7858,7 @@
     </row>
     <row r="26" spans="1:10" ht="25.5">
       <c r="A26" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="B26" s="1" t="s">
         <v>322</v>
@@ -7870,10 +7869,10 @@
     </row>
     <row r="27" spans="1:10" ht="25.5">
       <c r="A27" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="D27" s="18" t="s">
         <v>70</v>
@@ -7881,10 +7880,10 @@
     </row>
     <row r="28" spans="1:10" ht="25.5">
       <c r="A28" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="D28" s="18" t="s">
         <v>70</v>
@@ -7892,10 +7891,10 @@
     </row>
     <row r="29" spans="1:10" ht="51">
       <c r="A29" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="D29" s="18" t="s">
         <v>70</v>
@@ -7903,10 +7902,10 @@
     </row>
     <row r="30" spans="1:10" ht="51">
       <c r="A30" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="D30" s="18" t="s">
         <v>70</v>
@@ -7923,7 +7922,7 @@
         <v>117</v>
       </c>
       <c r="C32" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="D32" s="18" t="s">
         <v>254</v>
@@ -7949,18 +7948,18 @@
     </row>
     <row r="33" spans="1:10">
       <c r="A33" t="s">
+        <v>476</v>
+      </c>
+      <c r="B33" s="1" t="s">
         <v>477</v>
-      </c>
-      <c r="B33" s="1" t="s">
-        <v>478</v>
       </c>
     </row>
     <row r="34" spans="1:10" ht="38.25">
       <c r="A34" t="s">
+        <v>478</v>
+      </c>
+      <c r="B34" s="1" t="s">
         <v>479</v>
-      </c>
-      <c r="B34" s="1" t="s">
-        <v>480</v>
       </c>
     </row>
     <row r="36" spans="1:10">
@@ -7971,7 +7970,7 @@
         <v>119</v>
       </c>
       <c r="C36" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="D36" s="18" t="s">
         <v>254</v>
@@ -7997,7 +7996,7 @@
     </row>
     <row r="37" spans="1:10">
       <c r="A37" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="B37" t="s">
         <v>322</v>
@@ -8005,18 +8004,18 @@
     </row>
     <row r="38" spans="1:10">
       <c r="A38" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="B38" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
     </row>
     <row r="39" spans="1:10">
       <c r="A39" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="B39" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
     </row>
     <row r="41" spans="1:10">
@@ -8072,7 +8071,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:J42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="150" workbookViewId="0">
+    <sheetView topLeftCell="A7" zoomScale="150" workbookViewId="0">
       <selection activeCell="C16" sqref="C16:J16"/>
     </sheetView>
   </sheetViews>
@@ -8121,7 +8120,7 @@
         <v>122</v>
       </c>
       <c r="C2" t="s">
-        <v>541</v>
+        <v>538</v>
       </c>
       <c r="D2" t="s">
         <v>254</v>
@@ -8147,26 +8146,26 @@
     </row>
     <row r="3" spans="1:10">
       <c r="A3" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
       <c r="B3" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
     </row>
     <row r="4" spans="1:10">
       <c r="A4" t="s">
+        <v>525</v>
+      </c>
+      <c r="B4" t="s">
         <v>526</v>
-      </c>
-      <c r="B4" t="s">
-        <v>527</v>
       </c>
     </row>
     <row r="5" spans="1:10">
       <c r="A5" t="s">
+        <v>527</v>
+      </c>
+      <c r="B5" t="s">
         <v>528</v>
-      </c>
-      <c r="B5" t="s">
-        <v>529</v>
       </c>
     </row>
     <row r="7" spans="1:10">
@@ -8177,7 +8176,7 @@
         <v>126</v>
       </c>
       <c r="C7" s="18" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="D7" t="s">
         <v>128</v>
@@ -8203,10 +8202,10 @@
     </row>
     <row r="8" spans="1:10" ht="25.5">
       <c r="A8" s="18" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="B8" s="20" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="D8" t="s">
         <v>128</v>
@@ -8214,10 +8213,10 @@
     </row>
     <row r="9" spans="1:10" ht="25.5">
       <c r="A9" s="18" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="B9" s="20" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="D9" t="s">
         <v>128</v>
@@ -8235,7 +8234,7 @@
         <v>127</v>
       </c>
       <c r="C11" s="18" t="s">
-        <v>589</v>
+        <v>586</v>
       </c>
       <c r="D11" t="s">
         <v>70</v>
@@ -8261,10 +8260,10 @@
     </row>
     <row r="12" spans="1:10" ht="25.5">
       <c r="A12" s="18" t="s">
-        <v>553</v>
+        <v>550</v>
       </c>
       <c r="B12" s="20" t="s">
-        <v>554</v>
+        <v>551</v>
       </c>
       <c r="D12" t="s">
         <v>70</v>
@@ -8274,10 +8273,10 @@
     </row>
     <row r="13" spans="1:10" ht="25.5">
       <c r="A13" s="18" t="s">
-        <v>555</v>
+        <v>552</v>
       </c>
       <c r="B13" s="20" t="s">
-        <v>556</v>
+        <v>553</v>
       </c>
       <c r="D13" t="s">
         <v>70</v>
@@ -8287,10 +8286,10 @@
     </row>
     <row r="14" spans="1:10" ht="63.75">
       <c r="A14" s="18" t="s">
-        <v>557</v>
+        <v>554</v>
       </c>
       <c r="B14" s="20" t="s">
-        <v>558</v>
+        <v>555</v>
       </c>
       <c r="D14" t="s">
         <v>70</v>
@@ -8310,7 +8309,7 @@
         <v>261</v>
       </c>
       <c r="C16" s="18" t="s">
-        <v>590</v>
+        <v>587</v>
       </c>
       <c r="D16" t="s">
         <v>70</v>
@@ -8336,10 +8335,10 @@
     </row>
     <row r="17" spans="1:10" ht="25.5">
       <c r="A17" s="18" t="s">
-        <v>559</v>
+        <v>556</v>
       </c>
       <c r="B17" s="21" t="s">
-        <v>554</v>
+        <v>551</v>
       </c>
       <c r="D17" t="s">
         <v>70</v>
@@ -8349,10 +8348,10 @@
     </row>
     <row r="18" spans="1:10" ht="63.75">
       <c r="A18" s="18" t="s">
-        <v>560</v>
+        <v>557</v>
       </c>
       <c r="B18" s="21" t="s">
-        <v>561</v>
+        <v>558</v>
       </c>
       <c r="D18" t="s">
         <v>70</v>
@@ -8362,7 +8361,7 @@
     </row>
     <row r="19" spans="1:10">
       <c r="A19" s="18" t="s">
-        <v>562</v>
+        <v>559</v>
       </c>
       <c r="B19" s="18" t="s">
         <v>322</v>
@@ -8375,10 +8374,10 @@
     </row>
     <row r="20" spans="1:10" ht="51">
       <c r="A20" s="18" t="s">
-        <v>563</v>
+        <v>560</v>
       </c>
       <c r="B20" s="21" t="s">
-        <v>564</v>
+        <v>561</v>
       </c>
       <c r="D20" t="s">
         <v>70</v>
@@ -8397,7 +8396,7 @@
         <v>293</v>
       </c>
       <c r="C22" t="s">
-        <v>542</v>
+        <v>539</v>
       </c>
       <c r="D22" t="s">
         <v>254</v>
@@ -8423,26 +8422,26 @@
     </row>
     <row r="23" spans="1:10">
       <c r="A23" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="B23" s="18" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
     </row>
     <row r="24" spans="1:10">
       <c r="A24" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="B24" s="18" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
     </row>
     <row r="25" spans="1:10">
       <c r="A25" t="s">
+        <v>531</v>
+      </c>
+      <c r="B25" s="18" t="s">
         <v>532</v>
-      </c>
-      <c r="B25" s="18" t="s">
-        <v>533</v>
       </c>
     </row>
     <row r="26" spans="1:10">
@@ -8456,7 +8455,7 @@
         <v>297</v>
       </c>
       <c r="C27" s="18" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="D27" t="s">
         <v>128</v>
@@ -8482,10 +8481,10 @@
     </row>
     <row r="29" spans="1:10">
       <c r="A29" s="18" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="B29" s="20" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="D29" t="s">
         <v>128</v>
@@ -8493,10 +8492,10 @@
     </row>
     <row r="30" spans="1:10" ht="51">
       <c r="A30" s="18" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="B30" s="20" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="D30" t="s">
         <v>128</v>
@@ -8504,10 +8503,10 @@
     </row>
     <row r="31" spans="1:10" ht="63.75">
       <c r="A31" s="18" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="B31" s="20" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="D31" t="s">
         <v>128</v>
@@ -8515,10 +8514,10 @@
     </row>
     <row r="32" spans="1:10" ht="51">
       <c r="A32" s="18" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="B32" s="20" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="D32" t="s">
         <v>128</v>
@@ -8526,10 +8525,10 @@
     </row>
     <row r="33" spans="1:4" ht="51">
       <c r="A33" s="18" t="s">
+        <v>521</v>
+      </c>
+      <c r="B33" s="20" t="s">
         <v>522</v>
-      </c>
-      <c r="B33" s="20" t="s">
-        <v>523</v>
       </c>
       <c r="D33" t="s">
         <v>128</v>

</xml_diff>

<commit_message>
2 user stories implemented
</commit_message>
<xml_diff>
--- a/Team05Report.xlsx
+++ b/Team05Report.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="240" windowWidth="20730" windowHeight="11760" tabRatio="500" firstSheet="1" activeTab="3"/>
+    <workbookView xWindow="240" yWindow="240" windowWidth="20730" windowHeight="11760" tabRatio="500" firstSheet="1" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Team" sheetId="1" r:id="rId1"/>
@@ -62,7 +62,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1260" uniqueCount="591">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1314" uniqueCount="615">
   <si>
     <t>Date</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -1700,13 +1700,7 @@
     <t>T19.02</t>
   </si>
   <si>
-    <t>get the wife age</t>
-  </si>
-  <si>
     <t>T19.03</t>
-  </si>
-  <si>
-    <t>Chech the age between 18to 50</t>
   </si>
   <si>
     <t>T23.01</t>
@@ -1894,6 +1888,84 @@
   </si>
   <si>
     <t>In Family F4, wife I9(Elena /Wilson/) was born on 1 NOV 1941 while child I3(Katie /Brown/) was born on 14 FEB 1950</t>
+  </si>
+  <si>
+    <t>get the wife age and children age</t>
+  </si>
+  <si>
+    <t>Compare the ages between 18to 50</t>
+  </si>
+  <si>
+    <t>AT86</t>
+  </si>
+  <si>
+    <t>AT87</t>
+  </si>
+  <si>
+    <t>AT88</t>
+  </si>
+  <si>
+    <t>AT89</t>
+  </si>
+  <si>
+    <t>In Family F2, husband I2(Jianguo /Mao/) and child I1(Jacky /Gao/) don't have the same last name.</t>
+  </si>
+  <si>
+    <t>In Family F2, husband I2's last name is Mao, while child I1's last name is Gao</t>
+  </si>
+  <si>
+    <t>In Family F2, husband I2's last name is Mao, and child I5's last name is Mao</t>
+  </si>
+  <si>
+    <t>AT86~87</t>
+  </si>
+  <si>
+    <t>T25.01</t>
+  </si>
+  <si>
+    <t>T25.02</t>
+  </si>
+  <si>
+    <t>For each family, get the last name of the husband.</t>
+  </si>
+  <si>
+    <t>T25.03</t>
+  </si>
+  <si>
+    <t>Check if the last names of husband and children are the same</t>
+  </si>
+  <si>
+    <t>Get the last names of the children</t>
+  </si>
+  <si>
+    <t>In Family F2, there are more than 4 children born on the same day: I5(Emily /Mao/), I14(Emilya /Mao/), I15(Emilyb /Mao/), I16(Emilyc /Mao/), and I17(Emilyd /Mao/).</t>
+  </si>
+  <si>
+    <t>In Family F2, child I5, I14, I15, I16 and I17 were all born on 11 SEP 1971</t>
+  </si>
+  <si>
+    <t>In Family F2, only child I1 was born on 27 JAN 1970</t>
+  </si>
+  <si>
+    <t>AT88~89</t>
+  </si>
+  <si>
+    <t>T27.01</t>
+  </si>
+  <si>
+    <t>T27.02</t>
+  </si>
+  <si>
+    <t>T27.03</t>
+  </si>
+  <si>
+    <t>For each family, get the birthdays of all the children</t>
+  </si>
+  <si>
+    <t>Count the numbers of children that were born on the same day</t>
+  </si>
+  <si>
+    <t>Check if there are more than 4 children born on the same day in one family</t>
   </si>
 </sst>
 </file>
@@ -2200,25 +2272,25 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="226254848"/>
-        <c:axId val="226256384"/>
+        <c:axId val="227630464"/>
+        <c:axId val="231203968"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="226254848"/>
+        <c:axId val="227630464"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="m/d" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="226256384"/>
+        <c:crossAx val="231203968"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
         <c:baseTimeUnit val="days"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="226256384"/>
+        <c:axId val="231203968"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2226,7 +2298,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="226254848"/>
+        <c:crossAx val="227630464"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2236,7 +2308,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="1" l="0.750000000000003" r="0.750000000000003" t="1" header="0.5" footer="0.5"/>
+    <c:pageMargins b="1" l="0.75000000000000311" r="0.75000000000000311" t="1" header="0.5" footer="0.5"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -2710,10 +2782,10 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J7"/>
+  <dimension ref="A1:J18"/>
   <sheetViews>
     <sheetView zoomScale="150" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75"/>
@@ -2760,98 +2832,194 @@
       <c r="B2" s="18" t="s">
         <v>339</v>
       </c>
+      <c r="C2" s="18" t="s">
+        <v>598</v>
+      </c>
       <c r="D2" s="18" t="s">
         <v>128</v>
       </c>
+      <c r="E2" s="18" t="s">
+        <v>329</v>
+      </c>
       <c r="F2">
         <v>30</v>
       </c>
       <c r="G2">
         <v>35</v>
       </c>
-    </row>
-    <row r="3" spans="1:10">
-      <c r="A3" t="s">
+      <c r="H2">
+        <v>31</v>
+      </c>
+      <c r="I2">
+        <v>30</v>
+      </c>
+      <c r="J2" s="16">
+        <v>40652</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" ht="25.5">
+      <c r="A4" s="18" t="s">
+        <v>599</v>
+      </c>
+      <c r="B4" s="20" t="s">
+        <v>601</v>
+      </c>
+      <c r="D4" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" ht="25.5">
+      <c r="A5" s="18" t="s">
+        <v>600</v>
+      </c>
+      <c r="B5" s="20" t="s">
+        <v>604</v>
+      </c>
+      <c r="D5" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" ht="38.25">
+      <c r="A6" s="18" t="s">
+        <v>602</v>
+      </c>
+      <c r="B6" s="20" t="s">
+        <v>603</v>
+      </c>
+      <c r="D6" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10">
+      <c r="A8" t="s">
         <v>307</v>
       </c>
-      <c r="B3" s="18" t="s">
+      <c r="B8" s="18" t="s">
         <v>341</v>
       </c>
-      <c r="D3" s="18" t="s">
+      <c r="D8" s="18" t="s">
         <v>254</v>
       </c>
-      <c r="F3">
+      <c r="F8">
         <v>15</v>
       </c>
-      <c r="G3">
+      <c r="G8">
         <v>30</v>
       </c>
     </row>
-    <row r="4" spans="1:10">
-      <c r="A4" t="s">
+    <row r="10" spans="1:10">
+      <c r="A10" t="s">
         <v>340</v>
       </c>
-      <c r="B4" s="18" t="s">
+      <c r="B10" s="18" t="s">
         <v>347</v>
       </c>
-      <c r="D4" s="18" t="s">
+      <c r="C10" s="18" t="s">
+        <v>608</v>
+      </c>
+      <c r="D10" s="18" t="s">
         <v>128</v>
       </c>
-      <c r="F4">
+      <c r="E10" s="18" t="s">
+        <v>329</v>
+      </c>
+      <c r="F10">
         <v>35</v>
       </c>
-      <c r="G4">
+      <c r="G10">
         <v>70</v>
       </c>
-    </row>
-    <row r="5" spans="1:10">
-      <c r="A5" t="s">
+      <c r="H10">
+        <v>43</v>
+      </c>
+      <c r="I10">
+        <v>50</v>
+      </c>
+      <c r="J10" s="16">
+        <v>40652</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" ht="25.5">
+      <c r="A12" s="18" t="s">
+        <v>609</v>
+      </c>
+      <c r="B12" s="20" t="s">
+        <v>612</v>
+      </c>
+      <c r="D12" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" ht="38.25">
+      <c r="A13" s="18" t="s">
+        <v>610</v>
+      </c>
+      <c r="B13" s="20" t="s">
+        <v>613</v>
+      </c>
+      <c r="D13" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" ht="38.25">
+      <c r="A14" s="18" t="s">
+        <v>611</v>
+      </c>
+      <c r="B14" s="20" t="s">
+        <v>614</v>
+      </c>
+      <c r="D14" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10">
+      <c r="A16" t="s">
         <v>342</v>
       </c>
-      <c r="B5" s="18" t="s">
+      <c r="B16" s="18" t="s">
         <v>357</v>
       </c>
-      <c r="D5" s="18" t="s">
+      <c r="D16" s="18" t="s">
         <v>254</v>
       </c>
-      <c r="F5">
+      <c r="F16">
         <v>20</v>
       </c>
-      <c r="G5">
+      <c r="G16">
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:10">
-      <c r="A6" t="s">
+    <row r="17" spans="1:7">
+      <c r="A17" t="s">
         <v>343</v>
       </c>
-      <c r="B6" s="18" t="s">
+      <c r="B17" s="18" t="s">
         <v>354</v>
       </c>
-      <c r="D6" s="18" t="s">
+      <c r="D17" s="18" t="s">
         <v>70</v>
       </c>
-      <c r="F6">
+      <c r="F17">
         <v>35</v>
       </c>
-      <c r="G6">
+      <c r="G17">
         <v>40</v>
       </c>
     </row>
-    <row r="7" spans="1:10">
-      <c r="A7" t="s">
+    <row r="18" spans="1:7">
+      <c r="A18" t="s">
         <v>344</v>
       </c>
-      <c r="B7" s="18" t="s">
+      <c r="B18" s="18" t="s">
         <v>352</v>
       </c>
-      <c r="D7" s="18" t="s">
+      <c r="D18" s="18" t="s">
         <v>70</v>
       </c>
-      <c r="F7">
+      <c r="F18">
         <v>30</v>
       </c>
-      <c r="G7">
+      <c r="G18">
         <v>35</v>
       </c>
     </row>
@@ -2870,8 +3038,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:L31"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" zoomScale="150" workbookViewId="0">
-      <selection activeCell="D23" sqref="D23:K23"/>
+    <sheetView topLeftCell="B7" zoomScale="150" workbookViewId="0">
+      <selection activeCell="D28" sqref="D28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75"/>
@@ -3620,7 +3788,7 @@
         <v>122</v>
       </c>
       <c r="D20" t="s">
-        <v>538</v>
+        <v>536</v>
       </c>
       <c r="E20" t="s">
         <v>254</v>
@@ -3690,7 +3858,7 @@
         <v>127</v>
       </c>
       <c r="D22" s="18" t="s">
-        <v>586</v>
+        <v>584</v>
       </c>
       <c r="E22" t="s">
         <v>70</v>
@@ -3725,7 +3893,7 @@
         <v>261</v>
       </c>
       <c r="D23" s="18" t="s">
-        <v>587</v>
+        <v>585</v>
       </c>
       <c r="E23" t="s">
         <v>70</v>
@@ -3760,7 +3928,7 @@
         <v>293</v>
       </c>
       <c r="D24" t="s">
-        <v>539</v>
+        <v>537</v>
       </c>
       <c r="E24" t="s">
         <v>254</v>
@@ -3829,6 +3997,30 @@
       <c r="C26" s="18" t="s">
         <v>339</v>
       </c>
+      <c r="D26" s="18" t="s">
+        <v>598</v>
+      </c>
+      <c r="E26" s="18" t="s">
+        <v>128</v>
+      </c>
+      <c r="F26" s="18" t="s">
+        <v>329</v>
+      </c>
+      <c r="G26">
+        <v>30</v>
+      </c>
+      <c r="H26">
+        <v>35</v>
+      </c>
+      <c r="I26">
+        <v>31</v>
+      </c>
+      <c r="J26">
+        <v>30</v>
+      </c>
+      <c r="K26" s="16">
+        <v>40652</v>
+      </c>
       <c r="L26" s="7">
         <v>40610</v>
       </c>
@@ -3850,6 +4042,30 @@
       </c>
       <c r="C28" s="18" t="s">
         <v>347</v>
+      </c>
+      <c r="D28" s="18" t="s">
+        <v>608</v>
+      </c>
+      <c r="E28" s="18" t="s">
+        <v>128</v>
+      </c>
+      <c r="F28" s="18" t="s">
+        <v>329</v>
+      </c>
+      <c r="G28">
+        <v>35</v>
+      </c>
+      <c r="H28">
+        <v>70</v>
+      </c>
+      <c r="I28">
+        <v>43</v>
+      </c>
+      <c r="J28">
+        <v>50</v>
+      </c>
+      <c r="K28" s="16">
+        <v>40652</v>
       </c>
       <c r="L28" s="7">
         <v>40610</v>
@@ -3904,8 +4120,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F31"/>
   <sheetViews>
-    <sheetView topLeftCell="A14" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="C33" sqref="C33"/>
+    <sheetView tabSelected="1" topLeftCell="A14" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="D28" sqref="D28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75"/>
@@ -4308,7 +4524,7 @@
         <v>123</v>
       </c>
       <c r="D20" t="s">
-        <v>538</v>
+        <v>536</v>
       </c>
       <c r="E20">
         <v>50</v>
@@ -4348,7 +4564,7 @@
         <v>125</v>
       </c>
       <c r="D22" s="18" t="s">
-        <v>586</v>
+        <v>584</v>
       </c>
       <c r="E22">
         <v>100</v>
@@ -4368,7 +4584,7 @@
         <v>262</v>
       </c>
       <c r="D23" s="18" t="s">
-        <v>587</v>
+        <v>585</v>
       </c>
       <c r="E23">
         <v>70</v>
@@ -4388,7 +4604,7 @@
         <v>296</v>
       </c>
       <c r="D24" t="s">
-        <v>539</v>
+        <v>537</v>
       </c>
       <c r="E24">
         <v>75</v>
@@ -4427,6 +4643,9 @@
       <c r="C26" s="1" t="s">
         <v>348</v>
       </c>
+      <c r="D26" s="18" t="s">
+        <v>598</v>
+      </c>
       <c r="E26">
         <v>30</v>
       </c>
@@ -4459,7 +4678,10 @@
         <v>347</v>
       </c>
       <c r="C28" s="20" t="s">
-        <v>588</v>
+        <v>586</v>
+      </c>
+      <c r="D28" s="18" t="s">
+        <v>608</v>
       </c>
       <c r="E28">
         <v>35</v>
@@ -4534,8 +4756,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F100"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A71" zoomScale="145" zoomScaleNormal="145" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="D77" sqref="D77"/>
+    <sheetView topLeftCell="A80" zoomScale="145" zoomScaleNormal="145" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="A91" sqref="A91"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75"/>
@@ -5782,7 +6004,7 @@
         <v>500</v>
       </c>
       <c r="E62" s="20" t="s">
-        <v>540</v>
+        <v>538</v>
       </c>
       <c r="F62" t="s">
         <v>53</v>
@@ -5802,7 +6024,7 @@
         <v>501</v>
       </c>
       <c r="E63" s="20" t="s">
-        <v>541</v>
+        <v>539</v>
       </c>
       <c r="F63" t="s">
         <v>53</v>
@@ -5822,7 +6044,7 @@
         <v>502</v>
       </c>
       <c r="E64" s="20" t="s">
-        <v>542</v>
+        <v>540</v>
       </c>
       <c r="F64" t="s">
         <v>53</v>
@@ -5842,7 +6064,7 @@
         <v>503</v>
       </c>
       <c r="E65" s="20" t="s">
-        <v>543</v>
+        <v>541</v>
       </c>
       <c r="F65" t="s">
         <v>53</v>
@@ -5862,7 +6084,7 @@
         <v>504</v>
       </c>
       <c r="E66" s="20" t="s">
-        <v>544</v>
+        <v>542</v>
       </c>
       <c r="F66" t="s">
         <v>53</v>
@@ -5882,7 +6104,7 @@
         <v>505</v>
       </c>
       <c r="E67" s="20" t="s">
-        <v>545</v>
+        <v>543</v>
       </c>
       <c r="F67" t="s">
         <v>53</v>
@@ -5902,7 +6124,7 @@
         <v>506</v>
       </c>
       <c r="E68" s="20" t="s">
-        <v>546</v>
+        <v>544</v>
       </c>
       <c r="F68" t="s">
         <v>53</v>
@@ -5942,7 +6164,7 @@
         <v>508</v>
       </c>
       <c r="E70" s="20" t="s">
-        <v>547</v>
+        <v>545</v>
       </c>
       <c r="F70" t="s">
         <v>53</v>
@@ -5962,7 +6184,7 @@
         <v>509</v>
       </c>
       <c r="E71" s="20" t="s">
-        <v>548</v>
+        <v>546</v>
       </c>
       <c r="F71" t="s">
         <v>53</v>
@@ -5982,7 +6204,7 @@
         <v>510</v>
       </c>
       <c r="E72" s="20" t="s">
-        <v>549</v>
+        <v>547</v>
       </c>
       <c r="F72" t="s">
         <v>53</v>
@@ -6019,10 +6241,10 @@
         <v>122</v>
       </c>
       <c r="D74" s="20" t="s">
-        <v>590</v>
+        <v>588</v>
       </c>
       <c r="E74" s="20" t="s">
-        <v>589</v>
+        <v>587</v>
       </c>
       <c r="F74" s="18" t="s">
         <v>53</v>
@@ -6039,7 +6261,7 @@
         <v>122</v>
       </c>
       <c r="D75" s="1" t="s">
-        <v>534</v>
+        <v>532</v>
       </c>
       <c r="E75" s="1" t="s">
         <v>51</v>
@@ -6059,10 +6281,10 @@
         <v>293</v>
       </c>
       <c r="D76" s="1" t="s">
-        <v>536</v>
+        <v>534</v>
       </c>
       <c r="E76" s="1" t="s">
-        <v>535</v>
+        <v>533</v>
       </c>
       <c r="F76" s="18" t="s">
         <v>53</v>
@@ -6079,7 +6301,7 @@
         <v>293</v>
       </c>
       <c r="D77" s="1" t="s">
-        <v>537</v>
+        <v>535</v>
       </c>
       <c r="E77" s="1" t="s">
         <v>51</v>
@@ -6090,7 +6312,7 @@
     </row>
     <row r="78" spans="1:6" ht="25.5">
       <c r="A78" s="18" t="s">
-        <v>562</v>
+        <v>560</v>
       </c>
       <c r="B78" s="18" t="s">
         <v>91</v>
@@ -6099,10 +6321,10 @@
         <v>127</v>
       </c>
       <c r="D78" s="20" t="s">
-        <v>571</v>
+        <v>569</v>
       </c>
       <c r="E78" s="1" t="s">
-        <v>572</v>
+        <v>570</v>
       </c>
       <c r="F78" s="18" t="s">
         <v>53</v>
@@ -6110,7 +6332,7 @@
     </row>
     <row r="79" spans="1:6" ht="25.5">
       <c r="A79" t="s">
-        <v>563</v>
+        <v>561</v>
       </c>
       <c r="B79" s="18" t="s">
         <v>91</v>
@@ -6119,7 +6341,7 @@
         <v>127</v>
       </c>
       <c r="D79" s="20" t="s">
-        <v>573</v>
+        <v>571</v>
       </c>
       <c r="E79" s="1" t="s">
         <v>51</v>
@@ -6130,7 +6352,7 @@
     </row>
     <row r="80" spans="1:6" ht="25.5">
       <c r="A80" s="18" t="s">
-        <v>564</v>
+        <v>562</v>
       </c>
       <c r="B80" t="s">
         <v>92</v>
@@ -6139,10 +6361,10 @@
         <v>261</v>
       </c>
       <c r="D80" s="20" t="s">
-        <v>575</v>
+        <v>573</v>
       </c>
       <c r="E80" s="1" t="s">
-        <v>574</v>
+        <v>572</v>
       </c>
       <c r="F80" s="18" t="s">
         <v>53</v>
@@ -6150,7 +6372,7 @@
     </row>
     <row r="81" spans="1:6" ht="25.5">
       <c r="A81" t="s">
-        <v>565</v>
+        <v>563</v>
       </c>
       <c r="B81" s="18" t="s">
         <v>92</v>
@@ -6159,10 +6381,10 @@
         <v>261</v>
       </c>
       <c r="D81" s="20" t="s">
-        <v>576</v>
+        <v>574</v>
       </c>
       <c r="E81" s="1" t="s">
-        <v>577</v>
+        <v>575</v>
       </c>
       <c r="F81" s="18" t="s">
         <v>53</v>
@@ -6170,7 +6392,7 @@
     </row>
     <row r="82" spans="1:6" ht="25.5">
       <c r="A82" s="18" t="s">
-        <v>566</v>
+        <v>564</v>
       </c>
       <c r="B82" s="18" t="s">
         <v>92</v>
@@ -6179,10 +6401,10 @@
         <v>261</v>
       </c>
       <c r="D82" s="20" t="s">
-        <v>579</v>
+        <v>577</v>
       </c>
       <c r="E82" s="20" t="s">
-        <v>578</v>
+        <v>576</v>
       </c>
       <c r="F82" s="18" t="s">
         <v>53</v>
@@ -6190,7 +6412,7 @@
     </row>
     <row r="83" spans="1:6" ht="25.5">
       <c r="A83" t="s">
-        <v>567</v>
+        <v>565</v>
       </c>
       <c r="B83" s="18" t="s">
         <v>92</v>
@@ -6199,10 +6421,10 @@
         <v>261</v>
       </c>
       <c r="D83" s="20" t="s">
-        <v>580</v>
+        <v>578</v>
       </c>
       <c r="E83" s="20" t="s">
-        <v>581</v>
+        <v>579</v>
       </c>
       <c r="F83" s="18" t="s">
         <v>53</v>
@@ -6210,7 +6432,7 @@
     </row>
     <row r="84" spans="1:6" ht="25.5">
       <c r="A84" s="18" t="s">
-        <v>568</v>
+        <v>566</v>
       </c>
       <c r="B84" s="18" t="s">
         <v>92</v>
@@ -6219,7 +6441,7 @@
         <v>261</v>
       </c>
       <c r="D84" s="20" t="s">
-        <v>582</v>
+        <v>580</v>
       </c>
       <c r="E84" s="20" t="s">
         <v>51</v>
@@ -6230,7 +6452,7 @@
     </row>
     <row r="85" spans="1:6" ht="25.5">
       <c r="A85" t="s">
-        <v>569</v>
+        <v>567</v>
       </c>
       <c r="B85" s="18" t="s">
         <v>92</v>
@@ -6239,10 +6461,10 @@
         <v>261</v>
       </c>
       <c r="D85" s="20" t="s">
-        <v>584</v>
+        <v>582</v>
       </c>
       <c r="E85" s="20" t="s">
-        <v>583</v>
+        <v>581</v>
       </c>
       <c r="F85" s="18" t="s">
         <v>53</v>
@@ -6250,7 +6472,7 @@
     </row>
     <row r="86" spans="1:6" ht="25.5">
       <c r="A86" s="18" t="s">
-        <v>570</v>
+        <v>568</v>
       </c>
       <c r="B86" s="18" t="s">
         <v>92</v>
@@ -6259,7 +6481,7 @@
         <v>261</v>
       </c>
       <c r="D86" s="20" t="s">
-        <v>585</v>
+        <v>583</v>
       </c>
       <c r="E86" s="20" t="s">
         <v>51</v>
@@ -6268,15 +6490,88 @@
         <v>53</v>
       </c>
     </row>
-    <row r="87" spans="1:6">
-      <c r="F87" s="18"/>
-    </row>
-    <row r="88" spans="1:6">
-      <c r="A88" s="18"/>
-      <c r="F88" s="18"/>
-    </row>
-    <row r="90" spans="1:6">
-      <c r="A90" s="18"/>
+    <row r="87" spans="1:6" ht="38.25">
+      <c r="A87" s="18" t="s">
+        <v>591</v>
+      </c>
+      <c r="B87" t="s">
+        <v>95</v>
+      </c>
+      <c r="C87" s="18" t="s">
+        <v>339</v>
+      </c>
+      <c r="D87" s="20" t="s">
+        <v>596</v>
+      </c>
+      <c r="E87" s="20" t="s">
+        <v>595</v>
+      </c>
+      <c r="F87" s="18" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="88" spans="1:6" ht="25.5">
+      <c r="A88" s="18" t="s">
+        <v>592</v>
+      </c>
+      <c r="B88" t="s">
+        <v>95</v>
+      </c>
+      <c r="C88" s="18" t="s">
+        <v>339</v>
+      </c>
+      <c r="D88" s="20" t="s">
+        <v>597</v>
+      </c>
+      <c r="E88" s="20" t="s">
+        <v>51</v>
+      </c>
+      <c r="F88" s="18" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="89" spans="1:6" ht="63.75">
+      <c r="A89" s="18" t="s">
+        <v>593</v>
+      </c>
+      <c r="B89" t="s">
+        <v>340</v>
+      </c>
+      <c r="C89" s="18" t="s">
+        <v>347</v>
+      </c>
+      <c r="D89" s="20" t="s">
+        <v>606</v>
+      </c>
+      <c r="E89" s="20" t="s">
+        <v>605</v>
+      </c>
+      <c r="F89" s="18" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="90" spans="1:6" ht="25.5">
+      <c r="A90" s="18" t="s">
+        <v>594</v>
+      </c>
+      <c r="B90" t="s">
+        <v>340</v>
+      </c>
+      <c r="C90" s="18" t="s">
+        <v>347</v>
+      </c>
+      <c r="D90" s="20" t="s">
+        <v>607</v>
+      </c>
+      <c r="E90" s="20" t="s">
+        <v>51</v>
+      </c>
+      <c r="F90" s="18" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="91" spans="1:6">
+      <c r="A91" s="18"/>
     </row>
     <row r="92" spans="1:6">
       <c r="A92" s="18"/>
@@ -7509,7 +7804,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:J48"/>
   <sheetViews>
-    <sheetView topLeftCell="A33" zoomScale="150" workbookViewId="0">
+    <sheetView topLeftCell="A9" zoomScale="150" workbookViewId="0">
       <selection activeCell="B41" sqref="B41:B48"/>
     </sheetView>
   </sheetViews>
@@ -8071,8 +8366,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:J42"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" zoomScale="150" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16:J16"/>
+    <sheetView topLeftCell="A10" zoomScale="150" workbookViewId="0">
+      <selection activeCell="A8" sqref="A8:D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75"/>
@@ -8120,7 +8415,7 @@
         <v>122</v>
       </c>
       <c r="C2" t="s">
-        <v>538</v>
+        <v>536</v>
       </c>
       <c r="D2" t="s">
         <v>254</v>
@@ -8156,16 +8451,16 @@
       <c r="A4" t="s">
         <v>525</v>
       </c>
-      <c r="B4" t="s">
-        <v>526</v>
+      <c r="B4" s="18" t="s">
+        <v>589</v>
       </c>
     </row>
     <row r="5" spans="1:10">
       <c r="A5" t="s">
-        <v>527</v>
-      </c>
-      <c r="B5" t="s">
-        <v>528</v>
+        <v>526</v>
+      </c>
+      <c r="B5" s="18" t="s">
+        <v>590</v>
       </c>
     </row>
     <row r="7" spans="1:10">
@@ -8234,7 +8529,7 @@
         <v>127</v>
       </c>
       <c r="C11" s="18" t="s">
-        <v>586</v>
+        <v>584</v>
       </c>
       <c r="D11" t="s">
         <v>70</v>
@@ -8260,10 +8555,10 @@
     </row>
     <row r="12" spans="1:10" ht="25.5">
       <c r="A12" s="18" t="s">
-        <v>550</v>
+        <v>548</v>
       </c>
       <c r="B12" s="20" t="s">
-        <v>551</v>
+        <v>549</v>
       </c>
       <c r="D12" t="s">
         <v>70</v>
@@ -8273,10 +8568,10 @@
     </row>
     <row r="13" spans="1:10" ht="25.5">
       <c r="A13" s="18" t="s">
-        <v>552</v>
+        <v>550</v>
       </c>
       <c r="B13" s="20" t="s">
-        <v>553</v>
+        <v>551</v>
       </c>
       <c r="D13" t="s">
         <v>70</v>
@@ -8286,10 +8581,10 @@
     </row>
     <row r="14" spans="1:10" ht="63.75">
       <c r="A14" s="18" t="s">
-        <v>554</v>
+        <v>552</v>
       </c>
       <c r="B14" s="20" t="s">
-        <v>555</v>
+        <v>553</v>
       </c>
       <c r="D14" t="s">
         <v>70</v>
@@ -8309,7 +8604,7 @@
         <v>261</v>
       </c>
       <c r="C16" s="18" t="s">
-        <v>587</v>
+        <v>585</v>
       </c>
       <c r="D16" t="s">
         <v>70</v>
@@ -8335,10 +8630,10 @@
     </row>
     <row r="17" spans="1:10" ht="25.5">
       <c r="A17" s="18" t="s">
-        <v>556</v>
+        <v>554</v>
       </c>
       <c r="B17" s="21" t="s">
-        <v>551</v>
+        <v>549</v>
       </c>
       <c r="D17" t="s">
         <v>70</v>
@@ -8348,10 +8643,10 @@
     </row>
     <row r="18" spans="1:10" ht="63.75">
       <c r="A18" s="18" t="s">
-        <v>557</v>
+        <v>555</v>
       </c>
       <c r="B18" s="21" t="s">
-        <v>558</v>
+        <v>556</v>
       </c>
       <c r="D18" t="s">
         <v>70</v>
@@ -8361,7 +8656,7 @@
     </row>
     <row r="19" spans="1:10">
       <c r="A19" s="18" t="s">
-        <v>559</v>
+        <v>557</v>
       </c>
       <c r="B19" s="18" t="s">
         <v>322</v>
@@ -8374,10 +8669,10 @@
     </row>
     <row r="20" spans="1:10" ht="51">
       <c r="A20" s="18" t="s">
-        <v>560</v>
+        <v>558</v>
       </c>
       <c r="B20" s="21" t="s">
-        <v>561</v>
+        <v>559</v>
       </c>
       <c r="D20" t="s">
         <v>70</v>
@@ -8396,7 +8691,7 @@
         <v>293</v>
       </c>
       <c r="C22" t="s">
-        <v>539</v>
+        <v>537</v>
       </c>
       <c r="D22" t="s">
         <v>254</v>
@@ -8422,7 +8717,7 @@
     </row>
     <row r="23" spans="1:10">
       <c r="A23" t="s">
-        <v>529</v>
+        <v>527</v>
       </c>
       <c r="B23" s="18" t="s">
         <v>384</v>
@@ -8430,18 +8725,18 @@
     </row>
     <row r="24" spans="1:10">
       <c r="A24" t="s">
-        <v>530</v>
+        <v>528</v>
       </c>
       <c r="B24" s="18" t="s">
-        <v>533</v>
+        <v>531</v>
       </c>
     </row>
     <row r="25" spans="1:10">
       <c r="A25" t="s">
-        <v>531</v>
+        <v>529</v>
       </c>
       <c r="B25" s="18" t="s">
-        <v>532</v>
+        <v>530</v>
       </c>
     </row>
     <row r="26" spans="1:10">

</xml_diff>

<commit_message>
implemented two user stories
us 29, us 30 and complete the report
</commit_message>
<xml_diff>
--- a/Team05Report.xlsx
+++ b/Team05Report.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="240" windowWidth="20730" windowHeight="11760" tabRatio="500" firstSheet="1" activeTab="9"/>
+    <workbookView xWindow="240" yWindow="240" windowWidth="20730" windowHeight="11760" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Team" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
     <sheet name="Sprint4" sheetId="6" r:id="rId9"/>
     <sheet name="Sprint5" sheetId="8" r:id="rId10"/>
   </sheets>
-  <calcPr calcId="124519" concurrentCalc="0"/>
+  <calcPr calcId="145621" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -62,7 +62,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1366" uniqueCount="636">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1426" uniqueCount="667">
   <si>
     <t>Date</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -2030,17 +2030,110 @@
   </si>
   <si>
     <t>By using their birth date find the age difference</t>
+  </si>
+  <si>
+    <t>AT94</t>
+  </si>
+  <si>
+    <t>AT95</t>
+  </si>
+  <si>
+    <t>AT96</t>
+  </si>
+  <si>
+    <t>AT97</t>
+  </si>
+  <si>
+    <t>Child I1 (Jacky /Gao/)  of family F2 was born ( 27 JAN 1970)  before before parents' marriage.(7 JUL 1970)</t>
+  </si>
+  <si>
+    <t>AT98</t>
+  </si>
+  <si>
+    <t>Child I3 (Katie /Brown/)  of family F4 was born ( 14 FEB 1874)  before before parents' marriage.(1 JAN 1996)</t>
+  </si>
+  <si>
+    <t>Child I3 (Katie /Brown/)  of family F4 was married (7 JUL 1970)  before before parents' marriage.(1 JAN 1996)</t>
+  </si>
+  <si>
+    <t>child I3 of family F4 was married on 7 JUL 1970, parents' of family F4 was married on 1 Jan 1996</t>
+  </si>
+  <si>
+    <t>child  I6 of family F2 was born on 11 SEP 1970, parents' was married on 7 JUL 1970</t>
+  </si>
+  <si>
+    <t>child  I3 of family F4 was born on 14 FEB 1874, parents' was married on 1 Jan 1996</t>
+  </si>
+  <si>
+    <t>child  I1 of Family F2 was born on 27 Jan 1970, parents' was married on 7 JUL 1970</t>
+  </si>
+  <si>
+    <t>child  I1 of Family F2 was married on 1 Jan 1996, parents' of family f2 was married on 7 JUL 1970</t>
+  </si>
+  <si>
+    <t>AT94~96</t>
+  </si>
+  <si>
+    <t>AT97~98</t>
+  </si>
+  <si>
+    <t>T29.01</t>
+  </si>
+  <si>
+    <t>T29.02</t>
+  </si>
+  <si>
+    <t>T29.03</t>
+  </si>
+  <si>
+    <t>T29.04</t>
+  </si>
+  <si>
+    <t>get access to every child's record of each family</t>
+  </si>
+  <si>
+    <t>compare the child's birthday with parents' marriage date</t>
+  </si>
+  <si>
+    <t>if child was born before parent's marriage, return error message</t>
+  </si>
+  <si>
+    <t>T30.01</t>
+  </si>
+  <si>
+    <t>T30.02</t>
+  </si>
+  <si>
+    <t>T30.03</t>
+  </si>
+  <si>
+    <t>T30.04</t>
+  </si>
+  <si>
+    <t>get access to every child's fams record</t>
+  </si>
+  <si>
+    <t>if the child was married, get his/her marriage date</t>
+  </si>
+  <si>
+    <t>compare child's marriage date with parents'</t>
+  </si>
+  <si>
+    <t>T30.05</t>
+  </si>
+  <si>
+    <t>if the child was married before parents', return error message</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="m/d"/>
     <numFmt numFmtId="165" formatCode="0.0"/>
   </numFmts>
-  <fonts count="10">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Verdana"/>
@@ -2278,11 +2371,22 @@
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="1"/>
   <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
   <c:chart>
+    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
       <c:lineChart>
         <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
@@ -2306,6 +2410,9 @@
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>40644</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>40657</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2331,44 +2438,64 @@
                 <c:pt idx="4">
                   <c:v>6</c:v>
                 </c:pt>
+                <c:pt idx="5">
+                  <c:v>0</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:smooth val="0"/>
         </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
         <c:marker val="1"/>
-        <c:axId val="89646976"/>
-        <c:axId val="89648512"/>
+        <c:smooth val="0"/>
+        <c:axId val="42742144"/>
+        <c:axId val="42743680"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="89646976"/>
+        <c:axId val="42742144"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="b"/>
         <c:numFmt formatCode="m/d" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="89648512"/>
+        <c:crossAx val="42743680"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
         <c:baseTimeUnit val="days"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="89648512"/>
+        <c:axId val="42743680"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="89646976"/>
+        <c:crossAx val="42742144"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
@@ -2732,14 +2859,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView zoomScale="150" workbookViewId="0">
       <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="7.625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="6.375" customWidth="1"/>
@@ -2748,7 +2875,7 @@
     <col min="5" max="5" width="19.25" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="4" customFormat="1">
+    <row r="1" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>22</v>
       </c>
@@ -2765,7 +2892,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>70</v>
       </c>
@@ -2782,7 +2909,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>128</v>
       </c>
@@ -2799,7 +2926,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>254</v>
       </c>
@@ -2816,7 +2943,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="9" spans="1:5">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="D9" s="4" t="s">
         <v>67</v>
       </c>
@@ -2845,19 +2972,19 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J23"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:J34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="150" workbookViewId="0">
-      <selection activeCell="I8" sqref="I8"/>
+    <sheetView topLeftCell="A28" zoomScale="150" workbookViewId="0">
+      <selection activeCell="B39" sqref="B37:B39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="25.375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>3</v>
       </c>
@@ -2889,7 +3016,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:10">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>95</v>
       </c>
@@ -2921,7 +3048,7 @@
         <v>40652</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="25.5">
+    <row r="4" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A4" s="18" t="s">
         <v>599</v>
       </c>
@@ -2932,7 +3059,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="25.5">
+    <row r="5" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A5" s="18" t="s">
         <v>600</v>
       </c>
@@ -2943,7 +3070,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="6" spans="1:10" ht="38.25">
+    <row r="6" spans="1:10" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A6" s="18" t="s">
         <v>602</v>
       </c>
@@ -2954,7 +3081,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="8" spans="1:10">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>307</v>
       </c>
@@ -2983,7 +3110,7 @@
         <v>40656</v>
       </c>
     </row>
-    <row r="9" spans="1:10">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>627</v>
       </c>
@@ -2994,7 +3121,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="10" spans="1:10">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>628</v>
       </c>
@@ -3005,7 +3132,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="11" spans="1:10">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>629</v>
       </c>
@@ -3016,7 +3143,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="12" spans="1:10">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>340</v>
       </c>
@@ -3048,7 +3175,7 @@
         <v>40652</v>
       </c>
     </row>
-    <row r="14" spans="1:10" ht="25.5">
+    <row r="14" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A14" s="18" t="s">
         <v>609</v>
       </c>
@@ -3059,7 +3186,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="15" spans="1:10" ht="38.25">
+    <row r="15" spans="1:10" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A15" s="18" t="s">
         <v>610</v>
       </c>
@@ -3070,7 +3197,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="16" spans="1:10" ht="38.25">
+    <row r="16" spans="1:10" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A16" s="18" t="s">
         <v>611</v>
       </c>
@@ -3081,7 +3208,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="18" spans="1:10">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>342</v>
       </c>
@@ -3110,7 +3237,7 @@
         <v>40656</v>
       </c>
     </row>
-    <row r="19" spans="1:10" ht="25.5">
+    <row r="19" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>631</v>
       </c>
@@ -3121,7 +3248,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="20" spans="1:10" ht="25.5">
+    <row r="20" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>632</v>
       </c>
@@ -3132,7 +3259,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="21" spans="1:10" ht="25.5">
+    <row r="21" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>633</v>
       </c>
@@ -3143,38 +3270,167 @@
         <v>254</v>
       </c>
     </row>
-    <row r="22" spans="1:10">
-      <c r="A22" t="s">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B22" s="20"/>
+      <c r="D22" s="18"/>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
         <v>343</v>
       </c>
-      <c r="B22" s="18" t="s">
+      <c r="B23" s="18" t="s">
         <v>354</v>
       </c>
-      <c r="D22" s="18" t="s">
-        <v>70</v>
-      </c>
-      <c r="F22">
-        <v>35</v>
-      </c>
-      <c r="G22">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="23" spans="1:10">
-      <c r="A23" t="s">
-        <v>344</v>
-      </c>
-      <c r="B23" s="18" t="s">
-        <v>352</v>
+      <c r="C23" s="18" t="s">
+        <v>649</v>
       </c>
       <c r="D23" s="18" t="s">
         <v>70</v>
       </c>
+      <c r="E23" s="18" t="s">
+        <v>329</v>
+      </c>
       <c r="F23">
+        <v>35</v>
+      </c>
+      <c r="G23">
+        <v>40</v>
+      </c>
+      <c r="H23">
+        <v>15</v>
+      </c>
+      <c r="I23">
+        <v>10</v>
+      </c>
+      <c r="J23" s="16">
+        <v>40657</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>651</v>
+      </c>
+      <c r="B24" s="20" t="s">
+        <v>322</v>
+      </c>
+      <c r="C24" s="18"/>
+      <c r="D24" s="18"/>
+      <c r="E24" s="18"/>
+      <c r="J24" s="16"/>
+    </row>
+    <row r="25" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>652</v>
+      </c>
+      <c r="B25" s="20" t="s">
+        <v>655</v>
+      </c>
+      <c r="C25" s="18"/>
+      <c r="D25" s="18"/>
+      <c r="E25" s="18"/>
+      <c r="J25" s="16"/>
+    </row>
+    <row r="26" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>653</v>
+      </c>
+      <c r="B26" s="20" t="s">
+        <v>656</v>
+      </c>
+      <c r="C26" s="18"/>
+      <c r="D26" s="18"/>
+      <c r="E26" s="18"/>
+      <c r="J26" s="16"/>
+    </row>
+    <row r="27" spans="1:10" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>654</v>
+      </c>
+      <c r="B27" s="20" t="s">
+        <v>657</v>
+      </c>
+      <c r="C27" s="18"/>
+      <c r="D27" s="18"/>
+      <c r="E27" s="18"/>
+      <c r="J27" s="16"/>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B28" s="18"/>
+      <c r="C28" s="18"/>
+      <c r="D28" s="18"/>
+      <c r="E28" s="18"/>
+      <c r="J28" s="16"/>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>344</v>
+      </c>
+      <c r="B29" s="18" t="s">
+        <v>352</v>
+      </c>
+      <c r="C29" s="18" t="s">
+        <v>650</v>
+      </c>
+      <c r="D29" s="18" t="s">
+        <v>70</v>
+      </c>
+      <c r="E29" s="18" t="s">
+        <v>329</v>
+      </c>
+      <c r="F29">
         <v>30</v>
       </c>
-      <c r="G23">
+      <c r="G29">
         <v>35</v>
+      </c>
+      <c r="H29">
+        <v>18</v>
+      </c>
+      <c r="I29">
+        <v>15</v>
+      </c>
+      <c r="J29" s="16">
+        <v>40657</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>658</v>
+      </c>
+      <c r="B30" s="20" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>659</v>
+      </c>
+      <c r="B31" s="20" t="s">
+        <v>662</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>660</v>
+      </c>
+      <c r="B32" s="20" t="s">
+        <v>663</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>661</v>
+      </c>
+      <c r="B33" s="20" t="s">
+        <v>664</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>665</v>
+      </c>
+      <c r="B34" s="20" t="s">
+        <v>666</v>
       </c>
     </row>
   </sheetData>
@@ -3189,14 +3445,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L31"/>
   <sheetViews>
-    <sheetView topLeftCell="A14" zoomScale="150" workbookViewId="0">
-      <selection activeCell="N32" sqref="N32"/>
+    <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
+      <selection activeCell="I29" sqref="I26:I29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="6.625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="8.875" bestFit="1" customWidth="1"/>
@@ -3212,7 +3468,7 @@
     <col min="12" max="12" width="10.75" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="4" customFormat="1">
+    <row r="1" spans="1:12" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>40</v>
       </c>
@@ -3250,7 +3506,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:12">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -3288,7 +3544,7 @@
         <v>40598</v>
       </c>
     </row>
-    <row r="3" spans="1:12">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>1</v>
       </c>
@@ -3326,7 +3582,7 @@
         <v>40598</v>
       </c>
     </row>
-    <row r="4" spans="1:12">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>1</v>
       </c>
@@ -3364,7 +3620,7 @@
         <v>40598</v>
       </c>
     </row>
-    <row r="5" spans="1:12">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>1</v>
       </c>
@@ -3402,7 +3658,7 @@
         <v>40598</v>
       </c>
     </row>
-    <row r="6" spans="1:12">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>1</v>
       </c>
@@ -3440,7 +3696,7 @@
         <v>40598</v>
       </c>
     </row>
-    <row r="7" spans="1:12">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>1</v>
       </c>
@@ -3478,7 +3734,7 @@
         <v>40598</v>
       </c>
     </row>
-    <row r="8" spans="1:12">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>2</v>
       </c>
@@ -3516,7 +3772,7 @@
         <v>40598</v>
       </c>
     </row>
-    <row r="9" spans="1:12">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>2</v>
       </c>
@@ -3554,7 +3810,7 @@
         <v>40598</v>
       </c>
     </row>
-    <row r="10" spans="1:12">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>2</v>
       </c>
@@ -3592,7 +3848,7 @@
         <v>40598</v>
       </c>
     </row>
-    <row r="11" spans="1:12">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>2</v>
       </c>
@@ -3630,7 +3886,7 @@
         <v>40598</v>
       </c>
     </row>
-    <row r="12" spans="1:12">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>2</v>
       </c>
@@ -3668,7 +3924,7 @@
         <v>40598</v>
       </c>
     </row>
-    <row r="13" spans="1:12">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>2</v>
       </c>
@@ -3706,7 +3962,7 @@
         <v>40598</v>
       </c>
     </row>
-    <row r="14" spans="1:12">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>3</v>
       </c>
@@ -3744,7 +4000,7 @@
         <v>40598</v>
       </c>
     </row>
-    <row r="15" spans="1:12">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>3</v>
       </c>
@@ -3782,7 +4038,7 @@
         <v>40598</v>
       </c>
     </row>
-    <row r="16" spans="1:12">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>3</v>
       </c>
@@ -3820,7 +4076,7 @@
         <v>40598</v>
       </c>
     </row>
-    <row r="17" spans="1:12">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>3</v>
       </c>
@@ -3858,7 +4114,7 @@
         <v>40598</v>
       </c>
     </row>
-    <row r="18" spans="1:12">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>3</v>
       </c>
@@ -3896,7 +4152,7 @@
         <v>40598</v>
       </c>
     </row>
-    <row r="19" spans="1:12">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>3</v>
       </c>
@@ -3934,7 +4190,7 @@
         <v>40598</v>
       </c>
     </row>
-    <row r="20" spans="1:12">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>4</v>
       </c>
@@ -3972,7 +4228,7 @@
         <v>40598</v>
       </c>
     </row>
-    <row r="21" spans="1:12">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>4</v>
       </c>
@@ -4010,7 +4266,7 @@
         <v>40598</v>
       </c>
     </row>
-    <row r="22" spans="1:12">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>4</v>
       </c>
@@ -4048,7 +4304,7 @@
         <v>40598</v>
       </c>
     </row>
-    <row r="23" spans="1:12">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>4</v>
       </c>
@@ -4086,7 +4342,7 @@
         <v>40602</v>
       </c>
     </row>
-    <row r="24" spans="1:12">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>4</v>
       </c>
@@ -4124,7 +4380,7 @@
         <v>40602</v>
       </c>
     </row>
-    <row r="25" spans="1:12">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>4</v>
       </c>
@@ -4162,7 +4418,7 @@
         <v>40602</v>
       </c>
     </row>
-    <row r="26" spans="1:12">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>5</v>
       </c>
@@ -4200,7 +4456,7 @@
         <v>40610</v>
       </c>
     </row>
-    <row r="27" spans="1:12">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>5</v>
       </c>
@@ -4238,7 +4494,7 @@
         <v>40610</v>
       </c>
     </row>
-    <row r="28" spans="1:12">
+    <row r="28" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>5</v>
       </c>
@@ -4276,7 +4532,7 @@
         <v>40610</v>
       </c>
     </row>
-    <row r="29" spans="1:12">
+    <row r="29" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>5</v>
       </c>
@@ -4314,7 +4570,7 @@
         <v>40610</v>
       </c>
     </row>
-    <row r="30" spans="1:12">
+    <row r="30" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>5</v>
       </c>
@@ -4324,11 +4580,35 @@
       <c r="C30" s="18" t="s">
         <v>354</v>
       </c>
+      <c r="D30" s="18" t="s">
+        <v>649</v>
+      </c>
+      <c r="E30" s="18" t="s">
+        <v>70</v>
+      </c>
+      <c r="F30" s="18" t="s">
+        <v>329</v>
+      </c>
+      <c r="G30">
+        <v>35</v>
+      </c>
+      <c r="H30">
+        <v>40</v>
+      </c>
+      <c r="I30">
+        <v>15</v>
+      </c>
+      <c r="J30">
+        <v>10</v>
+      </c>
+      <c r="K30" s="16">
+        <v>40657</v>
+      </c>
       <c r="L30" s="7">
         <v>40610</v>
       </c>
     </row>
-    <row r="31" spans="1:12">
+    <row r="31" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>5</v>
       </c>
@@ -4337,6 +4617,30 @@
       </c>
       <c r="C31" s="18" t="s">
         <v>352</v>
+      </c>
+      <c r="D31" s="18" t="s">
+        <v>650</v>
+      </c>
+      <c r="E31" s="18" t="s">
+        <v>70</v>
+      </c>
+      <c r="F31" s="18" t="s">
+        <v>329</v>
+      </c>
+      <c r="G31">
+        <v>30</v>
+      </c>
+      <c r="H31">
+        <v>35</v>
+      </c>
+      <c r="I31">
+        <v>18</v>
+      </c>
+      <c r="J31">
+        <v>15</v>
+      </c>
+      <c r="K31" s="16">
+        <v>40657</v>
       </c>
       <c r="L31" s="7">
         <v>40610</v>
@@ -4355,14 +4659,14 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F31"/>
   <sheetViews>
-    <sheetView topLeftCell="A23" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="D29" sqref="D29"/>
+    <sheetView topLeftCell="A22" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="D31" sqref="D31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="8.875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="24.75" bestFit="1" customWidth="1"/>
@@ -4371,7 +4675,7 @@
     <col min="6" max="6" width="9" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>28</v>
       </c>
@@ -4391,7 +4695,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="25.5">
+    <row r="2" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>31</v>
       </c>
@@ -4411,7 +4715,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="25.5">
+    <row r="3" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>32</v>
       </c>
@@ -4431,7 +4735,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>34</v>
       </c>
@@ -4451,7 +4755,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>74</v>
       </c>
@@ -4471,7 +4775,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>75</v>
       </c>
@@ -4491,7 +4795,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="7" spans="1:6">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>76</v>
       </c>
@@ -4511,7 +4815,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="8" spans="1:6">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>77</v>
       </c>
@@ -4531,7 +4835,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:6">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>78</v>
       </c>
@@ -4551,7 +4855,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="10" spans="1:6">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>79</v>
       </c>
@@ -4571,7 +4875,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="11" spans="1:6">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>80</v>
       </c>
@@ -4591,7 +4895,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:6">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>81</v>
       </c>
@@ -4611,7 +4915,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:6">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>82</v>
       </c>
@@ -4631,7 +4935,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="25.5">
+    <row r="14" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A14" s="18" t="s">
         <v>83</v>
       </c>
@@ -4651,7 +4955,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="15" spans="1:6">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>84</v>
       </c>
@@ -4671,7 +4975,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="16" spans="1:6">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>85</v>
       </c>
@@ -4691,7 +4995,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="17" spans="1:6">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>86</v>
       </c>
@@ -4711,7 +5015,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="18" spans="1:6">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>87</v>
       </c>
@@ -4731,7 +5035,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="19" spans="1:6" ht="25.5">
+    <row r="19" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>88</v>
       </c>
@@ -4751,7 +5055,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="20" spans="1:6">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>89</v>
       </c>
@@ -4771,7 +5075,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="21" spans="1:6">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>90</v>
       </c>
@@ -4791,7 +5095,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="22" spans="1:6">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>91</v>
       </c>
@@ -4811,7 +5115,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="23" spans="1:6" ht="25.5">
+    <row r="23" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>92</v>
       </c>
@@ -4831,7 +5135,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="24" spans="1:6" ht="25.5">
+    <row r="24" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>93</v>
       </c>
@@ -4851,7 +5155,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="25" spans="1:6" ht="38.25">
+    <row r="25" spans="1:6" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>94</v>
       </c>
@@ -4871,7 +5175,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="26" spans="1:6">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>95</v>
       </c>
@@ -4891,7 +5195,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="27" spans="1:6" ht="25.5">
+    <row r="27" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>307</v>
       </c>
@@ -4911,7 +5215,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="28" spans="1:6" ht="25.5">
+    <row r="28" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>340</v>
       </c>
@@ -4931,7 +5235,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="29" spans="1:6">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>342</v>
       </c>
@@ -4951,7 +5255,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="30" spans="1:6">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>343</v>
       </c>
@@ -4961,6 +5265,9 @@
       <c r="C30" s="1" t="s">
         <v>353</v>
       </c>
+      <c r="D30" s="18" t="s">
+        <v>649</v>
+      </c>
       <c r="E30">
         <v>35</v>
       </c>
@@ -4968,7 +5275,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="31" spans="1:6">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>344</v>
       </c>
@@ -4977,6 +5284,9 @@
       </c>
       <c r="C31" s="1" t="s">
         <v>355</v>
+      </c>
+      <c r="D31" s="18" t="s">
+        <v>650</v>
       </c>
       <c r="E31">
         <v>30</v>
@@ -4997,14 +5307,14 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F100"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F101"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" zoomScale="145" zoomScaleNormal="145" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="A95" sqref="A95"/>
+    <sheetView topLeftCell="A91" zoomScale="145" zoomScaleNormal="145" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="B98" sqref="B98"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="6.375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="8.875" bestFit="1" customWidth="1"/>
@@ -5014,7 +5324,7 @@
     <col min="6" max="6" width="7.25" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>61</v>
       </c>
@@ -5034,7 +5344,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="47.25">
+    <row r="2" spans="1:6" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>54</v>
       </c>
@@ -5054,7 +5364,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="47.25">
+    <row r="3" spans="1:6" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>55</v>
       </c>
@@ -5074,7 +5384,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="47.25">
+    <row r="4" spans="1:6" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>56</v>
       </c>
@@ -5094,7 +5404,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="47.25">
+    <row r="5" spans="1:6" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>57</v>
       </c>
@@ -5114,7 +5424,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="47.25">
+    <row r="6" spans="1:6" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>58</v>
       </c>
@@ -5134,7 +5444,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="31.5">
+    <row r="7" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>59</v>
       </c>
@@ -5154,7 +5464,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="63">
+    <row r="8" spans="1:6" ht="63" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>150</v>
       </c>
@@ -5174,7 +5484,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="63">
+    <row r="9" spans="1:6" ht="63" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>154</v>
       </c>
@@ -5194,7 +5504,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="78.75">
+    <row r="10" spans="1:6" ht="78.75" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>155</v>
       </c>
@@ -5214,7 +5524,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="63">
+    <row r="11" spans="1:6" ht="63" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>157</v>
       </c>
@@ -5234,7 +5544,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="63">
+    <row r="12" spans="1:6" ht="63" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>158</v>
       </c>
@@ -5254,7 +5564,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="78.75">
+    <row r="13" spans="1:6" ht="78.75" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>159</v>
       </c>
@@ -5274,7 +5584,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="47.25">
+    <row r="14" spans="1:6" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>170</v>
       </c>
@@ -5294,7 +5604,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="47.25">
+    <row r="15" spans="1:6" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>172</v>
       </c>
@@ -5314,7 +5624,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="16" spans="1:6" ht="38.25">
+    <row r="16" spans="1:6" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>188</v>
       </c>
@@ -5334,7 +5644,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="17" spans="1:6" ht="38.25">
+    <row r="17" spans="1:6" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>189</v>
       </c>
@@ -5354,7 +5664,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="18" spans="1:6" ht="38.25">
+    <row r="18" spans="1:6" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>190</v>
       </c>
@@ -5374,7 +5684,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="19" spans="1:6" ht="38.25">
+    <row r="19" spans="1:6" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>191</v>
       </c>
@@ -5394,7 +5704,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="20" spans="1:6" ht="26.25">
+    <row r="20" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>192</v>
       </c>
@@ -5414,7 +5724,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="21" spans="1:6" ht="47.25">
+    <row r="21" spans="1:6" ht="47.25" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>193</v>
       </c>
@@ -5434,7 +5744,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="22" spans="1:6" ht="47.25">
+    <row r="22" spans="1:6" ht="47.25" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>194</v>
       </c>
@@ -5454,7 +5764,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="23" spans="1:6" ht="37.5" customHeight="1">
+    <row r="23" spans="1:6" ht="37.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>195</v>
       </c>
@@ -5474,7 +5784,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="24" spans="1:6" ht="26.25">
+    <row r="24" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>196</v>
       </c>
@@ -5494,7 +5804,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="25" spans="1:6" ht="25.5">
+    <row r="25" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>197</v>
       </c>
@@ -5514,7 +5824,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="26" spans="1:6">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>198</v>
       </c>
@@ -5534,7 +5844,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="27" spans="1:6" ht="25.5">
+    <row r="27" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>199</v>
       </c>
@@ -5554,7 +5864,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="28" spans="1:6" ht="25.5">
+    <row r="28" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>200</v>
       </c>
@@ -5574,7 +5884,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="29" spans="1:6" ht="25.5">
+    <row r="29" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>201</v>
       </c>
@@ -5594,7 +5904,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="30" spans="1:6" ht="38.25">
+    <row r="30" spans="1:6" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>202</v>
       </c>
@@ -5614,7 +5924,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="31" spans="1:6" ht="51">
+    <row r="31" spans="1:6" ht="51" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>203</v>
       </c>
@@ -5634,7 +5944,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="32" spans="1:6" ht="26.25">
+    <row r="32" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>204</v>
       </c>
@@ -5654,7 +5964,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="33" spans="1:6" ht="25.5">
+    <row r="33" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>205</v>
       </c>
@@ -5674,7 +5984,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="34" spans="1:6" ht="26.25">
+    <row r="34" spans="1:6" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>206</v>
       </c>
@@ -5694,7 +6004,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="35" spans="1:6" ht="25.5">
+    <row r="35" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>207</v>
       </c>
@@ -5714,7 +6024,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="36" spans="1:6" ht="38.25">
+    <row r="36" spans="1:6" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>208</v>
       </c>
@@ -5734,7 +6044,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="37" spans="1:6" ht="38.25">
+    <row r="37" spans="1:6" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>209</v>
       </c>
@@ -5754,7 +6064,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="38" spans="1:6" ht="38.25">
+    <row r="38" spans="1:6" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>210</v>
       </c>
@@ -5774,7 +6084,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="39" spans="1:6" ht="25.5">
+    <row r="39" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>211</v>
       </c>
@@ -5794,7 +6104,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="40" spans="1:6" ht="38.25">
+    <row r="40" spans="1:6" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>212</v>
       </c>
@@ -5814,7 +6124,7 @@
         <v>401</v>
       </c>
     </row>
-    <row r="41" spans="1:6" ht="25.5">
+    <row r="41" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>213</v>
       </c>
@@ -5834,7 +6144,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="42" spans="1:6" ht="38.25">
+    <row r="42" spans="1:6" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>214</v>
       </c>
@@ -5854,7 +6164,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="43" spans="1:6" ht="25.5">
+    <row r="43" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>215</v>
       </c>
@@ -5874,7 +6184,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="44" spans="1:6" ht="25.5">
+    <row r="44" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>216</v>
       </c>
@@ -5894,7 +6204,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="45" spans="1:6" ht="51">
+    <row r="45" spans="1:6" ht="51" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>217</v>
       </c>
@@ -5914,7 +6224,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="46" spans="1:6" ht="51">
+    <row r="46" spans="1:6" ht="51" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>218</v>
       </c>
@@ -5934,7 +6244,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="47" spans="1:6" ht="51">
+    <row r="47" spans="1:6" ht="51" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>219</v>
       </c>
@@ -5954,7 +6264,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="48" spans="1:6" ht="51">
+    <row r="48" spans="1:6" ht="51" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>220</v>
       </c>
@@ -5974,7 +6284,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="49" spans="1:6" ht="25.5">
+    <row r="49" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>221</v>
       </c>
@@ -5994,7 +6304,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="50" spans="1:6" ht="51">
+    <row r="50" spans="1:6" ht="51" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>222</v>
       </c>
@@ -6014,7 +6324,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="51" spans="1:6" ht="25.5">
+    <row r="51" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>223</v>
       </c>
@@ -6034,7 +6344,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="52" spans="1:6" ht="51">
+    <row r="52" spans="1:6" ht="51" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>224</v>
       </c>
@@ -6054,7 +6364,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="53" spans="1:6" ht="51">
+    <row r="53" spans="1:6" ht="51" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>225</v>
       </c>
@@ -6074,7 +6384,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="54" spans="1:6" ht="51">
+    <row r="54" spans="1:6" ht="51" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>226</v>
       </c>
@@ -6094,7 +6404,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="55" spans="1:6" ht="51">
+    <row r="55" spans="1:6" ht="51" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>227</v>
       </c>
@@ -6114,7 +6424,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="56" spans="1:6">
+    <row r="56" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>228</v>
       </c>
@@ -6134,7 +6444,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="57" spans="1:6">
+    <row r="57" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>229</v>
       </c>
@@ -6154,7 +6464,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="58" spans="1:6" ht="51">
+    <row r="58" spans="1:6" ht="51" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>230</v>
       </c>
@@ -6174,7 +6484,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="59" spans="1:6" ht="25.5">
+    <row r="59" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>231</v>
       </c>
@@ -6194,7 +6504,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="60" spans="1:6" ht="25.5">
+    <row r="60" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>232</v>
       </c>
@@ -6214,7 +6524,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="61" spans="1:6">
+    <row r="61" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>233</v>
       </c>
@@ -6234,7 +6544,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="62" spans="1:6" ht="25.5">
+    <row r="62" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
         <v>234</v>
       </c>
@@ -6254,7 +6564,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="63" spans="1:6" ht="25.5">
+    <row r="63" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>368</v>
       </c>
@@ -6274,7 +6584,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="64" spans="1:6" ht="25.5">
+    <row r="64" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
         <v>369</v>
       </c>
@@ -6294,7 +6604,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="65" spans="1:6" ht="25.5">
+    <row r="65" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
         <v>370</v>
       </c>
@@ -6314,7 +6624,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="66" spans="1:6">
+    <row r="66" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
         <v>371</v>
       </c>
@@ -6334,7 +6644,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="67" spans="1:6">
+    <row r="67" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
         <v>372</v>
       </c>
@@ -6354,7 +6664,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="68" spans="1:6" ht="25.5">
+    <row r="68" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
         <v>373</v>
       </c>
@@ -6374,7 +6684,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="69" spans="1:6" ht="25.5">
+    <row r="69" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
         <v>374</v>
       </c>
@@ -6394,7 +6704,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="70" spans="1:6" ht="25.5">
+    <row r="70" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
         <v>375</v>
       </c>
@@ -6414,7 +6724,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="71" spans="1:6" ht="25.5">
+    <row r="71" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
         <v>376</v>
       </c>
@@ -6434,7 +6744,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="72" spans="1:6" ht="25.5">
+    <row r="72" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
         <v>377</v>
       </c>
@@ -6454,7 +6764,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="73" spans="1:6" ht="25.5">
+    <row r="73" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
         <v>378</v>
       </c>
@@ -6474,7 +6784,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="74" spans="1:6" ht="51">
+    <row r="74" spans="1:6" ht="51" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
         <v>379</v>
       </c>
@@ -6494,7 +6804,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="75" spans="1:6" ht="25.5">
+    <row r="75" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
         <v>380</v>
       </c>
@@ -6514,7 +6824,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="76" spans="1:6" ht="25.5">
+    <row r="76" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
         <v>381</v>
       </c>
@@ -6534,7 +6844,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="77" spans="1:6" ht="25.5">
+    <row r="77" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
         <v>382</v>
       </c>
@@ -6554,7 +6864,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="78" spans="1:6" ht="25.5">
+    <row r="78" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A78" s="18" t="s">
         <v>560</v>
       </c>
@@ -6574,7 +6884,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="79" spans="1:6" ht="25.5">
+    <row r="79" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
         <v>561</v>
       </c>
@@ -6594,7 +6904,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="80" spans="1:6" ht="25.5">
+    <row r="80" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A80" s="18" t="s">
         <v>562</v>
       </c>
@@ -6614,7 +6924,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="81" spans="1:6" ht="25.5">
+    <row r="81" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
         <v>563</v>
       </c>
@@ -6634,7 +6944,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="82" spans="1:6" ht="25.5">
+    <row r="82" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A82" s="18" t="s">
         <v>564</v>
       </c>
@@ -6654,7 +6964,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="83" spans="1:6" ht="25.5">
+    <row r="83" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
         <v>565</v>
       </c>
@@ -6674,7 +6984,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="84" spans="1:6" ht="25.5">
+    <row r="84" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A84" s="18" t="s">
         <v>566</v>
       </c>
@@ -6694,7 +7004,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="85" spans="1:6" ht="25.5">
+    <row r="85" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
         <v>567</v>
       </c>
@@ -6714,7 +7024,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="86" spans="1:6" ht="25.5">
+    <row r="86" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A86" s="18" t="s">
         <v>568</v>
       </c>
@@ -6734,7 +7044,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="87" spans="1:6" ht="38.25">
+    <row r="87" spans="1:6" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A87" s="18" t="s">
         <v>591</v>
       </c>
@@ -6754,7 +7064,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="88" spans="1:6" ht="25.5">
+    <row r="88" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A88" s="18" t="s">
         <v>592</v>
       </c>
@@ -6774,7 +7084,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="89" spans="1:6" ht="63.75">
+    <row r="89" spans="1:6" ht="63.75" x14ac:dyDescent="0.2">
       <c r="A89" s="18" t="s">
         <v>593</v>
       </c>
@@ -6794,7 +7104,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="90" spans="1:6" ht="25.5">
+    <row r="90" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A90" s="18" t="s">
         <v>594</v>
       </c>
@@ -6814,7 +7124,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="91" spans="1:6" ht="25.5">
+    <row r="91" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A91" s="18" t="s">
         <v>615</v>
       </c>
@@ -6834,7 +7144,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="92" spans="1:6" ht="25.5">
+    <row r="92" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A92" s="18" t="s">
         <v>618</v>
       </c>
@@ -6854,7 +7164,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="93" spans="1:6" ht="51">
+    <row r="93" spans="1:6" ht="51" x14ac:dyDescent="0.2">
       <c r="A93" s="18" t="s">
         <v>620</v>
       </c>
@@ -6874,7 +7184,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="94" spans="1:6" ht="38.25">
+    <row r="94" spans="1:6" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A94" s="18" t="s">
         <v>623</v>
       </c>
@@ -6894,14 +7204,108 @@
         <v>53</v>
       </c>
     </row>
-    <row r="96" spans="1:6">
-      <c r="A96" s="18"/>
-    </row>
-    <row r="98" spans="1:1">
-      <c r="A98" s="18"/>
-    </row>
-    <row r="100" spans="1:1">
-      <c r="A100" s="18"/>
+    <row r="95" spans="1:6" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A95" s="18" t="s">
+        <v>636</v>
+      </c>
+      <c r="B95" t="s">
+        <v>343</v>
+      </c>
+      <c r="C95" s="18" t="s">
+        <v>354</v>
+      </c>
+      <c r="D95" s="1" t="s">
+        <v>647</v>
+      </c>
+      <c r="E95" s="1" t="s">
+        <v>640</v>
+      </c>
+      <c r="F95" s="18" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="96" spans="1:6" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A96" s="18" t="s">
+        <v>637</v>
+      </c>
+      <c r="B96" t="s">
+        <v>343</v>
+      </c>
+      <c r="C96" s="18" t="s">
+        <v>354</v>
+      </c>
+      <c r="D96" s="1" t="s">
+        <v>646</v>
+      </c>
+      <c r="E96" s="1" t="s">
+        <v>642</v>
+      </c>
+      <c r="F96" s="18" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="97" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A97" s="18" t="s">
+        <v>638</v>
+      </c>
+      <c r="B97" t="s">
+        <v>343</v>
+      </c>
+      <c r="C97" s="18" t="s">
+        <v>354</v>
+      </c>
+      <c r="D97" s="1" t="s">
+        <v>645</v>
+      </c>
+      <c r="E97" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="F97" s="18" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="98" spans="1:6" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A98" s="18" t="s">
+        <v>639</v>
+      </c>
+      <c r="B98" t="s">
+        <v>344</v>
+      </c>
+      <c r="C98" s="18" t="s">
+        <v>352</v>
+      </c>
+      <c r="D98" s="1" t="s">
+        <v>644</v>
+      </c>
+      <c r="E98" s="1" t="s">
+        <v>643</v>
+      </c>
+      <c r="F98" s="18" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="99" spans="1:6" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A99" s="18" t="s">
+        <v>641</v>
+      </c>
+      <c r="B99" t="s">
+        <v>344</v>
+      </c>
+      <c r="C99" s="18" t="s">
+        <v>352</v>
+      </c>
+      <c r="D99" s="1" t="s">
+        <v>648</v>
+      </c>
+      <c r="E99" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="F99" s="18" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="101" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A101" s="18"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -6916,14 +7320,14 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView zoomScale="150" workbookViewId="0">
-      <selection activeCell="I7" sqref="I7"/>
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="10.75" style="2"/>
     <col min="2" max="2" width="18.125" bestFit="1" customWidth="1"/>
@@ -6933,7 +7337,7 @@
     <col min="6" max="6" width="13.75" style="9" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="4" customFormat="1">
+    <row r="1" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -6953,7 +7357,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="2">
         <v>40598</v>
       </c>
@@ -6964,7 +7368,7 @@
         <v>598</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="2">
         <v>40602</v>
       </c>
@@ -6985,7 +7389,7 @@
         <v>100.61538461538461</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="2">
         <v>40611</v>
       </c>
@@ -7006,7 +7410,7 @@
         <v>124.15384615384616</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="2">
         <v>40630</v>
       </c>
@@ -7027,7 +7431,7 @@
         <v>109.5</v>
       </c>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" s="2">
         <v>40644</v>
       </c>
@@ -7048,10 +7452,25 @@
         <v>105.84615384615384</v>
       </c>
     </row>
-    <row r="7" spans="1:6">
-      <c r="F7" s="9" t="e">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A7" s="2">
+        <v>40657</v>
+      </c>
+      <c r="B7">
+        <v>0</v>
+      </c>
+      <c r="C7">
+        <v>6</v>
+      </c>
+      <c r="D7">
+        <v>2110</v>
+      </c>
+      <c r="E7">
+        <v>140</v>
+      </c>
+      <c r="F7" s="9">
         <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
+        <v>73.285714285714292</v>
       </c>
     </row>
   </sheetData>
@@ -7068,14 +7487,14 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J42"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" zoomScale="150" workbookViewId="0">
+    <sheetView topLeftCell="A31" zoomScale="150" workbookViewId="0">
       <selection activeCell="B34" sqref="B34:B42"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="8.875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="38.75" style="1" bestFit="1" customWidth="1"/>
@@ -7089,7 +7508,7 @@
     <col min="10" max="10" width="11" style="6" bestFit="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>11</v>
       </c>
@@ -7121,7 +7540,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:10">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>31</v>
       </c>
@@ -7153,7 +7572,7 @@
         <v>40600</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="25.5">
+    <row r="4" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>185</v>
       </c>
@@ -7164,7 +7583,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="25.5">
+    <row r="5" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>41</v>
       </c>
@@ -7175,7 +7594,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="6" spans="1:10" ht="25.5">
+    <row r="6" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>42</v>
       </c>
@@ -7186,7 +7605,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="7" spans="1:10" ht="25.5">
+    <row r="7" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>180</v>
       </c>
@@ -7197,7 +7616,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="9" spans="1:10">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>32</v>
       </c>
@@ -7229,7 +7648,7 @@
         <v>40601</v>
       </c>
     </row>
-    <row r="11" spans="1:10" ht="38.25">
+    <row r="11" spans="1:10" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>43</v>
       </c>
@@ -7240,7 +7659,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="12" spans="1:10" ht="38.25">
+    <row r="12" spans="1:10" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>44</v>
       </c>
@@ -7251,7 +7670,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="14" spans="1:10">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>156</v>
       </c>
@@ -7283,7 +7702,7 @@
         <v>40602</v>
       </c>
     </row>
-    <row r="15" spans="1:10">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>280</v>
       </c>
@@ -7295,7 +7714,7 @@
       </c>
       <c r="J15" s="7"/>
     </row>
-    <row r="16" spans="1:10">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>281</v>
       </c>
@@ -7306,7 +7725,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="17" spans="1:10">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>282</v>
       </c>
@@ -7317,7 +7736,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="18" spans="1:10" ht="25.5">
+    <row r="18" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>283</v>
       </c>
@@ -7329,10 +7748,10 @@
       </c>
       <c r="J18" s="7"/>
     </row>
-    <row r="19" spans="1:10">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
       <c r="J19" s="7"/>
     </row>
-    <row r="20" spans="1:10">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>75</v>
       </c>
@@ -7364,7 +7783,7 @@
         <v>40602</v>
       </c>
     </row>
-    <row r="21" spans="1:10">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>284</v>
       </c>
@@ -7376,7 +7795,7 @@
       </c>
       <c r="J21" s="7"/>
     </row>
-    <row r="22" spans="1:10">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>285</v>
       </c>
@@ -7387,7 +7806,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="23" spans="1:10">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>286</v>
       </c>
@@ -7396,10 +7815,10 @@
       </c>
       <c r="J23" s="7"/>
     </row>
-    <row r="24" spans="1:10">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.2">
       <c r="J24" s="7"/>
     </row>
-    <row r="25" spans="1:10">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>74</v>
       </c>
@@ -7431,7 +7850,7 @@
         <v>40601</v>
       </c>
     </row>
-    <row r="26" spans="1:10" ht="25.5">
+    <row r="26" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>287</v>
       </c>
@@ -7443,7 +7862,7 @@
       </c>
       <c r="J26" s="7"/>
     </row>
-    <row r="27" spans="1:10" ht="25.5">
+    <row r="27" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>288</v>
       </c>
@@ -7455,7 +7874,7 @@
       </c>
       <c r="J27" s="7"/>
     </row>
-    <row r="28" spans="1:10" ht="25.5">
+    <row r="28" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>289</v>
       </c>
@@ -7467,10 +7886,10 @@
       </c>
       <c r="J28" s="7"/>
     </row>
-    <row r="29" spans="1:10">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.2">
       <c r="J29" s="7"/>
     </row>
-    <row r="30" spans="1:10">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>76</v>
       </c>
@@ -7502,7 +7921,7 @@
         <v>40602</v>
       </c>
     </row>
-    <row r="31" spans="1:10" ht="25.5">
+    <row r="31" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>290</v>
       </c>
@@ -7514,7 +7933,7 @@
       </c>
       <c r="J31" s="7"/>
     </row>
-    <row r="32" spans="1:10" ht="25.5">
+    <row r="32" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>291</v>
       </c>
@@ -7526,49 +7945,49 @@
       </c>
       <c r="J32" s="7"/>
     </row>
-    <row r="33" spans="2:10">
+    <row r="33" spans="2:10" x14ac:dyDescent="0.2">
       <c r="J33" s="7"/>
     </row>
-    <row r="34" spans="2:10">
+    <row r="34" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B34" s="5" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="35" spans="2:10">
+    <row r="35" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B35" s="5"/>
     </row>
-    <row r="36" spans="2:10">
+    <row r="36" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B36" s="5" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="37" spans="2:10">
+    <row r="37" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B37" s="1" t="s">
         <v>299</v>
       </c>
     </row>
-    <row r="38" spans="2:10" ht="25.5">
+    <row r="38" spans="2:10" ht="25.5" x14ac:dyDescent="0.2">
       <c r="B38" s="1" t="s">
         <v>298</v>
       </c>
     </row>
-    <row r="39" spans="2:10" ht="38.25">
+    <row r="39" spans="2:10" ht="38.25" x14ac:dyDescent="0.2">
       <c r="B39" s="1" t="s">
         <v>301</v>
       </c>
       <c r="J39" s="7"/>
     </row>
-    <row r="40" spans="2:10" ht="25.5">
+    <row r="40" spans="2:10" ht="25.5" x14ac:dyDescent="0.2">
       <c r="B40" s="1" t="s">
         <v>300</v>
       </c>
     </row>
-    <row r="41" spans="2:10">
+    <row r="41" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B41" s="5" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="42" spans="2:10">
+    <row r="42" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B42" s="1" t="s">
         <v>63</v>
       </c>
@@ -7586,20 +8005,20 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J45"/>
   <sheetViews>
-    <sheetView topLeftCell="A25" zoomScale="150" workbookViewId="0">
+    <sheetView topLeftCell="A28" zoomScale="150" workbookViewId="0">
       <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="8.875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="24.125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>11</v>
       </c>
@@ -7631,7 +8050,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:10">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>77</v>
       </c>
@@ -7663,7 +8082,7 @@
         <v>40608</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="25.5">
+    <row r="4" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>315</v>
       </c>
@@ -7675,7 +8094,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="25.5">
+    <row r="5" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>316</v>
       </c>
@@ -7687,7 +8106,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="6" spans="1:10" ht="25.5">
+    <row r="6" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>317</v>
       </c>
@@ -7699,11 +8118,11 @@
         <v>128</v>
       </c>
     </row>
-    <row r="7" spans="1:10">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
     </row>
-    <row r="8" spans="1:10">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>78</v>
       </c>
@@ -7735,7 +8154,7 @@
         <v>40608</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="25.5">
+    <row r="10" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>318</v>
       </c>
@@ -7747,7 +8166,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="11" spans="1:10">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>319</v>
       </c>
@@ -7759,7 +8178,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="12" spans="1:10" ht="38.25">
+    <row r="12" spans="1:10" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>320</v>
       </c>
@@ -7771,7 +8190,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="14" spans="1:10">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>79</v>
       </c>
@@ -7803,7 +8222,7 @@
         <v>40610</v>
       </c>
     </row>
-    <row r="15" spans="1:10" ht="25.5">
+    <row r="15" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>321</v>
       </c>
@@ -7814,7 +8233,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="16" spans="1:10" ht="25.5">
+    <row r="16" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>323</v>
       </c>
@@ -7825,7 +8244,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="17" spans="1:10">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>324</v>
       </c>
@@ -7836,7 +8255,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="18" spans="1:10" ht="38.25">
+    <row r="18" spans="1:10" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>326</v>
       </c>
@@ -7848,10 +8267,10 @@
       </c>
       <c r="J18" s="16"/>
     </row>
-    <row r="19" spans="1:10">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
       <c r="J19" s="16"/>
     </row>
-    <row r="20" spans="1:10">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>80</v>
       </c>
@@ -7883,7 +8302,7 @@
         <v>40610</v>
       </c>
     </row>
-    <row r="21" spans="1:10" ht="25.5">
+    <row r="21" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>330</v>
       </c>
@@ -7894,7 +8313,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="22" spans="1:10" ht="38.25">
+    <row r="22" spans="1:10" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>331</v>
       </c>
@@ -7905,7 +8324,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="23" spans="1:10" ht="25.5">
+    <row r="23" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>333</v>
       </c>
@@ -7916,7 +8335,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="24" spans="1:10" ht="25.5">
+    <row r="24" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>335</v>
       </c>
@@ -7927,7 +8346,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="25" spans="1:10" ht="25.5">
+    <row r="25" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>337</v>
       </c>
@@ -7938,7 +8357,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="27" spans="1:10">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>81</v>
       </c>
@@ -7970,7 +8389,7 @@
         <v>40612</v>
       </c>
     </row>
-    <row r="28" spans="1:10" ht="25.5">
+    <row r="28" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>383</v>
       </c>
@@ -7979,7 +8398,7 @@
       </c>
       <c r="J28" s="16"/>
     </row>
-    <row r="29" spans="1:10" ht="38.25">
+    <row r="29" spans="1:10" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>385</v>
       </c>
@@ -7988,7 +8407,7 @@
       </c>
       <c r="J29" s="16"/>
     </row>
-    <row r="30" spans="1:10" ht="25.5">
+    <row r="30" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>387</v>
       </c>
@@ -7997,7 +8416,7 @@
       </c>
       <c r="J30" s="16"/>
     </row>
-    <row r="31" spans="1:10" ht="25.5">
+    <row r="31" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>389</v>
       </c>
@@ -8006,7 +8425,7 @@
       </c>
       <c r="J31" s="16"/>
     </row>
-    <row r="32" spans="1:10">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>82</v>
       </c>
@@ -8038,7 +8457,7 @@
         <v>40612</v>
       </c>
     </row>
-    <row r="33" spans="1:2" ht="25.5">
+    <row r="33" spans="1:2" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>391</v>
       </c>
@@ -8046,7 +8465,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="34" spans="1:2" ht="51">
+    <row r="34" spans="1:2" ht="51" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>392</v>
       </c>
@@ -8054,7 +8473,7 @@
         <v>393</v>
       </c>
     </row>
-    <row r="35" spans="1:2" ht="25.5">
+    <row r="35" spans="1:2" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>394</v>
       </c>
@@ -8062,43 +8481,43 @@
         <v>395</v>
       </c>
     </row>
-    <row r="37" spans="1:2">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B37" s="5" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="38" spans="1:2">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B38" s="5"/>
     </row>
-    <row r="39" spans="1:2">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B39" s="5" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="40" spans="1:2">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B40" s="1" t="s">
         <v>299</v>
       </c>
     </row>
-    <row r="41" spans="1:2" ht="25.5">
+    <row r="41" spans="1:2" ht="25.5" x14ac:dyDescent="0.2">
       <c r="B41" s="1" t="s">
         <v>298</v>
       </c>
     </row>
-    <row r="42" spans="1:2" ht="51">
+    <row r="42" spans="1:2" ht="51" x14ac:dyDescent="0.2">
       <c r="B42" s="1" t="s">
         <v>301</v>
       </c>
     </row>
-    <row r="43" spans="1:2">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B43" s="1"/>
     </row>
-    <row r="44" spans="1:2">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B44" s="5" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="45" spans="1:2" ht="25.5">
+    <row r="45" spans="1:2" ht="25.5" x14ac:dyDescent="0.2">
       <c r="B45" s="1" t="s">
         <v>63</v>
       </c>
@@ -8116,19 +8535,19 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J48"/>
   <sheetViews>
-    <sheetView zoomScale="150" workbookViewId="0">
+    <sheetView topLeftCell="A34" zoomScale="150" workbookViewId="0">
       <selection activeCell="B41" sqref="B41:B48"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="24.875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>3</v>
       </c>
@@ -8160,7 +8579,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:10">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" s="18" t="s">
         <v>83</v>
       </c>
@@ -8192,7 +8611,7 @@
         <v>40625</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="25.5">
+    <row r="4" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>417</v>
       </c>
@@ -8204,7 +8623,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="38.25">
+    <row r="5" spans="1:10" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>418</v>
       </c>
@@ -8216,7 +8635,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="6" spans="1:10" ht="38.25">
+    <row r="6" spans="1:10" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>419</v>
       </c>
@@ -8228,7 +8647,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="7" spans="1:10" ht="38.25">
+    <row r="7" spans="1:10" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>423</v>
       </c>
@@ -8240,7 +8659,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="8" spans="1:10" ht="25.5">
+    <row r="8" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>424</v>
       </c>
@@ -8248,7 +8667,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="9" spans="1:10" ht="51">
+    <row r="9" spans="1:10" ht="51" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>425</v>
       </c>
@@ -8260,7 +8679,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="38.25">
+    <row r="10" spans="1:10" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>427</v>
       </c>
@@ -8272,7 +8691,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="12" spans="1:10">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>84</v>
       </c>
@@ -8304,7 +8723,7 @@
         <v>40625</v>
       </c>
     </row>
-    <row r="14" spans="1:10" ht="25.5">
+    <row r="14" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>436</v>
       </c>
@@ -8316,7 +8735,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="15" spans="1:10" ht="38.25">
+    <row r="15" spans="1:10" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>437</v>
       </c>
@@ -8328,7 +8747,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="16" spans="1:10" ht="38.25">
+    <row r="16" spans="1:10" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>438</v>
       </c>
@@ -8340,11 +8759,11 @@
         <v>128</v>
       </c>
     </row>
-    <row r="17" spans="1:10">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
     </row>
-    <row r="18" spans="1:10">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>85</v>
       </c>
@@ -8376,7 +8795,7 @@
         <v>40628</v>
       </c>
     </row>
-    <row r="19" spans="1:10">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>456</v>
       </c>
@@ -8387,7 +8806,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="20" spans="1:10" ht="25.5">
+    <row r="20" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>458</v>
       </c>
@@ -8398,7 +8817,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="21" spans="1:10" ht="38.25">
+    <row r="21" spans="1:10" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>460</v>
       </c>
@@ -8409,7 +8828,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="22" spans="1:10" ht="51">
+    <row r="22" spans="1:10" ht="51" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>461</v>
       </c>
@@ -8420,7 +8839,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="23" spans="1:10" ht="25.5">
+    <row r="23" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>464</v>
       </c>
@@ -8431,10 +8850,10 @@
         <v>70</v>
       </c>
     </row>
-    <row r="24" spans="1:10">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.2">
       <c r="D24" s="18"/>
     </row>
-    <row r="25" spans="1:10">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>86</v>
       </c>
@@ -8466,7 +8885,7 @@
         <v>40628</v>
       </c>
     </row>
-    <row r="26" spans="1:10" ht="25.5">
+    <row r="26" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>466</v>
       </c>
@@ -8477,7 +8896,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="27" spans="1:10" ht="25.5">
+    <row r="27" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>467</v>
       </c>
@@ -8488,7 +8907,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="28" spans="1:10" ht="25.5">
+    <row r="28" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>468</v>
       </c>
@@ -8499,7 +8918,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="29" spans="1:10" ht="51">
+    <row r="29" spans="1:10" ht="51" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>469</v>
       </c>
@@ -8510,7 +8929,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="30" spans="1:10" ht="51">
+    <row r="30" spans="1:10" ht="51" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>472</v>
       </c>
@@ -8521,10 +8940,10 @@
         <v>70</v>
       </c>
     </row>
-    <row r="31" spans="1:10">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.2">
       <c r="D31" s="18"/>
     </row>
-    <row r="32" spans="1:10">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>87</v>
       </c>
@@ -8556,7 +8975,7 @@
         <v>40630</v>
       </c>
     </row>
-    <row r="33" spans="1:10">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>476</v>
       </c>
@@ -8564,7 +8983,7 @@
         <v>477</v>
       </c>
     </row>
-    <row r="34" spans="1:10" ht="38.25">
+    <row r="34" spans="1:10" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>478</v>
       </c>
@@ -8572,7 +8991,7 @@
         <v>479</v>
       </c>
     </row>
-    <row r="36" spans="1:10">
+    <row r="36" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>88</v>
       </c>
@@ -8604,7 +9023,7 @@
         <v>40630</v>
       </c>
     </row>
-    <row r="37" spans="1:10">
+    <row r="37" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>480</v>
       </c>
@@ -8612,7 +9031,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="38" spans="1:10">
+    <row r="38" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>482</v>
       </c>
@@ -8620,7 +9039,7 @@
         <v>459</v>
       </c>
     </row>
-    <row r="39" spans="1:10">
+    <row r="39" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>483</v>
       </c>
@@ -8628,40 +9047,40 @@
         <v>481</v>
       </c>
     </row>
-    <row r="41" spans="1:10">
+    <row r="41" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B41" s="5" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="42" spans="1:10">
+    <row r="42" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B42" s="5"/>
     </row>
-    <row r="43" spans="1:10">
+    <row r="43" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B43" s="5" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="44" spans="1:10">
+    <row r="44" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B44" s="1" t="s">
         <v>299</v>
       </c>
     </row>
-    <row r="45" spans="1:10" ht="25.5">
+    <row r="45" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
       <c r="B45" s="1" t="s">
         <v>298</v>
       </c>
     </row>
-    <row r="46" spans="1:10" ht="51">
+    <row r="46" spans="1:10" ht="51" x14ac:dyDescent="0.2">
       <c r="B46" s="1" t="s">
         <v>301</v>
       </c>
     </row>
-    <row r="47" spans="1:10">
+    <row r="47" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B47" s="5" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="48" spans="1:10" ht="25.5">
+    <row r="48" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
       <c r="B48" s="1" t="s">
         <v>63</v>
       </c>
@@ -8678,19 +9097,19 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J42"/>
   <sheetViews>
-    <sheetView topLeftCell="A17" zoomScale="150" workbookViewId="0">
+    <sheetView topLeftCell="A32" zoomScale="150" workbookViewId="0">
       <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="23.75" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>3</v>
       </c>
@@ -8722,7 +9141,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:10">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>89</v>
       </c>
@@ -8754,7 +9173,7 @@
         <v>40644</v>
       </c>
     </row>
-    <row r="3" spans="1:10">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>524</v>
       </c>
@@ -8762,7 +9181,7 @@
         <v>523</v>
       </c>
     </row>
-    <row r="4" spans="1:10">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>525</v>
       </c>
@@ -8770,7 +9189,7 @@
         <v>589</v>
       </c>
     </row>
-    <row r="5" spans="1:10">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>526</v>
       </c>
@@ -8778,7 +9197,7 @@
         <v>590</v>
       </c>
     </row>
-    <row r="7" spans="1:10">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>90</v>
       </c>
@@ -8810,7 +9229,7 @@
         <v>40638</v>
       </c>
     </row>
-    <row r="8" spans="1:10" ht="25.5">
+    <row r="8" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A8" s="18" t="s">
         <v>495</v>
       </c>
@@ -8821,7 +9240,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="9" spans="1:10" ht="25.5">
+    <row r="9" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A9" s="18" t="s">
         <v>496</v>
       </c>
@@ -8832,11 +9251,11 @@
         <v>128</v>
       </c>
     </row>
-    <row r="10" spans="1:10">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A10" s="18"/>
       <c r="B10" s="20"/>
     </row>
-    <row r="11" spans="1:10">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>91</v>
       </c>
@@ -8868,7 +9287,7 @@
         <v>40644</v>
       </c>
     </row>
-    <row r="12" spans="1:10" ht="25.5">
+    <row r="12" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A12" s="18" t="s">
         <v>548</v>
       </c>
@@ -8881,7 +9300,7 @@
       <c r="E12" s="18"/>
       <c r="J12" s="16"/>
     </row>
-    <row r="13" spans="1:10" ht="25.5">
+    <row r="13" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A13" s="18" t="s">
         <v>550</v>
       </c>
@@ -8894,7 +9313,7 @@
       <c r="E13" s="18"/>
       <c r="J13" s="16"/>
     </row>
-    <row r="14" spans="1:10" ht="63.75">
+    <row r="14" spans="1:10" ht="63.75" x14ac:dyDescent="0.2">
       <c r="A14" s="18" t="s">
         <v>552</v>
       </c>
@@ -8907,11 +9326,11 @@
       <c r="E14" s="18"/>
       <c r="J14" s="16"/>
     </row>
-    <row r="15" spans="1:10">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
       <c r="E15" s="18"/>
       <c r="J15" s="16"/>
     </row>
-    <row r="16" spans="1:10">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>92</v>
       </c>
@@ -8943,7 +9362,7 @@
         <v>40644</v>
       </c>
     </row>
-    <row r="17" spans="1:10" ht="25.5">
+    <row r="17" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A17" s="18" t="s">
         <v>554</v>
       </c>
@@ -8956,7 +9375,7 @@
       <c r="E17" s="18"/>
       <c r="J17" s="16"/>
     </row>
-    <row r="18" spans="1:10" ht="63.75">
+    <row r="18" spans="1:10" ht="63.75" x14ac:dyDescent="0.2">
       <c r="A18" s="18" t="s">
         <v>555</v>
       </c>
@@ -8969,7 +9388,7 @@
       <c r="E18" s="18"/>
       <c r="J18" s="16"/>
     </row>
-    <row r="19" spans="1:10">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A19" s="18" t="s">
         <v>557</v>
       </c>
@@ -8982,7 +9401,7 @@
       <c r="E19" s="18"/>
       <c r="J19" s="16"/>
     </row>
-    <row r="20" spans="1:10" ht="51">
+    <row r="20" spans="1:10" ht="51" x14ac:dyDescent="0.2">
       <c r="A20" s="18" t="s">
         <v>558</v>
       </c>
@@ -8995,10 +9414,10 @@
       <c r="E20" s="18"/>
       <c r="J20" s="16"/>
     </row>
-    <row r="21" spans="1:10">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B21" s="18"/>
     </row>
-    <row r="22" spans="1:10">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>93</v>
       </c>
@@ -9030,7 +9449,7 @@
         <v>40644</v>
       </c>
     </row>
-    <row r="23" spans="1:10">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>527</v>
       </c>
@@ -9038,7 +9457,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="24" spans="1:10">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>528</v>
       </c>
@@ -9046,7 +9465,7 @@
         <v>531</v>
       </c>
     </row>
-    <row r="25" spans="1:10">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>529</v>
       </c>
@@ -9054,10 +9473,10 @@
         <v>530</v>
       </c>
     </row>
-    <row r="26" spans="1:10">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B26" s="18"/>
     </row>
-    <row r="27" spans="1:10">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>94</v>
       </c>
@@ -9089,7 +9508,7 @@
         <v>40638</v>
       </c>
     </row>
-    <row r="29" spans="1:10">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A29" s="18" t="s">
         <v>513</v>
       </c>
@@ -9100,7 +9519,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="30" spans="1:10" ht="51">
+    <row r="30" spans="1:10" ht="51" x14ac:dyDescent="0.2">
       <c r="A30" s="18" t="s">
         <v>514</v>
       </c>
@@ -9111,7 +9530,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="31" spans="1:10" ht="63.75">
+    <row r="31" spans="1:10" ht="63.75" x14ac:dyDescent="0.2">
       <c r="A31" s="18" t="s">
         <v>518</v>
       </c>
@@ -9122,7 +9541,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="32" spans="1:10" ht="51">
+    <row r="32" spans="1:10" ht="51" x14ac:dyDescent="0.2">
       <c r="A32" s="18" t="s">
         <v>519</v>
       </c>
@@ -9133,7 +9552,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="33" spans="1:4" ht="51">
+    <row r="33" spans="1:4" ht="51" x14ac:dyDescent="0.2">
       <c r="A33" s="18" t="s">
         <v>521</v>
       </c>
@@ -9144,40 +9563,40 @@
         <v>128</v>
       </c>
     </row>
-    <row r="35" spans="1:4">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B35" s="5" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="36" spans="1:4">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B36" s="5"/>
     </row>
-    <row r="37" spans="1:4">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B37" s="5" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="38" spans="1:4" ht="25.5">
+    <row r="38" spans="1:4" ht="25.5" x14ac:dyDescent="0.2">
       <c r="B38" s="1" t="s">
         <v>299</v>
       </c>
     </row>
-    <row r="39" spans="1:4" ht="25.5">
+    <row r="39" spans="1:4" ht="25.5" x14ac:dyDescent="0.2">
       <c r="B39" s="1" t="s">
         <v>298</v>
       </c>
     </row>
-    <row r="40" spans="1:4" ht="51">
+    <row r="40" spans="1:4" ht="51" x14ac:dyDescent="0.2">
       <c r="B40" s="1" t="s">
         <v>301</v>
       </c>
     </row>
-    <row r="41" spans="1:4">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B41" s="5" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="42" spans="1:4" ht="25.5">
+    <row r="42" spans="1:4" ht="25.5" x14ac:dyDescent="0.2">
       <c r="B42" s="1" t="s">
         <v>63</v>
       </c>

</xml_diff>